<commit_message>
updated about page and some additional refactor
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BA8456-26B8-41AB-BC2F-EAF4A9832C58}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B0F380-B934-4279-8F09-3383B9D6C56D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7358" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="6135" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">IMAGES!$A$1:$F$82</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="0" concurrentCalc="0"/>
+  <calcPr calcId="181029" iterateDelta="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="569">
   <si>
     <t>cliff</t>
   </si>
@@ -1684,9 +1684,6 @@
     <t>IV+ &amp; f6b</t>
   </si>
   <si>
-    <t>portugal+RM10:Q10</t>
-  </si>
-  <si>
     <t xml:space="preserve">Meadinha is a dome of granite in North Portugal which makes for some brilliant pitches if you can handle the high technical grade! The route Queles is on the left side an is half trad climbing and half sport route.  The line is only 60m long, but the crag has some routes up to 200m. The other routes are either pure sport line or have challenging sport or aid sections with a little easy trad in them. Check out meadinha.com for more information if you fancy your hand at some of the more challenging parts of the cliff. </t>
   </si>
   <si>
@@ -1696,15 +1693,9 @@
     <t>https://www.allaboutportugal.pt/pt/arcos-de-valdevez/jardins/miradouro-do-penedo-da-meadinha</t>
   </si>
   <si>
-    <t>img/meadinha/meadina-topo-for-queles.jpg</t>
-  </si>
-  <si>
     <t>Topo for Queles on Meadinha in Portugal</t>
   </si>
   <si>
-    <t>img/meadinha/meadina-crag-in-north-portugal.jpg</t>
-  </si>
-  <si>
     <t>Meadinha Granite Dome in Portugal</t>
   </si>
   <si>
@@ -1726,7 +1717,31 @@
     <t>img/guidebooks/rock-climbs-in-portugal.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">A solid guidebook with clear topography that is well organised and covers bouldering, sport and trad. The book lacks detailed descriptions on the routes themselves, but this is probably a good thing for those with a string on-sight ethic. The book is not essential for climbing at Meadinha as the meadinah.com website has far more information but the book is a worthwhile purchase for someone traveling around Portugal, however the price tag feels a bit high all things considered. </t>
+    <t>Park in the nearby village of Peneda and Meadinha should be clearly visible a short walk up the hill.</t>
+  </si>
+  <si>
+    <t>FREE</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This publicly availible guidebook is so clear and comprehensive that I almost didn't bother adding Lion Rock to this website because its covered in far better detail in this guide. </t>
+  </si>
+  <si>
+    <t>img/topos/meadinha/meadina-crag-in-north-portugal.jpg</t>
+  </si>
+  <si>
+    <t>img/topos/meadinha/meadina-topo-for-queles.jpg</t>
+  </si>
+  <si>
+    <t>portugal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A solid guidebook with clear topography that is well organised and covers bouldering, sport and trad. The book lacks detailed descriptions on the routes themselves, but this is probably a good thing for those with a strong on-sight ethic. The book is not essential for climbing at Meadinha as the meadinah.com website has far more information but the book is a worthwhile purchase for someone traveling around Portugal, however the price tag feels a bit high all things considered. </t>
+  </si>
+  <si>
+    <t>img/guidebooks/rock-climbs-in-hong-kong.jpg</t>
   </si>
 </sst>
 </file>
@@ -2789,8 +2804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3398,7 +3413,7 @@
         <v>548</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>549</v>
+        <v>566</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>211</v>
@@ -3413,7 +3428,10 @@
         <v>42</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>560</v>
       </c>
       <c r="T10" s="2" t="s">
         <v>45</v>
@@ -4179,7 +4197,7 @@
   <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C75" sqref="A74:C75"/>
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6056,16 +6074,16 @@
         <v>119</v>
       </c>
       <c r="C80" t="s">
-        <v>553</v>
+        <v>565</v>
       </c>
       <c r="D80" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E80" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F80" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="2"/>
@@ -6080,13 +6098,13 @@
         <v>122</v>
       </c>
       <c r="C81" t="s">
-        <v>555</v>
+        <v>564</v>
       </c>
       <c r="D81" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E81" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="F81" t="s">
         <v>302</v>
@@ -6104,10 +6122,10 @@
         <v>114</v>
       </c>
       <c r="C82" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D82" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E82" t="s">
         <v>111</v>
@@ -6134,8 +6152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6422,10 +6440,10 @@
         <v>34</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="G10" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="I10">
         <v>34.950000000000003</v>
@@ -6754,8 +6772,36 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>399</v>
+      </c>
+      <c r="C22" t="s">
+        <v>521</v>
+      </c>
+      <c r="D22" t="s">
+        <v>562</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>563</v>
+      </c>
+      <c r="G22" t="s">
+        <v>568</v>
+      </c>
+      <c r="H22" t="s">
+        <v>541</v>
+      </c>
+      <c r="I22" t="s">
+        <v>561</v>
+      </c>
+      <c r="J22" t="s">
+        <v>561</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6768,7 +6814,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6940,10 +6986,10 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="C15" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -7299,7 +7345,7 @@
   <dimension ref="A1:V93"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="G56" sqref="A1:N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10165,8 +10211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10520,7 +10566,7 @@
       </c>
       <c r="E10">
         <f>IF(CLIMBS!S10&lt;&gt;0,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B10,"tile"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
@@ -10971,7 +11017,7 @@
       </c>
       <c r="G22">
         <f>_xlfn.IFNA(IF(VLOOKUP(B22,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <f>_xlfn.IFNA(IF(VLOOKUP(B22,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>

</xml_diff>

<commit_message>
fixed subscribe overlay style
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B0F380-B934-4279-8F09-3383B9D6C56D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C4D1BF-3554-4E52-9D3E-B967D396EC0D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="6135" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="573">
   <si>
     <t>cliff</t>
   </si>
@@ -1742,6 +1742,18 @@
   </si>
   <si>
     <t>img/guidebooks/rock-climbs-in-hong-kong.jpg</t>
+  </si>
+  <si>
+    <t>Diedro UBSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The South face of Peñón de Ifach in Costa Blanca offers a great array of climbing. Most of the routes are bolted but a small rack is more or less essential for most climbs. Diedro UBSA is one of the more popular climbs on the face and provides a long winding adventure including an 8 meter abseil at one point in order to progress the route to the top. The rock is loose in places so helmets are essential as is water due to the possible heat. </t>
+  </si>
+  <si>
+    <t>img/tiles/penon-costa-blanca.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peñón de Ifach rising out of the costline of Costa Blanca offers great climbing </t>
   </si>
 </sst>
 </file>
@@ -2804,8 +2816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4185,6 +4197,45 @@
       <c r="E23" s="2" t="s">
         <v>525</v>
       </c>
+      <c r="F23" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="G23" s="2">
+        <v>228</v>
+      </c>
+      <c r="H23" s="2">
+        <v>9</v>
+      </c>
+      <c r="I23" s="2">
+        <v>6</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="O23" s="2">
+        <v>20</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4194,10 +4245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6138,6 +6189,44 @@
         <v>9map</v>
       </c>
     </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <v>22</v>
+      </c>
+      <c r="B83" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <v>22</v>
+      </c>
+      <c r="B84" t="s">
+        <v>188</v>
+      </c>
+      <c r="C84" t="s">
+        <v>571</v>
+      </c>
+      <c r="D84" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <v>22</v>
+      </c>
+      <c r="B85" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>22</v>
+      </c>
+      <c r="B86" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F82" xr:uid="{BFB1D3BA-7B83-4CA6-BA2B-968EDE266848}"/>
   <hyperlinks>
@@ -6152,8 +6241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7344,7 +7433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745174B4-A8CA-45B8-ACCB-9B5B609F0D5D}">
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G56" sqref="A1:N61"/>
     </sheetView>
   </sheetViews>
@@ -11038,7 +11127,7 @@
       </c>
       <c r="D23">
         <f>IF(CLIMBS!R23&lt;&gt;0,1,0)+IF(CLIMBS!G23&lt;&gt;0,1,0)+IF(CLIMBS!H23&lt;&gt;0,1,0)+IF(CLIMBS!I23&lt;&gt;0,1,0)+IF(CLIMBS!J23&lt;&gt;0,1,0)+IF(CLIMBS!N23&lt;&gt;0,1,0)+IF(CLIMBS!M23&lt;&gt;0,1,0)+IF(CLIMBS!O23&lt;&gt;0,1,0)+IF(CLIMBS!P23&lt;&gt;0,1,0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E23">
         <f>IF(CLIMBS!S23&lt;&gt;0,1,0)</f>

</xml_diff>

<commit_message>
added penon de ifach in spain
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C4D1BF-3554-4E52-9D3E-B967D396EC0D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEB0D75-E6CD-4797-ABCE-C387C545AC82}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="587">
   <si>
     <t>cliff</t>
   </si>
@@ -1747,20 +1747,74 @@
     <t>Diedro UBSA</t>
   </si>
   <si>
-    <t xml:space="preserve">The South face of Peñón de Ifach in Costa Blanca offers a great array of climbing. Most of the routes are bolted but a small rack is more or less essential for most climbs. Diedro UBSA is one of the more popular climbs on the face and provides a long winding adventure including an 8 meter abseil at one point in order to progress the route to the top. The rock is loose in places so helmets are essential as is water due to the possible heat. </t>
-  </si>
-  <si>
     <t>img/tiles/penon-costa-blanca.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Peñón de Ifach rising out of the costline of Costa Blanca offers great climbing </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The South face of Peñón de Ifach in Costa Blanca offers a great array of climbing. Most of the routes are bolted but a small rack is more or less essential. Diedro UBSA is one of the more popular climbs on the face and provides a long winding adventure including an 8 meter abseil at one point in order to progress the route to the top. The rock is loose in places so remember your helmet. Pleanty of water is also recomended due to the heat you can get on the south face. </t>
+  </si>
+  <si>
+    <t>38.633896,0.074286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peñón is the obvious land mark you see from Calpe. It should also be well signposted. If you drive to the harbour you can park there and take a short walkaround the and scramble up to the start of this rout on the south face. From the summit there should be a path down through the mountain. </t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Pe%C3%B1%C3%B3n_de_Ifach,_Calpe,_Espa%C3%B1a,_2014-07-01,_DD_13.JPG</t>
+  </si>
+  <si>
+    <t>https://verticalfever.co.uk/2013/10/24/costa-blanca-round-up/</t>
+  </si>
+  <si>
+    <t>original: vertical fever</t>
+  </si>
+  <si>
+    <t>Diedro UBSA topo on the south face near Calpe</t>
+  </si>
+  <si>
+    <t>9781873341954</t>
+  </si>
+  <si>
+    <t>img/guidebooks/costa-blanca.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A brilliant book covering a wide and varied set of crags in sunny Spain. This Rockfax guide covers the climbs around Calpe including Diedre UBSA and many others. A great book for the multi-pitch climber with a penchant for trad. The old edition can be picked up cheap if you are on a budget, but the updated guide covers more routes and areas. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Peñón de Ifach is in both versions in detail. </t>
+    </r>
+  </si>
+  <si>
+    <t>img/topos/penon/penon-costa-blanca.jpg</t>
+  </si>
+  <si>
+    <t>img/topos/penon/penon-topo-for-diedre-UBSA.jpg</t>
+  </si>
+  <si>
+    <t>img/maps/penon-near-calp.png</t>
+  </si>
+  <si>
+    <t>Costa Blanca climbing location</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1916,6 +1970,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="38">
@@ -2290,7 +2350,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -2346,6 +2406,9 @@
     </xf>
     <xf numFmtId="1" fontId="20" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2814,10 +2877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4181,12 +4244,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>522</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" s="2">
         <v>22</v>
@@ -4218,6 +4281,9 @@
       <c r="M23" s="2" t="s">
         <v>221</v>
       </c>
+      <c r="N23" s="2" t="s">
+        <v>574</v>
+      </c>
       <c r="O23" s="2">
         <v>20</v>
       </c>
@@ -4228,13 +4294,24 @@
         <v>66</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>570</v>
+        <v>573</v>
+      </c>
+      <c r="S23" s="28" t="s">
+        <v>575</v>
       </c>
       <c r="T23" s="2" t="s">
         <v>245</v>
       </c>
       <c r="U23" s="2" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="S24" s="28"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" s="2" t="s">
+        <v>572</v>
       </c>
     </row>
   </sheetData>
@@ -4247,8 +4324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5681,7 +5758,7 @@
         <v>120</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" ref="H61:H82" si="2">CONCATENATE(A61,B61)</f>
+        <f t="shared" ref="H61:H86" si="2">CONCATENATE(A61,B61)</f>
         <v>17tile</v>
       </c>
     </row>
@@ -6196,6 +6273,22 @@
       <c r="B83" t="s">
         <v>122</v>
       </c>
+      <c r="C83" t="s">
+        <v>583</v>
+      </c>
+      <c r="D83" t="s">
+        <v>571</v>
+      </c>
+      <c r="E83" t="s">
+        <v>576</v>
+      </c>
+      <c r="F83" t="s">
+        <v>302</v>
+      </c>
+      <c r="H83" t="str">
+        <f t="shared" si="2"/>
+        <v>22crag</v>
+      </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A84">
@@ -6205,10 +6298,20 @@
         <v>188</v>
       </c>
       <c r="C84" t="s">
+        <v>570</v>
+      </c>
+      <c r="D84" t="s">
         <v>571</v>
       </c>
-      <c r="D84" t="s">
-        <v>572</v>
+      <c r="E84" t="s">
+        <v>576</v>
+      </c>
+      <c r="F84" t="s">
+        <v>302</v>
+      </c>
+      <c r="H84" t="str">
+        <f t="shared" si="2"/>
+        <v>22tile</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.45">
@@ -6218,6 +6321,22 @@
       <c r="B85" t="s">
         <v>119</v>
       </c>
+      <c r="C85" t="s">
+        <v>584</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="E85" t="s">
+        <v>577</v>
+      </c>
+      <c r="F85" t="s">
+        <v>578</v>
+      </c>
+      <c r="H85" t="str">
+        <f t="shared" si="2"/>
+        <v>22topo</v>
+      </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A86">
@@ -6225,6 +6344,22 @@
       </c>
       <c r="B86" t="s">
         <v>114</v>
+      </c>
+      <c r="C86" t="s">
+        <v>585</v>
+      </c>
+      <c r="D86" t="s">
+        <v>586</v>
+      </c>
+      <c r="E86" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F86" t="s">
+        <v>110</v>
+      </c>
+      <c r="H86" t="str">
+        <f t="shared" si="2"/>
+        <v>22map</v>
       </c>
     </row>
   </sheetData>
@@ -6239,10 +6374,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="F18" sqref="A1:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6890,6 +7025,35 @@
       </c>
       <c r="J22" t="s">
         <v>561</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="C23" t="s">
+        <v>525</v>
+      </c>
+      <c r="D23" t="s">
+        <v>271</v>
+      </c>
+      <c r="E23">
+        <v>267</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="G23" t="s">
+        <v>581</v>
+      </c>
+      <c r="I23">
+        <v>29.95</v>
+      </c>
+      <c r="J23">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -10301,7 +10465,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11123,26 +11287,26 @@
       </c>
       <c r="C23" t="str">
         <f>CLIMBS!B23</f>
-        <v>draft</v>
+        <v>publish</v>
       </c>
       <c r="D23">
         <f>IF(CLIMBS!R23&lt;&gt;0,1,0)+IF(CLIMBS!G23&lt;&gt;0,1,0)+IF(CLIMBS!H23&lt;&gt;0,1,0)+IF(CLIMBS!I23&lt;&gt;0,1,0)+IF(CLIMBS!J23&lt;&gt;0,1,0)+IF(CLIMBS!N23&lt;&gt;0,1,0)+IF(CLIMBS!M23&lt;&gt;0,1,0)+IF(CLIMBS!O23&lt;&gt;0,1,0)+IF(CLIMBS!P23&lt;&gt;0,1,0)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E23">
         <f>IF(CLIMBS!S23&lt;&gt;0,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F23" t="str">
+        <v>1</v>
+      </c>
+      <c r="F23">
         <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B23,"tile"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B23,"crag"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B23,"topo"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B23,"map"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
-        <v>missing</v>
+        <v>4</v>
       </c>
       <c r="G23">
         <f>_xlfn.IFNA(IF(VLOOKUP(B23,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <f>_xlfn.IFNA(IF(VLOOKUP(B23,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>

</xml_diff>

<commit_message>
fixed a image path
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDDD002-0218-4ED2-AE99-956621A93775}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30A722F-A5E7-4B2C-BC0F-D427776BBC84}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -1870,13 +1870,13 @@
     <t>img/topos/meteor/holy-ghost-crag-pillar-of-dreams-topo.jpg</t>
   </si>
   <si>
-    <t>img/maps/meteor-climbing</t>
-  </si>
-  <si>
     <t>Location of Meteor climbing in Greece</t>
   </si>
   <si>
     <t>Arguably one of the best sea stacks in the United Kingdom, The Old Man of Stoer (Stake), makes for an adventurous day out and an all round exceptional climb. The rock is Torridonian sandstone, meaning it was formed before any significant life on earth existed. The approach is either some wet rock hopping 100m north of the stack at the lowest tide or the more classic Tyrolean traverse which needs to be set up by swimming the 8 meter channel if there is not one left in place when you arrive. The route itself, Original Route, meanders the landward face. Larger cams and hexs are recommended. Be wary of nesting seagulls who first line of defence is usually to attack you with projectile vomit.</t>
+  </si>
+  <si>
+    <t>img/maps/meteor-climbing.png</t>
   </si>
 </sst>
 </file>
@@ -2939,7 +2939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
@@ -3079,7 +3079,7 @@
         <v>29</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>30</v>
@@ -4446,8 +4446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6564,10 +6564,10 @@
         <v>113</v>
       </c>
       <c r="C90" t="s">
+        <v>605</v>
+      </c>
+      <c r="D90" t="s">
         <v>603</v>
-      </c>
-      <c r="D90" t="s">
-        <v>604</v>
       </c>
       <c r="E90" s="12" t="s">
         <v>110</v>

</xml_diff>

<commit_message>
Warn IE users the site won't workfor their browser
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30A722F-A5E7-4B2C-BC0F-D427776BBC84}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B698068-6BAA-4905-A301-2C9B572A3E7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -4446,8 +4446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6592,10 +6592,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="A1:J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7272,6 +7272,11 @@
       </c>
       <c r="J23">
         <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" s="4">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -11560,7 +11565,7 @@
       </c>
       <c r="G24">
         <f>_xlfn.IFNA(IF(VLOOKUP(B24,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <f>_xlfn.IFNA(IF(VLOOKUP(B24,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>

</xml_diff>

<commit_message>
added google search console verification tag
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B698068-6BAA-4905-A301-2C9B572A3E7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB744558-FBCD-46E3-89FC-2704CD82B62B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="610">
   <si>
     <t>cliff</t>
   </si>
@@ -1877,6 +1877,18 @@
   </si>
   <si>
     <t>img/maps/meteor-climbing.png</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2UxZN8z</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2C1KKgp</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2RJohKd</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2zQOEY3</t>
   </si>
 </sst>
 </file>
@@ -6595,7 +6607,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6664,6 +6676,9 @@
       <c r="G2" t="s">
         <v>309</v>
       </c>
+      <c r="H2" t="s">
+        <v>606</v>
+      </c>
       <c r="I2">
         <v>24.99</v>
       </c>
@@ -6693,6 +6708,9 @@
       <c r="G3" t="s">
         <v>314</v>
       </c>
+      <c r="H3" t="s">
+        <v>607</v>
+      </c>
       <c r="I3">
         <v>25</v>
       </c>
@@ -6722,6 +6740,9 @@
       <c r="G4" t="s">
         <v>318</v>
       </c>
+      <c r="H4" s="13" t="s">
+        <v>608</v>
+      </c>
       <c r="I4">
         <v>24.99</v>
       </c>
@@ -6768,6 +6789,9 @@
       <c r="G6" t="s">
         <v>341</v>
       </c>
+      <c r="H6" t="s">
+        <v>609</v>
+      </c>
       <c r="I6">
         <v>20</v>
       </c>
@@ -6829,6 +6853,9 @@
       <c r="G8" t="s">
         <v>318</v>
       </c>
+      <c r="H8" s="13" t="s">
+        <v>608</v>
+      </c>
       <c r="I8">
         <v>24.99</v>
       </c>
@@ -6858,6 +6885,9 @@
       <c r="G9" t="s">
         <v>309</v>
       </c>
+      <c r="H9" t="s">
+        <v>606</v>
+      </c>
       <c r="I9">
         <v>24.99</v>
       </c>
@@ -6916,6 +6946,9 @@
       <c r="G11" t="s">
         <v>309</v>
       </c>
+      <c r="H11" t="s">
+        <v>606</v>
+      </c>
       <c r="I11">
         <v>24.99</v>
       </c>
@@ -6945,6 +6978,9 @@
       <c r="G12" t="s">
         <v>341</v>
       </c>
+      <c r="H12" t="s">
+        <v>609</v>
+      </c>
       <c r="I12">
         <v>20</v>
       </c>
@@ -6974,6 +7010,9 @@
       <c r="G13" t="s">
         <v>318</v>
       </c>
+      <c r="H13" s="13" t="s">
+        <v>608</v>
+      </c>
       <c r="I13">
         <v>24.99</v>
       </c>
@@ -7032,6 +7071,9 @@
       <c r="G15" t="s">
         <v>309</v>
       </c>
+      <c r="H15" t="s">
+        <v>606</v>
+      </c>
       <c r="I15">
         <v>24.99</v>
       </c>
@@ -7280,8 +7322,13 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{14007672-E4E3-4A8F-8DD0-45E59BDCCEDC}"/>
+    <hyperlink ref="H8" r:id="rId2" xr:uid="{B67B1897-7EEF-4BFD-B837-658E489AF517}"/>
+    <hyperlink ref="H13" r:id="rId3" xr:uid="{6357674A-8282-416E-BCEF-A2B394B14AEA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ga tracking value needs to be an int not a string
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB744558-FBCD-46E3-89FC-2704CD82B62B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859F3355-ADA4-489D-BFB4-3CB833A8D0B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6607,7 +6607,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7317,9 +7317,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A24" s="4">
-        <v>23</v>
-      </c>
+      <c r="A24" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -11612,7 +11610,7 @@
       </c>
       <c r="G24">
         <f>_xlfn.IFNA(IF(VLOOKUP(B24,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <f>_xlfn.IFNA(IF(VLOOKUP(B24,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>

</xml_diff>

<commit_message>
fixed nav height on mobile and other code style fixes
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859F3355-ADA4-489D-BFB4-3CB833A8D0B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BD8E86-4F5A-45D8-A131-78C3D15BD35D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="618">
   <si>
     <t>cliff</t>
   </si>
@@ -1676,9 +1676,6 @@
   </si>
   <si>
     <t>Região do Norte</t>
-  </si>
-  <si>
-    <t>IV+ &amp; f6b</t>
   </si>
   <si>
     <t xml:space="preserve">Meadinha is a dome of granite in North Portugal which makes for some brilliant pitches if you can handle the high technical grade! The route Queles is on the left side an is half trad climbing and half sport route.  The line is only 60m long, but the crag has some routes up to 200m. The other routes are either pure sport line or have challenging sport or aid sections with a little easy trad in them. Check out meadinha.com for more information if you fancy your hand at some of the more challenging parts of the cliff. </t>
@@ -1889,6 +1886,33 @@
   </si>
   <si>
     <t>https://amzn.to/2zQOEY3</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Aiguille Dibona</t>
+  </si>
+  <si>
+    <t>Hautes-Alpes</t>
+  </si>
+  <si>
+    <t>TD (f6a+)</t>
+  </si>
+  <si>
+    <t>IV+ &amp; (f6b)</t>
+  </si>
+  <si>
+    <t>france</t>
+  </si>
+  <si>
+    <t>Visite Obligatoire</t>
+  </si>
+  <si>
+    <t>44.961162,6.243941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The picturesque peak of Aiguille Dibona was re-named (formerly: Pain de Sucre du Soreiller) after Italian mountaineer Angelo Dibona after the first accent in 1913 with Guido Mayer. The route Visite Obligatoire or Obligatory Visit in English wasn’t climbed until 1988. This is a long, sustained route has mixed bolted and traditional protection. The peak finishes at an altitude just over 3,000m. Although the bottom half contains the technically hardest moves, the route doesn’t let up much. Its graded f6a+. Escape is much harder after the 8th pitch. </t>
   </si>
 </sst>
 </file>
@@ -2951,8 +2975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3091,7 +3115,7 @@
         <v>29</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>30</v>
@@ -3557,10 +3581,10 @@
         <v>61</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>547</v>
+        <v>613</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>210</v>
@@ -3575,10 +3599,10 @@
         <v>41</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="T10" s="2" t="s">
         <v>44</v>
@@ -4333,7 +4357,7 @@
         <v>524</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G23" s="2">
         <v>228</v>
@@ -4354,7 +4378,7 @@
         <v>220</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="O23" s="2">
         <v>20</v>
@@ -4366,10 +4390,10 @@
         <v>65</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="T23" s="2" t="s">
         <v>244</v>
@@ -4380,7 +4404,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>107</v>
@@ -4389,13 +4413,13 @@
         <v>23</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G24" s="2">
         <v>250</v>
@@ -4413,13 +4437,13 @@
         <v>26</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="O24" s="2">
         <v>21</v>
@@ -4431,10 +4455,10 @@
         <v>223</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="T24" s="2" t="s">
         <v>244</v>
@@ -4443,9 +4467,68 @@
         <v>345</v>
       </c>
     </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="2">
+        <v>24</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="G25" s="2">
+        <v>350</v>
+      </c>
+      <c r="H25" s="2">
+        <v>13</v>
+      </c>
+      <c r="I25" s="2">
+        <v>7</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="O25" s="2">
+        <v>190</v>
+      </c>
+      <c r="P25" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -6336,16 +6419,16 @@
         <v>118</v>
       </c>
       <c r="C80" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D80" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E80" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F80" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="2"/>
@@ -6360,13 +6443,13 @@
         <v>121</v>
       </c>
       <c r="C81" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D81" t="s">
+        <v>551</v>
+      </c>
+      <c r="E81" t="s">
         <v>552</v>
-      </c>
-      <c r="E81" t="s">
-        <v>553</v>
       </c>
       <c r="F81" t="s">
         <v>301</v>
@@ -6384,10 +6467,10 @@
         <v>113</v>
       </c>
       <c r="C82" t="s">
+        <v>553</v>
+      </c>
+      <c r="D82" t="s">
         <v>554</v>
-      </c>
-      <c r="D82" t="s">
-        <v>555</v>
       </c>
       <c r="E82" t="s">
         <v>110</v>
@@ -6408,13 +6491,13 @@
         <v>121</v>
       </c>
       <c r="C83" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D83" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E83" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F83" t="s">
         <v>301</v>
@@ -6432,13 +6515,13 @@
         <v>187</v>
       </c>
       <c r="C84" t="s">
+        <v>568</v>
+      </c>
+      <c r="D84" t="s">
         <v>569</v>
       </c>
-      <c r="D84" t="s">
-        <v>570</v>
-      </c>
       <c r="E84" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F84" t="s">
         <v>301</v>
@@ -6456,16 +6539,16 @@
         <v>118</v>
       </c>
       <c r="C85" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E85" t="s">
+        <v>575</v>
+      </c>
+      <c r="F85" t="s">
         <v>576</v>
-      </c>
-      <c r="F85" t="s">
-        <v>577</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="2"/>
@@ -6480,10 +6563,10 @@
         <v>113</v>
       </c>
       <c r="C86" t="s">
+        <v>583</v>
+      </c>
+      <c r="D86" t="s">
         <v>584</v>
-      </c>
-      <c r="D86" t="s">
-        <v>585</v>
       </c>
       <c r="E86" s="12" t="s">
         <v>110</v>
@@ -6504,16 +6587,16 @@
         <v>121</v>
       </c>
       <c r="C87" t="s">
+        <v>594</v>
+      </c>
+      <c r="D87" t="s">
         <v>595</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>596</v>
       </c>
-      <c r="E87" t="s">
+      <c r="F87" t="s">
         <v>597</v>
-      </c>
-      <c r="F87" t="s">
-        <v>598</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="2"/>
@@ -6528,13 +6611,13 @@
         <v>187</v>
       </c>
       <c r="C88" t="s">
+        <v>598</v>
+      </c>
+      <c r="D88" t="s">
+        <v>595</v>
+      </c>
+      <c r="E88" t="s">
         <v>599</v>
-      </c>
-      <c r="D88" t="s">
-        <v>596</v>
-      </c>
-      <c r="E88" t="s">
-        <v>600</v>
       </c>
       <c r="F88" t="s">
         <v>119</v>
@@ -6552,16 +6635,16 @@
         <v>118</v>
       </c>
       <c r="C89" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D89" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E89" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F89" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="2"/>
@@ -6576,10 +6659,10 @@
         <v>113</v>
       </c>
       <c r="C90" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D90" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E90" s="12" t="s">
         <v>110</v>
@@ -6606,7 +6689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -6677,7 +6760,7 @@
         <v>309</v>
       </c>
       <c r="H2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I2">
         <v>24.99</v>
@@ -6709,7 +6792,7 @@
         <v>314</v>
       </c>
       <c r="H3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I3">
         <v>25</v>
@@ -6741,7 +6824,7 @@
         <v>318</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I4">
         <v>24.99</v>
@@ -6790,7 +6873,7 @@
         <v>341</v>
       </c>
       <c r="H6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I6">
         <v>20</v>
@@ -6854,7 +6937,7 @@
         <v>318</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I8">
         <v>24.99</v>
@@ -6886,7 +6969,7 @@
         <v>309</v>
       </c>
       <c r="H9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I9">
         <v>24.99</v>
@@ -6912,10 +6995,10 @@
         <v>34</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G10" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I10">
         <v>34.950000000000003</v>
@@ -6947,7 +7030,7 @@
         <v>309</v>
       </c>
       <c r="H11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I11">
         <v>24.99</v>
@@ -6979,7 +7062,7 @@
         <v>341</v>
       </c>
       <c r="H12" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I12">
         <v>20</v>
@@ -7011,7 +7094,7 @@
         <v>318</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I13">
         <v>24.99</v>
@@ -7072,7 +7155,7 @@
         <v>309</v>
       </c>
       <c r="H15" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I15">
         <v>24.99</v>
@@ -7266,25 +7349,25 @@
         <v>520</v>
       </c>
       <c r="D22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E22">
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G22" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H22" t="s">
         <v>540</v>
       </c>
       <c r="I22" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J22" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
@@ -7292,7 +7375,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C23" t="s">
         <v>524</v>
@@ -7304,10 +7387,10 @@
         <v>267</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G23" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I23">
         <v>29.95</v>
@@ -7507,10 +7590,10 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
+        <v>555</v>
+      </c>
+      <c r="C15" t="s">
         <v>556</v>
-      </c>
-      <c r="C15" t="s">
-        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -10730,10 +10813,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11617,8 +11700,44 @@
         <v>0</v>
       </c>
     </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" t="str">
+        <f>CLIMBS!A25</f>
+        <v>Aiguille Dibona</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="str">
+        <f>CLIMBS!B25</f>
+        <v>draft</v>
+      </c>
+      <c r="D25">
+        <f>IF(CLIMBS!R25&lt;&gt;0,1,0)+IF(CLIMBS!G25&lt;&gt;0,1,0)+IF(CLIMBS!H25&lt;&gt;0,1,0)+IF(CLIMBS!I25&lt;&gt;0,1,0)+IF(CLIMBS!J25&lt;&gt;0,1,0)+IF(CLIMBS!N25&lt;&gt;0,1,0)+IF(CLIMBS!M25&lt;&gt;0,1,0)+IF(CLIMBS!O25&lt;&gt;0,1,0)+IF(CLIMBS!P25&lt;&gt;0,1,0)</f>
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <f>IF(CLIMBS!S25&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" t="str">
+        <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B25,"tile"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B25,"crag"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B25,"topo"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B25,"map"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
+        <v>missing</v>
+      </c>
+      <c r="G25">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B25,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B25,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
@@ -11626,7 +11745,7 @@
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C24">
+  <conditionalFormatting sqref="C2:C25">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"draft"</formula>
     </cfRule>
@@ -11636,12 +11755,12 @@
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C24">
+  <conditionalFormatting sqref="C3:C25">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E24">
+  <conditionalFormatting sqref="E2:E25">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -11649,7 +11768,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F24">
+  <conditionalFormatting sqref="F2:F25">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>4</formula>
     </cfRule>
@@ -11657,7 +11776,7 @@
       <formula>"missing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H24">
+  <conditionalFormatting sqref="G2:H25">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
adding the excel. Git -p wasn't doing it
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BD8E86-4F5A-45D8-A131-78C3D15BD35D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD97F11-9F02-4C41-B099-BBD7C293B55E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="671">
   <si>
     <t>cliff</t>
   </si>
@@ -1912,14 +1912,196 @@
     <t>44.961162,6.243941</t>
   </si>
   <si>
-    <t xml:space="preserve">The picturesque peak of Aiguille Dibona was re-named (formerly: Pain de Sucre du Soreiller) after Italian mountaineer Angelo Dibona after the first accent in 1913 with Guido Mayer. The route Visite Obligatoire or Obligatory Visit in English wasn’t climbed until 1988. This is a long, sustained route has mixed bolted and traditional protection. The peak finishes at an altitude just over 3,000m. Although the bottom half contains the technically hardest moves, the route doesn’t let up much. Its graded f6a+. Escape is much harder after the 8th pitch. </t>
+    <t>https://www.camptocamp.org/images/304934/fr/aiguille-dibona</t>
+  </si>
+  <si>
+    <t>original: RémiB</t>
+  </si>
+  <si>
+    <t>http://clive.rocks/aiguille-dibona/</t>
+  </si>
+  <si>
+    <t>img: Clive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aiguille Dibona in the Haute-Alps </t>
+  </si>
+  <si>
+    <t>The Obligatory Climb on Aiguille Dibona</t>
+  </si>
+  <si>
+    <t>img/topos/aiguille-dibona/aiguille-debona-visite-obligatoire.jpg</t>
+  </si>
+  <si>
+    <t>img/topos/aiguille-dibona/aiguille-debona.jpg</t>
+  </si>
+  <si>
+    <t>img/tiles/aiguille-debona.jpg</t>
+  </si>
+  <si>
+    <t>The picturesque peak of Aiguille Dibona was re-named (formerly: Pain de Sucre du Soreiller) after Italian mountaineer Angelo Dibona after the first accent in 1913 with Guido Mayer. The route Visite Obligatoire or Obligatory Visit in English wasn’t climbed until 1988. This is a long, sustained route that is reasonably well bolted but will require a trad rack of nuts and cams to supplement. The peak finishes at an altitude just over 3,000m. Although the bottom half contains the technically hardest moves, the route doesn’t let up much. Its graded f6a+ with an alpine grade of TD (très difficile) . Escape is much harder after the 8th pitch so make sure you consider this before pressing on.</t>
+  </si>
+  <si>
+    <t>Approach: Allow a few hours for the approach which can be made from Les Etages. There is mountain hut at the base of the mountain, Ref du Soreiller.
+Decent: This is done via a couple of assails off the back followed by a climbers path off the back of the mountain that weaves around to the front bringing climbers back to the hut.</t>
+  </si>
+  <si>
+    <t>img/maps/aiguille-debona.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aiguille Dibona location in the Haute-Alps </t>
+  </si>
+  <si>
+    <t>https://amzn.to/2QTmPrH</t>
+  </si>
+  <si>
+    <t>img/guidebooks/plaisir-selection.jpg</t>
+  </si>
+  <si>
+    <t>9783906087405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plaisir Selection </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want to recommend this guidebook but I just can’t. In some ways it’s brilliant, the hand drawn topos are very artistic, the book has 3 languages and it takes the approach of highlighting the best climbs on the cliff, much like the approach we have taken on multi-pitch.com. Sadly, a lot of the photography is poor to terrible. The “action” shots are from the belay to the leader or second, so give little in the way of inspiration and many of the mountain images are blurry silhouettes.  In addition, the images of the mountains are often just a third of the page. In this pocket-sized book, it means a 400m climb could be reduced to the size of your thumbnail. The final issue is the price which seem to be around £40. </t>
+  </si>
+  <si>
+    <t>https://soreiller.com/en/home/</t>
+  </si>
+  <si>
+    <t>Soreiller Refuge - Mountain Hut Info</t>
+  </si>
+  <si>
+    <t>Rock Climbing Europe</t>
+  </si>
+  <si>
+    <t>An old book presumably aimed at American climbers, however its truly brilliant can be picked up cheap. Described as the authoritative guide to the best climbing destinations in Western Europe, including Great Britain, France, Belgium, Spain, Italy, Switzerland, Greece, Germany, and Norway. The route topos are although black and white are accompanied by good route descriptions, equipment recommendations, and accurate route ratings. The book contains a good mixture of Trad and sport across single and multi-pitch climbs. Its basically a thick A4 book thou so not practical to take to the cliff. Highly recommended.</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2BwCB2b</t>
+  </si>
+  <si>
+    <t>img/guidebooks/rock-climbing-europe.jpg</t>
+  </si>
+  <si>
+    <t>9780762727179</t>
+  </si>
+  <si>
+    <t>https://www.needlesports.com/54396/products/portugal--rock-climbs-on-the-western-tip-of-europe.aspx</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2EmsTCn</t>
+  </si>
+  <si>
+    <t>https://www.needlesports.com/33708/products/montserrat-free-climbs.aspx</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2S4G1A6</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2Bp4EjV</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2Ep6xjN</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2BkLsnn</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2SKowVu</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2Emt6Wb</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>47.116966,8.985149</t>
+  </si>
+  <si>
+    <r>
+      <t>Br</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ü</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ggler</t>
+    </r>
+  </si>
+  <si>
+    <t>Direkte Plattenwand</t>
+  </si>
+  <si>
+    <t>Canton of Glarus</t>
+  </si>
+  <si>
+    <t>f5a</t>
+  </si>
+  <si>
+    <t>switzerland</t>
+  </si>
+  <si>
+    <t>img/topos/bruggler/bruggler-crag-switzerland.jpg</t>
+  </si>
+  <si>
+    <t>Bruggler offers great Rock Climbing</t>
+  </si>
+  <si>
+    <t>https://www.camptocamp.org/waypoints/42475/fr/brueggler</t>
+  </si>
+  <si>
+    <t>img: Camp To Crag</t>
+  </si>
+  <si>
+    <t>img/tiles/bruggler-crag-switzerland.jpg</t>
+  </si>
+  <si>
+    <t>img/maps/bruggler.png</t>
+  </si>
+  <si>
+    <t>Briggler is a great climbing location</t>
+  </si>
+  <si>
+    <t>img/topos/bruggler/bruggler-direct-route-topo.jpg</t>
+  </si>
+  <si>
+    <t>The Direct Route up Bruggler</t>
+  </si>
+  <si>
+    <t>http://blog.buschnick.net/2013/06/climbing-bruggler-hiking-speer-1950m.html</t>
+  </si>
+  <si>
+    <t>Original: Soren</t>
+  </si>
+  <si>
+    <t>Direkte Plattenwand, is one of the easier, more popular routes up the middle of Bruggler crag. The route is bolted but requires a small trad rack to ease some of the run out sections. There are many routes on this face, some can be climbed clean. Although it’s a big face with lots of options, expect some crowds. Be wary of rockfall from other parties of climbers and be careful not to dislodge rocks from the pitted limestone route.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approach: The route is best approached from Stattboden.
+Decent. Carefully move along the summit to the cross  on the left after the final pitch. From there a path can be followed to walk off the cliff. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2075,6 +2257,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="38">
@@ -2449,7 +2637,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -2506,6 +2694,7 @@
     <xf numFmtId="1" fontId="20" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2975,8 +3164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView topLeftCell="G18" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4472,7 +4661,7 @@
         <v>610</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" s="2">
         <v>24</v>
@@ -4520,9 +4709,80 @@
         <v>41</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>617</v>
+        <v>626</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="U25" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="2">
+        <v>25</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="G26" s="2">
+        <v>230</v>
+      </c>
+      <c r="H26" s="2">
+        <v>8</v>
+      </c>
+      <c r="I26" s="2">
+        <v>5</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="O26" s="2">
+        <v>70</v>
+      </c>
+      <c r="P26" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="U26" s="2" t="s">
         <v>201</v>
       </c>
     </row>
@@ -4539,10 +4799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5975,7 +6235,7 @@
         <v>119</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" ref="H61:H90" si="2">CONCATENATE(A61,B61)</f>
+        <f t="shared" ref="H61:H95" si="2">CONCATENATE(A61,B61)</f>
         <v>17tile</v>
       </c>
     </row>
@@ -6673,6 +6933,186 @@
       <c r="H90" t="str">
         <f t="shared" si="2"/>
         <v>23map</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A91">
+        <v>24</v>
+      </c>
+      <c r="B91" t="s">
+        <v>118</v>
+      </c>
+      <c r="C91" t="s">
+        <v>623</v>
+      </c>
+      <c r="D91" t="s">
+        <v>622</v>
+      </c>
+      <c r="E91" s="28" t="s">
+        <v>617</v>
+      </c>
+      <c r="F91" t="s">
+        <v>618</v>
+      </c>
+      <c r="H91" t="str">
+        <f t="shared" si="2"/>
+        <v>24topo</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <v>24</v>
+      </c>
+      <c r="B92" t="s">
+        <v>121</v>
+      </c>
+      <c r="C92" t="s">
+        <v>624</v>
+      </c>
+      <c r="D92" t="s">
+        <v>621</v>
+      </c>
+      <c r="E92" t="s">
+        <v>619</v>
+      </c>
+      <c r="F92" t="s">
+        <v>620</v>
+      </c>
+      <c r="H92" t="str">
+        <f t="shared" si="2"/>
+        <v>24crag</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A93">
+        <v>24</v>
+      </c>
+      <c r="B93" t="s">
+        <v>187</v>
+      </c>
+      <c r="C93" t="s">
+        <v>625</v>
+      </c>
+      <c r="D93" t="s">
+        <v>621</v>
+      </c>
+      <c r="E93" s="28" t="s">
+        <v>617</v>
+      </c>
+      <c r="F93" t="s">
+        <v>618</v>
+      </c>
+      <c r="H93" t="str">
+        <f t="shared" si="2"/>
+        <v>24tile</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A94">
+        <v>24</v>
+      </c>
+      <c r="B94" t="s">
+        <v>113</v>
+      </c>
+      <c r="C94" t="s">
+        <v>628</v>
+      </c>
+      <c r="D94" t="s">
+        <v>629</v>
+      </c>
+      <c r="E94" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F94" t="s">
+        <v>109</v>
+      </c>
+      <c r="H94" t="str">
+        <f t="shared" si="2"/>
+        <v>24map</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>25</v>
+      </c>
+      <c r="B95" t="s">
+        <v>121</v>
+      </c>
+      <c r="C95" t="s">
+        <v>658</v>
+      </c>
+      <c r="D95" t="s">
+        <v>659</v>
+      </c>
+      <c r="E95" t="s">
+        <v>660</v>
+      </c>
+      <c r="F95" t="s">
+        <v>661</v>
+      </c>
+      <c r="H95" t="str">
+        <f t="shared" si="2"/>
+        <v>25crag</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A96">
+        <v>25</v>
+      </c>
+      <c r="B96" t="s">
+        <v>187</v>
+      </c>
+      <c r="C96" t="s">
+        <v>662</v>
+      </c>
+      <c r="D96" t="s">
+        <v>659</v>
+      </c>
+      <c r="E96" t="s">
+        <v>660</v>
+      </c>
+      <c r="F96" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A97">
+        <v>25</v>
+      </c>
+      <c r="B97" t="s">
+        <v>113</v>
+      </c>
+      <c r="C97" t="s">
+        <v>663</v>
+      </c>
+      <c r="D97" t="s">
+        <v>664</v>
+      </c>
+      <c r="E97" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F97" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A98">
+        <v>25</v>
+      </c>
+      <c r="B98" t="s">
+        <v>118</v>
+      </c>
+      <c r="C98" t="s">
+        <v>665</v>
+      </c>
+      <c r="D98" t="s">
+        <v>666</v>
+      </c>
+      <c r="E98" t="s">
+        <v>667</v>
+      </c>
+      <c r="F98" t="s">
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -6687,10 +7127,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7000,6 +7440,9 @@
       <c r="G10" t="s">
         <v>557</v>
       </c>
+      <c r="H10" t="s">
+        <v>642</v>
+      </c>
       <c r="I10">
         <v>34.950000000000003</v>
       </c>
@@ -7125,6 +7568,9 @@
       <c r="G14" t="s">
         <v>387</v>
       </c>
+      <c r="H14" t="s">
+        <v>643</v>
+      </c>
       <c r="I14">
         <v>25</v>
       </c>
@@ -7186,6 +7632,9 @@
       <c r="G16" t="s">
         <v>397</v>
       </c>
+      <c r="H16" t="s">
+        <v>644</v>
+      </c>
       <c r="I16">
         <v>34</v>
       </c>
@@ -7215,6 +7664,9 @@
       <c r="G17" t="s">
         <v>412</v>
       </c>
+      <c r="H17" t="s">
+        <v>645</v>
+      </c>
       <c r="I17">
         <v>34.99</v>
       </c>
@@ -7244,6 +7696,9 @@
       <c r="G18" t="s">
         <v>462</v>
       </c>
+      <c r="H18" t="s">
+        <v>646</v>
+      </c>
       <c r="I18">
         <v>25</v>
       </c>
@@ -7273,6 +7728,9 @@
       <c r="G19" t="s">
         <v>466</v>
       </c>
+      <c r="H19" t="s">
+        <v>647</v>
+      </c>
       <c r="I19">
         <v>20</v>
       </c>
@@ -7302,6 +7760,9 @@
       <c r="G20" t="s">
         <v>514</v>
       </c>
+      <c r="H20" t="s">
+        <v>648</v>
+      </c>
       <c r="I20">
         <v>34.99</v>
       </c>
@@ -7331,6 +7792,9 @@
       <c r="G21" t="s">
         <v>515</v>
       </c>
+      <c r="H21" t="s">
+        <v>649</v>
+      </c>
       <c r="I21">
         <v>19.95</v>
       </c>
@@ -7392,6 +7856,9 @@
       <c r="G23" t="s">
         <v>579</v>
       </c>
+      <c r="H23" t="s">
+        <v>650</v>
+      </c>
       <c r="I23">
         <v>29.95</v>
       </c>
@@ -7400,7 +7867,100 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A24" s="4"/>
+      <c r="A24" s="4">
+        <v>24</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="C24" t="s">
+        <v>633</v>
+      </c>
+      <c r="D24" t="s">
+        <v>270</v>
+      </c>
+      <c r="E24">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
+        <v>634</v>
+      </c>
+      <c r="G24" t="s">
+        <v>631</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>630</v>
+      </c>
+      <c r="I24">
+        <v>38</v>
+      </c>
+      <c r="J24">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="C25" t="s">
+        <v>637</v>
+      </c>
+      <c r="D25" t="s">
+        <v>270</v>
+      </c>
+      <c r="E25">
+        <v>410</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="G25" t="s">
+        <v>640</v>
+      </c>
+      <c r="H25" t="s">
+        <v>639</v>
+      </c>
+      <c r="I25">
+        <v>10</v>
+      </c>
+      <c r="J25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="C26" t="s">
+        <v>633</v>
+      </c>
+      <c r="D26" t="s">
+        <v>270</v>
+      </c>
+      <c r="E26">
+        <v>300</v>
+      </c>
+      <c r="F26" t="s">
+        <v>634</v>
+      </c>
+      <c r="G26" t="s">
+        <v>631</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>630</v>
+      </c>
+      <c r="I26">
+        <v>38</v>
+      </c>
+      <c r="J26">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7415,10 +7975,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7594,6 +8154,17 @@
       </c>
       <c r="C15" t="s">
         <v>556</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>635</v>
+      </c>
+      <c r="C16" t="s">
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -7948,8 +8519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745174B4-A8CA-45B8-ACCB-9B5B609F0D5D}">
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G56" sqref="A1:N61"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10740,42 +11311,426 @@
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A62" s="15">
+        <v>24</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="C62" s="15">
+        <v>6</v>
+      </c>
+      <c r="D62" s="15">
+        <v>5</v>
+      </c>
+      <c r="E62" s="15">
+        <v>5</v>
+      </c>
+      <c r="F62" s="15">
+        <v>7</v>
+      </c>
+      <c r="G62" s="15">
+        <v>5</v>
+      </c>
+      <c r="H62" s="15">
+        <v>4</v>
+      </c>
+      <c r="I62" s="15">
+        <v>2</v>
+      </c>
+      <c r="J62" s="15">
+        <v>2</v>
+      </c>
+      <c r="K62" s="15">
+        <v>4</v>
+      </c>
+      <c r="L62" s="15">
+        <v>7</v>
+      </c>
+      <c r="M62" s="15">
+        <v>6</v>
+      </c>
+      <c r="N62" s="15">
+        <v>6</v>
+      </c>
       <c r="U62" s="8"/>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A63" s="14">
+        <v>24</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C63" s="14">
+        <v>1</v>
+      </c>
+      <c r="D63" s="14">
+        <v>2</v>
+      </c>
+      <c r="E63" s="14">
+        <v>7</v>
+      </c>
+      <c r="F63" s="14">
+        <v>9</v>
+      </c>
+      <c r="G63" s="14">
+        <v>14</v>
+      </c>
+      <c r="H63" s="14">
+        <v>18</v>
+      </c>
+      <c r="I63" s="14">
+        <v>21</v>
+      </c>
+      <c r="J63" s="14">
+        <v>21</v>
+      </c>
+      <c r="K63" s="14">
+        <v>16</v>
+      </c>
+      <c r="L63" s="14">
+        <v>11</v>
+      </c>
+      <c r="M63" s="14">
+        <v>5</v>
+      </c>
+      <c r="N63" s="14">
+        <v>1</v>
+      </c>
       <c r="U63" s="8"/>
     </row>
-    <row r="65" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A64" s="16">
+        <v>24</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="C64" s="16">
+        <v>-9</v>
+      </c>
+      <c r="D64" s="16">
+        <v>-8</v>
+      </c>
+      <c r="E64" s="16">
+        <v>-5</v>
+      </c>
+      <c r="F64" s="16">
+        <v>-3</v>
+      </c>
+      <c r="G64" s="16">
+        <v>1</v>
+      </c>
+      <c r="H64" s="16">
+        <v>4</v>
+      </c>
+      <c r="I64" s="16">
+        <v>7</v>
+      </c>
+      <c r="J64" s="16">
+        <v>7</v>
+      </c>
+      <c r="K64" s="16">
+        <v>3</v>
+      </c>
+      <c r="L64" s="16">
+        <v>0</v>
+      </c>
+      <c r="M64" s="16">
+        <v>-5</v>
+      </c>
+      <c r="N64" s="16">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A65" s="15">
+        <v>23</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="C65" s="15">
+        <v>5</v>
+      </c>
+      <c r="D65" s="15">
+        <v>6</v>
+      </c>
+      <c r="E65" s="15">
+        <v>5</v>
+      </c>
+      <c r="F65" s="15">
+        <v>5</v>
+      </c>
+      <c r="G65" s="15">
+        <v>5</v>
+      </c>
+      <c r="H65" s="15">
+        <v>3</v>
+      </c>
+      <c r="I65" s="15">
+        <v>2</v>
+      </c>
+      <c r="J65" s="15">
+        <v>2</v>
+      </c>
+      <c r="K65" s="15">
+        <v>2</v>
+      </c>
+      <c r="L65" s="15">
+        <v>5</v>
+      </c>
+      <c r="M65" s="15">
+        <v>6</v>
+      </c>
+      <c r="N65" s="15">
+        <v>6</v>
+      </c>
       <c r="U65" s="8"/>
     </row>
-    <row r="66" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A66" s="14">
+        <v>23</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C66" s="14">
+        <v>12</v>
+      </c>
+      <c r="D66" s="14">
+        <v>13</v>
+      </c>
+      <c r="E66" s="14">
+        <v>15</v>
+      </c>
+      <c r="F66" s="14">
+        <v>19</v>
+      </c>
+      <c r="G66" s="14">
+        <v>25</v>
+      </c>
+      <c r="H66" s="14">
+        <v>29</v>
+      </c>
+      <c r="I66" s="14">
+        <v>32</v>
+      </c>
+      <c r="J66" s="14">
+        <v>32</v>
+      </c>
+      <c r="K66" s="14">
+        <v>27</v>
+      </c>
+      <c r="L66" s="14">
+        <v>22</v>
+      </c>
+      <c r="M66" s="14">
+        <v>17</v>
+      </c>
+      <c r="N66" s="14">
+        <v>13</v>
+      </c>
       <c r="U66" s="8"/>
     </row>
-    <row r="68" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A67" s="16">
+        <v>23</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="C67" s="16">
+        <v>4</v>
+      </c>
+      <c r="D67" s="16">
+        <v>4</v>
+      </c>
+      <c r="E67" s="16">
+        <v>6</v>
+      </c>
+      <c r="F67" s="16">
+        <v>9</v>
+      </c>
+      <c r="G67" s="16">
+        <v>14</v>
+      </c>
+      <c r="H67" s="16">
+        <v>19</v>
+      </c>
+      <c r="I67" s="16">
+        <v>22</v>
+      </c>
+      <c r="J67" s="16">
+        <v>22</v>
+      </c>
+      <c r="K67" s="16">
+        <v>18</v>
+      </c>
+      <c r="L67" s="16">
+        <v>14</v>
+      </c>
+      <c r="M67" s="16">
+        <v>9</v>
+      </c>
+      <c r="N67" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A68" s="15">
+        <v>22</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="C68" s="15">
+        <v>4</v>
+      </c>
+      <c r="D68" s="15">
+        <v>3</v>
+      </c>
+      <c r="E68" s="15">
+        <v>4</v>
+      </c>
+      <c r="F68" s="15">
+        <v>4</v>
+      </c>
+      <c r="G68" s="15">
+        <v>4</v>
+      </c>
+      <c r="H68" s="15">
+        <v>2</v>
+      </c>
+      <c r="I68" s="15">
+        <v>1</v>
+      </c>
+      <c r="J68" s="15">
+        <v>1</v>
+      </c>
+      <c r="K68" s="15">
+        <v>3</v>
+      </c>
+      <c r="L68" s="15">
+        <v>4</v>
+      </c>
+      <c r="M68" s="15">
+        <v>4</v>
+      </c>
+      <c r="N68" s="15">
+        <v>4</v>
+      </c>
       <c r="U68" s="8"/>
     </row>
-    <row r="69" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A69" s="14">
+        <v>22</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C69" s="14">
+        <v>15</v>
+      </c>
+      <c r="D69" s="14">
+        <v>16</v>
+      </c>
+      <c r="E69" s="14">
+        <v>18</v>
+      </c>
+      <c r="F69" s="14">
+        <v>19</v>
+      </c>
+      <c r="G69" s="14">
+        <v>23</v>
+      </c>
+      <c r="H69" s="14">
+        <v>27</v>
+      </c>
+      <c r="I69" s="14">
+        <v>29</v>
+      </c>
+      <c r="J69" s="14">
+        <v>29</v>
+      </c>
+      <c r="K69" s="14">
+        <v>27</v>
+      </c>
+      <c r="L69" s="14">
+        <v>24</v>
+      </c>
+      <c r="M69" s="14">
+        <v>18</v>
+      </c>
+      <c r="N69" s="14">
+        <v>16</v>
+      </c>
       <c r="U69" s="8"/>
     </row>
-    <row r="71" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A70" s="16">
+        <v>22</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="C70" s="16">
+        <v>6</v>
+      </c>
+      <c r="D70" s="16">
+        <v>6</v>
+      </c>
+      <c r="E70" s="16">
+        <v>8</v>
+      </c>
+      <c r="F70" s="16">
+        <v>10</v>
+      </c>
+      <c r="G70" s="16">
+        <v>13</v>
+      </c>
+      <c r="H70" s="16">
+        <v>17</v>
+      </c>
+      <c r="I70" s="16">
+        <v>20</v>
+      </c>
+      <c r="J70" s="16">
+        <v>21</v>
+      </c>
+      <c r="K70" s="16">
+        <v>18</v>
+      </c>
+      <c r="L70" s="16">
+        <v>14</v>
+      </c>
+      <c r="M70" s="16">
+        <v>9</v>
+      </c>
+      <c r="N70" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U71" s="8"/>
     </row>
-    <row r="72" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U72" s="8"/>
     </row>
-    <row r="74" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U74" s="8"/>
     </row>
-    <row r="75" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U75" s="8"/>
     </row>
-    <row r="77" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U77" s="8"/>
     </row>
-    <row r="78" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U78" s="8"/>
     </row>
-    <row r="80" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U80" s="8"/>
     </row>
     <row r="81" spans="21:21" x14ac:dyDescent="0.45">
@@ -10815,8 +11770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11661,7 +12616,7 @@
       </c>
       <c r="H23">
         <f>_xlfn.IFNA(IF(VLOOKUP(B23,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
@@ -11693,11 +12648,11 @@
       </c>
       <c r="G24">
         <f>_xlfn.IFNA(IF(VLOOKUP(B24,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <f>_xlfn.IFNA(IF(VLOOKUP(B24,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
@@ -11710,7 +12665,7 @@
       </c>
       <c r="C25" t="str">
         <f>CLIMBS!B25</f>
-        <v>draft</v>
+        <v>publish</v>
       </c>
       <c r="D25">
         <f>IF(CLIMBS!R25&lt;&gt;0,1,0)+IF(CLIMBS!G25&lt;&gt;0,1,0)+IF(CLIMBS!H25&lt;&gt;0,1,0)+IF(CLIMBS!I25&lt;&gt;0,1,0)+IF(CLIMBS!J25&lt;&gt;0,1,0)+IF(CLIMBS!N25&lt;&gt;0,1,0)+IF(CLIMBS!M25&lt;&gt;0,1,0)+IF(CLIMBS!O25&lt;&gt;0,1,0)+IF(CLIMBS!P25&lt;&gt;0,1,0)</f>
@@ -11718,22 +12673,22 @@
       </c>
       <c r="E25">
         <f>IF(CLIMBS!S25&lt;&gt;0,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F25" t="str">
+        <v>1</v>
+      </c>
+      <c r="F25">
         <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B25,"tile"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B25,"crag"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B25,"topo"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B25,"map"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
-        <v>missing</v>
+        <v>4</v>
       </c>
       <c r="G25">
         <f>_xlfn.IFNA(IF(VLOOKUP(B25,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <f>_xlfn.IFNA(IF(VLOOKUP(B25,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made images on cards clickable
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD97F11-9F02-4C41-B099-BBD7C293B55E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547B907B-0F39-45F3-A68E-5FCF40B10090}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="674">
   <si>
     <t>cliff</t>
   </si>
@@ -2095,6 +2095,15 @@
   <si>
     <t xml:space="preserve">Approach: The route is best approached from Stattboden.
 Decent. Carefully move along the summit to the cross  on the left after the final pitch. From there a path can be followed to walk off the cliff. </t>
+  </si>
+  <si>
+    <t>Vajolet towers</t>
+  </si>
+  <si>
+    <t>46.460408,11.624514</t>
+  </si>
+  <si>
+    <t>South Tyrol</t>
   </si>
 </sst>
 </file>
@@ -3164,32 +3173,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView topLeftCell="G18" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.53125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.86328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="6.46484375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.86328125" style="2" customWidth="1"/>
-    <col min="11" max="12" width="9.46484375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="9.53125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="15.1328125" style="2" customWidth="1"/>
-    <col min="17" max="20" width="15.33203125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="4.53125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="2" customWidth="1"/>
+    <col min="11" max="12" width="9.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" style="2" customWidth="1"/>
+    <col min="17" max="20" width="15.28515625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3254,7 +3263,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -3313,7 +3322,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -3375,7 +3384,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
@@ -3437,7 +3446,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>56</v>
       </c>
@@ -3493,7 +3502,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>66</v>
       </c>
@@ -3555,7 +3564,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>75</v>
       </c>
@@ -3617,7 +3626,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>87</v>
       </c>
@@ -3673,7 +3682,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>93</v>
       </c>
@@ -3735,7 +3744,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>96</v>
       </c>
@@ -3797,7 +3806,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>100</v>
       </c>
@@ -3856,7 +3865,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>195</v>
       </c>
@@ -3918,7 +3927,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>216</v>
       </c>
@@ -3980,7 +3989,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>232</v>
       </c>
@@ -4039,7 +4048,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>250</v>
       </c>
@@ -4101,7 +4110,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>283</v>
       </c>
@@ -4166,7 +4175,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>354</v>
       </c>
@@ -4228,7 +4237,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>402</v>
       </c>
@@ -4290,7 +4299,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>440</v>
       </c>
@@ -4346,7 +4355,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>473</v>
       </c>
@@ -4408,7 +4417,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>478</v>
       </c>
@@ -4467,7 +4476,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>520</v>
       </c>
@@ -4529,7 +4538,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>521</v>
       </c>
@@ -4591,7 +4600,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>589</v>
       </c>
@@ -4656,7 +4665,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>610</v>
       </c>
@@ -4721,7 +4730,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>653</v>
       </c>
@@ -4786,7 +4795,27 @@
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="2">
+        <v>26</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" t="s">
+        <v>673</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>570</v>
       </c>
@@ -4805,17 +4834,17 @@
       <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.46484375" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
     <col min="7" max="7" width="4" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>127</v>
       </c>
@@ -4838,7 +4867,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4862,7 +4891,7 @@
         <v>1crag</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4886,7 +4915,7 @@
         <v>1topo</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4910,7 +4939,7 @@
         <v>1map</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4934,7 +4963,7 @@
         <v>2crag</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -4958,7 +4987,7 @@
         <v>2topo</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -4982,7 +5011,7 @@
         <v>2map</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -5006,7 +5035,7 @@
         <v>3crag</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -5030,7 +5059,7 @@
         <v>3topo</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -5054,7 +5083,7 @@
         <v>3map</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -5078,7 +5107,7 @@
         <v>5crag</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -5102,7 +5131,7 @@
         <v>5topo</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -5126,7 +5155,7 @@
         <v>5map</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -5150,7 +5179,7 @@
         <v>6crag</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -5174,7 +5203,7 @@
         <v>6topo</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -5198,7 +5227,7 @@
         <v>6map</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -5222,7 +5251,7 @@
         <v>7crag</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
@@ -5246,7 +5275,7 @@
         <v>7topo</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -5270,7 +5299,7 @@
         <v>7map</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
@@ -5294,7 +5323,7 @@
         <v>8crag</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
@@ -5318,7 +5347,7 @@
         <v>8topo</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
@@ -5342,7 +5371,7 @@
         <v>8map</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
@@ -5366,7 +5395,7 @@
         <v>10crag</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
@@ -5390,7 +5419,7 @@
         <v>10topo</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10</v>
       </c>
@@ -5414,7 +5443,7 @@
         <v>10map</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -5435,7 +5464,7 @@
         <v>2tile</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -5453,7 +5482,7 @@
         <v>1tile</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -5471,7 +5500,7 @@
         <v>3tile</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
@@ -5489,7 +5518,7 @@
         <v>4tile</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -5510,7 +5539,7 @@
         <v>5tile</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
@@ -5528,7 +5557,7 @@
         <v>6tile</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
@@ -5552,7 +5581,7 @@
         <v>7tile</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>8</v>
       </c>
@@ -5573,7 +5602,7 @@
         <v>8tile</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>9</v>
       </c>
@@ -5597,7 +5626,7 @@
         <v>9tile</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>10</v>
       </c>
@@ -5615,7 +5644,7 @@
         <v>10tile</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>11</v>
       </c>
@@ -5639,7 +5668,7 @@
         <v>11crag</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>11</v>
       </c>
@@ -5663,7 +5692,7 @@
         <v>11topo</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>11</v>
       </c>
@@ -5687,7 +5716,7 @@
         <v>11map</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>11</v>
       </c>
@@ -5711,7 +5740,7 @@
         <v>11tile</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>12</v>
       </c>
@@ -5735,7 +5764,7 @@
         <v>12crag</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>12</v>
       </c>
@@ -5759,7 +5788,7 @@
         <v>12topo</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>12</v>
       </c>
@@ -5783,7 +5812,7 @@
         <v>12tile</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>13</v>
       </c>
@@ -5807,7 +5836,7 @@
         <v>13tile</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>13</v>
       </c>
@@ -5831,7 +5860,7 @@
         <v>13crag</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>13</v>
       </c>
@@ -5855,7 +5884,7 @@
         <v>13topo</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>14</v>
       </c>
@@ -5879,7 +5908,7 @@
         <v>14crag</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>14</v>
       </c>
@@ -5903,7 +5932,7 @@
         <v>14topo</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>14</v>
       </c>
@@ -5927,7 +5956,7 @@
         <v>14tile</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>15</v>
       </c>
@@ -5951,7 +5980,7 @@
         <v>15topo</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>15</v>
       </c>
@@ -5975,7 +6004,7 @@
         <v>15tile</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -5999,7 +6028,7 @@
         <v>15crag</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>15</v>
       </c>
@@ -6023,7 +6052,7 @@
         <v>15map</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>16</v>
       </c>
@@ -6047,7 +6076,7 @@
         <v>16crag</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>16</v>
       </c>
@@ -6071,7 +6100,7 @@
         <v>16topo</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>16</v>
       </c>
@@ -6095,7 +6124,7 @@
         <v>16tile</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>14</v>
       </c>
@@ -6119,7 +6148,7 @@
         <v>14map</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>16</v>
       </c>
@@ -6143,7 +6172,7 @@
         <v>16map</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>12</v>
       </c>
@@ -6167,7 +6196,7 @@
         <v>12map</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>17</v>
       </c>
@@ -6191,7 +6220,7 @@
         <v>17topo</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>17</v>
       </c>
@@ -6215,7 +6244,7 @@
         <v>17crag</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>17</v>
       </c>
@@ -6239,7 +6268,7 @@
         <v>17tile</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>17</v>
       </c>
@@ -6263,7 +6292,7 @@
         <v>17map</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>13</v>
       </c>
@@ -6287,7 +6316,7 @@
         <v>13map</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>18</v>
       </c>
@@ -6311,7 +6340,7 @@
         <v>18topo</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>18</v>
       </c>
@@ -6335,7 +6364,7 @@
         <v>18crag</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>18</v>
       </c>
@@ -6359,7 +6388,7 @@
         <v>18tile</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>18</v>
       </c>
@@ -6383,7 +6412,7 @@
         <v>18map</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>20</v>
       </c>
@@ -6407,7 +6436,7 @@
         <v>20crag</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>20</v>
       </c>
@@ -6431,7 +6460,7 @@
         <v>20tile</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>20</v>
       </c>
@@ -6455,7 +6484,7 @@
         <v>20topo</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>20</v>
       </c>
@@ -6479,7 +6508,7 @@
         <v>20map</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>19</v>
       </c>
@@ -6503,7 +6532,7 @@
         <v>19crag</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>19</v>
       </c>
@@ -6527,7 +6556,7 @@
         <v>19tile</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>19</v>
       </c>
@@ -6551,7 +6580,7 @@
         <v>19topo</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>19</v>
       </c>
@@ -6575,7 +6604,7 @@
         <v>19map</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>21</v>
       </c>
@@ -6599,7 +6628,7 @@
         <v>21crag</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>21</v>
       </c>
@@ -6623,7 +6652,7 @@
         <v>21tile</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>21</v>
       </c>
@@ -6647,7 +6676,7 @@
         <v>21topo</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>21</v>
       </c>
@@ -6671,7 +6700,7 @@
         <v>21map</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>9</v>
       </c>
@@ -6695,7 +6724,7 @@
         <v>9topo</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>9</v>
       </c>
@@ -6719,7 +6748,7 @@
         <v>9crag</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>9</v>
       </c>
@@ -6743,7 +6772,7 @@
         <v>9map</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>22</v>
       </c>
@@ -6767,7 +6796,7 @@
         <v>22crag</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>22</v>
       </c>
@@ -6791,7 +6820,7 @@
         <v>22tile</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>22</v>
       </c>
@@ -6815,7 +6844,7 @@
         <v>22topo</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>22</v>
       </c>
@@ -6839,7 +6868,7 @@
         <v>22map</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>23</v>
       </c>
@@ -6863,7 +6892,7 @@
         <v>23crag</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>23</v>
       </c>
@@ -6887,7 +6916,7 @@
         <v>23tile</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>23</v>
       </c>
@@ -6911,7 +6940,7 @@
         <v>23topo</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>23</v>
       </c>
@@ -6935,7 +6964,7 @@
         <v>23map</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>24</v>
       </c>
@@ -6959,7 +6988,7 @@
         <v>24topo</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>24</v>
       </c>
@@ -6983,7 +7012,7 @@
         <v>24crag</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>24</v>
       </c>
@@ -7007,7 +7036,7 @@
         <v>24tile</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>24</v>
       </c>
@@ -7031,7 +7060,7 @@
         <v>24map</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>25</v>
       </c>
@@ -7055,7 +7084,7 @@
         <v>25crag</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>25</v>
       </c>
@@ -7075,7 +7104,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>25</v>
       </c>
@@ -7095,7 +7124,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>25</v>
       </c>
@@ -7129,23 +7158,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="34.1328125" customWidth="1"/>
-    <col min="4" max="4" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
     <col min="7" max="7" width="45" customWidth="1"/>
-    <col min="8" max="8" width="7.19921875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -7177,7 +7206,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>2</v>
       </c>
@@ -7209,7 +7238,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -7241,7 +7270,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -7273,7 +7302,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -7290,7 +7319,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -7322,7 +7351,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -7354,7 +7383,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -7386,7 +7415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -7418,7 +7447,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -7450,7 +7479,7 @@
         <v>34.950000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -7482,7 +7511,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>13</v>
       </c>
@@ -7514,7 +7543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>16</v>
       </c>
@@ -7546,7 +7575,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>11</v>
       </c>
@@ -7578,7 +7607,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -7610,7 +7639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>12</v>
       </c>
@@ -7642,7 +7671,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>17</v>
       </c>
@@ -7674,7 +7703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>18</v>
       </c>
@@ -7706,7 +7735,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>15</v>
       </c>
@@ -7738,7 +7767,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -7770,7 +7799,7 @@
         <v>34.99</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -7802,7 +7831,7 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -7834,7 +7863,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -7866,7 +7895,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>24</v>
       </c>
@@ -7898,7 +7927,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -7930,7 +7959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -7981,14 +8010,14 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.46484375" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.53125" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -8002,7 +8031,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -8013,7 +8042,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -8024,7 +8053,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -8035,7 +8064,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>16</v>
       </c>
@@ -8046,7 +8075,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>17</v>
       </c>
@@ -8057,7 +8086,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -8068,7 +8097,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12</v>
       </c>
@@ -8079,7 +8108,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -8090,7 +8119,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>15</v>
       </c>
@@ -8101,7 +8130,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>19</v>
       </c>
@@ -8112,7 +8141,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20</v>
       </c>
@@ -8123,7 +8152,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20</v>
       </c>
@@ -8134,7 +8163,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>21</v>
       </c>
@@ -8145,7 +8174,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -8156,7 +8185,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>24</v>
       </c>
@@ -8180,17 +8209,17 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.1328125" customWidth="1"/>
-    <col min="3" max="3" width="15.46484375" customWidth="1"/>
-    <col min="4" max="4" width="15.1328125" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="53.46484375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="53.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -8216,7 +8245,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -8239,7 +8268,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -8257,7 +8286,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -8275,7 +8304,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -8291,7 +8320,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -8307,7 +8336,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -8323,7 +8352,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -8339,7 +8368,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -8355,7 +8384,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -8371,7 +8400,7 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -8387,7 +8416,7 @@
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -8405,7 +8434,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -8423,7 +8452,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -8439,7 +8468,7 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -8457,7 +8486,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -8475,7 +8504,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -8501,7 +8530,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>21</v>
       </c>
@@ -8523,9 +8552,9 @@
       <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -8569,7 +8598,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>2</v>
       </c>
@@ -8613,7 +8642,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -8658,7 +8687,7 @@
       </c>
       <c r="U3" s="9"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -8702,7 +8731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -8746,7 +8775,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>3</v>
       </c>
@@ -8790,7 +8819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>3</v>
       </c>
@@ -8835,7 +8864,7 @@
       </c>
       <c r="S7" s="8"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>16</v>
       </c>
@@ -8879,7 +8908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>16</v>
       </c>
@@ -8924,7 +8953,7 @@
       </c>
       <c r="S9" s="8"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>16</v>
       </c>
@@ -8969,7 +8998,7 @@
       </c>
       <c r="S10" s="8"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>11</v>
       </c>
@@ -9013,7 +9042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -9058,7 +9087,7 @@
       </c>
       <c r="S12" s="8"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>11</v>
       </c>
@@ -9104,7 +9133,7 @@
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>1</v>
       </c>
@@ -9148,7 +9177,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>1</v>
       </c>
@@ -9194,7 +9223,7 @@
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>1</v>
       </c>
@@ -9240,7 +9269,7 @@
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>5</v>
       </c>
@@ -9284,7 +9313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>5</v>
       </c>
@@ -9330,7 +9359,7 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>5</v>
       </c>
@@ -9376,7 +9405,7 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>13</v>
       </c>
@@ -9420,7 +9449,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>13</v>
       </c>
@@ -9466,7 +9495,7 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>13</v>
       </c>
@@ -9512,7 +9541,7 @@
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>14</v>
       </c>
@@ -9556,7 +9585,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>14</v>
       </c>
@@ -9602,7 +9631,7 @@
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>14</v>
       </c>
@@ -9648,7 +9677,7 @@
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>7</v>
       </c>
@@ -9692,7 +9721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <v>7</v>
       </c>
@@ -9738,7 +9767,7 @@
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>7</v>
       </c>
@@ -9784,7 +9813,7 @@
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>12</v>
       </c>
@@ -9828,7 +9857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>12</v>
       </c>
@@ -9874,7 +9903,7 @@
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>12</v>
       </c>
@@ -9920,7 +9949,7 @@
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>17</v>
       </c>
@@ -9964,7 +9993,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>17</v>
       </c>
@@ -10010,7 +10039,7 @@
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>17</v>
       </c>
@@ -10056,7 +10085,7 @@
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>6</v>
       </c>
@@ -10100,7 +10129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>6</v>
       </c>
@@ -10146,7 +10175,7 @@
       <c r="R36" s="8"/>
       <c r="S36" s="8"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>6</v>
       </c>
@@ -10192,7 +10221,7 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>8</v>
       </c>
@@ -10236,7 +10265,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
         <v>8</v>
       </c>
@@ -10282,7 +10311,7 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <v>8</v>
       </c>
@@ -10328,7 +10357,7 @@
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>10</v>
       </c>
@@ -10372,7 +10401,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>10</v>
       </c>
@@ -10417,7 +10446,7 @@
       </c>
       <c r="R42" s="8"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
         <v>10</v>
       </c>
@@ -10462,7 +10491,7 @@
       </c>
       <c r="R43" s="8"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>18</v>
       </c>
@@ -10506,7 +10535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
         <v>18</v>
       </c>
@@ -10551,7 +10580,7 @@
       </c>
       <c r="R45" s="8"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>18</v>
       </c>
@@ -10600,7 +10629,7 @@
       <c r="U46" s="17"/>
       <c r="V46" s="17"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>15</v>
       </c>
@@ -10648,7 +10677,7 @@
       <c r="U47" s="17"/>
       <c r="V47" s="17"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
         <v>15</v>
       </c>
@@ -10696,7 +10725,7 @@
       <c r="U48" s="17"/>
       <c r="V48" s="17"/>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
         <v>15</v>
       </c>
@@ -10744,7 +10773,7 @@
       <c r="U49" s="17"/>
       <c r="V49" s="17"/>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <v>19</v>
       </c>
@@ -10792,7 +10821,7 @@
       <c r="U50" s="17"/>
       <c r="V50" s="17"/>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
         <v>19</v>
       </c>
@@ -10840,7 +10869,7 @@
       <c r="U51" s="17"/>
       <c r="V51" s="17"/>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>19</v>
       </c>
@@ -10888,7 +10917,7 @@
       <c r="U52" s="17"/>
       <c r="V52" s="17"/>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>20</v>
       </c>
@@ -10936,7 +10965,7 @@
       <c r="U53" s="17"/>
       <c r="V53" s="17"/>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="14">
         <v>20</v>
       </c>
@@ -10985,7 +11014,7 @@
       <c r="U54" s="17"/>
       <c r="V54" s="17"/>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
         <v>20</v>
       </c>
@@ -11034,7 +11063,7 @@
       <c r="U55" s="17"/>
       <c r="V55" s="17"/>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>21</v>
       </c>
@@ -11083,7 +11112,7 @@
       <c r="U56" s="17"/>
       <c r="V56" s="17"/>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="14">
         <v>21</v>
       </c>
@@ -11132,7 +11161,7 @@
       <c r="U57" s="8"/>
       <c r="V57" s="17"/>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="16">
         <v>21</v>
       </c>
@@ -11176,7 +11205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>9</v>
       </c>
@@ -11221,7 +11250,7 @@
       </c>
       <c r="U59" s="8"/>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="14">
         <v>9</v>
       </c>
@@ -11266,7 +11295,7 @@
       </c>
       <c r="U60" s="8"/>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
         <v>9</v>
       </c>
@@ -11310,7 +11339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <v>24</v>
       </c>
@@ -11355,7 +11384,7 @@
       </c>
       <c r="U62" s="8"/>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="14">
         <v>24</v>
       </c>
@@ -11400,7 +11429,7 @@
       </c>
       <c r="U63" s="8"/>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
         <v>24</v>
       </c>
@@ -11444,7 +11473,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>23</v>
       </c>
@@ -11489,7 +11518,7 @@
       </c>
       <c r="U65" s="8"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="14">
         <v>23</v>
       </c>
@@ -11534,7 +11563,7 @@
       </c>
       <c r="U66" s="8"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="16">
         <v>23</v>
       </c>
@@ -11578,7 +11607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <v>22</v>
       </c>
@@ -11623,7 +11652,7 @@
       </c>
       <c r="U68" s="8"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="14">
         <v>22</v>
       </c>
@@ -11668,7 +11697,7 @@
       </c>
       <c r="U69" s="8"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="16">
         <v>22</v>
       </c>
@@ -11712,52 +11741,52 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U71" s="8"/>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U72" s="8"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U74" s="8"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U75" s="8"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U77" s="8"/>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U78" s="8"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U80" s="8"/>
     </row>
-    <row r="81" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="81" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U81" s="8"/>
     </row>
-    <row r="83" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="83" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U83" s="8"/>
     </row>
-    <row r="84" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="84" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U84" s="8"/>
     </row>
-    <row r="86" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="86" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U86" s="8"/>
     </row>
-    <row r="87" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="87" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U87" s="8"/>
     </row>
-    <row r="89" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="89" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U89" s="8"/>
     </row>
-    <row r="90" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="90" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U90" s="8"/>
     </row>
-    <row r="92" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="92" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U92" s="8"/>
     </row>
-    <row r="93" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="93" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U93" s="8"/>
     </row>
   </sheetData>
@@ -11768,23 +11797,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.53125" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.53125" customWidth="1"/>
-    <col min="8" max="8" width="10.1328125" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>376</v>
       </c>
@@ -11810,7 +11839,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CLIMBS!A2</f>
         <v>Old Man of Stoer</v>
@@ -11847,7 +11876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CLIMBS!A3</f>
         <v>Bosigran</v>
@@ -11884,7 +11913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>CLIMBS!A4</f>
         <v>Clogwyn Du'r Arddu</v>
@@ -11921,7 +11950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>CLIMBS!A5</f>
         <v>Vratsa</v>
@@ -11958,7 +11987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>CLIMBS!A6</f>
         <v>Tormore Group</v>
@@ -11995,7 +12024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>CLIMBS!A7</f>
         <v>Sass Pordoi</v>
@@ -12032,7 +12061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>CLIMBS!A8</f>
         <v>Cwm Idwal</v>
@@ -12069,7 +12098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>CLIMBS!A9</f>
         <v>Lundy</v>
@@ -12106,7 +12135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CLIMBS!A10</f>
         <v>Meadinha</v>
@@ -12143,7 +12172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>CLIMBS!A11</f>
         <v>Cornakey Cliff</v>
@@ -12180,7 +12209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>CLIMBS!A12</f>
         <v>Cir Mhor</v>
@@ -12217,7 +12246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>CLIMBS!A13</f>
         <v>Roca Gris</v>
@@ -12254,7 +12283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>CLIMBS!A14</f>
         <v>Sail Rock</v>
@@ -12291,7 +12320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>CLIMBS!A15</f>
         <v>Chair Ladder</v>
@@ -12328,7 +12357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>CLIMBS!A16</f>
         <v>The Devils Tower</v>
@@ -12365,7 +12394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>CLIMBS!A17</f>
         <v>Lliwedd</v>
@@ -12402,7 +12431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>CLIMBS!A18</f>
         <v>Stetind</v>
@@ -12439,7 +12468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>CLIMBS!A19</f>
         <v>Scafell</v>
@@ -12475,7 +12504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>CLIMBS!A20</f>
         <v>Mount Indefatigable</v>
@@ -12511,7 +12540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>CLIMBS!A21</f>
         <v>Slieve Beg</v>
@@ -12547,7 +12576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>CLIMBS!A22</f>
         <v>Lion Rock</v>
@@ -12583,7 +12612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>CLIMBS!A23</f>
         <v>Peñón de Ifach</v>
@@ -12619,7 +12648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>CLIMBS!A24</f>
         <v>Heiliger Geist</v>
@@ -12655,7 +12684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>CLIMBS!A25</f>
         <v>Aiguille Dibona</v>
@@ -12691,8 +12720,80 @@
         <v>1</v>
       </c>
     </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>CLIMBS!A26</f>
+        <v>Brüggler</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="str">
+        <f>CLIMBS!B26</f>
+        <v>publish</v>
+      </c>
+      <c r="D26">
+        <f>IF(CLIMBS!R26&lt;&gt;0,1,0)+IF(CLIMBS!G26&lt;&gt;0,1,0)+IF(CLIMBS!H26&lt;&gt;0,1,0)+IF(CLIMBS!I26&lt;&gt;0,1,0)+IF(CLIMBS!J26&lt;&gt;0,1,0)+IF(CLIMBS!N26&lt;&gt;0,1,0)+IF(CLIMBS!M26&lt;&gt;0,1,0)+IF(CLIMBS!O26&lt;&gt;0,1,0)+IF(CLIMBS!P26&lt;&gt;0,1,0)</f>
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <f>IF(CLIMBS!S26&lt;&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F26" t="str">
+        <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B26,"tile"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B26,"crag"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B26,"topo"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B26,"map"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
+        <v>missing</v>
+      </c>
+      <c r="G26">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B26,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B26,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>CLIMBS!A27</f>
+        <v>Vajolet towers</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="str">
+        <f>CLIMBS!B27</f>
+        <v>draft</v>
+      </c>
+      <c r="D27">
+        <f>IF(CLIMBS!R27&lt;&gt;0,1,0)+IF(CLIMBS!G27&lt;&gt;0,1,0)+IF(CLIMBS!H27&lt;&gt;0,1,0)+IF(CLIMBS!I27&lt;&gt;0,1,0)+IF(CLIMBS!J27&lt;&gt;0,1,0)+IF(CLIMBS!N27&lt;&gt;0,1,0)+IF(CLIMBS!M27&lt;&gt;0,1,0)+IF(CLIMBS!O27&lt;&gt;0,1,0)+IF(CLIMBS!P27&lt;&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f>IF(CLIMBS!S27&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" t="str">
+        <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B27,"tile"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B27,"crag"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B27,"topo"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B27,"map"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
+        <v>missing</v>
+      </c>
+      <c r="G27">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B27,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B27,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
@@ -12700,7 +12801,7 @@
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C25">
+  <conditionalFormatting sqref="C2:C27">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"draft"</formula>
     </cfRule>
@@ -12710,12 +12811,12 @@
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C25">
+  <conditionalFormatting sqref="C3:C27">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E25">
+  <conditionalFormatting sqref="E2:E27">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -12723,7 +12824,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F25">
+  <conditionalFormatting sqref="F2:F27">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>4</formula>
     </cfRule>
@@ -12731,7 +12832,7 @@
       <formula>"missing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H25">
+  <conditionalFormatting sqref="G2:H27">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
human readable urls for better seo. This is a big change and some more bits are needed to give it the full impact. The js will also need a tidy up, but ill do that in a later commit
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F715009-64F9-47DB-9349-6F0EAE9D5662}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FB6B00-83B2-437D-8213-FABEB7F6DD9F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="686">
   <si>
     <t>cliff</t>
   </si>
@@ -2052,9 +2052,6 @@
     <t>The Vejolet Towers topo for Piaz Arete</t>
   </si>
   <si>
-    <t xml:space="preserve">The Vejolet Towers rock climbing location </t>
-  </si>
-  <si>
     <t>VI+ &amp; (f6b)</t>
   </si>
   <si>
@@ -2101,6 +2098,48 @@
   </si>
   <si>
     <t>img/topos/montserrat/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/stoer/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/bosigran/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/cloggy/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/cnoc/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/idwal/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/lundy/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/wreakers/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/meadinha/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/sail-rock/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/chair/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/devils-tower/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/mournes/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/lion-rock/maps/</t>
+  </si>
+  <si>
+    <t>img/topos/scafell/maps/</t>
   </si>
 </sst>
 </file>
@@ -3171,7 +3210,7 @@
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView topLeftCell="G3" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="I27" sqref="I27:R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3776,7 +3815,7 @@
         <v>60</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>540</v>
@@ -4024,7 +4063,7 @@
         <v>70</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="O14" s="2">
         <v>20</v>
@@ -4148,7 +4187,7 @@
         <v>279</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="O16" s="2">
         <v>5</v>
@@ -4393,7 +4432,7 @@
         <v>451</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="O20" s="2">
         <v>40</v>
@@ -4809,7 +4848,7 @@
         <v>644</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G27" s="2">
         <v>160</v>
@@ -4848,7 +4887,7 @@
         <v>646</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="U27" s="2" t="s">
         <v>243</v>
@@ -4867,11 +4906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4907,7 +4945,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4931,7 +4969,7 @@
         <v>1crag</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4939,7 +4977,7 @@
         <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>672</v>
       </c>
       <c r="D3" t="s">
         <v>114</v>
@@ -4962,6 +5000,9 @@
       <c r="B4" t="s">
         <v>111</v>
       </c>
+      <c r="C4" t="s">
+        <v>115</v>
+      </c>
       <c r="D4" t="s">
         <v>110</v>
       </c>
@@ -4976,52 +5017,46 @@
         <v>1map</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>2crag</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>1tile</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>2topo</v>
+        <v>2crag</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
@@ -5029,68 +5064,68 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>129</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="F7" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>2map</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>2topo</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>673</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E8" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="F8" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>3crag</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>2map</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>139</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>136</v>
-      </c>
-      <c r="F9" t="s">
-        <v>137</v>
+        <v>179</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>3topo</v>
+        <v>2tile</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
@@ -5098,358 +5133,352 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="F10" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>3map</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>3crag</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F11" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>5crag</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>3topo</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>674</v>
       </c>
       <c r="D12" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E12" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="F12" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>5topo</v>
+        <v>3map</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>178</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
-      </c>
-      <c r="E13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>5map</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>3tile</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="C14" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F14" t="s">
-        <v>151</v>
+        <v>182</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>6crag</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>4tile</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="E15" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="F15" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>6topo</v>
+        <v>5crag</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
-        <v>663</v>
+        <v>145</v>
       </c>
       <c r="D16" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E16" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="F16" t="s">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>6map</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>5topo</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
-        <v>156</v>
+        <v>675</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
       <c r="F17" t="s">
-        <v>151</v>
+        <v>108</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>7crag</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>5map</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="C18" t="s">
-        <v>158</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="E18" t="s">
-        <v>160</v>
-      </c>
-      <c r="F18" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>7topo</v>
+        <v>5tile</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>119</v>
+      </c>
+      <c r="C19" t="s">
+        <v>148</v>
       </c>
       <c r="D19" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="E19" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="F19" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>7map</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>6crag</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E20" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F20" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>8crag</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>6topo</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
-        <v>412</v>
+        <v>662</v>
       </c>
       <c r="D21" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="E21" t="s">
-        <v>168</v>
+        <v>109</v>
       </c>
       <c r="F21" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>8topo</v>
+        <v>6map</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
+        <v>178</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>147</v>
-      </c>
-      <c r="E22" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>8map</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>6tile</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
         <v>119</v>
       </c>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="D23" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="E23" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="F23" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>10crag</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>7crag</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
         <v>116</v>
       </c>
       <c r="C24" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="D24" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="E24" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F24" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>10topo</v>
+        <v>7topo</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
         <v>111</v>
       </c>
+      <c r="C25" t="s">
+        <v>676</v>
+      </c>
       <c r="D25" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="E25" t="s">
         <v>109</v>
@@ -5459,270 +5488,300 @@
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>10map</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>7map</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
         <v>178</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="E26" t="s">
-        <v>179</v>
+        <v>157</v>
+      </c>
+      <c r="F26" t="s">
+        <v>151</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>2tile</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>7tile</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>164</v>
+      </c>
+      <c r="E27" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" t="s">
+        <v>166</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>1tile</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>8crag</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>412</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>167</v>
+      </c>
+      <c r="E28" t="s">
+        <v>168</v>
+      </c>
+      <c r="F28" t="s">
+        <v>169</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>3tile</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>8topo</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>178</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>677</v>
       </c>
       <c r="D29" t="s">
-        <v>182</v>
+        <v>147</v>
+      </c>
+      <c r="E29" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" t="s">
+        <v>108</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>4tile</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>8map</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
         <v>178</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="D30" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="E30" t="s">
-        <v>143</v>
+        <v>180</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>5tile</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>8tile</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>178</v>
+        <v>111</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>679</v>
       </c>
       <c r="D31" t="s">
-        <v>149</v>
+        <v>530</v>
+      </c>
+      <c r="E31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" t="s">
+        <v>108</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>6tile</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>9map</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
         <v>178</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E32" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="F32" t="s">
-        <v>151</v>
+        <v>290</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
-        <v>7tile</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>9tile</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>539</v>
       </c>
       <c r="D33" t="s">
-        <v>164</v>
+        <v>527</v>
       </c>
       <c r="E33" t="s">
-        <v>180</v>
+        <v>526</v>
+      </c>
+      <c r="F33" t="s">
+        <v>525</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
-        <v>8tile</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>9topo</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>538</v>
       </c>
       <c r="D34" t="s">
-        <v>185</v>
+        <v>528</v>
       </c>
       <c r="E34" t="s">
-        <v>181</v>
+        <v>529</v>
       </c>
       <c r="F34" t="s">
         <v>290</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
-        <v>9tile</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>9crag</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="D35" t="s">
-        <v>184</v>
+        <v>171</v>
+      </c>
+      <c r="E35" t="s">
+        <v>172</v>
+      </c>
+      <c r="F35" t="s">
+        <v>173</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
-        <v>10tile</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>10crag</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C36" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="D36" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="E36" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="F36" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
-        <v>11crag</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>10topo</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="C37" t="s">
-        <v>197</v>
+        <v>101</v>
       </c>
       <c r="D37" t="s">
-        <v>205</v>
-      </c>
-      <c r="E37" t="s">
-        <v>194</v>
-      </c>
-      <c r="F37" t="s">
-        <v>112</v>
+        <v>184</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
-        <v>11topo</v>
+        <v>10tile</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
         <v>111</v>
       </c>
       <c r="C38" t="s">
-        <v>664</v>
+        <v>678</v>
       </c>
       <c r="D38" t="s">
-        <v>372</v>
+        <v>176</v>
       </c>
       <c r="E38" t="s">
         <v>109</v>
@@ -5732,21 +5791,21 @@
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
-        <v>11map</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>10map</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="C39" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E39" t="s">
         <v>189</v>
@@ -5756,545 +5815,551 @@
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
-        <v>11tile</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>11crag</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C40" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="D40" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E40" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="F40" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
-        <v>12crag</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>11topo</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="C41" t="s">
-        <v>222</v>
+        <v>196</v>
       </c>
       <c r="D41" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E41" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="F41" t="s">
-        <v>151</v>
+        <v>190</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
-        <v>12topo</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>11tile</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>178</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
-        <v>362</v>
+        <v>663</v>
       </c>
       <c r="D42" t="s">
-        <v>219</v>
+        <v>372</v>
       </c>
       <c r="E42" t="s">
-        <v>363</v>
+        <v>109</v>
       </c>
       <c r="F42" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
-        <v>12tile</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>11map</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="C43" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D43" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="E43" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="F43" t="s">
-        <v>229</v>
+        <v>117</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
-        <v>13tile</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>12crag</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C44" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D44" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="E44" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="F44" t="s">
-        <v>229</v>
+        <v>151</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v>13crag</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>12topo</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="C45" t="s">
-        <v>236</v>
+        <v>362</v>
       </c>
       <c r="D45" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="E45" t="s">
-        <v>238</v>
+        <v>363</v>
       </c>
       <c r="F45" t="s">
-        <v>239</v>
+        <v>112</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
-        <v>13topo</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>12tile</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C46" t="s">
-        <v>251</v>
+        <v>671</v>
       </c>
       <c r="D46" t="s">
-        <v>248</v>
-      </c>
-      <c r="E46" t="s">
-        <v>244</v>
-      </c>
-      <c r="F46" t="s">
-        <v>245</v>
+        <v>380</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>14crag</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>12map</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="C47" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="D47" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="E47" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="F47" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>14topo</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>13tile</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="C48" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="D48" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="E48" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="F48" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>14tile</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>13crag</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B49" t="s">
         <v>116</v>
       </c>
       <c r="C49" t="s">
-        <v>291</v>
+        <v>236</v>
       </c>
       <c r="D49" t="s">
-        <v>277</v>
+        <v>237</v>
       </c>
       <c r="E49" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="F49" t="s">
-        <v>287</v>
+        <v>239</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>15topo</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>13topo</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>178</v>
+        <v>111</v>
       </c>
       <c r="C50" t="s">
-        <v>284</v>
+        <v>680</v>
       </c>
       <c r="D50" t="s">
-        <v>285</v>
-      </c>
-      <c r="E50" t="s">
-        <v>286</v>
+        <v>410</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="F50" t="s">
-        <v>287</v>
+        <v>108</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>15tile</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>13map</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B51" t="s">
         <v>119</v>
       </c>
       <c r="C51" t="s">
-        <v>292</v>
+        <v>251</v>
       </c>
       <c r="D51" t="s">
-        <v>288</v>
+        <v>248</v>
       </c>
       <c r="E51" t="s">
-        <v>289</v>
+        <v>244</v>
       </c>
       <c r="F51" t="s">
-        <v>290</v>
+        <v>245</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>15crag</v>
+        <v>14crag</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>111</v>
+        <v>116</v>
+      </c>
+      <c r="C52" t="s">
+        <v>252</v>
       </c>
       <c r="D52" t="s">
-        <v>329</v>
+        <v>249</v>
       </c>
       <c r="E52" t="s">
-        <v>109</v>
+        <v>246</v>
       </c>
       <c r="F52" t="s">
-        <v>108</v>
+        <v>247</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>15map</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>14topo</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="C53" t="s">
-        <v>350</v>
+        <v>253</v>
       </c>
       <c r="D53" t="s">
-        <v>342</v>
+        <v>250</v>
       </c>
       <c r="E53" t="s">
-        <v>340</v>
+        <v>246</v>
       </c>
       <c r="F53" t="s">
-        <v>341</v>
+        <v>247</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
-        <v>16crag</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>14tile</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C54" t="s">
-        <v>351</v>
+        <v>681</v>
       </c>
       <c r="D54" t="s">
-        <v>347</v>
+        <v>378</v>
       </c>
       <c r="E54" t="s">
-        <v>348</v>
+        <v>109</v>
       </c>
       <c r="F54" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
-        <v>16topo</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>14map</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B55" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="C55" t="s">
-        <v>364</v>
+        <v>291</v>
       </c>
       <c r="D55" t="s">
-        <v>342</v>
+        <v>277</v>
       </c>
       <c r="E55" t="s">
-        <v>353</v>
+        <v>278</v>
       </c>
       <c r="F55" t="s">
-        <v>112</v>
+        <v>287</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>16tile</v>
+        <v>15topo</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>178</v>
+      </c>
+      <c r="C56" t="s">
+        <v>284</v>
       </c>
       <c r="D56" t="s">
-        <v>378</v>
+        <v>285</v>
       </c>
       <c r="E56" t="s">
-        <v>109</v>
+        <v>286</v>
       </c>
       <c r="F56" t="s">
-        <v>108</v>
+        <v>287</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
-        <v>14map</v>
+        <v>15tile</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C57" t="s">
-        <v>668</v>
+        <v>292</v>
       </c>
       <c r="D57" t="s">
-        <v>379</v>
+        <v>288</v>
       </c>
       <c r="E57" t="s">
-        <v>109</v>
+        <v>289</v>
       </c>
       <c r="F57" t="s">
-        <v>108</v>
+        <v>290</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" ref="H57:H60" si="1">CONCATENATE(A57,B57)</f>
-        <v>16map</v>
+        <v>15crag</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B58" t="s">
         <v>111</v>
       </c>
       <c r="C58" t="s">
-        <v>672</v>
+        <v>682</v>
       </c>
       <c r="D58" t="s">
-        <v>380</v>
-      </c>
-      <c r="E58" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="E58" t="s">
         <v>109</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" t="s">
         <v>108</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="1"/>
-        <v>12map</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>15map</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C59" t="s">
-        <v>408</v>
+        <v>350</v>
       </c>
       <c r="D59" t="s">
-        <v>402</v>
+        <v>342</v>
       </c>
       <c r="E59" t="s">
-        <v>392</v>
-      </c>
-      <c r="F59" s="12" t="s">
-        <v>393</v>
+        <v>340</v>
+      </c>
+      <c r="F59" t="s">
+        <v>341</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="1"/>
-        <v>17topo</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>16crag</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C60" t="s">
-        <v>407</v>
+        <v>351</v>
       </c>
       <c r="D60" t="s">
-        <v>404</v>
+        <v>347</v>
       </c>
       <c r="E60" t="s">
-        <v>403</v>
+        <v>348</v>
       </c>
       <c r="F60" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="1"/>
-        <v>17crag</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>16topo</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B61" t="s">
         <v>178</v>
       </c>
       <c r="C61" t="s">
-        <v>405</v>
+        <v>364</v>
       </c>
       <c r="D61" t="s">
-        <v>406</v>
+        <v>342</v>
       </c>
       <c r="E61" t="s">
-        <v>403</v>
+        <v>353</v>
       </c>
       <c r="F61" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" ref="H61:H74" si="2">CONCATENATE(A61,B61)</f>
-        <v>17tile</v>
+        <v>16tile</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
         <v>111</v>
       </c>
       <c r="C62" t="s">
-        <v>661</v>
+        <v>667</v>
       </c>
       <c r="D62" t="s">
-        <v>409</v>
-      </c>
-      <c r="E62" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="E62" t="s">
         <v>109</v>
       </c>
       <c r="F62" t="s">
@@ -6302,100 +6367,103 @@
       </c>
       <c r="H62" t="str">
         <f t="shared" si="2"/>
-        <v>17map</v>
+        <v>16map</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>111</v>
+        <v>116</v>
+      </c>
+      <c r="C63" t="s">
+        <v>408</v>
       </c>
       <c r="D63" t="s">
-        <v>410</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F63" t="s">
-        <v>108</v>
+        <v>402</v>
+      </c>
+      <c r="E63" t="s">
+        <v>392</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>393</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="2"/>
-        <v>13map</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>17topo</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C64" t="s">
-        <v>429</v>
+        <v>407</v>
       </c>
       <c r="D64" t="s">
-        <v>430</v>
+        <v>404</v>
       </c>
       <c r="E64" t="s">
-        <v>431</v>
+        <v>403</v>
       </c>
       <c r="F64" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="2"/>
-        <v>18topo</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>17crag</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="C65" t="s">
-        <v>432</v>
+        <v>405</v>
       </c>
       <c r="D65" t="s">
-        <v>434</v>
+        <v>406</v>
       </c>
       <c r="E65" t="s">
-        <v>435</v>
+        <v>403</v>
       </c>
       <c r="F65" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="2"/>
-        <v>18crag</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>17tile</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>178</v>
+        <v>111</v>
       </c>
       <c r="C66" t="s">
-        <v>433</v>
+        <v>660</v>
       </c>
       <c r="D66" t="s">
-        <v>434</v>
-      </c>
-      <c r="E66" t="s">
-        <v>435</v>
+        <v>409</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="F66" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="2"/>
-        <v>18tile</v>
+        <v>17map</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.45">
@@ -6403,281 +6471,287 @@
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>116</v>
+      </c>
+      <c r="C67" t="s">
+        <v>429</v>
       </c>
       <c r="D67" t="s">
-        <v>437</v>
-      </c>
-      <c r="E67" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="F67" s="12" t="s">
-        <v>108</v>
+        <v>430</v>
+      </c>
+      <c r="E67" t="s">
+        <v>431</v>
+      </c>
+      <c r="F67" t="s">
+        <v>112</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" si="2"/>
-        <v>18map</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>18topo</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B68" t="s">
         <v>119</v>
       </c>
       <c r="C68" t="s">
-        <v>473</v>
+        <v>432</v>
       </c>
       <c r="D68" t="s">
-        <v>464</v>
+        <v>434</v>
       </c>
       <c r="E68" t="s">
-        <v>465</v>
-      </c>
-      <c r="F68" s="12" t="s">
-        <v>466</v>
+        <v>435</v>
+      </c>
+      <c r="F68" t="s">
+        <v>137</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="2"/>
-        <v>20crag</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>18crag</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B69" t="s">
         <v>178</v>
       </c>
       <c r="C69" t="s">
-        <v>472</v>
+        <v>433</v>
       </c>
       <c r="D69" t="s">
-        <v>464</v>
+        <v>434</v>
       </c>
       <c r="E69" t="s">
-        <v>467</v>
-      </c>
-      <c r="F69" s="12" t="s">
-        <v>466</v>
+        <v>435</v>
+      </c>
+      <c r="F69" t="s">
+        <v>137</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="2"/>
-        <v>20tile</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>18tile</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C70" t="s">
-        <v>471</v>
+        <v>685</v>
       </c>
       <c r="D70" t="s">
-        <v>468</v>
-      </c>
-      <c r="E70" t="s">
-        <v>467</v>
+        <v>437</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>469</v>
+        <v>108</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="2"/>
-        <v>20topo</v>
+        <v>18map</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B71" t="s">
-        <v>111</v>
+        <v>119</v>
+      </c>
+      <c r="C71" t="s">
+        <v>485</v>
       </c>
       <c r="D71" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="E71" t="s">
-        <v>109</v>
+        <v>486</v>
       </c>
       <c r="F71" t="s">
-        <v>108</v>
+        <v>290</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="2"/>
-        <v>20map</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>19crag</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="C72" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="D72" t="s">
         <v>479</v>
       </c>
       <c r="E72" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="F72" t="s">
-        <v>290</v>
+        <v>481</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="2"/>
-        <v>19crag</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>19tile</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>19</v>
       </c>
       <c r="B73" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="C73" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="D73" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="E73" t="s">
         <v>480</v>
       </c>
       <c r="F73" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="2"/>
-        <v>19tile</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>19topo</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>19</v>
       </c>
       <c r="B74" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C74" t="s">
-        <v>484</v>
+        <v>661</v>
       </c>
       <c r="D74" t="s">
-        <v>483</v>
-      </c>
-      <c r="E74" t="s">
-        <v>480</v>
+        <v>490</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="F74" t="s">
-        <v>482</v>
+        <v>108</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="2"/>
-        <v>19topo</v>
+        <v>19map</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A75">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B75" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C75" t="s">
-        <v>662</v>
+        <v>473</v>
       </c>
       <c r="D75" t="s">
-        <v>490</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="F75" t="s">
-        <v>108</v>
+        <v>464</v>
+      </c>
+      <c r="E75" t="s">
+        <v>465</v>
+      </c>
+      <c r="F75" s="12" t="s">
+        <v>466</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" ref="H75" si="3">CONCATENATE(A75,B75)</f>
-        <v>19map</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>20crag</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="C76" t="s">
-        <v>514</v>
+        <v>472</v>
       </c>
       <c r="D76" t="s">
-        <v>511</v>
+        <v>464</v>
       </c>
       <c r="E76" t="s">
-        <v>512</v>
-      </c>
-      <c r="F76" t="s">
-        <v>513</v>
+        <v>467</v>
+      </c>
+      <c r="F76" s="12" t="s">
+        <v>466</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" ref="H76:H102" si="4">CONCATENATE(A76,B76)</f>
-        <v>21crag</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>20tile</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B77" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="C77" t="s">
-        <v>510</v>
+        <v>471</v>
       </c>
       <c r="D77" t="s">
-        <v>511</v>
+        <v>468</v>
       </c>
       <c r="E77" t="s">
-        <v>512</v>
-      </c>
-      <c r="F77" t="s">
-        <v>513</v>
+        <v>467</v>
+      </c>
+      <c r="F77" s="12" t="s">
+        <v>469</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="4"/>
-        <v>21tile</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>20topo</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C78" t="s">
-        <v>515</v>
+        <v>683</v>
       </c>
       <c r="D78" t="s">
-        <v>516</v>
+        <v>474</v>
       </c>
       <c r="E78" t="s">
-        <v>517</v>
+        <v>109</v>
       </c>
       <c r="F78" t="s">
-        <v>518</v>
+        <v>108</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="4"/>
-        <v>21topo</v>
+        <v>20map</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.45">
@@ -6685,81 +6759,87 @@
         <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>119</v>
+      </c>
+      <c r="C79" t="s">
+        <v>514</v>
       </c>
       <c r="D79" t="s">
-        <v>521</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>109</v>
+        <v>511</v>
+      </c>
+      <c r="E79" t="s">
+        <v>512</v>
       </c>
       <c r="F79" t="s">
-        <v>108</v>
+        <v>513</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="4"/>
-        <v>21map</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>21crag</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A80">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B80" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="C80" t="s">
-        <v>539</v>
+        <v>510</v>
       </c>
       <c r="D80" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
       <c r="E80" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="F80" t="s">
-        <v>525</v>
+        <v>513</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="4"/>
-        <v>9topo</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>21tile</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A81">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B81" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C81" t="s">
-        <v>538</v>
+        <v>515</v>
       </c>
       <c r="D81" t="s">
-        <v>528</v>
+        <v>516</v>
       </c>
       <c r="E81" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="F81" t="s">
-        <v>290</v>
+        <v>518</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="4"/>
-        <v>9crag</v>
+        <v>21topo</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A82">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B82" t="s">
         <v>111</v>
       </c>
+      <c r="C82" t="s">
+        <v>684</v>
+      </c>
       <c r="D82" t="s">
-        <v>530</v>
-      </c>
-      <c r="E82" t="s">
+        <v>521</v>
+      </c>
+      <c r="E82" s="12" t="s">
         <v>109</v>
       </c>
       <c r="F82" t="s">
@@ -6767,10 +6847,10 @@
       </c>
       <c r="H82" t="str">
         <f t="shared" si="4"/>
-        <v>9map</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+        <v>21map</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>22</v>
       </c>
@@ -6794,7 +6874,7 @@
         <v>22crag</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>22</v>
       </c>
@@ -6818,7 +6898,7 @@
         <v>22tile</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>22</v>
       </c>
@@ -6850,7 +6930,7 @@
         <v>111</v>
       </c>
       <c r="C86" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D86" t="s">
         <v>559</v>
@@ -6866,7 +6946,7 @@
         <v>22map</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>23</v>
       </c>
@@ -6890,7 +6970,7 @@
         <v>23crag</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>23</v>
       </c>
@@ -6914,7 +6994,7 @@
         <v>23tile</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>23</v>
       </c>
@@ -6946,7 +7026,7 @@
         <v>111</v>
       </c>
       <c r="C90" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D90" t="s">
         <v>577</v>
@@ -6962,7 +7042,7 @@
         <v>23map</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>24</v>
       </c>
@@ -6986,7 +7066,7 @@
         <v>24topo</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>24</v>
       </c>
@@ -7010,7 +7090,7 @@
         <v>24crag</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>24</v>
       </c>
@@ -7042,7 +7122,7 @@
         <v>111</v>
       </c>
       <c r="C94" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D94" t="s">
         <v>601</v>
@@ -7058,7 +7138,7 @@
         <v>24map</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>25</v>
       </c>
@@ -7082,7 +7162,7 @@
         <v>25crag</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>25</v>
       </c>
@@ -7114,7 +7194,7 @@
         <v>111</v>
       </c>
       <c r="C97" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D97" t="s">
         <v>635</v>
@@ -7130,7 +7210,7 @@
         <v>25map</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>25</v>
       </c>
@@ -7154,7 +7234,7 @@
         <v>25topo</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>26</v>
       </c>
@@ -7178,7 +7258,7 @@
         <v>26crag</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>26</v>
       </c>
@@ -7202,7 +7282,7 @@
         <v>26tile</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>26</v>
       </c>
@@ -7227,36 +7307,16 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A102">
-        <v>26</v>
-      </c>
-      <c r="B102" t="s">
-        <v>111</v>
-      </c>
-      <c r="D102" t="s">
-        <v>656</v>
-      </c>
-      <c r="E102" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="F102" t="s">
-        <v>108</v>
-      </c>
-      <c r="H102" t="str">
-        <f t="shared" si="4"/>
-        <v>26map</v>
-      </c>
+      <c r="E102" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F102" xr:uid="{BFB1D3BA-7B83-4CA6-BA2B-968EDE266848}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="map"/>
-      </filters>
-    </filterColumn>
+    <sortState ref="A2:F102">
+      <sortCondition ref="A1:A102"/>
+    </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E63" r:id="rId1" xr:uid="{35DF19F2-37DF-43EA-B6CA-AD2C731AF59E}"/>
+    <hyperlink ref="E50" r:id="rId1" xr:uid="{35DF19F2-37DF-43EA-B6CA-AD2C731AF59E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -12885,12 +12945,12 @@
         <f>IF(CLIMBS!S27&lt;&gt;0,1,0)</f>
         <v>1</v>
       </c>
-      <c r="F27">
+      <c r="F27" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B27,"tile"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B27,"crag"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B27,"topo"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B27,"map"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
-        <v>4</v>
+        <v>missing</v>
       </c>
       <c r="G27">
         <f>_xlfn.IFNA(IF(VLOOKUP(B27,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>

</xml_diff>

<commit_message>
added robits to fix search console error and removed null on routes without tech grade
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33997BC0-1EAC-4115-8593-864EE9655CF9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D687934-2F5D-4799-B324-616D88639810}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="696">
   <si>
     <t>cliff</t>
   </si>
@@ -2156,6 +2156,21 @@
   </si>
   <si>
     <t>tidal</t>
+  </si>
+  <si>
+    <t>Rock Around The World</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>img/guidebooks/rock-around-the-world.jpg</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2RmOhyX</t>
+  </si>
+  <si>
+    <t>9782952638876</t>
   </si>
 </sst>
 </file>
@@ -3225,7 +3240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="P29" sqref="P29"/>
     </sheetView>
@@ -7509,10 +7524,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8295,6 +8310,35 @@
       </c>
       <c r="I27">
         <v>29.95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="4">
+        <v>23</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>695</v>
+      </c>
+      <c r="C28" t="s">
+        <v>691</v>
+      </c>
+      <c r="D28" t="s">
+        <v>258</v>
+      </c>
+      <c r="E28" t="s">
+        <v>439</v>
+      </c>
+      <c r="F28" t="s">
+        <v>692</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>693</v>
+      </c>
+      <c r="H28" t="s">
+        <v>694</v>
+      </c>
+      <c r="I28">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed the duplicate template so all climb details use climbCard.js. Also added pitch by pitch info (example is Roca Gris and Wreakers slab). Also allow multiple guidebooks (example is Heiliger Geist). Some style changes for share on mobile as well as a possible fix for the iphone 10 scroll issue. I also removed the old map images (the google ones).
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BC9BCC-70EE-4D17-9713-0B9BE188C6CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E7C4D1-EDC8-4C6C-AF54-2C2885CA49AD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="6135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10785" windowHeight="4050" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="700">
   <si>
     <t>cliff</t>
   </si>
@@ -2167,32 +2167,52 @@
     <t>9782952638876</t>
   </si>
   <si>
-    <t>pitchs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It's fair to say everyone has a slightly different experience on wreakers slab, partly because the cliff is loose and the holds likely change regularly, even between the leader and the second! This makes helmets an absolute must. Due to its scale it's likely a lot of people also take slightly different lines, especially at the bottom and top pitches where the route is less clear. I think it justifies the grade of VS 4b. With the low technical grade it's an easy route to underestimate. A lot of the protection early on is marginal and some placements could actually make the climb more dangerous. For instance, a cam behind a large loose block could put the seconds life in danger. In short, it's not an ideal choice for those new to traditional multi-pitch climbing, but it offers stunning views and is a wonderful lengthy adventure if you have the experience lead it.
+    <t>Pitches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Park in the lower parking lot of Vinya Nova (41.585600, 1.816281). From there take the path north into the forest towards Torrent del Pont. Advance through the torrent and shortly after follow the path that goes to the right (milestones and white marks). Follow this uphill and arrive at a turnoff, head north. Pass by the foot of Pollegó de la Vinya Nova. Continue to the base of the Gray Rock.&lt;br /&gt;&lt;br /&gt;
+The decent requires 3 abseils of 40m, 40m and just under 60m. To find the anchor to abseil you need to walk along the ridge for 80m. You go over a couple of small peaks. You may want to stay roped for this slinging the occasional bush as the ground can be loose. If you use a pair of 50m ropes you can either use a tree to break the last abseil into 2 or create a trad anchor on the way or even abseil carefully off the end of the rope and downclimb the last 10m. All these options have risk especially if you end up doing it in the dark. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esparraguera offers an exciting 190m HVS (f5c) multi-pitch climb on the fantastic conglomerate rock of Montserrat in Spain. The route is sustained and consistent in grade. The hardest pitch is steep but has big holds and is well bolted, this may well feel like the easiest pitch if you are used to indoor climbing / bouldering. Whilst described as a clean trad route in many guidebooks, Esparraguera has a good amount bolts (17) and pitons (2) in sections in the middle pitches. Most of the harder moves are protected by old bolts. You will need a full trad rack of nuts and cams. Tri cams are particularly helpful for the pockets. The last pitch has no fixed protection. The route is given f5c in some guides or UIAA V+ in others, it is hard to convert to British grades but given the protection is good at the harder sections, the British grade of HVS 5a (maybe 5b) seems best. If anything feels hard, take some time and search for better holds, there will be some. The decent requires 3 abseils of 40m, 40m and just under 60m. </t>
+  </si>
+  <si>
+    <t>pitchInfo</t>
+  </si>
+  <si>
+    <t>It's fair to say everyone has a slightly different experience on wreckers slab, partly because the cliff is loose and the holds likely change regularly, even between the leader and the second! This makes helmets an absolute must. Due to its scale it's likely a lot of people also take slightly different lines, especially at the bottom and top pitches where the route is less clear. I think it justifies the grade of VS 4b. With the low technical grade it's an easy route to underestimate. A lot of the protection early on is marginal and some placements could actually make the climb more dangerous. For instance, a cam behind a large loose block could put the seconds life in danger. In short, it's not an ideal choice for those new to traditional multi-pitch climbing, but it offers stunning views and is a wonderful lengthy adventure if you have the experience lead it.
 &lt;br /&gt;
-&lt;strong&gt;Pitch 1&lt;/strong&gt;&lt;br /&gt;
-My experience here is reasonably worthless except to say if you leave the guidebook at the top of the cliff (because who wants to climb with a guide book in their bag), then the chances are you won’t actually know exactly which way to go and may attack the first belay head on. This takes you over loose ground with little or no gear and possibly makes the route a harder grade. Instead I’d recommend you don’t start too far right, climb up a few of meters to where the cliff eases off then traverse all the way left and head up to the belay.
+&lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;40m&lt;/span&gt; &lt;span class="pitchGrade""&gt;4a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+My experience here is reasonably worthless except to say if you leave the guidebook at the top of the cliff (because who wants to climb with a guide book in their bag), then the chances are you won’t actually know exactly which way to go and may attack the first belay head on. This takes you over loose ground with little or no gear and possibly makes the route a harder grade. Instead I’d recommend you don’t start too far right, climb up a few of meters to where the cliff eases off then traverse all the way left to the arete and head up to the belay.
 &lt;br /&gt;
 There are 2 pegs that you can use to form part of your belay. I’d highly recommend a 3 or 4 point anchor in addition to them. I placed my gear below the pegs giving a reasonably comfy ledge to belay from. Your nut tool comes in handy to clean the cracks when you lead this pitch!
 &lt;br /&gt;
-&lt;strong&gt;Pitch 2&lt;/strong&gt;&lt;br /&gt;
-Head up and around the overhanging block just above the belay. Whilst this is probably the steepest part of the climb it’s not fully vertical making gear placements easier than it looks. Be careful not to throw too many handholds at the belay below and follow the reasonably obvious crack up to a big grassy ledge with a pillar of rock on it.  There are lots of options for a multi-point anchor here. You can use the front of the pillar, side or even the nearby crack.
+&lt;strong class="pitch-title"&gt;Pitch 2 – &lt;span class="length"&gt;40m&lt;/span&gt; &lt;span class="pitchGrade""&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Head up and around the overhanging block just above the belay. Whilst this is probably the steepest part of the climb it’s not fully vertical making gear placements easier than it looks. Be careful not to throw too many handholds at the belay below and follow the reasonably obvious crack up to a big grassy ledge with a pillar of rock on it.  There are lots of options to build a traditional anchor here. You can use the front of the pillar, side or even the nearby crack further up.
 &lt;br /&gt;
-&lt;strong&gt;Pitch 3&lt;/strong&gt;&lt;br /&gt;
-This is where the rock climbing becomes utterly enjoyable. For the most part the rock is solid and there are plenty of placements for gear the left hand ridge is recommended with its stunning if a little intense views. Guidebooks suggest the pitch is 45m, but a the full 50m will take you over the top and right a little. A good belay can be built on the other side of the top ridge. Consider belaying your partner off the top 10m walk. It would be a stretch to call it a 4th pitch, but placing a couple of pieces of gear makes it a safer scrable.
-</t>
-  </si>
-  <si>
-    <t>Pitches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Park in the lower parking lot of Vinya Nova (41.585600, 1.816281). From there take the path north into the forest towards Torrent del Pont. Advance through the torrent and shortly after follow the path that goes to the right (milestones and white marks). Follow this uphill and arrive at a turnoff, head north. Pass by the foot of Pollegó de la Vinya Nova. Continue to the base of the Gray Rock.&lt;br /&gt;&lt;br /&gt;
-The decent requires 3 abseils of 40m, 40m and just under 60m. To find the anchor to abseil you need to walk along the ridge for 80m. You go over a couple of small peaks. You may want to stay roped for this slinging the occasional bush as the ground can be loose. If you use a pair of 50m ropes you can either use a tree to break the last abseil into 2 or create a trad anchor on the way or even abseil carefully off the end of the rope and downclimb the last 10m. All these options have risk especially if you end up doing it in the dark. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esparraguera offers an exciting 190m HVS (f5c) multi-pitch climb on the fantastic conglomerate rock of Montserrat in Spain. The route is sustained and consistent in grade. The hardest pitch is steep but has big holds and is well bolted, this may well feel like the easiest pitch if you are used to indoor climbing / bouldering. Whilst described as a clean trad route in many guidebooks, Esparraguera has a good amount bolts (17) and pitons (2) in sections in the middle pitches. Most of the harder moves are protected by old bolts. You will need a full trad rack of nuts and cams. Tri cams are particularly helpful for the pockets. The last pitch has no fixed protection. The route is given f5c in some guides or UIAA V+ in others, it is hard to convert to British grades but given the protection is good at the harder sections, the British grade of HVS 5a seems best. If anything feels hard, take some time and search for better holds, there will be some. The decent requires 3 abseils of 40m, 40m and just under 60m. </t>
+&lt;strong class="pitch-title"&gt;Pitch 3 – &lt;span class="length"&gt;50m&lt;/span&gt; &lt;span class="pitchGrade""&gt;4a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+This is where the rock climbing becomes utterly enjoyable. For the most part the rock is solid and there are plenty of placements for gear, the left ridge is recommended with its stunning if a little intense views. Guidebooks suggest the pitch is 45m, but a the full 50m will take you over the top and right a little. A good belay can be built on the other side of the top ridge. Consider belaying your partner off the top 10m walk. It would be a stretch to call it a 4th pitch, but placing a couple of pieces of gear makes it a safer scramble.</t>
+  </si>
+  <si>
+    <t>This route is a popular mixed multi-pitch rock climb. Because it’s an absolute classic it can be popular, even out of season. The climb is interesting and sustained, with a mixture of delicate slab work and a few big moves on a steep wall on the 3rd pitch. The views are incredible looking out over the valley and the exposure is immense in places.  Especially where the climb moves between the spires, up the middle of the 4th pitch and the travers across a ledge on the 5th pitch. The route could be climbed clean without use of the bolts if you have the confidence, time, patience and stamina to find protection on the slab sections which can be quite blank. It’s quicker and likely more enjoyable if you climb the route mixed, using the in-situ bolts and with additional gear to protect the run out sections on the 1st, 4th and 5th pitches and protection for the entire 6th pitch. A set of cams, nuts and tri-cams should cover you. Larger pieces could be helpful on the last pitch. 50m ropes are enough to get to the top, but 60m ropes are needed for the decent to save down climbing the last abseil or using a tree / bush for the last part. The rock can be loose, especially on pitch 1. Loose rocks also tend to gather on the ledges, so make sure you wear helmet and try to avid dislodging rock onto the path below which can be popular with hikers (who won’t have helmets). All the belay points have 3 expansion bolts which can be used for the anchors, except the top of the route where you will need to sling a bush or two and make sure you are not belaying more weight up than can be comfortably held. If climbing as a 3, it would be safer to belay the 2nd and 3rd climber separately on this pitch.
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;35m&lt;/span&gt; &lt;span class="pitchGrade" uiaa"&gt;IV+&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+The first pitch moves up to some trees on the ledge then left onto the ridge and directly up the centre of the slab spire to the belay. 
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 2 –&lt;span class="length"&gt;40m&lt;/span&gt; &lt;span class="pitchGrade" uiaa"&gt;V&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Climb up the spire to some harder moves not long after the belay. These are well protected by bolts and pitons. This pitch then eases off near the top to a belay behind the next spire.
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;25m&lt;/span&gt; &lt;span class="pitchGrade" uiaa"&gt;V+&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Climb the steep face using the big pockets which make for jug sized hand holds. Follow the bolts up onto the summit of this little spire and find the anchor in the gap between the next spire. This pitch is a quite different in style to the others, so although the crux on paper it may fell super easy to someone comfortable with bouldering.
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 4 –&lt;span class="length"&gt;50m&lt;/span&gt; &lt;span class="pitchGrade" uiaa"&gt;V&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+A long, exposed climb up the largest spire. Harder moves early on that change into a lower angled slab with no bolts and limited protection options.  The anchor is to the right near where this spire joins the next. Don’t climb to the top of this spire. 
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 5 –&lt;span class="length"&gt;25m&lt;/span&gt; &lt;span class="pitchGrade" uiaa"&gt;IV&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+The is a single bolt on this pitch and no clear path to the next anchor. Moving up to a ledge and wall offers good hand holds and some pockets for protection, before a traverse right to the anchor. 
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 6 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade" uiaa"&gt;IV+&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Move straight up following the crack system. There is no fixed protection but a number of placements can be found. Move over a small ledge to the summit. This is a sustained pitch of UIAA grave IV or IV+ all the way. There are no bolts at the top so you will need to sling a bush or two and make sure you are not belaying more weight up than can be comfortably held. If climbing as a 3, it would be safer to belay the 2nd and 3rd climber separately on this pitch.</t>
   </si>
 </sst>
 </file>
@@ -3282,9 +3302,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R13" sqref="R13"/>
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3368,7 +3388,7 @@
         <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>18</v>
@@ -4001,7 +4021,7 @@
         <v>104</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>189</v>
@@ -4095,7 +4115,7 @@
         <v>190</v>
       </c>
       <c r="H13" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I13" s="2">
         <v>6</v>
@@ -4125,16 +4145,21 @@
         <v>212</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>697</v>
-      </c>
-      <c r="T13" s="3"/>
+        <v>695</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>699</v>
+      </c>
       <c r="V13" s="2" t="s">
         <v>190</v>
       </c>
       <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
         <v>1</v>
       </c>
     </row>
@@ -4571,10 +4596,9 @@
       <c r="R20" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="S20" t="s">
+      <c r="S20" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="T20"/>
       <c r="U20" s="2" t="s">
         <v>189</v>
       </c>
@@ -5038,8 +5062,8 @@
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="S28" s="17"/>
-      <c r="T28" s="17"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
@@ -7584,8 +7608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="116" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="116" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12247,7 +12271,7 @@
         <v>366</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
@@ -12698,7 +12722,7 @@
       </c>
       <c r="I12">
         <f>IF(CLIMBS!T13 &lt;&gt;0,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
added guidebook info an a css change
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E7C4D1-EDC8-4C6C-AF54-2C2885CA49AD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C180321C-D64F-43A0-B15B-76A934A129EC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10785" windowHeight="4050" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="700">
   <si>
     <t>cliff</t>
   </si>
@@ -2155,9 +2155,6 @@
     <t>Rock Around The World</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>img/guidebooks/rock-around-the-world.jpg</t>
   </si>
   <si>
@@ -2213,6 +2210,9 @@
 &lt;br /&gt;
 &lt;strong class="pitch-title"&gt;Pitch 6 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade" uiaa"&gt;IV+&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
 Move straight up following the crack system. There is no fixed protection but a number of placements can be found. Move over a small ledge to the summit. This is a sustained pitch of UIAA grave IV or IV+ all the way. There are no bolts at the top so you will need to sling a bush or two and make sure you are not belaying more weight up than can be comfortably held. If climbing as a 3, it would be safer to belay the 2nd and 3rd climber separately on this pitch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The book is in French and English and covers regions around the world. The book has clear photo topographies of most routes and good descriptions including gear recommendations. The book covers trad, sport and mixed protection routes like Traumpfeiler. The only issue is, its not a cheap book, but it's well designed and tends to cover harder longer routes with most graded TD / ED alpine grades which is low to mid E grades in the British system, i.e. serious climbs. </t>
   </si>
 </sst>
 </file>
@@ -3388,7 +3388,7 @@
         <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>18</v>
@@ -4021,7 +4021,7 @@
         <v>104</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>189</v>
@@ -4145,13 +4145,13 @@
         <v>212</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="V13" s="2" t="s">
         <v>190</v>
@@ -7609,7 +7609,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="116" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8399,7 +8399,7 @@
         <v>23</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C28" t="s">
         <v>689</v>
@@ -8407,17 +8407,17 @@
       <c r="D28" t="s">
         <v>257</v>
       </c>
-      <c r="E28" t="s">
-        <v>437</v>
+      <c r="E28">
+        <v>157</v>
       </c>
       <c r="F28" t="s">
+        <v>699</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>690</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="H28" t="s">
         <v>691</v>
-      </c>
-      <c r="H28" t="s">
-        <v>692</v>
       </c>
       <c r="I28">
         <v>35</v>
@@ -12271,7 +12271,7 @@
         <v>366</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
added a super zoom for roca gris, fixed a favicon loading issue, deffered the tracking to the  bottom of the page for faster crucial content loading,oh and added some meta descriptions. I did it all on the boat yesterday but had no interwebs
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C180321C-D64F-43A0-B15B-76A934A129EC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACCE890-6378-41CE-9A6D-8A20D0E870DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10785" windowHeight="4050" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10785" windowHeight="4050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="716">
   <si>
     <t>cliff</t>
   </si>
@@ -2213,6 +2213,54 @@
   </si>
   <si>
     <t xml:space="preserve">The book is in French and English and covers regions around the world. The book has clear photo topographies of most routes and good descriptions including gear recommendations. The book covers trad, sport and mixed protection routes like Traumpfeiler. The only issue is, its not a cheap book, but it's well designed and tends to cover harder longer routes with most graded TD / ED alpine grades which is low to mid E grades in the British system, i.e. serious climbs. </t>
+  </si>
+  <si>
+    <t>jordan</t>
+  </si>
+  <si>
+    <t>Sandstone</t>
+  </si>
+  <si>
+    <t>Jodan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wadi Rum </t>
+  </si>
+  <si>
+    <t>Rum Doodle</t>
+  </si>
+  <si>
+    <t>Difficile</t>
+  </si>
+  <si>
+    <t>Djebel Rum</t>
+  </si>
+  <si>
+    <t>29.569981,35.406197</t>
+  </si>
+  <si>
+    <t>super</t>
+  </si>
+  <si>
+    <t>Super Zoom for Grey Rock climb in Montserrat</t>
+  </si>
+  <si>
+    <t>https://www.multi-pitch.com</t>
+  </si>
+  <si>
+    <t>img/topos/montserrat/zoom/</t>
+  </si>
+  <si>
+    <t>Cathedral Rock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teneriffe </t>
+  </si>
+  <si>
+    <t>28.2222531,-16.6373766</t>
+  </si>
+  <si>
+    <t>Via Mendez &amp; Guillermo</t>
   </si>
 </sst>
 </file>
@@ -3302,9 +3350,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5062,8 +5110,112 @@
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>706</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="2">
+        <v>27</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="G28" s="2">
+        <v>250</v>
+      </c>
+      <c r="H28" s="2">
+        <v>9</v>
+      </c>
+      <c r="I28" s="2">
+        <v>4</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="O28" s="2">
+        <v>30</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>701</v>
+      </c>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="2">
+        <v>28</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="G29" s="2">
+        <v>115</v>
+      </c>
+      <c r="H29" s="2">
+        <v>3</v>
+      </c>
+      <c r="I29" s="2">
+        <v>6</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="O29" s="2">
+        <v>15</v>
+      </c>
+      <c r="P29" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
@@ -5080,9 +5232,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="103" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="103" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7504,9 +7656,27 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>12</v>
+      </c>
+      <c r="B103" t="s">
+        <v>708</v>
+      </c>
+      <c r="C103" t="s">
+        <v>711</v>
+      </c>
+      <c r="D103" t="s">
+        <v>709</v>
+      </c>
+      <c r="E103" s="13" t="s">
+        <v>710</v>
+      </c>
+      <c r="F103" t="s">
+        <v>171</v>
+      </c>
       <c r="H103" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>12super</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.45">
@@ -7599,8 +7769,11 @@
       <sortCondition ref="A1:A102"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="E103" r:id="rId1" xr:uid="{0A321C65-D310-4F4B-93FB-7FA86D5B9B94}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7608,7 +7781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="116" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="116" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -8439,7 +8612,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C24:C25"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8638,7 +8811,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12229,10 +12402,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13331,8 +13504,48 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" t="str">
+        <f>CLIMBS!A28</f>
+        <v>Djebel Rum</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" t="str">
+        <f>CLIMBS!B28</f>
+        <v>draft</v>
+      </c>
+      <c r="D28">
+        <f>IF(CLIMBS!R28&lt;&gt;0,1,0)+IF(CLIMBS!G28&lt;&gt;0,1,0)+IF(CLIMBS!H28&lt;&gt;0,1,0)+IF(CLIMBS!I28&lt;&gt;0,1,0)+IF(CLIMBS!J28&lt;&gt;0,1,0)+IF(CLIMBS!N28&lt;&gt;0,1,0)+IF(CLIMBS!M28&lt;&gt;0,1,0)+IF(CLIMBS!O28&lt;&gt;0,1,0)+IF(CLIMBS!P28&lt;&gt;0,1,0)</f>
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <f>IF(CLIMBS!S28&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B28,"tile"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B28,"crag"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B28,"topo"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B28,"map"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B28,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B28,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f>IF(CLIMBS!T29 &lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
@@ -13340,7 +13553,7 @@
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C27">
+  <conditionalFormatting sqref="C2:C28">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"draft"</formula>
     </cfRule>
@@ -13350,12 +13563,12 @@
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C27">
+  <conditionalFormatting sqref="C3:C28">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E27">
+  <conditionalFormatting sqref="E2:E28">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -13371,7 +13584,7 @@
       <formula>"missing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H27">
+  <conditionalFormatting sqref="G2:H28">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -13379,7 +13592,7 @@
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I27">
+  <conditionalFormatting sqref="I2:I28">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
fixed zoom for production
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACCE890-6378-41CE-9A6D-8A20D0E870DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2609BFBC-3488-40BE-8642-7DB9F60618FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10785" windowHeight="4050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="718">
   <si>
     <t>cliff</t>
   </si>
@@ -2261,6 +2261,12 @@
   </si>
   <si>
     <t>Via Mendez &amp; Guillermo</t>
+  </si>
+  <si>
+    <t>Refs</t>
+  </si>
+  <si>
+    <t>3a</t>
   </si>
 </sst>
 </file>
@@ -3350,9 +3356,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R29" sqref="R29"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3859,6 +3865,9 @@
       </c>
       <c r="J8" s="2" t="s">
         <v>89</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>717</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>51</v>
@@ -12402,10 +12411,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12416,9 +12425,10 @@
     <col min="6" max="6" width="8.265625" customWidth="1"/>
     <col min="7" max="7" width="11.59765625" customWidth="1"/>
     <col min="8" max="8" width="10.1328125" customWidth="1"/>
+    <col min="9" max="9" width="7.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="11" t="s">
         <v>361</v>
       </c>
@@ -12444,10 +12454,13 @@
         <v>366</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>716</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>CLIMBS!A2</f>
         <v>Old Man of Stoer</v>
@@ -12484,11 +12497,15 @@
         <v>1</v>
       </c>
       <c r="I2">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B2,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
         <f>IF(CLIMBS!T3 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f>CLIMBS!A3</f>
         <v>Bosigran</v>
@@ -12525,11 +12542,15 @@
         <v>1</v>
       </c>
       <c r="I3">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B3,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
         <f>IF(CLIMBS!T4 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f>CLIMBS!A4</f>
         <v>Clogwyn Du'r Arddu</v>
@@ -12566,11 +12587,15 @@
         <v>1</v>
       </c>
       <c r="I4">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B4,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J4">
         <f>IF(CLIMBS!T5 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f>CLIMBS!A5</f>
         <v>Vratsa</v>
@@ -12607,11 +12632,15 @@
         <v>0</v>
       </c>
       <c r="I5">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B5,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J5">
         <f>IF(CLIMBS!T6 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
         <f>CLIMBS!A6</f>
         <v>Tormore Group</v>
@@ -12648,11 +12677,15 @@
         <v>1</v>
       </c>
       <c r="I6">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B6,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J6">
         <f>IF(CLIMBS!T7 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <f>CLIMBS!A7</f>
         <v>Sass Pordoi</v>
@@ -12689,11 +12722,15 @@
         <v>1</v>
       </c>
       <c r="I7">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B7,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J7">
         <f>IF(CLIMBS!T8 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
         <f>CLIMBS!A8</f>
         <v>Cwm Idwal</v>
@@ -12730,11 +12767,15 @@
         <v>1</v>
       </c>
       <c r="I8">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B8,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J8">
         <f>IF(CLIMBS!T9 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="str">
         <f>CLIMBS!A9</f>
         <v>Lundy</v>
@@ -12771,11 +12812,15 @@
         <v>1</v>
       </c>
       <c r="I9">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B9,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J9">
         <f>IF(CLIMBS!T10 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
         <f>CLIMBS!A10</f>
         <v>Meadinha</v>
@@ -12812,11 +12857,15 @@
         <v>1</v>
       </c>
       <c r="I10">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B10,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J10">
         <f>IF(CLIMBS!T11 &lt;&gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="str">
         <f>CLIMBS!A11</f>
         <v>Cornakey Cliff</v>
@@ -12853,11 +12902,15 @@
         <v>1</v>
       </c>
       <c r="I11">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B11,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J11">
         <f>IF(CLIMBS!T12 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="str">
         <f>CLIMBS!A12</f>
         <v>Cir Mhor</v>
@@ -12894,11 +12947,15 @@
         <v>1</v>
       </c>
       <c r="I12">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B12,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J12">
         <f>IF(CLIMBS!T13 &lt;&gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="str">
         <f>CLIMBS!A13</f>
         <v>Roca Gris</v>
@@ -12935,11 +12992,15 @@
         <v>1</v>
       </c>
       <c r="I13">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B13,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J13">
         <f>IF(CLIMBS!T14 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="str">
         <f>CLIMBS!A14</f>
         <v>Sail Rock</v>
@@ -12976,11 +13037,15 @@
         <v>1</v>
       </c>
       <c r="I14">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B14,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J14">
         <f>IF(CLIMBS!T15 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="str">
         <f>CLIMBS!A15</f>
         <v>Chair Ladder</v>
@@ -13017,11 +13082,15 @@
         <v>1</v>
       </c>
       <c r="I15">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B15,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
         <f>IF(CLIMBS!T16 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="str">
         <f>CLIMBS!A16</f>
         <v>The Devils Tower</v>
@@ -13058,11 +13127,15 @@
         <v>1</v>
       </c>
       <c r="I16">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B16,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J16">
         <f>IF(CLIMBS!T17 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="str">
         <f>CLIMBS!A17</f>
         <v>Lliwedd</v>
@@ -13099,11 +13172,15 @@
         <v>1</v>
       </c>
       <c r="I17">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B17,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J17">
         <f>IF(CLIMBS!T18 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="str">
         <f>CLIMBS!A18</f>
         <v>Stetind</v>
@@ -13140,11 +13217,15 @@
         <v>1</v>
       </c>
       <c r="I18">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B18,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J18">
         <f>IF(CLIMBS!T19 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="str">
         <f>CLIMBS!A19</f>
         <v>Scafell</v>
@@ -13180,11 +13261,15 @@
         <v>1</v>
       </c>
       <c r="I19">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B19,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J19">
         <f>IF(CLIMBS!T20 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="str">
         <f>CLIMBS!A20</f>
         <v>Mount Indefatigable</v>
@@ -13220,11 +13305,15 @@
         <v>1</v>
       </c>
       <c r="I20">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B20,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J20">
         <f>IF(CLIMBS!T21 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="str">
         <f>CLIMBS!A21</f>
         <v>Slieve Beg</v>
@@ -13260,11 +13349,15 @@
         <v>1</v>
       </c>
       <c r="I21">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B21,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J21">
         <f>IF(CLIMBS!T22 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="str">
         <f>CLIMBS!A22</f>
         <v>Lion Rock</v>
@@ -13300,11 +13393,15 @@
         <v>1</v>
       </c>
       <c r="I22">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B22,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J22">
         <f>IF(CLIMBS!T23 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="str">
         <f>CLIMBS!A23</f>
         <v>Peñón de Ifach</v>
@@ -13340,11 +13437,15 @@
         <v>1</v>
       </c>
       <c r="I23">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B23,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
         <f>IF(CLIMBS!T24 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="str">
         <f>CLIMBS!A24</f>
         <v>Heiliger Geist</v>
@@ -13380,11 +13481,15 @@
         <v>1</v>
       </c>
       <c r="I24">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B24,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J24">
         <f>IF(CLIMBS!T25 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="str">
         <f>CLIMBS!A25</f>
         <v>Aiguille Dibona</v>
@@ -13420,11 +13525,15 @@
         <v>1</v>
       </c>
       <c r="I25">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B25,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J25">
         <f>IF(CLIMBS!T26 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="str">
         <f>CLIMBS!A26</f>
         <v>Brüggler</v>
@@ -13460,11 +13569,15 @@
         <v>0</v>
       </c>
       <c r="I26">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B26,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
         <f>IF(CLIMBS!T27 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="str">
         <f>CLIMBS!A27</f>
         <v>Vajolet towers</v>
@@ -13500,17 +13613,21 @@
         <v>0</v>
       </c>
       <c r="I27">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B27,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J27">
         <f>IF(CLIMBS!T28 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="str">
         <f>CLIMBS!A28</f>
         <v>Djebel Rum</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" t="str">
         <f>CLIMBS!B28</f>
@@ -13524,28 +13641,76 @@
         <f>IF(CLIMBS!S28&lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
-      <c r="F28">
+      <c r="F28" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B28,"tile"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B28,"crag"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B28,"topo"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B28,"map"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
-        <v>4</v>
+        <v>missing</v>
       </c>
       <c r="G28">
         <f>_xlfn.IFNA(IF(VLOOKUP(B28,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28">
         <f>_xlfn.IFNA(IF(VLOOKUP(B28,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
         <v>0</v>
       </c>
       <c r="I28">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B28,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J28">
         <f>IF(CLIMBS!T29 &lt;&gt;0,1,0)</f>
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" t="str">
+        <f>CLIMBS!A29</f>
+        <v>Cathedral Rock</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="str">
+        <f>CLIMBS!B29</f>
+        <v>draft</v>
+      </c>
+      <c r="D29">
+        <f>IF(CLIMBS!R29&lt;&gt;0,1,0)+IF(CLIMBS!G29&lt;&gt;0,1,0)+IF(CLIMBS!H29&lt;&gt;0,1,0)+IF(CLIMBS!I29&lt;&gt;0,1,0)+IF(CLIMBS!J29&lt;&gt;0,1,0)+IF(CLIMBS!N29&lt;&gt;0,1,0)+IF(CLIMBS!M29&lt;&gt;0,1,0)+IF(CLIMBS!O29&lt;&gt;0,1,0)+IF(CLIMBS!P29&lt;&gt;0,1,0)</f>
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <f>IF(CLIMBS!S29&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F29" t="str">
+        <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B29,"tile"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B29,"crag"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B29,"topo"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B29,"map"),IMAGES!H:H,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
+        <v>missing</v>
+      </c>
+      <c r="G29">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B29,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B29,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B29,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f>IF(CLIMBS!T30 &lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
@@ -13553,7 +13718,7 @@
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C28">
+  <conditionalFormatting sqref="C2:C29">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"draft"</formula>
     </cfRule>
@@ -13563,12 +13728,12 @@
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C28">
+  <conditionalFormatting sqref="C3:C29">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E28">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -13584,7 +13749,7 @@
       <formula>"missing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H28">
+  <conditionalFormatting sqref="G2:I29">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -13592,7 +13757,7 @@
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I28">
+  <conditionalFormatting sqref="J2:J29">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
added topo builder v0.1. Plus removing google from critical path page load
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2609BFBC-3488-40BE-8642-7DB9F60618FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BAA883-B103-49BF-83D3-FB9B94E0EC33}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="15390" windowHeight="9532" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="722">
   <si>
     <t>cliff</t>
   </si>
@@ -2267,6 +2267,18 @@
   </si>
   <si>
     <t>3a</t>
+  </si>
+  <si>
+    <t>Setesdal</t>
+  </si>
+  <si>
+    <t>https://earth.app.goo.gl/XCHT6i</t>
+  </si>
+  <si>
+    <t>location on Google Earth</t>
+  </si>
+  <si>
+    <t>Brilliant drawn topo and blog</t>
   </si>
 </sst>
 </file>
@@ -3356,9 +3368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K8" sqref="K8"/>
+      <selection pane="topRight" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5226,6 +5238,17 @@
         <v>701</v>
       </c>
     </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="2">
+        <v>29</v>
+      </c>
+    </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>541</v>
@@ -5242,8 +5265,8 @@
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView zoomScale="103" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7686,66 +7709,6 @@
       <c r="H103" t="str">
         <f t="shared" si="4"/>
         <v>12super</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H104" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H105" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H106" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H107" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H108" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H109" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H110" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H111" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H112" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="113" spans="8:8" x14ac:dyDescent="0.45">
-      <c r="H113" t="str">
-        <f t="shared" si="4"/>
-        <v/>
       </c>
     </row>
     <row r="114" spans="8:8" x14ac:dyDescent="0.45">
@@ -8618,10 +8581,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8808,6 +8771,28 @@
       </c>
       <c r="C16" t="s">
         <v>603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>719</v>
+      </c>
+      <c r="C17" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" t="s">
+        <v>721</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
so much maths, so much code, even I'm surprised it works most of the time! One bug in the topo if drawn with belay missing but absail in (edge case).
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BAA883-B103-49BF-83D3-FB9B94E0EC33}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F007D28-1814-4DF7-8D2E-B40B4D4CC797}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="15390" windowHeight="9532" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="723">
   <si>
     <t>cliff</t>
   </si>
@@ -2279,6 +2279,9 @@
   </si>
   <si>
     <t>Brilliant drawn topo and blog</t>
+  </si>
+  <si>
+    <t>El Catedral, (the Cathedral in English) is a volcanic plug that stands in Teide National Park in the centre of Tenerife. It offers a variety of traditional multipitch climbs that tend to be around 3 or 4 pitches in length to reach that summit via just over 100 meters of climbing. Whilst Tenerife has a lot of incredible climbing the majority of it is single pitch sport routes. El Catedral offers some of the best trad multi-pitch climbing on the island.  In order to climb there, you need to seek permission from the national park which seems to be a straightforward process (see links in references section below). The route Via Mendez &amp; Guillermo is not the original route up the face but offers a high quality adventure at grade UIAA V+. Whilst a completely different grading system it sits around VS. There are easier options to the summit if needed like the original route which is graded UIAA IV or around VDiff in British grades.</t>
   </si>
 </sst>
 </file>
@@ -3368,9 +3371,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y31" sqref="Y31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5235,7 +5238,13 @@
         <v>1</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>701</v>
+        <v>41</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.45">
@@ -5264,8 +5273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
@@ -8583,7 +8592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -9147,8 +9156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745174B4-A8CA-45B8-ACCB-9B5B609F0D5D}">
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="N70" sqref="N70"/>
+    <sheetView topLeftCell="A50" zoomScale="94" workbookViewId="0">
+      <selection activeCell="O74" sqref="O74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12341,16 +12350,272 @@
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A71" s="15">
+        <v>25</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="C71" s="15">
+        <v>10</v>
+      </c>
+      <c r="D71" s="15">
+        <v>10</v>
+      </c>
+      <c r="E71" s="15">
+        <v>12</v>
+      </c>
+      <c r="F71" s="15">
+        <v>14</v>
+      </c>
+      <c r="G71" s="15">
+        <v>16</v>
+      </c>
+      <c r="H71" s="15">
+        <v>17</v>
+      </c>
+      <c r="I71" s="15">
+        <v>17</v>
+      </c>
+      <c r="J71" s="15">
+        <v>16</v>
+      </c>
+      <c r="K71" s="15">
+        <v>13</v>
+      </c>
+      <c r="L71" s="15">
+        <v>10</v>
+      </c>
+      <c r="M71" s="15">
+        <v>11</v>
+      </c>
+      <c r="N71" s="15">
+        <v>12</v>
+      </c>
       <c r="U71" s="8"/>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A72" s="14">
+        <v>25</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C72" s="14">
+        <v>-7</v>
+      </c>
+      <c r="D72" s="14">
+        <v>-8</v>
+      </c>
+      <c r="E72" s="14">
+        <v>-5</v>
+      </c>
+      <c r="F72" s="14">
+        <v>-2</v>
+      </c>
+      <c r="G72" s="14">
+        <v>1</v>
+      </c>
+      <c r="H72" s="14">
+        <v>5</v>
+      </c>
+      <c r="I72" s="14">
+        <v>7</v>
+      </c>
+      <c r="J72" s="14">
+        <v>8</v>
+      </c>
+      <c r="K72" s="14">
+        <v>4</v>
+      </c>
+      <c r="L72" s="14">
+        <v>1</v>
+      </c>
+      <c r="M72" s="14">
+        <v>-4</v>
+      </c>
+      <c r="N72" s="14">
+        <v>-6</v>
+      </c>
       <c r="U72" s="8"/>
     </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A73" s="16">
+        <v>25</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="C73" s="16">
+        <v>-1</v>
+      </c>
+      <c r="D73" s="16">
+        <v>-1</v>
+      </c>
+      <c r="E73" s="16">
+        <v>2</v>
+      </c>
+      <c r="F73" s="16">
+        <v>6</v>
+      </c>
+      <c r="G73" s="16">
+        <v>10</v>
+      </c>
+      <c r="H73" s="16">
+        <v>12</v>
+      </c>
+      <c r="I73" s="16">
+        <v>15</v>
+      </c>
+      <c r="J73" s="16">
+        <v>16</v>
+      </c>
+      <c r="K73" s="16">
+        <v>13</v>
+      </c>
+      <c r="L73" s="16">
+        <v>10</v>
+      </c>
+      <c r="M73" s="16">
+        <v>3</v>
+      </c>
+      <c r="N73" s="16">
+        <v>-1</v>
+      </c>
+    </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A74" s="15">
+        <v>28</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="C74" s="15">
+        <v>4</v>
+      </c>
+      <c r="D74" s="15">
+        <v>4</v>
+      </c>
+      <c r="E74" s="15">
+        <v>4</v>
+      </c>
+      <c r="F74" s="15">
+        <v>4</v>
+      </c>
+      <c r="G74" s="15">
+        <v>4</v>
+      </c>
+      <c r="H74" s="15">
+        <v>2</v>
+      </c>
+      <c r="I74" s="15">
+        <v>0</v>
+      </c>
+      <c r="J74" s="15">
+        <v>1</v>
+      </c>
+      <c r="K74" s="15">
+        <v>2</v>
+      </c>
+      <c r="L74" s="15">
+        <v>4</v>
+      </c>
+      <c r="M74" s="15">
+        <v>5</v>
+      </c>
+      <c r="N74" s="15">
+        <v>4</v>
+      </c>
       <c r="U74" s="8"/>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A75" s="14">
+        <v>28</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C75" s="14">
+        <v>15</v>
+      </c>
+      <c r="D75" s="14">
+        <v>16</v>
+      </c>
+      <c r="E75" s="14">
+        <v>18</v>
+      </c>
+      <c r="F75" s="14">
+        <v>21</v>
+      </c>
+      <c r="G75" s="14">
+        <v>24</v>
+      </c>
+      <c r="H75" s="14">
+        <v>29</v>
+      </c>
+      <c r="I75" s="14">
+        <v>31</v>
+      </c>
+      <c r="J75" s="14">
+        <v>32</v>
+      </c>
+      <c r="K75" s="14">
+        <v>28</v>
+      </c>
+      <c r="L75" s="14">
+        <v>23</v>
+      </c>
+      <c r="M75" s="14">
+        <v>18</v>
+      </c>
+      <c r="N75" s="14">
+        <v>16</v>
+      </c>
       <c r="U75" s="8"/>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A76" s="16">
+        <v>28</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="C76" s="16">
+        <v>5</v>
+      </c>
+      <c r="D76" s="16">
+        <v>5</v>
+      </c>
+      <c r="E76" s="16">
+        <v>7</v>
+      </c>
+      <c r="F76" s="16">
+        <v>9</v>
+      </c>
+      <c r="G76" s="16">
+        <v>13</v>
+      </c>
+      <c r="H76" s="16">
+        <v>17</v>
+      </c>
+      <c r="I76" s="16">
+        <v>19</v>
+      </c>
+      <c r="J76" s="16">
+        <v>20</v>
+      </c>
+      <c r="K76" s="16">
+        <v>17</v>
+      </c>
+      <c r="L76" s="16">
+        <v>14</v>
+      </c>
+      <c r="M76" s="16">
+        <v>9</v>
+      </c>
+      <c r="N76" s="16">
+        <v>6</v>
+      </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U77" s="8"/>
@@ -12398,8 +12663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13551,7 +13816,7 @@
       </c>
       <c r="H26">
         <f>_xlfn.IFNA(IF(VLOOKUP(B26,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <f>_xlfn.IFNA(IF(VLOOKUP(B26,REFERANCES!A:A,1,FALSE),1,0),0)</f>
@@ -13664,7 +13929,7 @@
       </c>
       <c r="D29">
         <f>IF(CLIMBS!R29&lt;&gt;0,1,0)+IF(CLIMBS!G29&lt;&gt;0,1,0)+IF(CLIMBS!H29&lt;&gt;0,1,0)+IF(CLIMBS!I29&lt;&gt;0,1,0)+IF(CLIMBS!J29&lt;&gt;0,1,0)+IF(CLIMBS!N29&lt;&gt;0,1,0)+IF(CLIMBS!M29&lt;&gt;0,1,0)+IF(CLIMBS!O29&lt;&gt;0,1,0)+IF(CLIMBS!P29&lt;&gt;0,1,0)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E29">
         <f>IF(CLIMBS!S29&lt;&gt;0,1,0)</f>
@@ -13683,7 +13948,7 @@
       </c>
       <c r="H29">
         <f>_xlfn.IFNA(IF(VLOOKUP(B29,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <f>_xlfn.IFNA(IF(VLOOKUP(B29,REFERANCES!A:A,1,FALSE),1,0),0)</f>

</xml_diff>

<commit_message>
some refactoring and minor bug fixing
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D275F52-0BDD-442F-828A-C1BB5918D289}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD0843A-1AD3-4712-BC71-DF81D4AE2BEA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="690">
   <si>
     <t>cliff</t>
   </si>
@@ -2012,9 +2012,6 @@
 The decent requires 3 abseils of 40m, 40m and just under 60m. To find the anchor to abseil you need to walk along the ridge for 80m. You go over a couple of small peaks. You may want to stay roped for this slinging the occasional bush as the ground can be loose. If you use a pair of 50m ropes you can either use a tree to break the last abseil into 2 or create a trad anchor on the way or even abseil carefully off the end of the rope and downclimb the last 10m. All these options have risk especially if you end up doing it in the dark. </t>
   </si>
   <si>
-    <t xml:space="preserve">Esparraguera offers an exciting 190m HVS (f5c) multi-pitch climb on the fantastic conglomerate rock of Montserrat in Spain. The route is sustained and consistent in grade. The hardest pitch is steep but has big holds and is well bolted, this may well feel like the easiest pitch if you are used to indoor climbing / bouldering. Whilst described as a clean trad route in many guidebooks, Esparraguera has a good amount bolts (17) and pitons (2) in sections in the middle pitches. Most of the harder moves are protected by old bolts. You will need a full trad rack of nuts and cams. Tri cams are particularly helpful for the pockets. The last pitch has no fixed protection. The route is given f5c in some guides or UIAA V+ in others, it is hard to convert to British grades but given the protection is good at the harder sections, the British grade of HVS 5a (maybe 5b) seems best. If anything feels hard, take some time and search for better holds, there will be some. The decent requires 3 abseils of 40m, 40m and just under 60m. </t>
-  </si>
-  <si>
     <t>pitchInfo</t>
   </si>
   <si>
@@ -2172,12 +2169,50 @@
   <si>
     <t>topo data</t>
   </si>
+  <si>
+    <t xml:space="preserve">Esparraguera offers an exciting 190m VS (f5c) multi-pitch climb on the fantastic conglomerate rock of Montserrat in Spain. The route is sustained and consistent in grade. The hardest pitch is steep but has big holds and is well bolted, this may well feel like the easiest pitch if you are used to indoor climbing / bouldering. Whilst described as a clean trad route in many guidebooks, Esparraguera has a good amount bolts (17) and pitons (2) in sections in the middle pitches. Most of the harder moves are protected by old bolts. You will need a full trad rack of nuts and cams. Tri cams are particularly helpful for the pockets. The last pitch has no fixed protection. The route is given f5c in some guides or UIAA V+ in others, it is hard to convert to British grades but given the protection is good at the harder sections, the British grade of VS 5a (maybe HVS 5b) seems best. If anything feels hard, take some time and search for better holds, there will be some. The decent requires 3 abseils of 40m, 40m and just under 60m. </t>
+  </si>
+  <si>
+    <t>0901601616</t>
+  </si>
+  <si>
+    <r>
+      <t>You would imagine a climbing guide dedicated to Lliwedd would be perfect for climbing this Welsh Mountain crag. Kelvin Neal’s 4</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> edition of this guidebook certainly offers and good amount of detail (95 pages) and it comes in a small portable format. However, that’s where the positive points end.  Like most Climbers Climb guides, it focuses on text-based descriptions with little or no imagery. If you are looking for a very loose suggestion of where to go, when climbing almost 1,000 feet, this book might suite. And yes, despite the fourth edition being published in 1998 it still uses the imperial system of feet. Fun fact: The original first edition was published in 1909 and was one of the first guidebooks to ever be published!  To summarise, it’s not going to be hugely helpful with route finding, but it’s a cheap enough guidebook with good historical relevance.  </t>
+    </r>
+  </si>
+  <si>
+    <t>https://amzn.to/2TYdPUI</t>
+  </si>
+  <si>
+    <t>img/guidebooks/lliwedd-guidebook.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2339,6 +2374,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="38">
@@ -2813,167 +2856,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3457,8 +3340,8 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N28" sqref="N28"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3542,7 +3425,7 @@
         <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>18</v>
@@ -3967,7 +3850,7 @@
         <v>89</v>
       </c>
       <c r="K8" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="M8" t="s">
         <v>51</v>
@@ -4178,7 +4061,7 @@
         <v>104</v>
       </c>
       <c r="T11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="U11" t="s">
         <v>174</v>
@@ -4275,10 +4158,10 @@
         <v>6</v>
       </c>
       <c r="I13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J13" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="K13" t="s">
         <v>26</v>
@@ -4302,13 +4185,13 @@
         <v>194</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>642</v>
+        <v>685</v>
       </c>
       <c r="S13" s="2" t="s">
         <v>641</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="V13" t="s">
         <v>175</v>
@@ -5220,7 +5103,7 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B28" t="s">
         <v>107</v>
@@ -5229,13 +5112,13 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
+        <v>648</v>
+      </c>
+      <c r="E28" t="s">
         <v>649</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>650</v>
-      </c>
-      <c r="F28" t="s">
-        <v>651</v>
       </c>
       <c r="G28">
         <v>250</v>
@@ -5253,13 +5136,13 @@
         <v>38</v>
       </c>
       <c r="L28" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="M28" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="N28" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="O28">
         <v>30</v>
@@ -5268,14 +5151,14 @@
         <v>1</v>
       </c>
       <c r="Q28" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B29" t="s">
         <v>106</v>
@@ -5284,13 +5167,13 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E29" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F29" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G29">
         <v>115</v>
@@ -5314,7 +5197,7 @@
         <v>191</v>
       </c>
       <c r="N29" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="O29">
         <v>15</v>
@@ -5326,10 +5209,10 @@
         <v>41</v>
       </c>
       <c r="R29" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="S29" s="2" t="s">
         <v>677</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>678</v>
       </c>
       <c r="W29">
         <v>1</v>
@@ -5337,7 +5220,7 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B30" t="s">
         <v>107</v>
@@ -5397,7 +5280,7 @@
         <v>117</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>334</v>
@@ -5423,7 +5306,7 @@
         <v>110</v>
       </c>
       <c r="I2" t="str">
-        <f>CONCATENATE(A2,B2)</f>
+        <f t="shared" ref="I2:I33" si="0">CONCATENATE(A2,B2)</f>
         <v>1topo</v>
       </c>
     </row>
@@ -5441,7 +5324,7 @@
         <v>116</v>
       </c>
       <c r="I3" t="str">
-        <f>CONCATENATE(A3,B3)</f>
+        <f t="shared" si="0"/>
         <v>1tile</v>
       </c>
     </row>
@@ -5465,7 +5348,7 @@
         <v>634</v>
       </c>
       <c r="I4" t="str">
-        <f>CONCATENATE(A4,B4)</f>
+        <f t="shared" si="0"/>
         <v>1map</v>
       </c>
     </row>
@@ -5489,7 +5372,7 @@
         <v>126</v>
       </c>
       <c r="I5" t="str">
-        <f>CONCATENATE(A5,B5)</f>
+        <f t="shared" si="0"/>
         <v>2topo</v>
       </c>
     </row>
@@ -5510,7 +5393,7 @@
         <v>162</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE(A6,B6)</f>
+        <f t="shared" si="0"/>
         <v>2tile</v>
       </c>
     </row>
@@ -5534,7 +5417,7 @@
         <v>634</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE(A7,B7)</f>
+        <f t="shared" si="0"/>
         <v>2map</v>
       </c>
     </row>
@@ -5558,7 +5441,7 @@
         <v>130</v>
       </c>
       <c r="I8" t="str">
-        <f>CONCATENATE(A8,B8)</f>
+        <f t="shared" si="0"/>
         <v>3topo</v>
       </c>
     </row>
@@ -5576,7 +5459,7 @@
         <v>128</v>
       </c>
       <c r="I9" t="str">
-        <f>CONCATENATE(A9,B9)</f>
+        <f t="shared" si="0"/>
         <v>3tile</v>
       </c>
     </row>
@@ -5600,7 +5483,7 @@
         <v>634</v>
       </c>
       <c r="I10" t="str">
-        <f>CONCATENATE(A10,B10)</f>
+        <f t="shared" si="0"/>
         <v>3map</v>
       </c>
     </row>
@@ -5618,7 +5501,7 @@
         <v>165</v>
       </c>
       <c r="I11" t="str">
-        <f>CONCATENATE(A11,B11)</f>
+        <f t="shared" si="0"/>
         <v>4tile</v>
       </c>
     </row>
@@ -5642,7 +5525,7 @@
         <v>136</v>
       </c>
       <c r="I12" t="str">
-        <f>CONCATENATE(A12,B12)</f>
+        <f t="shared" si="0"/>
         <v>5topo</v>
       </c>
     </row>
@@ -5663,7 +5546,7 @@
         <v>135</v>
       </c>
       <c r="I13" t="str">
-        <f>CONCATENATE(A13,B13)</f>
+        <f t="shared" si="0"/>
         <v>5tile</v>
       </c>
     </row>
@@ -5687,7 +5570,7 @@
         <v>634</v>
       </c>
       <c r="I14" t="str">
-        <f>CONCATENATE(A14,B14)</f>
+        <f t="shared" si="0"/>
         <v>5map</v>
       </c>
     </row>
@@ -5711,7 +5594,7 @@
         <v>126</v>
       </c>
       <c r="I15" t="str">
-        <f>CONCATENATE(A15,B15)</f>
+        <f t="shared" si="0"/>
         <v>6topo</v>
       </c>
     </row>
@@ -5729,7 +5612,7 @@
         <v>140</v>
       </c>
       <c r="I16" t="str">
-        <f>CONCATENATE(A16,B16)</f>
+        <f t="shared" si="0"/>
         <v>6tile</v>
       </c>
     </row>
@@ -5753,7 +5636,7 @@
         <v>634</v>
       </c>
       <c r="I17" t="str">
-        <f>CONCATENATE(A17,B17)</f>
+        <f t="shared" si="0"/>
         <v>6map</v>
       </c>
     </row>
@@ -5777,7 +5660,7 @@
         <v>150</v>
       </c>
       <c r="I18" t="str">
-        <f>CONCATENATE(A18,B18)</f>
+        <f t="shared" si="0"/>
         <v>7topo</v>
       </c>
     </row>
@@ -5801,7 +5684,7 @@
         <v>141</v>
       </c>
       <c r="I19" t="str">
-        <f>CONCATENATE(A19,B19)</f>
+        <f t="shared" si="0"/>
         <v>7tile</v>
       </c>
     </row>
@@ -5825,7 +5708,7 @@
         <v>634</v>
       </c>
       <c r="I20" t="str">
-        <f>CONCATENATE(A20,B20)</f>
+        <f t="shared" si="0"/>
         <v>7map</v>
       </c>
     </row>
@@ -5849,7 +5732,7 @@
         <v>155</v>
       </c>
       <c r="I21" t="str">
-        <f>CONCATENATE(A21,B21)</f>
+        <f t="shared" si="0"/>
         <v>8topo</v>
       </c>
     </row>
@@ -5870,7 +5753,7 @@
         <v>163</v>
       </c>
       <c r="I22" t="str">
-        <f>CONCATENATE(A22,B22)</f>
+        <f t="shared" si="0"/>
         <v>8tile</v>
       </c>
     </row>
@@ -5894,7 +5777,7 @@
         <v>634</v>
       </c>
       <c r="I23" t="str">
-        <f>CONCATENATE(A23,B23)</f>
+        <f t="shared" si="0"/>
         <v>8map</v>
       </c>
     </row>
@@ -5918,7 +5801,7 @@
         <v>479</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE(A24,B24)</f>
+        <f t="shared" si="0"/>
         <v>9topo</v>
       </c>
     </row>
@@ -5942,7 +5825,7 @@
         <v>258</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE(A25,B25)</f>
+        <f t="shared" si="0"/>
         <v>9tile</v>
       </c>
     </row>
@@ -5966,7 +5849,7 @@
         <v>634</v>
       </c>
       <c r="I26" t="str">
-        <f>CONCATENATE(A26,B26)</f>
+        <f t="shared" si="0"/>
         <v>9map</v>
       </c>
     </row>
@@ -5990,7 +5873,7 @@
         <v>157</v>
       </c>
       <c r="I27" t="str">
-        <f>CONCATENATE(A27,B27)</f>
+        <f t="shared" si="0"/>
         <v>10topo</v>
       </c>
     </row>
@@ -6008,7 +5891,7 @@
         <v>167</v>
       </c>
       <c r="I28" t="str">
-        <f>CONCATENATE(A28,B28)</f>
+        <f t="shared" si="0"/>
         <v>10tile</v>
       </c>
     </row>
@@ -6032,7 +5915,7 @@
         <v>634</v>
       </c>
       <c r="I29" t="str">
-        <f>CONCATENATE(A29,B29)</f>
+        <f t="shared" si="0"/>
         <v>10map</v>
       </c>
     </row>
@@ -6056,7 +5939,7 @@
         <v>110</v>
       </c>
       <c r="I30" t="str">
-        <f>CONCATENATE(A30,B30)</f>
+        <f t="shared" si="0"/>
         <v>11topo</v>
       </c>
     </row>
@@ -6080,7 +5963,7 @@
         <v>173</v>
       </c>
       <c r="I31" t="str">
-        <f>CONCATENATE(A31,B31)</f>
+        <f t="shared" si="0"/>
         <v>11tile</v>
       </c>
     </row>
@@ -6104,7 +5987,7 @@
         <v>634</v>
       </c>
       <c r="I32" t="str">
-        <f>CONCATENATE(A32,B32)</f>
+        <f t="shared" si="0"/>
         <v>11map</v>
       </c>
     </row>
@@ -6122,7 +6005,7 @@
         <v>196</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F33" t="s">
         <v>157</v>
@@ -6131,7 +6014,7 @@
         <v>5</v>
       </c>
       <c r="I33" t="str">
-        <f>CONCATENATE(A33,B33)</f>
+        <f t="shared" si="0"/>
         <v>12topo</v>
       </c>
     </row>
@@ -6155,7 +6038,7 @@
         <v>110</v>
       </c>
       <c r="I34" t="str">
-        <f>CONCATENATE(A34,B34)</f>
+        <f t="shared" ref="I34:I65" si="1">CONCATENATE(A34,B34)</f>
         <v>12tile</v>
       </c>
     </row>
@@ -6164,22 +6047,22 @@
         <v>12</v>
       </c>
       <c r="B35" t="s">
+        <v>654</v>
+      </c>
+      <c r="C35" t="s">
+        <v>657</v>
+      </c>
+      <c r="D35" t="s">
         <v>655</v>
       </c>
-      <c r="C35" t="s">
-        <v>658</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" s="10" t="s">
         <v>656</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>657</v>
       </c>
       <c r="F35" t="s">
         <v>157</v>
       </c>
       <c r="I35" t="str">
-        <f>CONCATENATE(A35,B35)</f>
+        <f t="shared" si="1"/>
         <v>12super</v>
       </c>
     </row>
@@ -6203,7 +6086,7 @@
         <v>634</v>
       </c>
       <c r="I36" t="str">
-        <f>CONCATENATE(A36,B36)</f>
+        <f t="shared" si="1"/>
         <v>12map</v>
       </c>
     </row>
@@ -6227,7 +6110,7 @@
         <v>214</v>
       </c>
       <c r="I37" t="str">
-        <f>CONCATENATE(A37,B37)</f>
+        <f t="shared" si="1"/>
         <v>13topo</v>
       </c>
     </row>
@@ -6251,7 +6134,7 @@
         <v>205</v>
       </c>
       <c r="I38" t="str">
-        <f>CONCATENATE(A38,B38)</f>
+        <f t="shared" si="1"/>
         <v>13tile</v>
       </c>
     </row>
@@ -6275,7 +6158,7 @@
         <v>634</v>
       </c>
       <c r="I39" t="str">
-        <f>CONCATENATE(A39,B39)</f>
+        <f t="shared" si="1"/>
         <v>13map</v>
       </c>
     </row>
@@ -6299,7 +6182,7 @@
         <v>220</v>
       </c>
       <c r="I40" t="str">
-        <f>CONCATENATE(A40,B40)</f>
+        <f t="shared" si="1"/>
         <v>14topo</v>
       </c>
     </row>
@@ -6323,7 +6206,7 @@
         <v>220</v>
       </c>
       <c r="I41" t="str">
-        <f>CONCATENATE(A41,B41)</f>
+        <f t="shared" si="1"/>
         <v>14tile</v>
       </c>
     </row>
@@ -6347,7 +6230,7 @@
         <v>634</v>
       </c>
       <c r="I42" t="str">
-        <f>CONCATENATE(A42,B42)</f>
+        <f t="shared" si="1"/>
         <v>14map</v>
       </c>
     </row>
@@ -6371,7 +6254,7 @@
         <v>257</v>
       </c>
       <c r="I43" t="str">
-        <f>CONCATENATE(A43,B43)</f>
+        <f t="shared" si="1"/>
         <v>15topo</v>
       </c>
     </row>
@@ -6395,7 +6278,7 @@
         <v>257</v>
       </c>
       <c r="I44" t="str">
-        <f>CONCATENATE(A44,B44)</f>
+        <f t="shared" si="1"/>
         <v>15tile</v>
       </c>
     </row>
@@ -6419,7 +6302,7 @@
         <v>634</v>
       </c>
       <c r="I45" t="str">
-        <f>CONCATENATE(A45,B45)</f>
+        <f t="shared" si="1"/>
         <v>15map</v>
       </c>
     </row>
@@ -6443,7 +6326,7 @@
         <v>110</v>
       </c>
       <c r="I46" t="str">
-        <f>CONCATENATE(A46,B46)</f>
+        <f t="shared" si="1"/>
         <v>16topo</v>
       </c>
     </row>
@@ -6467,7 +6350,7 @@
         <v>110</v>
       </c>
       <c r="I47" t="str">
-        <f>CONCATENATE(A47,B47)</f>
+        <f t="shared" si="1"/>
         <v>16tile</v>
       </c>
     </row>
@@ -6491,7 +6374,7 @@
         <v>634</v>
       </c>
       <c r="I48" t="str">
-        <f>CONCATENATE(A48,B48)</f>
+        <f t="shared" si="1"/>
         <v>16map</v>
       </c>
     </row>
@@ -6515,7 +6398,7 @@
         <v>356</v>
       </c>
       <c r="I49" t="str">
-        <f>CONCATENATE(A49,B49)</f>
+        <f t="shared" si="1"/>
         <v>17topo</v>
       </c>
     </row>
@@ -6539,7 +6422,7 @@
         <v>115</v>
       </c>
       <c r="I50" t="str">
-        <f>CONCATENATE(A50,B50)</f>
+        <f t="shared" si="1"/>
         <v>17tile</v>
       </c>
     </row>
@@ -6563,7 +6446,7 @@
         <v>634</v>
       </c>
       <c r="I51" t="str">
-        <f>CONCATENATE(A51,B51)</f>
+        <f t="shared" si="1"/>
         <v>17map</v>
       </c>
     </row>
@@ -6587,7 +6470,7 @@
         <v>110</v>
       </c>
       <c r="I52" t="str">
-        <f>CONCATENATE(A52,B52)</f>
+        <f t="shared" si="1"/>
         <v>18topo</v>
       </c>
     </row>
@@ -6611,7 +6494,7 @@
         <v>130</v>
       </c>
       <c r="I53" t="str">
-        <f>CONCATENATE(A53,B53)</f>
+        <f t="shared" si="1"/>
         <v>18tile</v>
       </c>
     </row>
@@ -6635,7 +6518,7 @@
         <v>634</v>
       </c>
       <c r="I54" t="str">
-        <f>CONCATENATE(A54,B54)</f>
+        <f t="shared" si="1"/>
         <v>18map</v>
       </c>
     </row>
@@ -6659,7 +6542,7 @@
         <v>439</v>
       </c>
       <c r="I55" t="str">
-        <f>CONCATENATE(A55,B55)</f>
+        <f t="shared" si="1"/>
         <v>19topo</v>
       </c>
     </row>
@@ -6683,7 +6566,7 @@
         <v>438</v>
       </c>
       <c r="I56" t="str">
-        <f>CONCATENATE(A56,B56)</f>
+        <f t="shared" si="1"/>
         <v>19tile</v>
       </c>
     </row>
@@ -6707,7 +6590,7 @@
         <v>634</v>
       </c>
       <c r="I57" t="str">
-        <f>CONCATENATE(A57,B57)</f>
+        <f t="shared" si="1"/>
         <v>19map</v>
       </c>
     </row>
@@ -6731,7 +6614,7 @@
         <v>427</v>
       </c>
       <c r="I58" t="str">
-        <f>CONCATENATE(A58,B58)</f>
+        <f t="shared" si="1"/>
         <v>20topo</v>
       </c>
     </row>
@@ -6755,7 +6638,7 @@
         <v>424</v>
       </c>
       <c r="I59" t="str">
-        <f>CONCATENATE(A59,B59)</f>
+        <f t="shared" si="1"/>
         <v>20tile</v>
       </c>
     </row>
@@ -6779,7 +6662,7 @@
         <v>634</v>
       </c>
       <c r="I60" t="str">
-        <f>CONCATENATE(A60,B60)</f>
+        <f t="shared" si="1"/>
         <v>20map</v>
       </c>
     </row>
@@ -6803,7 +6686,7 @@
         <v>472</v>
       </c>
       <c r="I61" t="str">
-        <f>CONCATENATE(A61,B61)</f>
+        <f t="shared" si="1"/>
         <v>21topo</v>
       </c>
     </row>
@@ -6827,7 +6710,7 @@
         <v>468</v>
       </c>
       <c r="I62" t="str">
-        <f>CONCATENATE(A62,B62)</f>
+        <f t="shared" si="1"/>
         <v>21tile</v>
       </c>
     </row>
@@ -6851,7 +6734,7 @@
         <v>634</v>
       </c>
       <c r="I63" t="str">
-        <f>CONCATENATE(A63,B63)</f>
+        <f t="shared" si="1"/>
         <v>21map</v>
       </c>
     </row>
@@ -6875,7 +6758,7 @@
         <v>503</v>
       </c>
       <c r="I64" t="str">
-        <f>CONCATENATE(A64,B64)</f>
+        <f t="shared" si="1"/>
         <v>22topo</v>
       </c>
     </row>
@@ -6899,7 +6782,7 @@
         <v>258</v>
       </c>
       <c r="I65" t="str">
-        <f>CONCATENATE(A65,B65)</f>
+        <f t="shared" si="1"/>
         <v>22tile</v>
       </c>
     </row>
@@ -6923,7 +6806,7 @@
         <v>634</v>
       </c>
       <c r="I66" t="str">
-        <f>CONCATENATE(A66,B66)</f>
+        <f t="shared" ref="I66:I81" si="2">CONCATENATE(A66,B66)</f>
         <v>22map</v>
       </c>
     </row>
@@ -6947,7 +6830,7 @@
         <v>479</v>
       </c>
       <c r="I67" t="str">
-        <f>CONCATENATE(A67,B67)</f>
+        <f t="shared" si="2"/>
         <v>23topo</v>
       </c>
     </row>
@@ -6971,7 +6854,7 @@
         <v>115</v>
       </c>
       <c r="I68" t="str">
-        <f>CONCATENATE(A68,B68)</f>
+        <f t="shared" si="2"/>
         <v>23tile</v>
       </c>
     </row>
@@ -6995,7 +6878,7 @@
         <v>634</v>
       </c>
       <c r="I69" t="str">
-        <f>CONCATENATE(A69,B69)</f>
+        <f t="shared" si="2"/>
         <v>23map</v>
       </c>
     </row>
@@ -7019,7 +6902,7 @@
         <v>538</v>
       </c>
       <c r="I70" t="str">
-        <f>CONCATENATE(A70,B70)</f>
+        <f t="shared" si="2"/>
         <v>24topo</v>
       </c>
     </row>
@@ -7043,7 +6926,7 @@
         <v>538</v>
       </c>
       <c r="I71" t="str">
-        <f>CONCATENATE(A71,B71)</f>
+        <f t="shared" si="2"/>
         <v>24tile</v>
       </c>
     </row>
@@ -7067,7 +6950,7 @@
         <v>634</v>
       </c>
       <c r="I72" t="str">
-        <f>CONCATENATE(A72,B72)</f>
+        <f t="shared" si="2"/>
         <v>24map</v>
       </c>
     </row>
@@ -7091,7 +6974,7 @@
         <v>582</v>
       </c>
       <c r="I73" t="str">
-        <f>CONCATENATE(A73,B73)</f>
+        <f t="shared" si="2"/>
         <v>25topo</v>
       </c>
     </row>
@@ -7115,7 +6998,7 @@
         <v>576</v>
       </c>
       <c r="I74" t="str">
-        <f>CONCATENATE(A74,B74)</f>
+        <f t="shared" si="2"/>
         <v>25tile</v>
       </c>
     </row>
@@ -7139,7 +7022,7 @@
         <v>634</v>
       </c>
       <c r="I75" t="str">
-        <f>CONCATENATE(A75,B75)</f>
+        <f t="shared" si="2"/>
         <v>25map</v>
       </c>
     </row>
@@ -7163,7 +7046,7 @@
         <v>595</v>
       </c>
       <c r="I76" t="str">
-        <f>CONCATENATE(A76,B76)</f>
+        <f t="shared" si="2"/>
         <v>26topo</v>
       </c>
     </row>
@@ -7187,7 +7070,7 @@
         <v>592</v>
       </c>
       <c r="I77" t="str">
-        <f>CONCATENATE(A77,B77)</f>
+        <f t="shared" si="2"/>
         <v>26tile</v>
       </c>
     </row>
@@ -7211,7 +7094,7 @@
         <v>634</v>
       </c>
       <c r="I78" t="str">
-        <f>CONCATENATE(A78,B78)</f>
+        <f t="shared" si="2"/>
         <v>26map</v>
       </c>
     </row>
@@ -7223,22 +7106,22 @@
         <v>114</v>
       </c>
       <c r="C79" t="s">
+        <v>667</v>
+      </c>
+      <c r="D79" t="s">
         <v>668</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" s="10" t="s">
         <v>669</v>
       </c>
-      <c r="E79" s="10" t="s">
+      <c r="F79" s="14" t="s">
         <v>670</v>
-      </c>
-      <c r="F79" s="14" t="s">
-        <v>671</v>
       </c>
       <c r="G79" s="14">
         <v>2</v>
       </c>
       <c r="I79" t="str">
-        <f>CONCATENATE(A79,B79)</f>
+        <f t="shared" si="2"/>
         <v>28topo</v>
       </c>
     </row>
@@ -7250,19 +7133,19 @@
         <v>161</v>
       </c>
       <c r="C80" t="s">
+        <v>671</v>
+      </c>
+      <c r="D80" t="s">
+        <v>682</v>
+      </c>
+      <c r="E80" t="s">
+        <v>673</v>
+      </c>
+      <c r="F80" t="s">
         <v>672</v>
       </c>
-      <c r="D80" t="s">
-        <v>683</v>
-      </c>
-      <c r="E80" t="s">
-        <v>674</v>
-      </c>
-      <c r="F80" t="s">
-        <v>673</v>
-      </c>
       <c r="I80" t="str">
-        <f>CONCATENATE(A80,B80)</f>
+        <f t="shared" si="2"/>
         <v>28tile</v>
       </c>
     </row>
@@ -7274,10 +7157,10 @@
         <v>109</v>
       </c>
       <c r="C81" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D81" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E81" t="s">
         <v>633</v>
@@ -7286,7 +7169,7 @@
         <v>634</v>
       </c>
       <c r="I81" t="str">
-        <f>CONCATENATE(A81,B81)</f>
+        <f t="shared" si="2"/>
         <v>28map</v>
       </c>
     </row>
@@ -7335,10 +7218,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="116" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="116" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8140,7 +8023,7 @@
         <v>157</v>
       </c>
       <c r="F28" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>637</v>
@@ -8150,6 +8033,35 @@
       </c>
       <c r="I28">
         <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>16</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>686</v>
+      </c>
+      <c r="C29" t="s">
+        <v>307</v>
+      </c>
+      <c r="D29" t="s">
+        <v>231</v>
+      </c>
+      <c r="E29">
+        <v>34</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G29" t="s">
+        <v>689</v>
+      </c>
+      <c r="H29" t="s">
+        <v>688</v>
+      </c>
+      <c r="I29">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -8362,10 +8274,10 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
+        <v>664</v>
+      </c>
+      <c r="C17" t="s">
         <v>665</v>
-      </c>
-      <c r="C17" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -8376,7 +8288,7 @@
         <v>195</v>
       </c>
       <c r="C18" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -8384,10 +8296,10 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
+        <v>674</v>
+      </c>
+      <c r="C19" t="s">
         <v>675</v>
-      </c>
-      <c r="C19" t="s">
-        <v>676</v>
       </c>
     </row>
   </sheetData>
@@ -12227,7 +12139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -12263,7 +12175,7 @@
         <v>331</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>332</v>
@@ -12272,7 +12184,7 @@
         <v>333</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>640</v>
@@ -13613,69 +13525,69 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D29">
-    <cfRule type="cellIs" dxfId="32" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="lessThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C29">
-    <cfRule type="cellIs" dxfId="30" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"draft"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="29" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C29">
-    <cfRule type="cellIs" dxfId="28" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E29">
-    <cfRule type="cellIs" dxfId="27" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G30">
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"missing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J29">
-    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K29">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G29">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added dynamic topo for cloggy
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C3FF69-D606-4605-96EC-8A1FA0C01674}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811E57A6-EBCA-4C25-8BF6-B40CFAF68E01}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="695">
   <si>
     <t>cliff</t>
   </si>
@@ -958,13 +958,7 @@
     <t>Topo for Avalanch to Red Wall to Longlands Continuation</t>
   </si>
   <si>
-    <t>https://www.summitpost.org/y-lliwedd/268799</t>
-  </si>
-  <si>
     <t>A brilliant guidebok with a good section on Lliwedd. Overall this book covers a good selection of climbs from a good selection of cliffs, including the 300m routes up Lliwedd</t>
-  </si>
-  <si>
-    <t>img/topos/lliwedd/longlands-red-wall-avalanche-topo-on-lliwedd.jpg</t>
   </si>
   <si>
     <t>Longlands Continuation</t>
@@ -2129,9 +2123,6 @@
   </si>
   <si>
     <t>dataFile</t>
-  </si>
-  <si>
-    <t>Via Mendez and Guillermo</t>
   </si>
   <si>
     <t>Cathederal Rock in Tenerife offers great climbing</t>
@@ -2209,6 +2200,27 @@
   </si>
   <si>
     <t xml:space="preserve">Rock Climbing Wyoming describes 11 major climbing areas in the state of Wyoming. It offers approximately 550 climbing routes. Falcon guides have maps, good topos, and action photos accompanying clearly written descriptions of the routes. The book is ideal for a trip to Wyoming, but enough of the information on the devils tower is available online for those looking to save some money. </t>
+  </si>
+  <si>
+    <t>Mendez and Guillermo</t>
+  </si>
+  <si>
+    <t>img/topos/lliwedd/longlands-continuation-climb-on-lliwedd.jpg</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/arg_flickr/14442887130/</t>
+  </si>
+  <si>
+    <t>https://www.rockfax.com/wp-content/uploads/intros/north-wales-climbs-preview.pdf</t>
+  </si>
+  <si>
+    <t>Rockfax preview covering the Great Slab climb on Cloggy</t>
+  </si>
+  <si>
+    <t>Rockfax preview covering  key climbs up Lliwedd</t>
+  </si>
+  <si>
+    <t>originl image: BMC super zoom</t>
   </si>
 </sst>
 </file>
@@ -3353,9 +3365,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A11" sqref="A11:D11"/>
+      <selection pane="topRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3439,7 +3451,7 @@
         <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>18</v>
@@ -3448,13 +3460,13 @@
         <v>19</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -3507,7 +3519,7 @@
         <v>29</v>
       </c>
       <c r="R2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="S2" t="s">
         <v>30</v>
@@ -3675,7 +3687,7 @@
         <v>7</v>
       </c>
       <c r="J5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K5" t="s">
         <v>60</v>
@@ -3864,7 +3876,7 @@
         <v>89</v>
       </c>
       <c r="K8" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="M8" t="s">
         <v>51</v>
@@ -3941,10 +3953,10 @@
         <v>41</v>
       </c>
       <c r="R9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="S9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="U9" t="s">
         <v>171</v>
@@ -3970,7 +3982,7 @@
         <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F10" t="s">
         <v>97</v>
@@ -3985,16 +3997,16 @@
         <v>7</v>
       </c>
       <c r="J10" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K10" t="s">
         <v>60</v>
       </c>
       <c r="L10" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="M10" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="N10" t="s">
         <v>179</v>
@@ -4009,10 +4021,10 @@
         <v>41</v>
       </c>
       <c r="R10" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="T10" s="2"/>
       <c r="U10" t="s">
@@ -4075,7 +4087,7 @@
         <v>104</v>
       </c>
       <c r="T11" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="U11" t="s">
         <v>171</v>
@@ -4199,13 +4211,13 @@
         <v>191</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="V13" t="s">
         <v>172</v>
@@ -4255,7 +4267,7 @@
         <v>70</v>
       </c>
       <c r="N14" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="O14">
         <v>20</v>
@@ -4377,13 +4389,13 @@
         <v>199</v>
       </c>
       <c r="L16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="M16" t="s">
         <v>247</v>
       </c>
       <c r="N16" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="O16">
         <v>5</v>
@@ -4398,7 +4410,7 @@
         <v>257</v>
       </c>
       <c r="S16" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="U16" t="s">
         <v>44</v>
@@ -4427,7 +4439,7 @@
         <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G17">
         <v>280</v>
@@ -4460,7 +4472,7 @@
         <v>53</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>307</v>
@@ -4475,7 +4487,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B18" t="s">
         <v>106</v>
@@ -4484,13 +4496,13 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E18" t="s">
+        <v>344</v>
+      </c>
+      <c r="F18" t="s">
         <v>346</v>
-      </c>
-      <c r="F18" t="s">
-        <v>348</v>
       </c>
       <c r="G18">
         <v>575</v>
@@ -4502,19 +4514,19 @@
         <v>7</v>
       </c>
       <c r="J18" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K18" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L18" t="s">
+        <v>347</v>
+      </c>
+      <c r="M18" t="s">
         <v>349</v>
       </c>
-      <c r="M18" t="s">
-        <v>351</v>
-      </c>
       <c r="N18" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="O18">
         <v>90</v>
@@ -4523,13 +4535,13 @@
         <v>2</v>
       </c>
       <c r="Q18" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="S18" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="U18" t="s">
         <v>207</v>
@@ -4540,7 +4552,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B19" t="s">
         <v>106</v>
@@ -4552,10 +4564,10 @@
         <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F19" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G19">
         <v>74</v>
@@ -4567,16 +4579,16 @@
         <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K19" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="M19" t="s">
         <v>39</v>
       </c>
       <c r="N19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="O19">
         <v>70</v>
@@ -4588,16 +4600,16 @@
         <v>53</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="T19" s="2"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B20" t="s">
         <v>106</v>
@@ -4606,13 +4618,13 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E20" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F20" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G20">
         <v>300</v>
@@ -4630,13 +4642,13 @@
         <v>79</v>
       </c>
       <c r="L20" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="M20" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="N20" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="O20">
         <v>40</v>
@@ -4648,10 +4660,10 @@
         <v>64</v>
       </c>
       <c r="R20" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="S20" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="U20" t="s">
         <v>171</v>
@@ -4659,7 +4671,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B21" t="s">
         <v>106</v>
@@ -4671,10 +4683,10 @@
         <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F21" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G21">
         <v>80</v>
@@ -4695,7 +4707,7 @@
         <v>70</v>
       </c>
       <c r="N21" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="O21">
         <v>90</v>
@@ -4707,10 +4719,10 @@
         <v>41</v>
       </c>
       <c r="R21" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="S21" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="V21" t="s">
         <v>215</v>
@@ -4718,7 +4730,7 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B22" t="s">
         <v>106</v>
@@ -4727,13 +4739,13 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E22" t="s">
+        <v>450</v>
+      </c>
+      <c r="F22" t="s">
         <v>452</v>
-      </c>
-      <c r="F22" t="s">
-        <v>454</v>
       </c>
       <c r="G22">
         <v>80</v>
@@ -4748,13 +4760,13 @@
         <v>59</v>
       </c>
       <c r="K22" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="M22" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="N22" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="O22">
         <v>40</v>
@@ -4766,13 +4778,13 @@
         <v>41</v>
       </c>
       <c r="R22" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="S22" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="U22" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="V22" t="s">
         <v>45</v>
@@ -4780,7 +4792,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B23" t="s">
         <v>106</v>
@@ -4792,10 +4804,10 @@
         <v>185</v>
       </c>
       <c r="E23" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F23" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G23">
         <v>228</v>
@@ -4816,7 +4828,7 @@
         <v>188</v>
       </c>
       <c r="N23" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="O23">
         <v>20</v>
@@ -4828,10 +4840,10 @@
         <v>64</v>
       </c>
       <c r="R23" t="s">
+        <v>491</v>
+      </c>
+      <c r="S23" t="s">
         <v>493</v>
-      </c>
-      <c r="S23" t="s">
-        <v>495</v>
       </c>
       <c r="U23" t="s">
         <v>207</v>
@@ -4845,7 +4857,7 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B24" t="s">
         <v>106</v>
@@ -4854,13 +4866,13 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
+        <v>504</v>
+      </c>
+      <c r="E24" t="s">
         <v>506</v>
       </c>
-      <c r="E24" t="s">
-        <v>508</v>
-      </c>
       <c r="F24" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="G24">
         <v>250</v>
@@ -4878,13 +4890,13 @@
         <v>26</v>
       </c>
       <c r="L24" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="M24" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="N24" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="O24">
         <v>21</v>
@@ -4896,10 +4908,10 @@
         <v>191</v>
       </c>
       <c r="R24" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="S24" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U24" t="s">
         <v>207</v>
@@ -4913,7 +4925,7 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B25" t="s">
         <v>106</v>
@@ -4922,13 +4934,13 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
+        <v>523</v>
+      </c>
+      <c r="E25" t="s">
         <v>525</v>
       </c>
-      <c r="E25" t="s">
-        <v>527</v>
-      </c>
       <c r="F25" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="G25">
         <v>350</v>
@@ -4940,19 +4952,19 @@
         <v>7</v>
       </c>
       <c r="J25" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K25" t="s">
         <v>60</v>
       </c>
       <c r="L25" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="M25" t="s">
+        <v>527</v>
+      </c>
+      <c r="N25" t="s">
         <v>529</v>
-      </c>
-      <c r="N25" t="s">
-        <v>531</v>
       </c>
       <c r="O25">
         <v>190</v>
@@ -4964,10 +4976,10 @@
         <v>41</v>
       </c>
       <c r="R25" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="T25" s="2"/>
       <c r="U25" t="s">
@@ -4982,7 +4994,7 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B26" t="s">
         <v>106</v>
@@ -4991,13 +5003,13 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E26" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F26" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="G26">
         <v>230</v>
@@ -5015,13 +5027,13 @@
         <v>199</v>
       </c>
       <c r="L26" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="M26" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="N26" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="O26">
         <v>70</v>
@@ -5033,10 +5045,10 @@
         <v>64</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="T26" s="2"/>
       <c r="U26" t="s">
@@ -5048,7 +5060,7 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B27" t="s">
         <v>106</v>
@@ -5060,10 +5072,10 @@
         <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F27" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="G27">
         <v>160</v>
@@ -5078,7 +5090,7 @@
         <v>37</v>
       </c>
       <c r="K27" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="L27" t="s">
         <v>80</v>
@@ -5087,7 +5099,7 @@
         <v>81</v>
       </c>
       <c r="N27" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="O27">
         <v>80</v>
@@ -5099,10 +5111,10 @@
         <v>83</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="T27" s="2"/>
       <c r="U27" t="s">
@@ -5117,7 +5129,7 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B28" t="s">
         <v>107</v>
@@ -5126,13 +5138,13 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
+        <v>641</v>
+      </c>
+      <c r="E28" t="s">
+        <v>642</v>
+      </c>
+      <c r="F28" t="s">
         <v>643</v>
-      </c>
-      <c r="E28" t="s">
-        <v>644</v>
-      </c>
-      <c r="F28" t="s">
-        <v>645</v>
       </c>
       <c r="G28">
         <v>250</v>
@@ -5150,13 +5162,13 @@
         <v>38</v>
       </c>
       <c r="L28" t="s">
+        <v>644</v>
+      </c>
+      <c r="M28" t="s">
+        <v>639</v>
+      </c>
+      <c r="N28" t="s">
         <v>646</v>
-      </c>
-      <c r="M28" t="s">
-        <v>641</v>
-      </c>
-      <c r="N28" t="s">
-        <v>648</v>
       </c>
       <c r="O28">
         <v>30</v>
@@ -5165,14 +5177,14 @@
         <v>1</v>
       </c>
       <c r="Q28" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B29" t="s">
         <v>106</v>
@@ -5181,13 +5193,13 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E29" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F29" t="s">
-        <v>672</v>
+        <v>688</v>
       </c>
       <c r="G29">
         <v>115</v>
@@ -5205,13 +5217,13 @@
         <v>199</v>
       </c>
       <c r="L29" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="M29" t="s">
         <v>188</v>
       </c>
       <c r="N29" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="O29">
         <v>15</v>
@@ -5223,10 +5235,10 @@
         <v>41</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="W29">
         <v>1</v>
@@ -5234,7 +5246,7 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B30" t="s">
         <v>107</v>
@@ -5245,7 +5257,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -5258,9 +5270,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5294,10 +5306,10 @@
         <v>117</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5350,16 +5362,16 @@
         <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D4" t="s">
         <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F4" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -5374,16 +5386,16 @@
         <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="D5" t="s">
         <v>123</v>
       </c>
       <c r="E5" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="F5" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -5422,16 +5434,16 @@
         <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D7" t="s">
         <v>125</v>
       </c>
       <c r="E7" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F7" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -5455,7 +5467,10 @@
         <v>127</v>
       </c>
       <c r="F8" t="s">
-        <v>128</v>
+        <v>694</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -5488,16 +5503,16 @@
         <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D10" t="s">
         <v>131</v>
       </c>
       <c r="E10" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F10" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -5575,16 +5590,16 @@
         <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D14" t="s">
         <v>137</v>
       </c>
       <c r="E14" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F14" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
@@ -5641,16 +5656,16 @@
         <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D17" t="s">
         <v>143</v>
       </c>
       <c r="E17" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F17" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -5713,16 +5728,16 @@
         <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D20" t="s">
         <v>149</v>
       </c>
       <c r="E20" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F20" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -5737,7 +5752,7 @@
         <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D21" t="s">
         <v>151</v>
@@ -5782,16 +5797,16 @@
         <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D23" t="s">
         <v>137</v>
       </c>
       <c r="E23" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F23" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -5806,16 +5821,16 @@
         <v>114</v>
       </c>
       <c r="C24" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
@@ -5854,16 +5869,16 @@
         <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D26" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E26" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F26" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
@@ -5878,7 +5893,7 @@
         <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="D27" t="s">
         <v>156</v>
@@ -5923,16 +5938,16 @@
         <v>109</v>
       </c>
       <c r="C29" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D29" t="s">
         <v>157</v>
       </c>
       <c r="E29" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F29" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
@@ -5995,16 +6010,16 @@
         <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D32" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E32" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F32" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="0"/>
@@ -6025,7 +6040,7 @@
         <v>193</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="F33" t="s">
         <v>155</v>
@@ -6046,13 +6061,13 @@
         <v>158</v>
       </c>
       <c r="C34" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D34" t="s">
         <v>194</v>
       </c>
       <c r="E34" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F34" t="s">
         <v>110</v>
@@ -6070,16 +6085,16 @@
         <v>109</v>
       </c>
       <c r="C35" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D35" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E35" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F35" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="1"/>
@@ -6142,16 +6157,16 @@
         <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D38" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E38" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F38" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="1"/>
@@ -6214,16 +6229,16 @@
         <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D41" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E41" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F41" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="1"/>
@@ -6286,16 +6301,16 @@
         <v>109</v>
       </c>
       <c r="C44" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D44" t="s">
         <v>292</v>
       </c>
       <c r="E44" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F44" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="1"/>
@@ -6310,16 +6325,19 @@
         <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>311</v>
+        <v>689</v>
       </c>
       <c r="D45" t="s">
         <v>308</v>
       </c>
       <c r="E45" t="s">
-        <v>309</v>
+        <v>690</v>
       </c>
       <c r="F45" t="s">
-        <v>110</v>
+        <v>684</v>
+      </c>
+      <c r="G45">
+        <v>5</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="1"/>
@@ -6334,13 +6352,13 @@
         <v>158</v>
       </c>
       <c r="C46" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D46" t="s">
         <v>303</v>
       </c>
       <c r="E46" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F46" t="s">
         <v>110</v>
@@ -6358,16 +6376,16 @@
         <v>109</v>
       </c>
       <c r="C47" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D47" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E47" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F47" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="1"/>
@@ -6382,16 +6400,16 @@
         <v>114</v>
       </c>
       <c r="C48" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D48" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E48" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F48" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="1"/>
@@ -6406,13 +6424,13 @@
         <v>158</v>
       </c>
       <c r="C49" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D49" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E49" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F49" t="s">
         <v>115</v>
@@ -6430,16 +6448,16 @@
         <v>109</v>
       </c>
       <c r="C50" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D50" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E50" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F50" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="1"/>
@@ -6454,13 +6472,13 @@
         <v>114</v>
       </c>
       <c r="C51" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D51" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="F51" t="s">
         <v>110</v>
@@ -6478,13 +6496,13 @@
         <v>158</v>
       </c>
       <c r="C52" t="s">
+        <v>386</v>
+      </c>
+      <c r="D52" t="s">
+        <v>387</v>
+      </c>
+      <c r="E52" t="s">
         <v>388</v>
-      </c>
-      <c r="D52" t="s">
-        <v>389</v>
-      </c>
-      <c r="E52" t="s">
-        <v>390</v>
       </c>
       <c r="F52" t="s">
         <v>128</v>
@@ -6502,16 +6520,16 @@
         <v>109</v>
       </c>
       <c r="C53" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D53" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E53" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F53" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="1"/>
@@ -6526,16 +6544,16 @@
         <v>114</v>
       </c>
       <c r="C54" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D54" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E54" t="s">
+        <v>430</v>
+      </c>
+      <c r="F54" t="s">
         <v>432</v>
-      </c>
-      <c r="F54" t="s">
-        <v>434</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="1"/>
@@ -6550,16 +6568,16 @@
         <v>158</v>
       </c>
       <c r="C55" t="s">
+        <v>428</v>
+      </c>
+      <c r="D55" t="s">
+        <v>429</v>
+      </c>
+      <c r="E55" t="s">
         <v>430</v>
       </c>
-      <c r="D55" t="s">
+      <c r="F55" t="s">
         <v>431</v>
-      </c>
-      <c r="E55" t="s">
-        <v>432</v>
-      </c>
-      <c r="F55" t="s">
-        <v>433</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="1"/>
@@ -6574,16 +6592,16 @@
         <v>109</v>
       </c>
       <c r="C56" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D56" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E56" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F56" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I56" t="str">
         <f t="shared" si="1"/>
@@ -6598,16 +6616,16 @@
         <v>114</v>
       </c>
       <c r="C57" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D57" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E57" t="s">
+        <v>418</v>
+      </c>
+      <c r="F57" t="s">
         <v>420</v>
-      </c>
-      <c r="F57" t="s">
-        <v>422</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="1"/>
@@ -6622,16 +6640,16 @@
         <v>158</v>
       </c>
       <c r="C58" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D58" t="s">
+        <v>416</v>
+      </c>
+      <c r="E58" t="s">
         <v>418</v>
       </c>
-      <c r="E58" t="s">
-        <v>420</v>
-      </c>
       <c r="F58" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" si="1"/>
@@ -6646,16 +6664,16 @@
         <v>109</v>
       </c>
       <c r="C59" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D59" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E59" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F59" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="1"/>
@@ -6670,16 +6688,16 @@
         <v>114</v>
       </c>
       <c r="C60" t="s">
+        <v>462</v>
+      </c>
+      <c r="D60" t="s">
+        <v>463</v>
+      </c>
+      <c r="E60" t="s">
         <v>464</v>
       </c>
-      <c r="D60" t="s">
+      <c r="F60" t="s">
         <v>465</v>
-      </c>
-      <c r="E60" t="s">
-        <v>466</v>
-      </c>
-      <c r="F60" t="s">
-        <v>467</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" si="1"/>
@@ -6694,16 +6712,16 @@
         <v>158</v>
       </c>
       <c r="C61" t="s">
+        <v>458</v>
+      </c>
+      <c r="D61" t="s">
+        <v>459</v>
+      </c>
+      <c r="E61" t="s">
         <v>460</v>
       </c>
-      <c r="D61" t="s">
+      <c r="F61" t="s">
         <v>461</v>
-      </c>
-      <c r="E61" t="s">
-        <v>462</v>
-      </c>
-      <c r="F61" t="s">
-        <v>463</v>
       </c>
       <c r="I61" t="str">
         <f t="shared" si="1"/>
@@ -6718,16 +6736,16 @@
         <v>109</v>
       </c>
       <c r="C62" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D62" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E62" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F62" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I62" t="str">
         <f t="shared" si="1"/>
@@ -6742,16 +6760,16 @@
         <v>114</v>
       </c>
       <c r="C63" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D63" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E63" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F63" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I63" t="str">
         <f t="shared" si="1"/>
@@ -6766,13 +6784,13 @@
         <v>158</v>
       </c>
       <c r="C64" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D64" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E64" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F64" t="s">
         <v>255</v>
@@ -6790,16 +6808,16 @@
         <v>109</v>
       </c>
       <c r="C65" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D65" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E65" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F65" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I65" t="str">
         <f t="shared" ref="I65:I80" si="2">CONCATENATE(A65,B65)</f>
@@ -6814,16 +6832,16 @@
         <v>114</v>
       </c>
       <c r="C66" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D66" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E66" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F66" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I66" t="str">
         <f t="shared" si="2"/>
@@ -6838,13 +6856,13 @@
         <v>158</v>
       </c>
       <c r="C67" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D67" t="s">
+        <v>512</v>
+      </c>
+      <c r="E67" t="s">
         <v>514</v>
-      </c>
-      <c r="E67" t="s">
-        <v>516</v>
       </c>
       <c r="F67" t="s">
         <v>115</v>
@@ -6862,16 +6880,16 @@
         <v>109</v>
       </c>
       <c r="C68" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D68" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E68" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F68" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I68" t="str">
         <f t="shared" si="2"/>
@@ -6886,16 +6904,16 @@
         <v>114</v>
       </c>
       <c r="C69" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D69" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E69" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F69" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="I69" t="str">
         <f t="shared" si="2"/>
@@ -6910,16 +6928,16 @@
         <v>158</v>
       </c>
       <c r="C70" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D70" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E70" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F70" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" si="2"/>
@@ -6934,16 +6952,16 @@
         <v>109</v>
       </c>
       <c r="C71" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D71" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E71" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F71" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="2"/>
@@ -6958,16 +6976,16 @@
         <v>114</v>
       </c>
       <c r="C72" t="s">
+        <v>572</v>
+      </c>
+      <c r="D72" t="s">
+        <v>573</v>
+      </c>
+      <c r="E72" t="s">
         <v>574</v>
       </c>
-      <c r="D72" t="s">
+      <c r="F72" t="s">
         <v>575</v>
-      </c>
-      <c r="E72" t="s">
-        <v>576</v>
-      </c>
-      <c r="F72" t="s">
-        <v>577</v>
       </c>
       <c r="I72" t="str">
         <f t="shared" si="2"/>
@@ -6982,16 +7000,16 @@
         <v>158</v>
       </c>
       <c r="C73" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D73" t="s">
+        <v>567</v>
+      </c>
+      <c r="E73" t="s">
+        <v>568</v>
+      </c>
+      <c r="F73" t="s">
         <v>569</v>
-      </c>
-      <c r="E73" t="s">
-        <v>570</v>
-      </c>
-      <c r="F73" t="s">
-        <v>571</v>
       </c>
       <c r="I73" t="str">
         <f t="shared" si="2"/>
@@ -7006,16 +7024,16 @@
         <v>109</v>
       </c>
       <c r="C74" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D74" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E74" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F74" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I74" t="str">
         <f t="shared" si="2"/>
@@ -7030,16 +7048,16 @@
         <v>114</v>
       </c>
       <c r="C75" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D75" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E75" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F75" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="I75" t="str">
         <f t="shared" si="2"/>
@@ -7054,16 +7072,16 @@
         <v>158</v>
       </c>
       <c r="C76" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D76" t="s">
+        <v>583</v>
+      </c>
+      <c r="E76" t="s">
+        <v>584</v>
+      </c>
+      <c r="F76" t="s">
         <v>585</v>
-      </c>
-      <c r="E76" t="s">
-        <v>586</v>
-      </c>
-      <c r="F76" t="s">
-        <v>587</v>
       </c>
       <c r="I76" t="str">
         <f t="shared" si="2"/>
@@ -7078,16 +7096,16 @@
         <v>109</v>
       </c>
       <c r="C77" t="s">
+        <v>624</v>
+      </c>
+      <c r="D77" t="s">
+        <v>625</v>
+      </c>
+      <c r="E77" t="s">
         <v>626</v>
       </c>
-      <c r="D77" t="s">
+      <c r="F77" t="s">
         <v>627</v>
-      </c>
-      <c r="E77" t="s">
-        <v>628</v>
-      </c>
-      <c r="F77" t="s">
-        <v>629</v>
       </c>
       <c r="I77" t="str">
         <f t="shared" si="2"/>
@@ -7102,16 +7120,16 @@
         <v>114</v>
       </c>
       <c r="C78" t="s">
+        <v>656</v>
+      </c>
+      <c r="D78" t="s">
+        <v>657</v>
+      </c>
+      <c r="E78" s="10" t="s">
         <v>658</v>
       </c>
-      <c r="D78" t="s">
+      <c r="F78" s="14" t="s">
         <v>659</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>660</v>
-      </c>
-      <c r="F78" s="14" t="s">
-        <v>661</v>
       </c>
       <c r="G78" s="14">
         <v>2</v>
@@ -7129,16 +7147,16 @@
         <v>158</v>
       </c>
       <c r="C79" t="s">
+        <v>660</v>
+      </c>
+      <c r="D79" t="s">
+        <v>670</v>
+      </c>
+      <c r="E79" t="s">
         <v>662</v>
       </c>
-      <c r="D79" t="s">
-        <v>673</v>
-      </c>
-      <c r="E79" t="s">
-        <v>664</v>
-      </c>
       <c r="F79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="I79" t="str">
         <f t="shared" si="2"/>
@@ -7153,16 +7171,16 @@
         <v>109</v>
       </c>
       <c r="C80" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D80" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="E80" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F80" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I80" t="str">
         <f t="shared" si="2"/>
@@ -7216,7 +7234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="116" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -7283,7 +7301,7 @@
         <v>261</v>
       </c>
       <c r="H2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="I2">
         <v>24.99</v>
@@ -7312,7 +7330,7 @@
         <v>266</v>
       </c>
       <c r="H3" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I3">
         <v>25</v>
@@ -7341,7 +7359,7 @@
         <v>270</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I4">
         <v>24.99</v>
@@ -7387,7 +7405,7 @@
         <v>293</v>
       </c>
       <c r="H6" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="I6">
         <v>20</v>
@@ -7445,7 +7463,7 @@
         <v>270</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I8">
         <v>24.99</v>
@@ -7474,7 +7492,7 @@
         <v>261</v>
       </c>
       <c r="H9" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="I9">
         <v>24.99</v>
@@ -7497,13 +7515,13 @@
         <v>34</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G10" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H10" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="I10">
         <v>34.950000000000003</v>
@@ -7532,7 +7550,7 @@
         <v>261</v>
       </c>
       <c r="H11" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="I11">
         <v>24.99</v>
@@ -7561,7 +7579,7 @@
         <v>293</v>
       </c>
       <c r="H12" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="I12">
         <v>20</v>
@@ -7584,13 +7602,13 @@
         <v>156</v>
       </c>
       <c r="F13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G13" t="s">
         <v>270</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I13">
         <v>24.99</v>
@@ -7601,10 +7619,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D14" t="s">
         <v>228</v>
@@ -7613,13 +7631,13 @@
         <v>32</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H14" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="I14">
         <v>25</v>
@@ -7642,13 +7660,13 @@
         <v>258</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G15" t="s">
         <v>261</v>
       </c>
       <c r="H15" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="I15">
         <v>24.99</v>
@@ -7659,10 +7677,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C16" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D16" t="s">
         <v>228</v>
@@ -7671,13 +7689,13 @@
         <v>162</v>
       </c>
       <c r="F16" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H16" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="I16">
         <v>34</v>
@@ -7688,10 +7706,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C17" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D17" t="s">
         <v>228</v>
@@ -7700,13 +7718,13 @@
         <v>354</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G17" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H17" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="I17">
         <v>34.99</v>
@@ -7717,25 +7735,25 @@
         <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D18" t="s">
         <v>228</v>
       </c>
       <c r="E18" t="s">
+        <v>395</v>
+      </c>
+      <c r="F18" t="s">
+        <v>396</v>
+      </c>
+      <c r="G18" t="s">
         <v>397</v>
       </c>
-      <c r="F18" t="s">
-        <v>398</v>
-      </c>
-      <c r="G18" t="s">
-        <v>399</v>
-      </c>
       <c r="H18" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I18">
         <v>25</v>
@@ -7746,25 +7764,25 @@
         <v>15</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C19" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D19" t="s">
         <v>228</v>
       </c>
       <c r="E19" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F19" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="G19" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H19" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="I19">
         <v>20</v>
@@ -7775,25 +7793,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C20" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D20" t="s">
         <v>228</v>
       </c>
       <c r="E20" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F20" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G20" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H20" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="I20">
         <v>34.99</v>
@@ -7804,10 +7822,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C21" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D21" t="s">
         <v>228</v>
@@ -7816,13 +7834,13 @@
         <v>129</v>
       </c>
       <c r="F21" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G21" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H21" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="I21">
         <v>19.95</v>
@@ -7833,28 +7851,28 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C22" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D22" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E22">
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G22" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H22" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I22" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -7862,10 +7880,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C23" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D23" t="s">
         <v>228</v>
@@ -7874,13 +7892,13 @@
         <v>267</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H23" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="I23">
         <v>29.95</v>
@@ -7891,10 +7909,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C24" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D24" t="s">
         <v>228</v>
@@ -7903,13 +7921,13 @@
         <v>34</v>
       </c>
       <c r="F24" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G24" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H24" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="I24">
         <v>38</v>
@@ -7920,10 +7938,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C25" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D25" t="s">
         <v>228</v>
@@ -7932,13 +7950,13 @@
         <v>410</v>
       </c>
       <c r="F25" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="G25" t="s">
         <v>549</v>
       </c>
-      <c r="G25" t="s">
-        <v>551</v>
-      </c>
       <c r="H25" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I25">
         <v>10</v>
@@ -7949,10 +7967,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C26" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D26" t="s">
         <v>228</v>
@@ -7961,13 +7979,13 @@
         <v>300</v>
       </c>
       <c r="F26" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G26" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H26" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="I26">
         <v>38</v>
@@ -7990,7 +8008,7 @@
         <v>86</v>
       </c>
       <c r="F27" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>299</v>
@@ -8007,10 +8025,10 @@
         <v>23</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C28" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D28" t="s">
         <v>228</v>
@@ -8019,13 +8037,13 @@
         <v>157</v>
       </c>
       <c r="F28" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="H28" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="I28">
         <v>35</v>
@@ -8036,7 +8054,7 @@
         <v>16</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="C29" t="s">
         <v>304</v>
@@ -8048,13 +8066,13 @@
         <v>34</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="G29" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="H29" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="I29">
         <v>10</v>
@@ -8073,10 +8091,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8141,7 +8159,7 @@
         <v>306</v>
       </c>
       <c r="C5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -8149,10 +8167,10 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -8160,10 +8178,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -8171,10 +8189,10 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -8182,10 +8200,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8193,10 +8211,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8204,10 +8222,10 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C11" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -8215,10 +8233,10 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -8226,10 +8244,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C13" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -8237,10 +8255,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C14" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -8248,10 +8266,10 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C15" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -8259,10 +8277,10 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C16" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -8270,10 +8288,10 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C17" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -8284,7 +8302,7 @@
         <v>192</v>
       </c>
       <c r="C18" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -8292,10 +8310,10 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C19" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -8303,10 +8321,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="C20" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -8314,10 +8332,32 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="C21" t="s">
-        <v>682</v>
+        <v>679</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>691</v>
+      </c>
+      <c r="C22" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>691</v>
+      </c>
+      <c r="C23" t="s">
+        <v>693</v>
       </c>
     </row>
   </sheetData>
@@ -8357,7 +8397,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>290</v>
@@ -8383,16 +8423,16 @@
         <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -8620,16 +8660,16 @@
         <v>171</v>
       </c>
       <c r="D17" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H17" t="s">
         <v>273</v>
@@ -12179,7 +12219,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -12188,28 +12228,28 @@
         <v>105</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>330</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -12345,7 +12385,7 @@
       </c>
       <c r="G4">
         <f>SUMIFS(IMAGES!G:G,IMAGES!A:A,'to-do-score-card'!B4,IMAGES!B:B,"topo")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H4">
         <f>_xlfn.IFNA(IF(VLOOKUP(B4,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
@@ -13021,7 +13061,7 @@
       </c>
       <c r="G17">
         <f>SUMIFS(IMAGES!G:G,IMAGES!A:A,'to-do-score-card'!B17,IMAGES!B:B,"topo")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H17">
         <f>_xlfn.IFNA(IF(VLOOKUP(B17,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>

</xml_diff>

<commit_message>
Added Static icons to improve perfomance, also added temp. Hopefully didn't break anything else
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B97238-7C6A-44C6-8DE5-DFA3B2EED0DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3761CE5D-B84E-40D5-9B6B-573537A27009}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,18 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">IMAGES!$A$1:$I$116</definedName>
   </definedNames>
   <calcPr calcId="181029" iterateDelta="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="704">
   <si>
     <t>cliff</t>
   </si>
@@ -2271,6 +2278,21 @@
   </si>
   <si>
     <t>Red Wall details on Mountain Project</t>
+  </si>
+  <si>
+    <t>Sepage</t>
+  </si>
+  <si>
+    <t>Wintour's Leap</t>
+  </si>
+  <si>
+    <t>Middlefell Butress</t>
+  </si>
+  <si>
+    <t>Wye Valley</t>
+  </si>
+  <si>
+    <t>Lake District</t>
   </si>
 </sst>
 </file>
@@ -3413,11 +3435,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A17" sqref="A17:B17"/>
+      <selection pane="topRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3442,7 +3464,7 @@
     <col min="23" max="23" width="5.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3518,8 +3540,11 @@
       <c r="Y1" s="1" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="Z1" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -3584,7 +3609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3646,7 +3671,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -3707,8 +3732,11 @@
       <c r="V4" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="Z4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -3764,7 +3792,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -3832,7 +3860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -3894,7 +3922,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -3953,7 +3981,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -4018,7 +4046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -4081,7 +4109,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -4146,7 +4174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -4208,7 +4236,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>184</v>
       </c>
@@ -4279,7 +4307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>196</v>
       </c>
@@ -4341,7 +4369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>212</v>
       </c>
@@ -4404,7 +4432,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>241</v>
       </c>
@@ -4472,7 +4500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>304</v>
       </c>
@@ -4536,8 +4564,11 @@
       <c r="V17" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="Z17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>344</v>
       </c>
@@ -4602,7 +4633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>377</v>
       </c>
@@ -4658,8 +4689,11 @@
         <v>382</v>
       </c>
       <c r="T19" s="2"/>
-    </row>
-    <row r="20" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="Z19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>406</v>
       </c>
@@ -4721,7 +4755,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>410</v>
       </c>
@@ -4779,8 +4813,11 @@
       <c r="V21" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="Z21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>446</v>
       </c>
@@ -4842,7 +4879,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>447</v>
       </c>
@@ -4907,7 +4944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>506</v>
       </c>
@@ -4975,7 +5012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>523</v>
       </c>
@@ -5044,7 +5081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>561</v>
       </c>
@@ -5110,7 +5147,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>577</v>
       </c>
@@ -5179,7 +5216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>643</v>
       </c>
@@ -5234,7 +5271,7 @@
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
-    <row r="29" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>645</v>
       </c>
@@ -5296,7 +5333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>650</v>
       </c>
@@ -5305,6 +5342,43 @@
       </c>
       <c r="C30">
         <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>700</v>
+      </c>
+      <c r="B31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>701</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32">
+        <v>31</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -8145,7 +8219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added wintours leap climb
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3761CE5D-B84E-40D5-9B6B-573537A27009}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD28B01-2CFD-4F2F-83DD-D74540E3ADB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="711">
   <si>
     <t>cliff</t>
   </si>
@@ -2052,9 +2052,6 @@
   </si>
   <si>
     <t>3a</t>
-  </si>
-  <si>
-    <t>Setesdal</t>
   </si>
   <si>
     <t>https://earth.app.goo.gl/XCHT6i</t>
@@ -2283,16 +2280,40 @@
     <t>Sepage</t>
   </si>
   <si>
-    <t>Wintour's Leap</t>
-  </si>
-  <si>
-    <t>Middlefell Butress</t>
-  </si>
-  <si>
-    <t>Wye Valley</t>
-  </si>
-  <si>
-    <t>Lake District</t>
+    <t>Wintours Leap</t>
+  </si>
+  <si>
+    <t>Gloucestershire</t>
+  </si>
+  <si>
+    <t>Right Hand Route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The right-hand route is in many ways the opposite twin to the left hand route. It has better pitches at the top where the left-hand route has better pitches at the bottom. While the right-hand route looks heavily vegetated from the bottom its surprisingly clean. That’s not to say its perfect, just better than it looks. It has good variety and is more sustained in grade when compared to the left hand route, which has a hard start and then eases off. It’s a classic limestone route with a small crack section, and exposed thin ledge system and a steeper juggy section at the end. Check the BMC RAD Database for route exit information. </t>
+  </si>
+  <si>
+    <t>img/tiles/wintours-leap-wye-valley-climbing.jpg</t>
+  </si>
+  <si>
+    <t>Limestone Outcrop Wintours Leap in the Wye Valley</t>
+  </si>
+  <si>
+    <t>Right Hand Route Climb at Wintours Leap in the Wye Valley</t>
+  </si>
+  <si>
+    <t>img/topos/wye-valley/wye-valley-wintours-leap-right-hand-route.png</t>
+  </si>
+  <si>
+    <t>51.664827,-2.664312</t>
+  </si>
+  <si>
+    <t>There is a grassy parking space for several cars above the outcrop at 51.666565, -2.665006. From there, continue on the road you came in on and take the first obvious path left not long after leaving the parking area. Follow the path and take the next obvious left after the old stone arches. After following this path until you come to the old chapel near the river. Pass it and turn left at h the river. Follow this path for a short distance until you near the outcrop then take a left up a climbers path to the base of the cliff.</t>
+  </si>
+  <si>
+    <t>img/topos/wye-valley/maps/</t>
+  </si>
+  <si>
+    <t>Location of Wintours Leap Climbing in the Wye Valley</t>
   </si>
 </sst>
 </file>
@@ -2954,7 +2975,147 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3437,9 +3598,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="65" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F31" sqref="F31"/>
+      <selection pane="topRight" activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3541,7 +3702,7 @@
         <v>627</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -4289,13 +4450,13 @@
         <v>191</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="S13" s="2" t="s">
         <v>633</v>
       </c>
       <c r="T13" s="14" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V13" t="s">
         <v>172</v>
@@ -4553,10 +4714,10 @@
         <v>318</v>
       </c>
       <c r="S17" s="14" t="s">
+        <v>694</v>
+      </c>
+      <c r="T17" s="14" t="s">
         <v>695</v>
-      </c>
-      <c r="T17" s="14" t="s">
-        <v>696</v>
       </c>
       <c r="U17" t="s">
         <v>171</v>
@@ -5288,7 +5449,7 @@
         <v>646</v>
       </c>
       <c r="F29" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G29">
         <v>115</v>
@@ -5324,10 +5485,10 @@
         <v>41</v>
       </c>
       <c r="R29" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="S29" s="2" t="s">
         <v>663</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>664</v>
       </c>
       <c r="W29">
         <v>1</v>
@@ -5335,50 +5496,58 @@
     </row>
     <row r="30" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>650</v>
+        <v>699</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" t="s">
         <v>700</v>
       </c>
-      <c r="B31" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31">
-        <v>30</v>
-      </c>
-      <c r="D31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="F30" t="s">
+        <v>701</v>
+      </c>
+      <c r="G30">
+        <v>87</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>4</v>
+      </c>
+      <c r="J30" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" t="s">
+        <v>38</v>
+      </c>
+      <c r="M30" t="s">
+        <v>39</v>
+      </c>
+      <c r="N30" t="s">
+        <v>707</v>
+      </c>
+      <c r="O30">
+        <v>20</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>64</v>
+      </c>
+      <c r="R30" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>701</v>
-      </c>
-      <c r="B32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32">
-        <v>31</v>
-      </c>
-      <c r="D32" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" t="s">
-        <v>703</v>
+      <c r="S30" s="2" t="s">
+        <v>708</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -5396,9 +5565,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5432,7 +5601,7 @@
         <v>117</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>328</v>
@@ -5512,16 +5681,16 @@
         <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D5" t="s">
         <v>123</v>
       </c>
       <c r="E5" t="s">
+        <v>680</v>
+      </c>
+      <c r="F5" t="s">
         <v>681</v>
-      </c>
-      <c r="F5" t="s">
-        <v>682</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -5593,7 +5762,7 @@
         <v>127</v>
       </c>
       <c r="F8" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -6019,7 +6188,7 @@
         <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D27" t="s">
         <v>156</v>
@@ -6166,7 +6335,7 @@
         <v>193</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F33" t="s">
         <v>155</v>
@@ -6451,16 +6620,16 @@
         <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D45" t="s">
         <v>307</v>
       </c>
       <c r="E45" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="F45" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G45">
         <v>5</v>
@@ -6604,7 +6773,7 @@
         <v>384</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="F51" t="s">
         <v>110</v>
@@ -6946,7 +7115,7 @@
         <v>626</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" ref="I65:I80" si="2">CONCATENATE(A65,B65)</f>
+        <f t="shared" ref="I65:I83" si="2">CONCATENATE(A65,B65)</f>
         <v>22map</v>
       </c>
     </row>
@@ -7246,16 +7415,16 @@
         <v>114</v>
       </c>
       <c r="C78" t="s">
+        <v>653</v>
+      </c>
+      <c r="D78" t="s">
         <v>654</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" s="10" t="s">
         <v>655</v>
       </c>
-      <c r="E78" s="10" t="s">
+      <c r="F78" s="14" t="s">
         <v>656</v>
-      </c>
-      <c r="F78" s="14" t="s">
-        <v>657</v>
       </c>
       <c r="G78" s="14">
         <v>2</v>
@@ -7273,16 +7442,16 @@
         <v>158</v>
       </c>
       <c r="C79" t="s">
+        <v>657</v>
+      </c>
+      <c r="D79" t="s">
+        <v>667</v>
+      </c>
+      <c r="E79" t="s">
+        <v>659</v>
+      </c>
+      <c r="F79" t="s">
         <v>658</v>
-      </c>
-      <c r="D79" t="s">
-        <v>668</v>
-      </c>
-      <c r="E79" t="s">
-        <v>660</v>
-      </c>
-      <c r="F79" t="s">
-        <v>659</v>
       </c>
       <c r="I79" t="str">
         <f t="shared" si="2"/>
@@ -7297,10 +7466,10 @@
         <v>109</v>
       </c>
       <c r="C80" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D80" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E80" t="s">
         <v>625</v>
@@ -7313,7 +7482,82 @@
         <v>28map</v>
       </c>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>29</v>
+      </c>
+      <c r="B81" t="s">
+        <v>158</v>
+      </c>
+      <c r="C81" t="s">
+        <v>703</v>
+      </c>
+      <c r="D81" t="s">
+        <v>704</v>
+      </c>
+      <c r="E81" t="s">
+        <v>154</v>
+      </c>
+      <c r="F81" t="s">
+        <v>155</v>
+      </c>
+      <c r="I81" t="str">
+        <f t="shared" si="2"/>
+        <v>29tile</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <v>29</v>
+      </c>
+      <c r="B82" t="s">
+        <v>114</v>
+      </c>
+      <c r="C82" t="s">
+        <v>706</v>
+      </c>
+      <c r="D82" t="s">
+        <v>705</v>
+      </c>
+      <c r="E82" t="s">
+        <v>154</v>
+      </c>
+      <c r="F82" t="s">
+        <v>155</v>
+      </c>
+      <c r="G82">
+        <v>5</v>
+      </c>
+      <c r="I82" t="str">
+        <f t="shared" si="2"/>
+        <v>29topo</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <v>29</v>
+      </c>
+      <c r="B83" t="s">
+        <v>109</v>
+      </c>
+      <c r="C83" t="s">
+        <v>709</v>
+      </c>
+      <c r="D83" t="s">
+        <v>710</v>
+      </c>
+      <c r="E83" t="s">
+        <v>625</v>
+      </c>
+      <c r="F83" t="s">
+        <v>626</v>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" si="2"/>
+        <v>29map</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E91" s="10"/>
     </row>
     <row r="113" spans="9:9" x14ac:dyDescent="0.45">
@@ -7902,7 +8146,7 @@
         <v>394</v>
       </c>
       <c r="F19" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G19" t="s">
         <v>399</v>
@@ -8180,7 +8424,7 @@
         <v>16</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C29" t="s">
         <v>304</v>
@@ -8192,13 +8436,13 @@
         <v>34</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="G29" t="s">
+        <v>673</v>
+      </c>
+      <c r="H29" t="s">
         <v>672</v>
-      </c>
-      <c r="G29" t="s">
-        <v>674</v>
-      </c>
-      <c r="H29" t="s">
-        <v>673</v>
       </c>
       <c r="I29">
         <v>10</v>
@@ -8414,10 +8658,10 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
+        <v>650</v>
+      </c>
+      <c r="C17" t="s">
         <v>651</v>
-      </c>
-      <c r="C17" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -8428,7 +8672,7 @@
         <v>192</v>
       </c>
       <c r="C18" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -8436,10 +8680,10 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
+        <v>660</v>
+      </c>
+      <c r="C19" t="s">
         <v>661</v>
-      </c>
-      <c r="C19" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -8447,10 +8691,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="C20" t="s">
         <v>679</v>
-      </c>
-      <c r="C20" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -8458,10 +8702,10 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
+        <v>675</v>
+      </c>
+      <c r="C21" t="s">
         <v>676</v>
-      </c>
-      <c r="C21" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -8469,10 +8713,10 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
+        <v>688</v>
+      </c>
+      <c r="C22" t="s">
         <v>689</v>
-      </c>
-      <c r="C22" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -8480,10 +8724,10 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C23" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -8491,7 +8735,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C24" t="s">
         <v>371</v>
@@ -8502,10 +8746,10 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
+        <v>696</v>
+      </c>
+      <c r="C25" t="s">
         <v>697</v>
-      </c>
-      <c r="C25" t="s">
-        <v>698</v>
       </c>
     </row>
   </sheetData>
@@ -12346,10 +12590,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -12385,7 +12629,7 @@
         <v>325</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>326</v>
@@ -13845,76 +14089,127 @@
         <v/>
       </c>
     </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A30" t="str">
+        <f>CLIMBS!A30</f>
+        <v>Wintours Leap</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="str">
+        <f>CLIMBS!B30</f>
+        <v>publish</v>
+      </c>
+      <c r="D30">
+        <f>IF(CLIMBS!R30&lt;&gt;0,1,0)+IF(CLIMBS!G30&lt;&gt;0,1,0)+IF(CLIMBS!H30&lt;&gt;0,1,0)+IF(CLIMBS!I30&lt;&gt;0,1,0)+IF(CLIMBS!J30&lt;&gt;0,1,0)+IF(CLIMBS!N30&lt;&gt;0,1,0)+IF(CLIMBS!M30&lt;&gt;0,1,0)+IF(CLIMBS!O30&lt;&gt;0,1,0)+IF(CLIMBS!P30&lt;&gt;0,1,0)</f>
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <f>IF(CLIMBS!S30&lt;&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B30,"tile"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B30,"topo"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B30,"map"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <f>SUMIFS(IMAGES!G:G,IMAGES!A:A,'to-do-score-card'!B30,IMAGES!B:B,"topo")</f>
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B30,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B30,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B30,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <f>IF(VLOOKUP(B30,CLIMBS!C:T,18,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="25" t="str">
+        <f t="shared" ref="L30" si="1">IF(SUM(D30:K30)=22,"DONE","")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="greaterThan">
+  <conditionalFormatting sqref="D2:D30">
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="17" operator="lessThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C29">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+  <conditionalFormatting sqref="C2:C30">
+    <cfRule type="cellIs" dxfId="28" priority="15" operator="equal">
       <formula>"draft"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C29">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+  <conditionalFormatting sqref="C3:C30">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E29">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
+  <conditionalFormatting sqref="E2:E30">
+    <cfRule type="cellIs" dxfId="25" priority="11" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G30">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>"missing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:J29">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+  <conditionalFormatting sqref="H2:J30">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K29">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="K2:K30">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+  <conditionalFormatting sqref="G2:G30">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F29">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="F2:F30">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added loads more info to wintours leap climb and compressed images and added decent
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD28B01-2CFD-4F2F-83DD-D74540E3ADB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4108A245-2DAD-4726-9874-934EFD2B8F5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="720">
   <si>
     <t>cliff</t>
   </si>
@@ -2289,31 +2289,69 @@
     <t>Right Hand Route</t>
   </si>
   <si>
-    <t xml:space="preserve">The right-hand route is in many ways the opposite twin to the left hand route. It has better pitches at the top where the left-hand route has better pitches at the bottom. While the right-hand route looks heavily vegetated from the bottom its surprisingly clean. That’s not to say its perfect, just better than it looks. It has good variety and is more sustained in grade when compared to the left hand route, which has a hard start and then eases off. It’s a classic limestone route with a small crack section, and exposed thin ledge system and a steeper juggy section at the end. Check the BMC RAD Database for route exit information. </t>
-  </si>
-  <si>
-    <t>img/tiles/wintours-leap-wye-valley-climbing.jpg</t>
-  </si>
-  <si>
     <t>Limestone Outcrop Wintours Leap in the Wye Valley</t>
   </si>
   <si>
     <t>Right Hand Route Climb at Wintours Leap in the Wye Valley</t>
   </si>
   <si>
-    <t>img/topos/wye-valley/wye-valley-wintours-leap-right-hand-route.png</t>
-  </si>
-  <si>
     <t>51.664827,-2.664312</t>
   </si>
   <si>
-    <t>There is a grassy parking space for several cars above the outcrop at 51.666565, -2.665006. From there, continue on the road you came in on and take the first obvious path left not long after leaving the parking area. Follow the path and take the next obvious left after the old stone arches. After following this path until you come to the old chapel near the river. Pass it and turn left at h the river. Follow this path for a short distance until you near the outcrop then take a left up a climbers path to the base of the cliff.</t>
-  </si>
-  <si>
     <t>img/topos/wye-valley/maps/</t>
   </si>
   <si>
     <t>Location of Wintours Leap Climbing in the Wye Valley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Approach:&lt;/strong&gt; There is a grassy parking space for several cars above the outcrop at 51.666565, -2.665006. From there, continue on the road you came in on and take the first obvious path left not long after leaving the parking area. Follow the path and take the next obvious left after the old stone arches. After following this path until you come to the old chapel near the river. Pass it and turn left at h the river. Follow this path for a short distance until you near the outcrop then take a left up a climbers path to the base of the cliff. &lt;br /&gt;&lt;br /&gt;
+&lt;strong&gt;Descent:&lt;/strong&gt; following a change of ownership of the house above this section of crag, the previous arrangement to exit through it’s garden is not longer possible. Please do not top out on any North Wall routes - only abseil descent from below the top of the crag is allowed. For those who don't wan't to climb above the Great Ledge, an abseil descent can be made from one of the two bolted abseil stations above The Tap or Joe’s Route. Two further abseil stations have been established just below the top of North Wall (using rope slings and rings around trees) allowing the last pitch of the more popular routes to be climbed and an abseil descent to the Great Ledge be made. 
+</t>
+  </si>
+  <si>
+    <t>https://www.thebmc.co.uk/modules/RAD/View.aspx?id=744</t>
+  </si>
+  <si>
+    <t>BMC RAD database Page</t>
+  </si>
+  <si>
+    <t>img/tiles/wintours-leap-wye-valley-climbs.jpg</t>
+  </si>
+  <si>
+    <t>img/topos/wye-valley/wye-valley-wintours-leap-right-hand-route.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Right Hand Route takes a route up good rock weaving round trees and foliage and makes good use of ledges for belay points. 
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;18m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;3c&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Climb the cracked gully diagonally right to get round some bushes then cut back left above them. There is a small stance and a decent tree belay just above the main ledge. The tree can be backed up with some protection in the rock behind. &lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 2 –&lt;span class="length"&gt;21m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+The second pitch ups the grade a bit after an easy start. Climb straight up behind the belay past some vegetation. Keep moving up until your below a left leaning thin crack that leads to another small ledge with a tree belay (again back it up in the rock behind). The crack offers good holds and protection but can feel a bit exposed and is a slight step change in the grade, especially if you can’t find the good holds.&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;17m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Climb up and slightly right onto some ledges. Take the left of two groves, this should have a peg you could use for additional protection. After that there should be a short neat slab and easier ground up onto the great ledge where there is a peg and tree belay at the back. Traversing left on a thin finger ledge before the great ledge offers a lovely if exposed climb with a big mantle move up. &lt;br/&gt;
+&lt;strong class="pitch-title"&gt;Pitch 4 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+A brilliant and rewarding pitch with great protection. Essentially you are looking to head though the broken V shape in the headwall above the ledge. The route has good holds, making it easer than it looks. After the broken V climb the short wall above and then keep heading up to slings and an abseil ring set up on a tree. You can climb the chimney or the wall directly below the abseil and anchor point. Both are short but fun. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The right hand route is in many ways the opposite twin to the left hand route (also a Hard Severe climb). It has better pitches at the top where the left-hand route has better pitches at the bottom. While the right hand route looks heavily vegetated from the bottom it’s surprisingly clean. That’s not to say its perfect, just better than it looks. It has good variety and is more sustained in grade when compared to the left-hand route, which has a hard start and then eases off. It’s a classic limestone route with a small crack section, and exposed thin ledge system and a steeper juggy section at the end. Check the BMC RAD Database for route exit information (see references), but at the time of writing abseiling off is required (see descent info). </t>
+  </si>
+  <si>
+    <t>Setdastal</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2XxjnCx</t>
+  </si>
+  <si>
+    <t>9780901601797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower Wye Valley </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The guidebook &lt;em&gt;Lower Wye Valley: Climbers' Club Guides to the Wye Valley and Forest of Dean&lt;/em&gt; has a good amount of information and climbs. The photos are for the most part very clear. However, the way the book is organised makes it very difficult to use. In true climber’s club style, there are no route numbers or page references on topos making it slow to find the details. When you do find the climb details, they use complex language and terminology, making it hard work to understand. Unfortunately there are not any other guidebook options for Wintour’s Leap, making this guidebook a must. </t>
+  </si>
+  <si>
+    <t>img/guidebooks/lower-wye-valley-climbing-guidebook.jpg</t>
   </si>
 </sst>
 </file>
@@ -2872,7 +2910,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2929,6 +2967,8 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2975,147 +3015,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3600,7 +3500,7 @@
   <sheetViews>
     <sheetView zoomScale="65" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q25" sqref="Q25"/>
+      <selection pane="topRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3766,9 +3666,6 @@
       <c r="W2">
         <v>1</v>
       </c>
-      <c r="Y2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -5532,7 +5429,7 @@
         <v>39</v>
       </c>
       <c r="N30" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="O30">
         <v>20</v>
@@ -5544,10 +5441,30 @@
         <v>64</v>
       </c>
       <c r="R30" t="s">
-        <v>702</v>
-      </c>
-      <c r="S30" s="2" t="s">
-        <v>708</v>
+        <v>713</v>
+      </c>
+      <c r="S30" s="14" t="s">
+        <v>707</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="U30" t="s">
+        <v>207</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>714</v>
+      </c>
+      <c r="B31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -5565,9 +5482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
+      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7490,10 +7407,10 @@
         <v>158</v>
       </c>
       <c r="C81" t="s">
-        <v>703</v>
+        <v>710</v>
       </c>
       <c r="D81" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="E81" t="s">
         <v>154</v>
@@ -7514,10 +7431,10 @@
         <v>114</v>
       </c>
       <c r="C82" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
       <c r="D82" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="E82" t="s">
         <v>154</v>
@@ -7541,10 +7458,10 @@
         <v>109</v>
       </c>
       <c r="C83" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D83" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="E83" t="s">
         <v>625</v>
@@ -7602,10 +7519,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="116" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A16" zoomScale="116" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8448,6 +8365,35 @@
         <v>10</v>
       </c>
     </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="C30" t="s">
+        <v>717</v>
+      </c>
+      <c r="D30" t="s">
+        <v>228</v>
+      </c>
+      <c r="E30">
+        <v>101</v>
+      </c>
+      <c r="F30" t="s">
+        <v>718</v>
+      </c>
+      <c r="G30" t="s">
+        <v>719</v>
+      </c>
+      <c r="H30" t="s">
+        <v>715</v>
+      </c>
+      <c r="I30">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1" xr:uid="{14007672-E4E3-4A8F-8DD0-45E59BDCCEDC}"/>
@@ -8461,10 +8407,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8655,7 +8601,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>650</v>
@@ -8750,6 +8696,17 @@
       </c>
       <c r="C25" t="s">
         <v>697</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>708</v>
+      </c>
+      <c r="C26" t="s">
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -9085,8 +9042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745174B4-A8CA-45B8-ACCB-9B5B609F0D5D}">
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="94" workbookViewId="0">
-      <selection activeCell="Q67" sqref="Q67"/>
+    <sheetView topLeftCell="A65" zoomScale="94" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12547,10 +12504,138 @@
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A77" s="12">
+        <v>29</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C77" s="12">
+        <v>13</v>
+      </c>
+      <c r="D77" s="12">
+        <v>9</v>
+      </c>
+      <c r="E77" s="12">
+        <v>11</v>
+      </c>
+      <c r="F77" s="12">
+        <v>9</v>
+      </c>
+      <c r="G77" s="12">
+        <v>8</v>
+      </c>
+      <c r="H77" s="12">
+        <v>8</v>
+      </c>
+      <c r="I77" s="12">
+        <v>7</v>
+      </c>
+      <c r="J77" s="12">
+        <v>8</v>
+      </c>
+      <c r="K77" s="12">
+        <v>9</v>
+      </c>
+      <c r="L77" s="12">
+        <v>11</v>
+      </c>
+      <c r="M77" s="12">
+        <v>10</v>
+      </c>
+      <c r="N77" s="12">
+        <v>11</v>
+      </c>
       <c r="U77" s="7"/>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A78" s="11">
+        <v>29</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C78" s="26">
+        <v>7</v>
+      </c>
+      <c r="D78" s="26">
+        <v>7.3</v>
+      </c>
+      <c r="E78" s="26">
+        <v>9.6</v>
+      </c>
+      <c r="F78" s="26">
+        <v>12.7</v>
+      </c>
+      <c r="G78" s="26">
+        <v>16</v>
+      </c>
+      <c r="H78" s="26">
+        <v>19.2</v>
+      </c>
+      <c r="I78" s="26">
+        <v>20.7</v>
+      </c>
+      <c r="J78" s="26">
+        <v>20.2</v>
+      </c>
+      <c r="K78" s="26">
+        <v>17.7</v>
+      </c>
+      <c r="L78" s="26">
+        <v>14.1</v>
+      </c>
+      <c r="M78" s="26">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="N78" s="26">
+        <v>7.9</v>
+      </c>
       <c r="U78" s="7"/>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A79" s="13">
+        <v>29</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C79" s="27">
+        <v>1.6</v>
+      </c>
+      <c r="D79" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="E79" s="27">
+        <v>2.8</v>
+      </c>
+      <c r="F79" s="27">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G79" s="27">
+        <v>7.7</v>
+      </c>
+      <c r="H79" s="27">
+        <v>10.7</v>
+      </c>
+      <c r="I79" s="27">
+        <v>12.2</v>
+      </c>
+      <c r="J79" s="27">
+        <v>12</v>
+      </c>
+      <c r="K79" s="27">
+        <v>10</v>
+      </c>
+      <c r="L79" s="27">
+        <v>7.4</v>
+      </c>
+      <c r="M79" s="27">
+        <v>4</v>
+      </c>
+      <c r="N79" s="27">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U80" s="7"/>
@@ -12592,8 +12677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="87" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -12692,7 +12777,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="25" t="str">
-        <f t="shared" ref="L2:L29" si="0">IF(SUM(D2:K2)=22,"DONE","")</f>
+        <f t="shared" ref="L2:L30" si="0">IF(SUM(D2:K2)=22,"DONE","")</f>
         <v/>
       </c>
     </row>
@@ -14121,11 +14206,11 @@
       </c>
       <c r="H30">
         <f>_xlfn.IFNA(IF(VLOOKUP(B30,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30">
         <f>_xlfn.IFNA(IF(VLOOKUP(B30,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30">
         <f>_xlfn.IFNA(IF(VLOOKUP(B30,REFERANCES!A:A,1,FALSE),1,0),0)</f>
@@ -14133,83 +14218,83 @@
       </c>
       <c r="K30">
         <f>IF(VLOOKUP(B30,CLIMBS!C:T,18,FALSE)&gt;0,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="25" t="str">
-        <f t="shared" ref="L30" si="1">IF(SUM(D30:K30)=22,"DONE","")</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>DONE</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D30">
-    <cfRule type="cellIs" dxfId="30" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="lessThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C30">
-    <cfRule type="cellIs" dxfId="28" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"draft"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C30">
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E30">
-    <cfRule type="cellIs" dxfId="25" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G30">
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"missing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J30">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K30">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G30">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F30">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
+ improved link contracts for accessibility + removed some unused CSS + adjusted the weather score, downweighting future weather + updated text for wintours leap for readability
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4108A245-2DAD-4726-9874-934EFD2B8F5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70897733-0D3D-489F-8A7A-9C987552E775}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -2277,9 +2277,6 @@
     <t>Red Wall details on Mountain Project</t>
   </si>
   <si>
-    <t>Sepage</t>
-  </si>
-  <si>
     <t>Wintours Leap</t>
   </si>
   <si>
@@ -2321,37 +2318,40 @@
     <t>img/topos/wye-valley/wye-valley-wintours-leap-right-hand-route.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">The Right Hand Route takes a route up good rock weaving round trees and foliage and makes good use of ledges for belay points. 
+    <t xml:space="preserve">The right hand route is in many ways the opposite twin to the left hand route (also a Hard Severe climb). It has better pitches at the top where the left-hand route has better pitches at the bottom. While the right hand route looks heavily vegetated from the bottom it’s surprisingly clean. That’s not to say its perfect, just better than it looks. It has good variety and is more sustained in grade when compared to the left-hand route, which has a hard start and then eases off. It’s a classic limestone route with a small crack section, and exposed thin ledge system and a steeper juggy section at the end. Check the BMC RAD Database for route exit information (see references), but at the time of writing abseiling off is required (see descent info). </t>
+  </si>
+  <si>
+    <t>Setdastal</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2XxjnCx</t>
+  </si>
+  <si>
+    <t>9780901601797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower Wye Valley </t>
+  </si>
+  <si>
+    <t>img/guidebooks/lower-wye-valley-climbing-guidebook.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The guidebook &lt;em&gt;Lower Wye Valley: Climbers' Club Guides to the Wye Valley and Forest of Dean&lt;/em&gt; has a good amount of information and climbs. The photos are, for the most part very clear. However, the way the book is organised makes it difficult to use. In true climber’s club style, there are no route numbers on the descriptions or page references on the photo topos, making it slow to find the details. When you do find the climb details, they use complex language and terminology, making it hard to understand. Unfortunately, there are not any other guidebook options for Wintour’s Leap. All things said, the guidebook is not too expensive a must for getting the most out of the area. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Right Hand Route takes a line up good rock, weaving around trees and foliage and makes good use of ledges for belay points. 
 &lt;br /&gt;
 &lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;18m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;3c&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
-Climb the cracked gully diagonally right to get round some bushes then cut back left above them. There is a small stance and a decent tree belay just above the main ledge. The tree can be backed up with some protection in the rock behind. &lt;br /&gt;
+Climb the cracked gully diagonally right to get around some bushes then cut back left above them. There is a small stance and a decent tree belay just above the main ledge. The tree can be backed up with some protection in the rock. &lt;br /&gt;
 &lt;strong class="pitch-title"&gt;Pitch 2 –&lt;span class="length"&gt;21m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
-The second pitch ups the grade a bit after an easy start. Climb straight up behind the belay past some vegetation. Keep moving up until your below a left leaning thin crack that leads to another small ledge with a tree belay (again back it up in the rock behind). The crack offers good holds and protection but can feel a bit exposed and is a slight step change in the grade, especially if you can’t find the good holds.&lt;br /&gt;
+The second pitch ups the grade after an easy start. Climb straight up behind the belay past some vegetation. Keep moving up until you’re below a left leaning thin crack that leads to another small ledge with a tree belay (again back it up with the rock). The crack offers good holds and protection but can feel a bit exposed and is a slight step up in the grade, especially if you can’t find the good holds.&lt;br /&gt;
 &lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;17m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
 Climb up and slightly right onto some ledges. Take the left of two groves, this should have a peg you could use for additional protection. After that there should be a short neat slab and easier ground up onto the great ledge where there is a peg and tree belay at the back. Traversing left on a thin finger ledge before the great ledge offers a lovely if exposed climb with a big mantle move up. &lt;br/&gt;
 &lt;strong class="pitch-title"&gt;Pitch 4 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
-A brilliant and rewarding pitch with great protection. Essentially you are looking to head though the broken V shape in the headwall above the ledge. The route has good holds, making it easer than it looks. After the broken V climb the short wall above and then keep heading up to slings and an abseil ring set up on a tree. You can climb the chimney or the wall directly below the abseil and anchor point. Both are short but fun. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The right hand route is in many ways the opposite twin to the left hand route (also a Hard Severe climb). It has better pitches at the top where the left-hand route has better pitches at the bottom. While the right hand route looks heavily vegetated from the bottom it’s surprisingly clean. That’s not to say its perfect, just better than it looks. It has good variety and is more sustained in grade when compared to the left-hand route, which has a hard start and then eases off. It’s a classic limestone route with a small crack section, and exposed thin ledge system and a steeper juggy section at the end. Check the BMC RAD Database for route exit information (see references), but at the time of writing abseiling off is required (see descent info). </t>
-  </si>
-  <si>
-    <t>Setdastal</t>
-  </si>
-  <si>
-    <t>https://amzn.to/2XxjnCx</t>
-  </si>
-  <si>
-    <t>9780901601797</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lower Wye Valley </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The guidebook &lt;em&gt;Lower Wye Valley: Climbers' Club Guides to the Wye Valley and Forest of Dean&lt;/em&gt; has a good amount of information and climbs. The photos are for the most part very clear. However, the way the book is organised makes it very difficult to use. In true climber’s club style, there are no route numbers or page references on topos making it slow to find the details. When you do find the climb details, they use complex language and terminology, making it hard work to understand. Unfortunately there are not any other guidebook options for Wintour’s Leap, making this guidebook a must. </t>
-  </si>
-  <si>
-    <t>img/guidebooks/lower-wye-valley-climbing-guidebook.jpg</t>
+A brilliant and rewarding pitch with great protection. Essentially you are looking to head though the broken V shape in the headwall above the ledge. The route has good holds, making it easer than it looks. After the broken V, climb the short wall above and then keep heading up to slings and an abseil ring set up on a tree. You can climb the chimney or the wall directly below the abseil and anchor point. Both are short but fun. </t>
+  </si>
+  <si>
+    <t>seepage</t>
   </si>
 </sst>
 </file>
@@ -3498,9 +3498,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView zoomScale="65" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z26" sqref="Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3602,7 +3602,7 @@
         <v>627</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>698</v>
+        <v>719</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -3791,7 +3791,7 @@
         <v>273</v>
       </c>
       <c r="Z4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -4623,7 +4623,7 @@
         <v>273</v>
       </c>
       <c r="Z17">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="T19" s="2"/>
       <c r="Z19">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -4872,7 +4872,7 @@
         <v>215</v>
       </c>
       <c r="Z21">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -5393,7 +5393,7 @@
     </row>
     <row r="30" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B30" t="s">
         <v>106</v>
@@ -5405,10 +5405,10 @@
         <v>32</v>
       </c>
       <c r="E30" t="s">
+        <v>699</v>
+      </c>
+      <c r="F30" t="s">
         <v>700</v>
-      </c>
-      <c r="F30" t="s">
-        <v>701</v>
       </c>
       <c r="G30">
         <v>87</v>
@@ -5429,7 +5429,7 @@
         <v>39</v>
       </c>
       <c r="N30" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="O30">
         <v>20</v>
@@ -5441,13 +5441,13 @@
         <v>64</v>
       </c>
       <c r="R30" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="S30" s="14" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="T30" s="3" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="U30" t="s">
         <v>207</v>
@@ -5458,7 +5458,7 @@
     </row>
     <row r="31" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B31" t="s">
         <v>107</v>
@@ -7407,10 +7407,10 @@
         <v>158</v>
       </c>
       <c r="C81" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D81" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E81" t="s">
         <v>154</v>
@@ -7431,10 +7431,10 @@
         <v>114</v>
       </c>
       <c r="C82" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D82" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E82" t="s">
         <v>154</v>
@@ -7458,10 +7458,10 @@
         <v>109</v>
       </c>
       <c r="C83" t="s">
+        <v>704</v>
+      </c>
+      <c r="D83" t="s">
         <v>705</v>
-      </c>
-      <c r="D83" t="s">
-        <v>706</v>
       </c>
       <c r="E83" t="s">
         <v>625</v>
@@ -7522,7 +7522,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="116" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8370,10 +8370,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C30" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D30" t="s">
         <v>228</v>
@@ -8382,13 +8382,13 @@
         <v>101</v>
       </c>
       <c r="F30" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="G30" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="H30" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="I30">
         <v>25</v>
@@ -8703,10 +8703,10 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
+        <v>707</v>
+      </c>
+      <c r="C26" t="s">
         <v>708</v>
-      </c>
-      <c r="C26" t="s">
-        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -12677,7 +12677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="87" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="87" workbookViewId="0">
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added current weather to details (only if it loads). Also fixed some tracking.
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70897733-0D3D-489F-8A7A-9C987552E775}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD6D6D5-1B94-46FB-AD44-BC0F669D3FED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="724">
   <si>
     <t>cliff</t>
   </si>
@@ -2091,9 +2091,6 @@
   </si>
   <si>
     <t>El Catedral, (the Cathedral in English) is a volcanic plug that stands in Teide National Park in the centre of Tenerife. It offers a variety of traditional multi-pitch climbs that tend to be around 3 or 4 pitches in length to reach that summit via just over 100 meters of climbing. Whilst Tenerife has a lot of incredible climbing the majority of it is single pitch sport routes. El Catedral offers some of the best trad multi-pitch climbing on the island.  In order to climb there, you need to seek permission from the national park which seems to be a straightforward process (see links in references section below). The route Via Mendez &amp; Guillermo is not the original route up the face but offers a high quality adventure at grade UIAA V+. Whilst a completely different grading system it sits around VS. There are easier options to the summit if needed like the original route which is graded UIAA IV or around VDiff in British grades.</t>
-  </si>
-  <si>
-    <t>coming soon</t>
   </si>
   <si>
     <t>Catherderal Rock Climbing in the national park Tenerife</t>
@@ -2352,6 +2349,23 @@
   </si>
   <si>
     <t>seepage</t>
+  </si>
+  <si>
+    <t>UKC Page</t>
+  </si>
+  <si>
+    <t>https://www.ukclimbing.com/logbook/crag.php?id=17495#overview</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Approach&lt;/strong&gt;: There is limited parking at Parador del Teide which is a short walk away. Alternatively, there are coach services up to here in the national park. The Cathedral rock climbing is south West past Roques de García.
+&lt;br /&gt;
+&lt;strong&gt;Decent&lt;/strong&gt;: The Decent requires 2 two abseils. Once from the top of the route, the other off to the side which can be tricky to find.  See route topo above.</t>
+  </si>
+  <si>
+    <t>http://anuestraputabolacroquis.blogspot.com/search/label/P.N.%20DEL%20TEIDE</t>
+  </si>
+  <si>
+    <t>Good Local trad climbing info for the area including this route</t>
   </si>
 </sst>
 </file>
@@ -3498,9 +3512,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z26" sqref="Z26"/>
+    <sheetView topLeftCell="A5" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3602,7 +3616,7 @@
         <v>627</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -4347,13 +4361,13 @@
         <v>191</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="S13" s="2" t="s">
         <v>633</v>
       </c>
       <c r="T13" s="14" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="V13" t="s">
         <v>172</v>
@@ -4611,10 +4625,10 @@
         <v>318</v>
       </c>
       <c r="S17" s="14" t="s">
+        <v>693</v>
+      </c>
+      <c r="T17" s="14" t="s">
         <v>694</v>
-      </c>
-      <c r="T17" s="14" t="s">
-        <v>695</v>
       </c>
       <c r="U17" t="s">
         <v>171</v>
@@ -5346,7 +5360,7 @@
         <v>646</v>
       </c>
       <c r="F29" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G29">
         <v>115</v>
@@ -5384,8 +5398,8 @@
       <c r="R29" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="S29" s="2" t="s">
-        <v>663</v>
+      <c r="S29" s="14" t="s">
+        <v>721</v>
       </c>
       <c r="W29">
         <v>1</v>
@@ -5393,7 +5407,7 @@
     </row>
     <row r="30" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B30" t="s">
         <v>106</v>
@@ -5405,10 +5419,10 @@
         <v>32</v>
       </c>
       <c r="E30" t="s">
+        <v>698</v>
+      </c>
+      <c r="F30" t="s">
         <v>699</v>
-      </c>
-      <c r="F30" t="s">
-        <v>700</v>
       </c>
       <c r="G30">
         <v>87</v>
@@ -5429,7 +5443,7 @@
         <v>39</v>
       </c>
       <c r="N30" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="O30">
         <v>20</v>
@@ -5441,13 +5455,13 @@
         <v>64</v>
       </c>
       <c r="R30" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="S30" s="14" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="T30" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="U30" t="s">
         <v>207</v>
@@ -5458,7 +5472,7 @@
     </row>
     <row r="31" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B31" t="s">
         <v>107</v>
@@ -5518,7 +5532,7 @@
         <v>117</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>328</v>
@@ -5598,16 +5612,16 @@
         <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D5" t="s">
         <v>123</v>
       </c>
       <c r="E5" t="s">
+        <v>679</v>
+      </c>
+      <c r="F5" t="s">
         <v>680</v>
-      </c>
-      <c r="F5" t="s">
-        <v>681</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -5679,7 +5693,7 @@
         <v>127</v>
       </c>
       <c r="F8" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -6105,7 +6119,7 @@
         <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D27" t="s">
         <v>156</v>
@@ -6252,7 +6266,7 @@
         <v>193</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="F33" t="s">
         <v>155</v>
@@ -6537,16 +6551,16 @@
         <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D45" t="s">
         <v>307</v>
       </c>
       <c r="E45" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="F45" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G45">
         <v>5</v>
@@ -6690,7 +6704,7 @@
         <v>384</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="F51" t="s">
         <v>110</v>
@@ -7362,7 +7376,7 @@
         <v>657</v>
       </c>
       <c r="D79" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E79" t="s">
         <v>659</v>
@@ -7383,10 +7397,10 @@
         <v>109</v>
       </c>
       <c r="C80" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D80" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E80" t="s">
         <v>625</v>
@@ -7407,10 +7421,10 @@
         <v>158</v>
       </c>
       <c r="C81" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D81" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E81" t="s">
         <v>154</v>
@@ -7431,10 +7445,10 @@
         <v>114</v>
       </c>
       <c r="C82" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D82" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E82" t="s">
         <v>154</v>
@@ -7458,10 +7472,10 @@
         <v>109</v>
       </c>
       <c r="C83" t="s">
+        <v>703</v>
+      </c>
+      <c r="D83" t="s">
         <v>704</v>
-      </c>
-      <c r="D83" t="s">
-        <v>705</v>
       </c>
       <c r="E83" t="s">
         <v>625</v>
@@ -8063,7 +8077,7 @@
         <v>394</v>
       </c>
       <c r="F19" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G19" t="s">
         <v>399</v>
@@ -8341,7 +8355,7 @@
         <v>16</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C29" t="s">
         <v>304</v>
@@ -8353,13 +8367,13 @@
         <v>34</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="G29" t="s">
+        <v>672</v>
+      </c>
+      <c r="H29" t="s">
         <v>671</v>
-      </c>
-      <c r="G29" t="s">
-        <v>673</v>
-      </c>
-      <c r="H29" t="s">
-        <v>672</v>
       </c>
       <c r="I29">
         <v>10</v>
@@ -8370,10 +8384,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="C30" t="s">
         <v>714</v>
-      </c>
-      <c r="C30" t="s">
-        <v>715</v>
       </c>
       <c r="D30" t="s">
         <v>228</v>
@@ -8382,13 +8396,13 @@
         <v>101</v>
       </c>
       <c r="F30" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="G30" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="H30" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="I30">
         <v>25</v>
@@ -8407,10 +8421,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8637,10 +8651,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="C20" t="s">
         <v>678</v>
-      </c>
-      <c r="C20" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -8648,10 +8662,10 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
+        <v>674</v>
+      </c>
+      <c r="C21" t="s">
         <v>675</v>
-      </c>
-      <c r="C21" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -8659,10 +8673,10 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
+        <v>687</v>
+      </c>
+      <c r="C22" t="s">
         <v>688</v>
-      </c>
-      <c r="C22" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -8670,10 +8684,10 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -8681,7 +8695,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C24" t="s">
         <v>371</v>
@@ -8692,10 +8706,10 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
+        <v>695</v>
+      </c>
+      <c r="C25" t="s">
         <v>696</v>
-      </c>
-      <c r="C25" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -8703,15 +8717,38 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
+        <v>706</v>
+      </c>
+      <c r="C26" t="s">
         <v>707</v>
       </c>
-      <c r="C26" t="s">
-        <v>708</v>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>28</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="C27" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>722</v>
+      </c>
+      <c r="C28" t="s">
+        <v>723</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B20" r:id="rId1" xr:uid="{B8B4C84F-4B9B-4B98-AA47-BE6674672F64}"/>
+    <hyperlink ref="B27" r:id="rId2" location="overview" xr:uid="{AAF53F3C-824D-46A3-8C66-5CFC2A7E56BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9042,8 +9079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745174B4-A8CA-45B8-ACCB-9B5B609F0D5D}">
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="94" workbookViewId="0">
+      <selection activeCell="O80" sqref="O80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12638,33 +12675,161 @@
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A80" s="12">
+        <v>26</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C80" s="12">
+        <v>9</v>
+      </c>
+      <c r="D80" s="12">
+        <v>7</v>
+      </c>
+      <c r="E80" s="12">
+        <v>10</v>
+      </c>
+      <c r="F80" s="12">
+        <v>10</v>
+      </c>
+      <c r="G80" s="12">
+        <v>12</v>
+      </c>
+      <c r="H80" s="12">
+        <v>14</v>
+      </c>
+      <c r="I80" s="12">
+        <v>15</v>
+      </c>
+      <c r="J80" s="12">
+        <v>14</v>
+      </c>
+      <c r="K80" s="12">
+        <v>10</v>
+      </c>
+      <c r="L80" s="12">
+        <v>7</v>
+      </c>
+      <c r="M80" s="12">
+        <v>9</v>
+      </c>
+      <c r="N80" s="12">
+        <v>9</v>
+      </c>
       <c r="U80" s="7"/>
     </row>
-    <row r="81" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A81" s="11">
+        <v>26</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C81" s="26">
+        <v>-7</v>
+      </c>
+      <c r="D81" s="26">
+        <v>-4</v>
+      </c>
+      <c r="E81" s="26">
+        <v>2</v>
+      </c>
+      <c r="F81" s="26">
+        <v>5</v>
+      </c>
+      <c r="G81" s="26">
+        <v>10</v>
+      </c>
+      <c r="H81" s="26">
+        <v>14</v>
+      </c>
+      <c r="I81" s="26">
+        <v>16</v>
+      </c>
+      <c r="J81" s="26">
+        <v>15</v>
+      </c>
+      <c r="K81" s="26">
+        <v>10</v>
+      </c>
+      <c r="L81" s="26">
+        <v>4</v>
+      </c>
+      <c r="M81" s="26">
+        <v>-3</v>
+      </c>
+      <c r="N81" s="26">
+        <v>-7</v>
+      </c>
       <c r="U81" s="7"/>
     </row>
-    <row r="83" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A82" s="13">
+        <v>26</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C82" s="27">
+        <v>-18</v>
+      </c>
+      <c r="D82" s="27">
+        <v>-15</v>
+      </c>
+      <c r="E82" s="27">
+        <v>-11</v>
+      </c>
+      <c r="F82" s="27">
+        <v>-7</v>
+      </c>
+      <c r="G82" s="27">
+        <v>-3</v>
+      </c>
+      <c r="H82" s="27">
+        <v>0</v>
+      </c>
+      <c r="I82" s="27">
+        <v>2</v>
+      </c>
+      <c r="J82" s="27">
+        <v>2</v>
+      </c>
+      <c r="K82" s="27">
+        <v>-2</v>
+      </c>
+      <c r="L82" s="27">
+        <v>-7</v>
+      </c>
+      <c r="M82" s="27">
+        <v>-13</v>
+      </c>
+      <c r="N82" s="27">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U83" s="7"/>
     </row>
-    <row r="84" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U84" s="7"/>
     </row>
-    <row r="86" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U86" s="7"/>
     </row>
-    <row r="87" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U87" s="7"/>
     </row>
-    <row r="89" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U89" s="7"/>
     </row>
-    <row r="90" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U90" s="7"/>
     </row>
-    <row r="92" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U92" s="7"/>
     </row>
-    <row r="93" spans="21:21" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U93" s="7"/>
     </row>
   </sheetData>
@@ -12677,8 +12842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="87" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView topLeftCell="A8" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -12714,7 +12879,7 @@
         <v>325</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>326</v>
@@ -14057,7 +14222,7 @@
       </c>
       <c r="I27">
         <f>_xlfn.IFNA(IF(VLOOKUP(B27,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27">
         <f>_xlfn.IFNA(IF(VLOOKUP(B27,REFERANCES!A:A,1,FALSE),1,0),0)</f>

</xml_diff>

<commit_message>
node wrangler.... updating conversion file to work with latest version of excel reader. it now takes an object not integer
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD6D6D5-1B94-46FB-AD44-BC0F669D3FED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A0F34B-C8B0-49C4-B0AF-A29B936B61B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="724">
   <si>
     <t>cliff</t>
   </si>
@@ -2318,9 +2318,6 @@
     <t xml:space="preserve">The right hand route is in many ways the opposite twin to the left hand route (also a Hard Severe climb). It has better pitches at the top where the left-hand route has better pitches at the bottom. While the right hand route looks heavily vegetated from the bottom it’s surprisingly clean. That’s not to say its perfect, just better than it looks. It has good variety and is more sustained in grade when compared to the left-hand route, which has a hard start and then eases off. It’s a classic limestone route with a small crack section, and exposed thin ledge system and a steeper juggy section at the end. Check the BMC RAD Database for route exit information (see references), but at the time of writing abseiling off is required (see descent info). </t>
   </si>
   <si>
-    <t>Setdastal</t>
-  </si>
-  <si>
     <t>https://amzn.to/2XxjnCx</t>
   </si>
   <si>
@@ -2366,6 +2363,9 @@
   </si>
   <si>
     <t>Good Local trad climbing info for the area including this route</t>
+  </si>
+  <si>
+    <t>https://pixabay.com/photos/sass-pordoi-sella-massif-2738856/</t>
   </si>
 </sst>
 </file>
@@ -3512,9 +3512,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3616,7 +3616,7 @@
         <v>627</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -5399,7 +5399,7 @@
         <v>662</v>
       </c>
       <c r="S29" s="14" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="W29">
         <v>1</v>
@@ -5461,24 +5461,13 @@
         <v>705</v>
       </c>
       <c r="T30" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="U30" t="s">
         <v>207</v>
       </c>
       <c r="W30">
         <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>711</v>
-      </c>
-      <c r="B31" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31">
-        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -5497,8 +5486,8 @@
   <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5868,6 +5857,9 @@
       </c>
       <c r="D16" t="s">
         <v>138</v>
+      </c>
+      <c r="E16" t="s">
+        <v>723</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
@@ -8384,10 +8376,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="C30" t="s">
         <v>713</v>
-      </c>
-      <c r="C30" t="s">
-        <v>714</v>
       </c>
       <c r="D30" t="s">
         <v>228</v>
@@ -8396,13 +8388,13 @@
         <v>101</v>
       </c>
       <c r="F30" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="G30" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="H30" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="I30">
         <v>25</v>
@@ -8728,10 +8720,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C27" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -8739,10 +8731,10 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
+        <v>721</v>
+      </c>
+      <c r="C28" t="s">
         <v>722</v>
-      </c>
-      <c r="C28" t="s">
-        <v>723</v>
       </c>
     </row>
   </sheetData>
@@ -9079,7 +9071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745174B4-A8CA-45B8-ACCB-9B5B609F0D5D}">
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="94" workbookViewId="0">
+    <sheetView topLeftCell="A64" zoomScale="94" workbookViewId="0">
       <selection activeCell="O80" sqref="O80"/>
     </sheetView>
   </sheetViews>
@@ -12842,8 +12834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="87" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A12" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
added avon gorge climb
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82059617-5F6C-4F2E-A510-969BEF472597}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C9740B-AD94-4EA5-AEAE-83FDC9E20F1C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="745">
   <si>
     <t>cliff</t>
   </si>
@@ -2368,12 +2368,6 @@
     <t>Avon Gorge</t>
   </si>
   <si>
-    <t>Draft</t>
-  </si>
-  <si>
-    <t>Gronk</t>
-  </si>
-  <si>
     <t>https://www.ukclimbing.com/logbook/crag.php?id=300</t>
   </si>
   <si>
@@ -2396,6 +2390,58 @@
   </si>
   <si>
     <t>img/topos/stoer/old-man-of-stoer-climbing-topo.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morpheus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Approach&lt;/strong&gt;: The easiest option is to park in the Sea Walls free car park directly below the cliff (51.468013, -2.632912). There is space for a dozen cars but it can fill up quickly at weekends. It’s also possible to park above the cliff and climb the fence to gain the path down. &lt;br /&gt;
+&lt;strong&gt;Decent&lt;/strong&gt;: To descend you can follow the path back down (assuming you parked at the bottom) to the car. The path is obvious and leads to the main road just right of the Sea Walls climbing area in Bristol. 
+</t>
+  </si>
+  <si>
+    <t>51.468490,-2.633171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morpheus is an enjoyable and varied multi-pitch climb originally graded Hard Very Difficult. The climb starts at the same point as Gronk on the left-hand part of the Sea Walls main area in Avon Gorge. Because it’s partially quarried limestone, the route offers and mix of climbing styles including moves on large crimps, laybacks on a flake, some delicate sloping moves and no doubt at least one mantle onto one of the many ledges. Protection is good and requires mostly wires, but finger sized cams are also useful. Whilst the crux was originally the moves off the ground at the start, I’d suggest the corner crack on the 3rd pitch is now much harder. This is because the limited footholds have been polished to a glass like texture by the feet of many thousand climbers. The rest of the route is mostly not too polished. The Sea Walls are a real city crag and some of the most accessible multi-pitch rock climbing in the UK because you can park right at the cliff. However the disadvantage is the main road that runs below the crag is very noisy and can make verbal communication difficult on this climb. </t>
+  </si>
+  <si>
+    <t>img/topos/avon/morpheus-climb-on-the-sea-walls.jpg</t>
+  </si>
+  <si>
+    <t>Morpheus route on the Sea Walls in Avon</t>
+  </si>
+  <si>
+    <t>img/tiles/sea-walls-avon-gorge.jpg</t>
+  </si>
+  <si>
+    <t>The Sea Walls City Multi-pitch Climbing in Bristol</t>
+  </si>
+  <si>
+    <t>https://www.ukclimbing.com/logbook/c.php?i=29806</t>
+  </si>
+  <si>
+    <t>UKC Page for Morpheus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The climb Morpheus takes a diagonal but weaving line up some of the easiest rock on the Sea Walls.  It makes for a great introduction to multipitch climbing due to plentiful ledge systems and a reasonably amenable grade (Hard Very Difficult / Severe). It’s possible to link he first two pitches into one long pitch providing you manage rope drag by extending runners and have a good level of confidence on the rock.
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;28m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Climb the short wall to a ledge with some better gear options. The initial wall does have some good holds, but they are well disguised in the limestone. Once on the first ledge, carefully walk right to a blocky corner. Place gear and move up this a little before cutting back left to create a belay at the white stained block that allows good protection behind it. 
+&lt;br /&gt;&lt;strong class="pitch-title"&gt;Pitch 2 –&lt;span class="length"&gt;16m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;3c&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Climb the block either by layback or reaching up and over while moving the feet up. From above the block move slightly right to good holds and climb onto one smaller ledge before moving up to a large ledge with some broken blocks below a corners system with a crack running through it. A belay can be created in the crack below the corner. 
+&lt;br /&gt;&lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;10m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Originally not a graded pitch, years of climber’s feet have polished the stone here to make it arguably the hardest part of Morpheus whichever way you climb it. The original route suggests moving up the corner to the piton then moving out to the right before going up to the next belay. Whilst arguably still the easiest option, the move requires the climber to trust their feet on a highly polished hold where the foot slipping mid move could lead to an awkward fall. The alternative is to climb the corner directly. This means harder moves, especially for the shorter climber, however it feels much less exposed in the corner. Once this section is dealt with there are a couple of easy moves up onto a ledge with a stone seat and decent options for an anchor in the wall behind.
+&lt;br /&gt;&lt;strong class="pitch-title"&gt;Pitch 4 –&lt;span class="length"&gt;12m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;3b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+This pitch is much easier than it looks. Take good holds diagonally right, initially passing a under a small bush. A belay can be made at the end of the climbing. Alternatively, there is a good tree belay around the corner, however verbal communication with your partner here will be impossible. &lt;br /&gt;
+It’s a short scramble up the back wall and a walk off after the tree belay point. </t>
+  </si>
+  <si>
+    <t>img/topos/avon/maps/</t>
+  </si>
+  <si>
+    <t>Location of Sea Walls climbing in Avon Gorge</t>
   </si>
 </sst>
 </file>
@@ -3542,9 +3588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A8" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5511,7 +5557,7 @@
         <v>723</v>
       </c>
       <c r="B31" t="s">
-        <v>724</v>
+        <v>106</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -5520,33 +5566,57 @@
         <v>32</v>
       </c>
       <c r="E31" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F31" t="s">
-        <v>725</v>
+        <v>732</v>
       </c>
       <c r="G31">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="H31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I31">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J31" t="s">
-        <v>25</v>
+        <v>171</v>
       </c>
       <c r="K31" t="s">
-        <v>198</v>
+        <v>79</v>
       </c>
       <c r="M31" t="s">
         <v>39</v>
       </c>
+      <c r="N31" t="s">
+        <v>734</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>64</v>
+      </c>
+      <c r="R31" t="s">
+        <v>735</v>
+      </c>
+      <c r="S31" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="T31" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="U31" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="32" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B32" t="s">
         <v>107</v>
@@ -5574,8 +5644,8 @@
   <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86:F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5623,7 +5693,7 @@
         <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D2" t="s">
         <v>112</v>
@@ -7129,7 +7199,7 @@
         <v>625</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" ref="I65:I83" si="2">CONCATENATE(A65,B65)</f>
+        <f t="shared" ref="I65:I86" si="2">CONCATENATE(A65,B65)</f>
         <v>22map</v>
       </c>
     </row>
@@ -7569,6 +7639,81 @@
       <c r="I83" t="str">
         <f t="shared" si="2"/>
         <v>29map</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <v>30</v>
+      </c>
+      <c r="B84" t="s">
+        <v>113</v>
+      </c>
+      <c r="C84" t="s">
+        <v>736</v>
+      </c>
+      <c r="D84" t="s">
+        <v>737</v>
+      </c>
+      <c r="E84" t="s">
+        <v>153</v>
+      </c>
+      <c r="F84" t="s">
+        <v>154</v>
+      </c>
+      <c r="G84">
+        <v>5</v>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="2"/>
+        <v>30topo</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <v>30</v>
+      </c>
+      <c r="B85" t="s">
+        <v>157</v>
+      </c>
+      <c r="C85" t="s">
+        <v>738</v>
+      </c>
+      <c r="D85" t="s">
+        <v>739</v>
+      </c>
+      <c r="E85" t="s">
+        <v>153</v>
+      </c>
+      <c r="F85" t="s">
+        <v>154</v>
+      </c>
+      <c r="I85" t="str">
+        <f t="shared" si="2"/>
+        <v>30tile</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>30</v>
+      </c>
+      <c r="B86" t="s">
+        <v>109</v>
+      </c>
+      <c r="C86" t="s">
+        <v>743</v>
+      </c>
+      <c r="D86" t="s">
+        <v>744</v>
+      </c>
+      <c r="E86" t="s">
+        <v>624</v>
+      </c>
+      <c r="F86" t="s">
+        <v>625</v>
+      </c>
+      <c r="I86" t="str">
+        <f t="shared" si="2"/>
+        <v>30map</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
@@ -8504,10 +8649,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8698,7 +8843,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
         <v>649</v>
@@ -8833,7 +8978,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C29" t="s">
         <v>717</v>
@@ -8844,10 +8989,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C30" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
@@ -8855,10 +9000,21 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C31" t="s">
-        <v>730</v>
+        <v>728</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>740</v>
+      </c>
+      <c r="C32" t="s">
+        <v>741</v>
       </c>
     </row>
   </sheetData>
@@ -9197,7 +9353,7 @@
   <dimension ref="A1:V93"/>
   <sheetViews>
     <sheetView topLeftCell="A64" zoomScale="94" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+      <selection activeCell="N78" sqref="N78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12926,10 +13082,138 @@
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A83" s="12">
+        <v>30</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="C83" s="12">
+        <v>13</v>
+      </c>
+      <c r="D83" s="12">
+        <v>9</v>
+      </c>
+      <c r="E83" s="12">
+        <v>11</v>
+      </c>
+      <c r="F83" s="12">
+        <v>9</v>
+      </c>
+      <c r="G83" s="12">
+        <v>8</v>
+      </c>
+      <c r="H83" s="12">
+        <v>8</v>
+      </c>
+      <c r="I83" s="12">
+        <v>7</v>
+      </c>
+      <c r="J83" s="12">
+        <v>8</v>
+      </c>
+      <c r="K83" s="12">
+        <v>9</v>
+      </c>
+      <c r="L83" s="12">
+        <v>11</v>
+      </c>
+      <c r="M83" s="12">
+        <v>10</v>
+      </c>
+      <c r="N83" s="12">
+        <v>11</v>
+      </c>
       <c r="U83" s="7"/>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A84" s="11">
+        <v>30</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="C84" s="26">
+        <v>8</v>
+      </c>
+      <c r="D84" s="26">
+        <v>8</v>
+      </c>
+      <c r="E84" s="26">
+        <v>11</v>
+      </c>
+      <c r="F84" s="26">
+        <v>13</v>
+      </c>
+      <c r="G84" s="26">
+        <v>17</v>
+      </c>
+      <c r="H84" s="26">
+        <v>19</v>
+      </c>
+      <c r="I84" s="26">
+        <v>22</v>
+      </c>
+      <c r="J84" s="26">
+        <v>21</v>
+      </c>
+      <c r="K84" s="26">
+        <v>18</v>
+      </c>
+      <c r="L84" s="26">
+        <v>15</v>
+      </c>
+      <c r="M84" s="26">
+        <v>11</v>
+      </c>
+      <c r="N84" s="26">
+        <v>9</v>
+      </c>
       <c r="U84" s="7"/>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A85" s="13">
+        <v>30</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C85" s="27">
+        <v>3</v>
+      </c>
+      <c r="D85" s="27">
+        <v>3</v>
+      </c>
+      <c r="E85" s="27">
+        <v>5</v>
+      </c>
+      <c r="F85" s="27">
+        <v>6</v>
+      </c>
+      <c r="G85" s="27">
+        <v>9</v>
+      </c>
+      <c r="H85" s="27">
+        <v>12</v>
+      </c>
+      <c r="I85" s="27">
+        <v>14</v>
+      </c>
+      <c r="J85" s="27">
+        <v>14</v>
+      </c>
+      <c r="K85" s="27">
+        <v>12</v>
+      </c>
+      <c r="L85" s="27">
+        <v>9</v>
+      </c>
+      <c r="M85" s="27">
+        <v>6</v>
+      </c>
+      <c r="N85" s="27">
+        <v>4</v>
+      </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.45">
       <c r="U86" s="7"/>
@@ -12957,10 +13241,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A8" zoomScale="87" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -14507,8 +14791,110 @@
         <v>DONE</v>
       </c>
     </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A31" t="str">
+        <f>CLIMBS!A31</f>
+        <v>Avon Gorge</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="str">
+        <f>CLIMBS!B31</f>
+        <v>publish</v>
+      </c>
+      <c r="D31">
+        <f>IF(CLIMBS!R31&lt;&gt;0,1,0)+IF(CLIMBS!G31&lt;&gt;0,1,0)+IF(CLIMBS!H31&lt;&gt;0,1,0)+IF(CLIMBS!I31&lt;&gt;0,1,0)+IF(CLIMBS!J31&lt;&gt;0,1,0)+IF(CLIMBS!N31&lt;&gt;0,1,0)+IF(CLIMBS!M31&lt;&gt;0,1,0)+IF(CLIMBS!O31&lt;&gt;0,1,0)+IF(CLIMBS!P31&lt;&gt;0,1,0)</f>
+        <v>9</v>
+      </c>
+      <c r="E31">
+        <f>IF(CLIMBS!S31&lt;&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B31,"tile"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B31,"topo"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B31,"map"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <f>SUMIFS(IMAGES!G:G,IMAGES!A:A,'to-do-score-card'!B31,IMAGES!B:B,"topo")</f>
+        <v>5</v>
+      </c>
+      <c r="H31">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B31,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B31,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B31,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <f>IF(VLOOKUP(B31,CLIMBS!C:T,18,FALSE)&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L31" s="25" t="str">
+        <f t="shared" ref="L31:L32" si="1">IF(SUM(D31:K31)=22,"DONE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A32" t="str">
+        <f>CLIMBS!A32</f>
+        <v>Setdastal</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="str">
+        <f>CLIMBS!B32</f>
+        <v>draft</v>
+      </c>
+      <c r="D32">
+        <f>IF(CLIMBS!R32&lt;&gt;0,1,0)+IF(CLIMBS!G32&lt;&gt;0,1,0)+IF(CLIMBS!H32&lt;&gt;0,1,0)+IF(CLIMBS!I32&lt;&gt;0,1,0)+IF(CLIMBS!J32&lt;&gt;0,1,0)+IF(CLIMBS!N32&lt;&gt;0,1,0)+IF(CLIMBS!M32&lt;&gt;0,1,0)+IF(CLIMBS!O32&lt;&gt;0,1,0)+IF(CLIMBS!P32&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f>IF(CLIMBS!S32&lt;&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F32" t="str">
+        <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B32,"tile"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B32,"topo"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B32,"map"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
+        <v>missing</v>
+      </c>
+      <c r="G32">
+        <f>SUMIFS(IMAGES!G:G,IMAGES!A:A,'to-do-score-card'!B32,IMAGES!B:B,"topo")</f>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B32,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B32,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B32,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <f>IF(VLOOKUP(B32,CLIMBS!C:T,18,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="25" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="cellIs" dxfId="16" priority="16" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
@@ -14516,7 +14902,7 @@
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C30">
+  <conditionalFormatting sqref="C2:C32">
     <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"draft"</formula>
     </cfRule>
@@ -14526,12 +14912,12 @@
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C30">
+  <conditionalFormatting sqref="C3:C32">
     <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E30">
+  <conditionalFormatting sqref="E2:E32">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -14539,7 +14925,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:G30">
+  <conditionalFormatting sqref="F2:G32">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
@@ -14547,7 +14933,7 @@
       <formula>"missing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:J30">
+  <conditionalFormatting sqref="H2:J32">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -14555,7 +14941,7 @@
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K30">
+  <conditionalFormatting sqref="K2:K32">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -14563,7 +14949,7 @@
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G32">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>1</formula>
       <formula>4</formula>
@@ -14575,7 +14961,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F30">
+  <conditionalFormatting sqref="F2:F32">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>3</formula>
     </cfRule>

</xml_diff>

<commit_message>
added fix for avon
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C9740B-AD94-4EA5-AEAE-83FDC9E20F1C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B238D4-B847-43FA-BC1F-0023C532950E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -2365,9 +2365,6 @@
     <t>https://pixabay.com/photos/sass-pordoi-sella-massif-2738856/</t>
   </si>
   <si>
-    <t>Avon Gorge</t>
-  </si>
-  <si>
     <t>https://www.ukclimbing.com/logbook/crag.php?id=300</t>
   </si>
   <si>
@@ -2395,40 +2392,46 @@
     <t xml:space="preserve">Morpheus </t>
   </si>
   <si>
+    <t>51.468490,-2.633171</t>
+  </si>
+  <si>
+    <t>img/topos/avon/morpheus-climb-on-the-sea-walls.jpg</t>
+  </si>
+  <si>
+    <t>Morpheus route on the Sea Walls in Avon</t>
+  </si>
+  <si>
+    <t>img/tiles/sea-walls-avon-gorge.jpg</t>
+  </si>
+  <si>
+    <t>The Sea Walls City Multi-pitch Climbing in Bristol</t>
+  </si>
+  <si>
+    <t>https://www.ukclimbing.com/logbook/c.php?i=29806</t>
+  </si>
+  <si>
+    <t>UKC Page for Morpheus</t>
+  </si>
+  <si>
+    <t>img/topos/avon/maps/</t>
+  </si>
+  <si>
+    <t>Location of Sea Walls climbing in Avon Gorge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morpheus is an enjoyable and varied multi-pitch climb originally graded Hard Very Difficult. The climb starts at the same point as Gronk on the left-hand part of the Sea Walls main area in Avon Gorge. Because it’s partially quarried limestone, the route offers and mix of climbing styles including moves on large crimps, laybacks on a flake, some delicate sloping moves and no doubt at least one mantle onto one of the many ledges. Protection is good and requires mostly wires, but some cams are also useful. Whilst the crux was originally the moves off the ground at the start, recent ecperiance suggest the corner crack on the 3rd pitch is now much harder. This is because the limited footholds have been polished to a glass like texture by the feet of many thousand climbers. The rest of the route is mostly not too polished. The Sea Walls at Avon Gorge are a real city crag and some of the most accessible multi-pitch rock climbing in the UK because you can park right at the cliff. However the disadvantage is the main road that runs below the crag is very noisy and can make verbal communication difficult on this climb. </t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;strong&gt;Approach&lt;/strong&gt;: The easiest option is to park in the Sea Walls free car park directly below the cliff (51.468013, -2.632912). There is space for a dozen cars but it can fill up quickly at weekends. It’s also possible to park above the cliff and climb the fence to gain the path down. &lt;br /&gt;
-&lt;strong&gt;Decent&lt;/strong&gt;: To descend you can follow the path back down (assuming you parked at the bottom) to the car. The path is obvious and leads to the main road just right of the Sea Walls climbing area in Bristol. 
+&lt;strong&gt;Decent&lt;/strong&gt;: To descend you can follow the path back down (assuming you parked at the bottom) to the car. The path is obvious and leads to the main road just right of the Sea Walls climbing area in Avon Gorge, Bristol. 
 </t>
   </si>
   <si>
-    <t>51.468490,-2.633171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morpheus is an enjoyable and varied multi-pitch climb originally graded Hard Very Difficult. The climb starts at the same point as Gronk on the left-hand part of the Sea Walls main area in Avon Gorge. Because it’s partially quarried limestone, the route offers and mix of climbing styles including moves on large crimps, laybacks on a flake, some delicate sloping moves and no doubt at least one mantle onto one of the many ledges. Protection is good and requires mostly wires, but finger sized cams are also useful. Whilst the crux was originally the moves off the ground at the start, I’d suggest the corner crack on the 3rd pitch is now much harder. This is because the limited footholds have been polished to a glass like texture by the feet of many thousand climbers. The rest of the route is mostly not too polished. The Sea Walls are a real city crag and some of the most accessible multi-pitch rock climbing in the UK because you can park right at the cliff. However the disadvantage is the main road that runs below the crag is very noisy and can make verbal communication difficult on this climb. </t>
-  </si>
-  <si>
-    <t>img/topos/avon/morpheus-climb-on-the-sea-walls.jpg</t>
-  </si>
-  <si>
-    <t>Morpheus route on the Sea Walls in Avon</t>
-  </si>
-  <si>
-    <t>img/tiles/sea-walls-avon-gorge.jpg</t>
-  </si>
-  <si>
-    <t>The Sea Walls City Multi-pitch Climbing in Bristol</t>
-  </si>
-  <si>
-    <t>https://www.ukclimbing.com/logbook/c.php?i=29806</t>
-  </si>
-  <si>
-    <t>UKC Page for Morpheus</t>
-  </si>
-  <si>
     <t xml:space="preserve">
-The climb Morpheus takes a diagonal but weaving line up some of the easiest rock on the Sea Walls.  It makes for a great introduction to multipitch climbing due to plentiful ledge systems and a reasonably amenable grade (Hard Very Difficult / Severe). It’s possible to link he first two pitches into one long pitch providing you manage rope drag by extending runners and have a good level of confidence on the rock.
+The climb Morpheus takes a diagonal but weaving line up some of the easiest rock on the Sea Walls.  It makes for a great introduction to multipitch climbing due to plentiful ledge systems and a reasonably amenable grade (Hard Very Difficult / Severe). It’s possible to link the first two pitches into one long pitch providing you manage rope drag by extending runners and have a good level of confidence on the rock.
 &lt;br /&gt;
 &lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;28m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
-Climb the short wall to a ledge with some better gear options. The initial wall does have some good holds, but they are well disguised in the limestone. Once on the first ledge, carefully walk right to a blocky corner. Place gear and move up this a little before cutting back left to create a belay at the white stained block that allows good protection behind it. 
+Climb the short wall to a ledge with some better gear options. The initial wall does have some good holds, but they are well disguised in the limestone. Once on the first ledge, carefully walk right to a blocky corner. Place gear and move up this a little, before cutting back left. The next belay is a crack on the left side of the white stained block. It allows good protection behind it. 
 &lt;br /&gt;&lt;strong class="pitch-title"&gt;Pitch 2 –&lt;span class="length"&gt;16m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;3c&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
 Climb the block either by layback or reaching up and over while moving the feet up. From above the block move slightly right to good holds and climb onto one smaller ledge before moving up to a large ledge with some broken blocks below a corners system with a crack running through it. A belay can be created in the crack below the corner. 
 &lt;br /&gt;&lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;10m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
@@ -2438,10 +2441,7 @@
 It’s a short scramble up the back wall and a walk off after the tree belay point. </t>
   </si>
   <si>
-    <t>img/topos/avon/maps/</t>
-  </si>
-  <si>
-    <t>Location of Sea Walls climbing in Avon Gorge</t>
+    <t>Avon Gorge</t>
   </si>
 </sst>
 </file>
@@ -3588,9 +3588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T31" sqref="T31"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5554,7 +5554,7 @@
     </row>
     <row r="31" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>723</v>
+        <v>744</v>
       </c>
       <c r="B31" t="s">
         <v>106</v>
@@ -5566,10 +5566,10 @@
         <v>32</v>
       </c>
       <c r="E31" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="F31" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G31">
         <v>67</v>
@@ -5590,7 +5590,7 @@
         <v>39</v>
       </c>
       <c r="N31" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="O31">
         <v>1</v>
@@ -5602,13 +5602,13 @@
         <v>64</v>
       </c>
       <c r="R31" t="s">
-        <v>735</v>
+        <v>741</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>733</v>
+        <v>742</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="U31" t="s">
         <v>170</v>
@@ -5616,7 +5616,7 @@
     </row>
     <row r="32" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B32" t="s">
         <v>107</v>
@@ -5643,7 +5643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E86" sqref="E86:F86"/>
     </sheetView>
@@ -5693,7 +5693,7 @@
         <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D2" t="s">
         <v>112</v>
@@ -7649,10 +7649,10 @@
         <v>113</v>
       </c>
       <c r="C84" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="D84" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="E84" t="s">
         <v>153</v>
@@ -7676,10 +7676,10 @@
         <v>157</v>
       </c>
       <c r="C85" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="D85" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="E85" t="s">
         <v>153</v>
@@ -7700,10 +7700,10 @@
         <v>109</v>
       </c>
       <c r="C86" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D86" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="E86" t="s">
         <v>624</v>
@@ -7763,7 +7763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="116" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -8978,7 +8978,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C29" t="s">
         <v>717</v>
@@ -8989,10 +8989,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="10" t="s">
+        <v>724</v>
+      </c>
+      <c r="C30" t="s">
         <v>725</v>
-      </c>
-      <c r="C30" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
@@ -9000,10 +9000,10 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>726</v>
+      </c>
+      <c r="C31" t="s">
         <v>727</v>
-      </c>
-      <c r="C31" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
@@ -9011,10 +9011,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="C32" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed map by removing async and fixed spelling on about
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B238D4-B847-43FA-BC1F-0023C532950E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF810A39-6BFC-4BEF-9AC1-AC0A7D4D97EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3588,9 +3588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R31" sqref="R31"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3824,6 +3824,12 @@
       <c r="V3" t="s">
         <v>45</v>
       </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -4584,6 +4590,12 @@
       </c>
       <c r="V15" t="s">
         <v>214</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
added some guidebook info
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16430EF2-AD02-4048-ABBC-9807FDB8543E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9104AAFF-6045-48D9-8070-84978CF389D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="793">
   <si>
     <t>cliff</t>
   </si>
@@ -2615,6 +2615,21 @@
   </si>
   <si>
     <t>https://climbing-bulgaria.com/2017/09/13/vratsa-region/</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2ZiZPHr</t>
+  </si>
+  <si>
+    <t>9781852841553</t>
+  </si>
+  <si>
+    <t>Selected Rock Climbs in Belgium and Luxembourg</t>
+  </si>
+  <si>
+    <t>img/guidebooks/selected-rock-climbs-in-belgium-and-luxembourg.jpg</t>
+  </si>
+  <si>
+    <t>Published in 1995 this climbing guidebook is best described as classic. It covers a number of climbs at Freyr including Le Merinos and La Savonnette. It’s written in English and is one of the early guidebooks from Chris Crags probably better known for his more recent work with Rockfax. The guide has decent route descriptions and uses British grades. There are pictures for some climbs but not these one on the Merinos face. Whilst it can be picked up cheaply there are newer guides to the area, although most are sadly not in English.</t>
   </si>
 </sst>
 </file>
@@ -6785,7 +6800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E90" sqref="E90"/>
     </sheetView>
@@ -9034,10 +9049,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9949,6 +9964,38 @@
       <c r="I31">
         <v>24.99</v>
       </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A32" s="3">
+        <v>32</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="C32" t="s">
+        <v>790</v>
+      </c>
+      <c r="D32" t="s">
+        <v>222</v>
+      </c>
+      <c r="E32">
+        <v>20</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="G32" t="s">
+        <v>791</v>
+      </c>
+      <c r="H32" t="s">
+        <v>788</v>
+      </c>
+      <c r="I32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -16475,7 +16522,7 @@
       </c>
       <c r="H33">
         <f>_xlfn.IFNA(IF(VLOOKUP(B33,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
         <f>_xlfn.IFNA(IF(VLOOKUP(B33,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>

</xml_diff>

<commit_message>
color coded map pins. Also minor bug fixes
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1684D5-E250-4520-A286-4C75F552332C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552F4200-C73C-48F8-BED5-6398E97558C9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,6 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">IMAGES!$A$1:$I$116</definedName>
   </definedNames>
   <calcPr calcId="181029" iterateDelta="0" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2633,7 +2634,31 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Corse Granite with a series of cracks and ledges make this an interesting but sustained climb with a number of British 4b graded moves. The route is reasonably easy to protect with the exception of the grass ledge at the end of pitch one. Cams, ti-cams as well as offset nuts seemed to work very well. The last short pitch is able to consume a significant number of 1-3 finger width cams.
+    <t>img/topos/mournes/poetic-justice-climb-on-slieve-beg-in-the-mournes.jpg</t>
+  </si>
+  <si>
+    <t>img/tiles/slieve-beg-crag-in-the-mourne-mountains.jpg</t>
+  </si>
+  <si>
+    <t>grassLegdes</t>
+  </si>
+  <si>
+    <t>boat</t>
+  </si>
+  <si>
+    <t>approachDifficulty</t>
+  </si>
+  <si>
+    <t>approachTime</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>polished</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corse Granite with a series of cracks and ledges make this an interesting but sustained climb with a number of British 4b graded moves. The route is reasonably easy to protect with the exception of the grass ledge at the end of pitch one. Cams, tri-cams as well as offset nuts seemed to work very well. The last short pitch is able to consume a significant number of 1-3 finger width cams.
 &lt;br/&gt;
 &lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;45m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br&gt;
 Starting 3m left of the right hand edge of the main face, climb up and left moving towards a corner with good holds. Climb up over the corner and onto the thin slab with a significant crack running up the middle. Keep climbing more or less straight up, and at one point around the halfway mark you veer a little right to a good ledge that’s very exposed. The route then continues up and over the broken ledge covered in grass, bilberry bushes and heather. This section is both hard to climb and hard to protect. It’s possible to use an ice axe to help climb the turf, however the small benefit and safety gained by taking an ice axe is outweighed but the inconvenience of carrying it on the following pitches. After the ledge, you can make a move up onto a ledge in the corner to build an anchor. This will be at more or less a full 50m rope length. The rope drag can be significant over the grass which is exactly where you don’t want it. Therefore, it’s recommended to break up pitch one at one of the reasonable ledges in the middle of the first pitch. 
@@ -2644,30 +2669,6 @@
 &lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;12m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br&gt;
 A short steep pitch that requires a mix of bridging and laybacks on what are, for the most part very good holds, all the way up to the summit. An anchor can be built from the rocks just back from the crag edge. 
 </t>
-  </si>
-  <si>
-    <t>img/topos/mournes/poetic-justice-climb-on-slieve-beg-in-the-mournes.jpg</t>
-  </si>
-  <si>
-    <t>img/tiles/slieve-beg-crag-in-the-mourne-mountains.jpg</t>
-  </si>
-  <si>
-    <t>grassLegdes</t>
-  </si>
-  <si>
-    <t>boat</t>
-  </si>
-  <si>
-    <t>approachDifficulty</t>
-  </si>
-  <si>
-    <t>approachTime</t>
-  </si>
-  <si>
-    <t>Approach</t>
-  </si>
-  <si>
-    <t>polished</t>
   </si>
 </sst>
 </file>
@@ -2860,7 +2861,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3070,6 +3071,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -3232,7 +3239,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3299,6 +3306,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4683,9 +4707,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4756,10 +4780,10 @@
         <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>13</v>
@@ -4786,13 +4810,13 @@
         <v>603</v>
       </c>
       <c r="Y1" s="29" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="Z1" s="29" t="s">
         <v>609</v>
       </c>
       <c r="AA1" s="29" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="AB1" s="29" t="s">
         <v>740</v>
@@ -4801,7 +4825,7 @@
         <v>698</v>
       </c>
       <c r="AD1" s="29" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>738</v>
@@ -4878,73 +4902,80 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="32">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="32">
         <v>67</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="32">
         <v>3</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="32">
         <v>4</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="32">
         <v>10</v>
       </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="P3" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="32" t="s">
         <v>729</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="32" t="s">
         <v>728</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="33" t="s">
         <v>727</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V3" s="30" t="s">
+      <c r="V3" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="AC3" s="30">
-        <v>1</v>
-      </c>
+      <c r="W3" s="34"/>
+      <c r="X3" s="34"/>
+      <c r="Y3" s="34"/>
+      <c r="Z3" s="34"/>
+      <c r="AA3" s="34"/>
+      <c r="AB3" s="34"/>
+      <c r="AC3" s="34">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="34"/>
     </row>
     <row r="4" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -5011,70 +5042,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="5" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="32">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="32">
         <v>400</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="32">
         <v>11</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="32">
         <v>7</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="32">
         <v>40</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="32">
         <v>2</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="32" t="s">
         <v>775</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="S5" s="35" t="s">
         <v>776</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V5" s="30" t="s">
+      <c r="V5" s="34" t="s">
         <v>165</v>
       </c>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="34"/>
+      <c r="AD5" s="34"/>
     </row>
     <row r="6" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -5150,67 +5189,76 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="7" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="32">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="32">
         <v>555</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="32">
         <v>16</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="32">
         <v>4</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="32">
         <v>45</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="32">
         <v>2</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" s="32" t="s">
         <v>40</v>
       </c>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34"/>
+      <c r="X7" s="34"/>
+      <c r="Y7" s="34"/>
+      <c r="Z7" s="34"/>
+      <c r="AA7" s="34"/>
+      <c r="AB7" s="34"/>
+      <c r="AC7" s="34"/>
+      <c r="AD7" s="34"/>
     </row>
     <row r="8" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -5271,70 +5319,77 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="32">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="32">
         <v>117</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="32">
         <v>5</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="32">
         <v>4</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="32">
         <v>120</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="32">
         <v>3</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="32" t="s">
         <v>357</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="32" t="s">
         <v>358</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U9" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="V9" s="30" t="s">
+      <c r="V9" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="W9" s="30">
-        <v>1</v>
-      </c>
+      <c r="W9" s="34">
+        <v>1</v>
+      </c>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="34"/>
+      <c r="AA9" s="34"/>
+      <c r="AB9" s="34"/>
+      <c r="AC9" s="34"/>
+      <c r="AD9" s="34"/>
     </row>
     <row r="10" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -5399,73 +5454,80 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="32">
         <v>10</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="32">
         <v>130</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="32">
         <v>3</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="32">
         <v>5</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="32">
         <v>50</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="32">
         <v>2</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S11" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="32" t="s">
         <v>617</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U11" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="Z11" s="30">
-        <v>1</v>
-      </c>
-      <c r="AB11" s="30">
-        <v>1</v>
-      </c>
+      <c r="V11" s="34"/>
+      <c r="W11" s="34"/>
+      <c r="X11" s="34"/>
+      <c r="Y11" s="34"/>
+      <c r="Z11" s="34">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="34"/>
+      <c r="AB11" s="34">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="34"/>
+      <c r="AD11" s="34"/>
     </row>
     <row r="12" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -5529,79 +5591,84 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="13" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="32">
         <v>12</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="32">
         <v>190</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="32">
         <v>6</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="32">
         <v>5</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="32">
         <v>35</v>
       </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="Q13" t="s">
+      <c r="P13" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="R13" s="2" t="s">
+      <c r="R13" s="35" t="s">
         <v>650</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="S13" s="35" t="s">
         <v>615</v>
       </c>
-      <c r="T13" s="14" t="s">
+      <c r="T13" s="36" t="s">
         <v>673</v>
       </c>
-      <c r="V13" s="30" t="s">
+      <c r="V13" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="W13" s="30">
-        <v>1</v>
-      </c>
-      <c r="X13" s="30">
-        <v>1</v>
-      </c>
-      <c r="AB13" s="30">
-        <v>1</v>
-      </c>
+      <c r="W13" s="34">
+        <v>1</v>
+      </c>
+      <c r="X13" s="34">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="34"/>
+      <c r="Z13" s="34"/>
+      <c r="AA13" s="34"/>
+      <c r="AB13" s="34">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="34"/>
+      <c r="AD13" s="34"/>
     </row>
     <row r="14" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
@@ -5665,73 +5732,80 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="15" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="32">
         <v>14</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="32">
         <v>70</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="32">
         <v>3</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="32">
         <v>4</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="32">
         <v>25</v>
       </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15" t="s">
+      <c r="P15" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="R15" s="2" t="s">
+      <c r="R15" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="S15" s="2" t="s">
+      <c r="S15" s="35" t="s">
         <v>736</v>
       </c>
-      <c r="T15" s="14" t="s">
+      <c r="T15" s="36" t="s">
         <v>737</v>
       </c>
-      <c r="U15" t="s">
+      <c r="U15" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="V15" s="30" t="s">
+      <c r="V15" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="Z15" s="30">
-        <v>1</v>
-      </c>
+      <c r="W15" s="34"/>
+      <c r="X15" s="34"/>
+      <c r="Y15" s="34"/>
+      <c r="Z15" s="34">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="34"/>
+      <c r="AB15" s="34"/>
+      <c r="AC15" s="34"/>
+      <c r="AD15" s="34"/>
     </row>
     <row r="16" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -5801,73 +5875,80 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="17" spans="1:31" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="32">
         <v>16</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="32" t="s">
         <v>300</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="32">
         <v>280</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="32">
         <v>12</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="32">
         <v>3</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="32">
         <v>70</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="32">
         <v>2</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="R17" s="2" t="s">
+      <c r="R17" s="35" t="s">
         <v>309</v>
       </c>
-      <c r="S17" s="14" t="s">
+      <c r="S17" s="36" t="s">
         <v>674</v>
       </c>
-      <c r="T17" s="14" t="s">
+      <c r="T17" s="36" t="s">
         <v>675</v>
       </c>
-      <c r="U17" t="s">
+      <c r="U17" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="V17" s="30" t="s">
+      <c r="V17" s="34" t="s">
         <v>264</v>
       </c>
-      <c r="AC17" s="30">
-        <v>1</v>
-      </c>
+      <c r="W17" s="34"/>
+      <c r="X17" s="34"/>
+      <c r="Y17" s="34"/>
+      <c r="Z17" s="34"/>
+      <c r="AA17" s="34"/>
+      <c r="AB17" s="34"/>
+      <c r="AC17" s="34">
+        <v>1</v>
+      </c>
+      <c r="AD17" s="34"/>
     </row>
     <row r="18" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
@@ -5934,65 +6015,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="19" spans="1:31" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="32" t="s">
         <v>366</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="32">
         <v>18</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="32" t="s">
         <v>367</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="32">
         <v>74</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="32">
         <v>3</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="32">
         <v>2</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="32" t="s">
         <v>370</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="32" t="s">
         <v>417</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="32" t="s">
         <v>369</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="32">
         <v>70</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="32">
         <v>2</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="Q19" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="R19" s="2" t="s">
+      <c r="R19" s="35" t="s">
         <v>377</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="S19" s="35" t="s">
         <v>371</v>
       </c>
-      <c r="T19" s="2"/>
-      <c r="AC19" s="30">
-        <v>1</v>
-      </c>
+      <c r="T19" s="35"/>
+      <c r="V19" s="34"/>
+      <c r="W19" s="34"/>
+      <c r="X19" s="34"/>
+      <c r="Y19" s="34"/>
+      <c r="Z19" s="34"/>
+      <c r="AA19" s="34"/>
+      <c r="AB19" s="34"/>
+      <c r="AC19" s="34">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="34"/>
     </row>
     <row r="20" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
@@ -6057,73 +6146,80 @@
       </c>
       <c r="AE20" s="31"/>
     </row>
-    <row r="21" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="21" spans="1:31" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="32" t="s">
         <v>399</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="32">
         <v>20</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="32" t="s">
         <v>400</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="32" t="s">
         <v>398</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="32">
         <v>80</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="32">
         <v>4</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="32">
         <v>5</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="32" t="s">
         <v>401</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="32">
         <v>90</v>
       </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
-      <c r="Q21" t="s">
+      <c r="P21" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="R21" s="2" t="s">
+      <c r="R21" s="35" t="s">
         <v>783</v>
       </c>
-      <c r="S21" s="3" t="s">
+      <c r="S21" s="33" t="s">
         <v>784</v>
       </c>
-      <c r="T21" s="3" t="s">
-        <v>785</v>
-      </c>
-      <c r="V21" s="30" t="s">
+      <c r="T21" s="33" t="s">
+        <v>793</v>
+      </c>
+      <c r="V21" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="AC21" s="30">
-        <v>1</v>
-      </c>
-      <c r="AE21" s="31">
+      <c r="W21" s="34"/>
+      <c r="X21" s="34"/>
+      <c r="Y21" s="34"/>
+      <c r="Z21" s="34"/>
+      <c r="AA21" s="34"/>
+      <c r="AB21" s="34"/>
+      <c r="AC21" s="34">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="34"/>
+      <c r="AE21" s="37">
         <f ca="1">NOW()</f>
-        <v>43720.403596064818</v>
+        <v>43721.638431712963</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -6188,70 +6284,77 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="23" spans="1:31" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="32" t="s">
         <v>429</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="32">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="32" t="s">
         <v>432</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="32" t="s">
         <v>468</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="32">
         <v>228</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="32">
         <v>9</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="32">
         <v>6</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="32" t="s">
         <v>473</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="32">
         <v>20</v>
       </c>
-      <c r="P23">
-        <v>1</v>
-      </c>
-      <c r="Q23" t="s">
+      <c r="P23" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R23" s="32" t="s">
         <v>472</v>
       </c>
-      <c r="S23" t="s">
+      <c r="S23" s="32" t="s">
         <v>474</v>
       </c>
-      <c r="U23" t="s">
+      <c r="U23" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="V23" s="30" t="s">
+      <c r="V23" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="W23" s="30">
-        <v>1</v>
-      </c>
+      <c r="W23" s="34">
+        <v>1</v>
+      </c>
+      <c r="X23" s="34"/>
+      <c r="Y23" s="34"/>
+      <c r="Z23" s="34"/>
+      <c r="AA23" s="34"/>
+      <c r="AB23" s="34"/>
+      <c r="AC23" s="34"/>
+      <c r="AD23" s="34"/>
     </row>
     <row r="24" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
@@ -6279,7 +6382,7 @@
         <v>9</v>
       </c>
       <c r="I24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
@@ -6321,74 +6424,81 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="25" spans="1:31" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="32" t="s">
         <v>505</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="32">
         <v>24</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="32" t="s">
         <v>504</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="32" t="s">
         <v>506</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="32" t="s">
         <v>509</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="32">
         <v>350</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="32">
         <v>13</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="32">
         <v>7</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="32" t="s">
         <v>507</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="32" t="s">
         <v>508</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" s="32" t="s">
         <v>510</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="32">
         <v>190</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="32">
         <v>2</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="Q25" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="R25" t="s">
+      <c r="R25" s="32" t="s">
         <v>517</v>
       </c>
-      <c r="S25" s="2" t="s">
+      <c r="S25" s="35" t="s">
         <v>518</v>
       </c>
-      <c r="T25" s="2"/>
-      <c r="U25" t="s">
+      <c r="T25" s="35"/>
+      <c r="U25" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="V25" s="30" t="s">
+      <c r="V25" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="W25" s="30">
-        <v>1</v>
-      </c>
+      <c r="W25" s="34">
+        <v>1</v>
+      </c>
+      <c r="X25" s="34"/>
+      <c r="Y25" s="34"/>
+      <c r="Z25" s="34"/>
+      <c r="AA25" s="34"/>
+      <c r="AB25" s="34"/>
+      <c r="AC25" s="34"/>
+      <c r="AD25" s="34"/>
     </row>
     <row r="26" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
@@ -6456,74 +6566,81 @@
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="27" spans="1:31" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="32" t="s">
         <v>559</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="32">
         <v>26</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="32" t="s">
         <v>561</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="32" t="s">
         <v>573</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="32">
         <v>160</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="32">
         <v>6</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="32">
         <v>4</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="32" t="s">
         <v>562</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N27" s="32" t="s">
         <v>560</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="32">
         <v>80</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="32">
         <v>3</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="Q27" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="R27" s="6" t="s">
+      <c r="R27" s="38" t="s">
         <v>563</v>
       </c>
-      <c r="S27" s="2" t="s">
+      <c r="S27" s="35" t="s">
         <v>601</v>
       </c>
-      <c r="T27" s="2"/>
-      <c r="U27" t="s">
+      <c r="T27" s="35"/>
+      <c r="U27" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="V27" s="30" t="s">
+      <c r="V27" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="W27" s="30">
-        <v>1</v>
-      </c>
+      <c r="W27" s="34">
+        <v>1</v>
+      </c>
+      <c r="X27" s="34"/>
+      <c r="Y27" s="34"/>
+      <c r="Z27" s="34"/>
+      <c r="AA27" s="34"/>
+      <c r="AB27" s="34"/>
+      <c r="AC27" s="34"/>
+      <c r="AD27" s="34"/>
     </row>
     <row r="28" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
@@ -6580,67 +6697,75 @@
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
-    <row r="29" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="29" spans="1:31" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="32" t="s">
         <v>627</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="32">
         <v>28</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="32" t="s">
         <v>628</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="32" t="s">
         <v>628</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="32" t="s">
         <v>665</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="32">
         <v>115</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="32">
         <v>3</v>
       </c>
-      <c r="I29">
-        <v>6</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="I29" s="32">
+        <v>5</v>
+      </c>
+      <c r="J29" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L29" s="32" t="s">
         <v>490</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M29" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N29" s="32" t="s">
         <v>629</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="32">
         <v>15</v>
       </c>
-      <c r="P29">
-        <v>1</v>
-      </c>
-      <c r="Q29" t="s">
+      <c r="P29" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="R29" s="2" t="s">
+      <c r="R29" s="35" t="s">
         <v>644</v>
       </c>
-      <c r="S29" s="14" t="s">
+      <c r="S29" s="36" t="s">
         <v>701</v>
       </c>
-      <c r="W29" s="30">
-        <v>1</v>
-      </c>
+      <c r="V29" s="34"/>
+      <c r="W29" s="34">
+        <v>1</v>
+      </c>
+      <c r="X29" s="34"/>
+      <c r="Y29" s="34"/>
+      <c r="Z29" s="34"/>
+      <c r="AA29" s="34"/>
+      <c r="AB29" s="34"/>
+      <c r="AC29" s="34"/>
+      <c r="AD29" s="34"/>
     </row>
     <row r="30" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
@@ -6707,70 +6832,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+    <row r="31" spans="1:31" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="32" t="s">
         <v>726</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="32">
         <v>30</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="32" t="s">
         <v>710</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="32" t="s">
         <v>713</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="32">
         <v>67</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="32">
         <v>4</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="32">
         <v>3</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M31" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N31" s="32" t="s">
         <v>714</v>
       </c>
-      <c r="O31">
-        <v>1</v>
-      </c>
-      <c r="P31">
-        <v>1</v>
-      </c>
-      <c r="Q31" t="s">
+      <c r="O31" s="32">
+        <v>1</v>
+      </c>
+      <c r="P31" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="R31" t="s">
+      <c r="R31" s="32" t="s">
         <v>723</v>
       </c>
-      <c r="S31" s="3" t="s">
+      <c r="S31" s="33" t="s">
         <v>724</v>
       </c>
-      <c r="T31" s="3" t="s">
+      <c r="T31" s="33" t="s">
         <v>725</v>
       </c>
-      <c r="U31" t="s">
+      <c r="U31" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="AA31" s="30">
-        <v>1</v>
-      </c>
+      <c r="V31" s="34"/>
+      <c r="W31" s="34"/>
+      <c r="X31" s="34"/>
+      <c r="Y31" s="34"/>
+      <c r="Z31" s="34"/>
+      <c r="AA31" s="34">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="34"/>
+      <c r="AC31" s="34"/>
+      <c r="AD31" s="34"/>
     </row>
     <row r="32" spans="1:31" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
@@ -6786,72 +6919,79 @@
         <v>332</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="33" spans="1:30" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="32" t="s">
         <v>742</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="32">
         <v>32</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="32" t="s">
         <v>741</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="32" t="s">
         <v>743</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="32" t="s">
         <v>744</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="32">
         <v>100</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="32">
         <v>4</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="32">
         <v>3</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="L33" t="s">
+      <c r="L33" s="32" t="s">
         <v>748</v>
       </c>
-      <c r="M33" t="s">
+      <c r="M33" s="32" t="s">
         <v>745</v>
       </c>
-      <c r="N33" t="s">
+      <c r="N33" s="32" t="s">
         <v>747</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="32">
         <v>20</v>
       </c>
-      <c r="P33">
-        <v>1</v>
-      </c>
-      <c r="Q33" t="s">
+      <c r="P33" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="R33" s="2" t="s">
+      <c r="R33" s="35" t="s">
         <v>760</v>
       </c>
-      <c r="S33" s="3" t="s">
+      <c r="S33" s="33" t="s">
         <v>759</v>
       </c>
-      <c r="V33" s="30" t="s">
+      <c r="V33" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="AA33" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W33" s="34"/>
+      <c r="X33" s="34"/>
+      <c r="Y33" s="34"/>
+      <c r="Z33" s="34"/>
+      <c r="AA33" s="34">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="34"/>
+      <c r="AC33" s="34"/>
+      <c r="AD33" s="34"/>
+    </row>
+    <row r="35" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>471</v>
       </c>
@@ -8224,7 +8364,7 @@
         <v>109</v>
       </c>
       <c r="C57" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D57" t="s">
         <v>405</v>
@@ -8251,7 +8391,7 @@
         <v>152</v>
       </c>
       <c r="C58" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D58" t="s">
         <v>404</v>
@@ -14888,7 +15028,7 @@
         <v>314</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>315</v>

</xml_diff>

<commit_message>
fix for topo media Query meaning full size images were downloaded every time! eeek. Also fix for grande fermeda topo
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4830E5F0-0288-4035-993C-8F03276741A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F11F308-0772-476C-B84B-319D9D2561F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -4775,7 +4775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AH31" sqref="AH31"/>
     </sheetView>
@@ -9560,8 +9560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10517,7 +10517,7 @@
         <v>220</v>
       </c>
       <c r="E33">
-        <v>175</v>
+        <v>240</v>
       </c>
       <c r="F33" t="s">
         <v>813</v>

</xml_diff>

<commit_message>
added ksar rock in morocco
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F024CFA2-DC6A-4799-B2D8-1541B817B3F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C04279-5186-456F-95F8-CB8AE983B2FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="846">
   <si>
     <t>cliff</t>
   </si>
@@ -2758,6 +2758,81 @@
   </si>
   <si>
     <t xml:space="preserve">The Devils slide was first climbed in the early 1960's. The face has been claimed to be the tallest granite slab in Europe. Whilst untrue, it is one of the tallest slab climbs in England and certainly a must climb classic. It makes for an exceptional climb at an amenable grade. This popular route was climbed, or perhaps more accurately "walked", feet only by Jonny Dawes in 2017. Although Lundy (meaning Puffin Island in Norse) has climbing restrictions some of the year, the devils slide and a number of other areas are exempt. The slide doesn't have nesting birds, likely because it's so exposed, bare that in mind when you plan. To get to Lundy a ferry can be taken from Ilfracombe in Devon. Climb up the right-hand side of the slab following the groove. For the last pitch take the obvious traverse left under the headwall. Whilst originally 5 pitches of climbing, it can be done in as few as three with long ropes and careful runner placments. See references below for more info. </t>
+  </si>
+  <si>
+    <t>Ksar Rock</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>East Butress</t>
+  </si>
+  <si>
+    <t>morocco</t>
+  </si>
+  <si>
+    <t>29.81270,-9.06676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Souss-Massa</t>
+  </si>
+  <si>
+    <t>https://issuu.com/oxfordalpineclub/docs/100cc_preview_reduced</t>
+  </si>
+  <si>
+    <t>Climb Info: Sample of Climb Tafraout | 100 Classic Climbs covering Ksar Rock</t>
+  </si>
+  <si>
+    <t>http://www.the-mountain-people.com/blog/morocco-trad-climbing-tafraout-recce-trip/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article: Morocco Trad Climbing | Tafraout </t>
+  </si>
+  <si>
+    <t>img/tiles/ksar-rock-trad-climbing-morocco.jpg</t>
+  </si>
+  <si>
+    <t>Ksar rock trad climbing Morocco</t>
+  </si>
+  <si>
+    <t>The Mountain People</t>
+  </si>
+  <si>
+    <t>origina: The Mountain People</t>
+  </si>
+  <si>
+    <t>img/topos/ksar-rock/ksar-rock-east-buttress-climb-morocco.jpg</t>
+  </si>
+  <si>
+    <t>Ksar rock offers easy trad climbing Morocco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ksar rock offers great multi-pitch rock climbing up to around 200 meters with grades from Severe to E1. This is a popular destination for its quick approach, easy access and quality routes that get great winter sun on the south face. The East Buttress route is one of the easiest climbs up Ksar Rock and an can be upgraded to Very Sever by taking a direct line on the 4th pitch. </t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Approach:&lt;/strong&gt;
+Park outside of Anammar Village, then follow the track into the village. The track ends at Ksar Rock Guesthouse (see references below for this accommodation option). Before the guesthouse, which is last on the left, turn left down an alleyway and then follow this left again towards the base of Ksar Rock and the East Buttress climb. 
+&lt;/p&gt;&lt;p&gt;
+&lt;strong&gt;Descent:&lt;/strong&gt; Head over the top of the cliff and descend down the north side before heading around to the west and coming down the west gully.</t>
+  </si>
+  <si>
+    <t>https://amzn.to/32OTqBc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A fantastic guidebook to the quartzite trad climbing around the Jebel el Kest and Jebel Taskra massifs. Mostly multi-pitch climbs up to to 800m mountain adventures.This is a selective guide in that it describes 79 of the best crags, but does offer comprehensive coverage of those crags. It covers the East Buttress climb on Ksar rock in exceptional detail. </t>
+  </si>
+  <si>
+    <t>Climb Tafraout - 100 Classic Climbs</t>
+  </si>
+  <si>
+    <t>img/guidebooks/climb-tafraout-100-classic-climbs.jpg</t>
+  </si>
+  <si>
+    <t>img/topos/ksar-rock/maps/</t>
+  </si>
+  <si>
+    <t>Location of Ksar Rock in Morocco</t>
   </si>
 </sst>
 </file>
@@ -3722,7 +3797,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7</c:v>
@@ -4798,11 +4873,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF35"/>
+  <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R9" sqref="R9"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y36" sqref="Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4997,7 +5072,7 @@
       <c r="AE2" s="40">
         <v>43668</v>
       </c>
-      <c r="AF2" s="38">
+      <c r="AF2" s="41">
         <f>(AE2-DATE(1970,1,1))*86400</f>
         <v>1563753600</v>
       </c>
@@ -5504,6 +5579,13 @@
       <c r="AB9" s="34"/>
       <c r="AC9" s="34"/>
       <c r="AD9" s="34"/>
+      <c r="AE9" s="39">
+        <v>43727</v>
+      </c>
+      <c r="AF9" s="38">
+        <f>(AE9-DATE(1970,1,1))*86400</f>
+        <v>1568851200</v>
+      </c>
     </row>
     <row r="10" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -7244,6 +7326,76 @@
       <c r="AB35" s="34"/>
       <c r="AC35" s="34"/>
       <c r="AD35" s="34"/>
+    </row>
+    <row r="36" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>822</v>
+      </c>
+      <c r="B36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>823</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>827</v>
+      </c>
+      <c r="F36" t="s">
+        <v>824</v>
+      </c>
+      <c r="G36">
+        <v>120</v>
+      </c>
+      <c r="H36">
+        <v>6</v>
+      </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
+      <c r="J36" t="s">
+        <v>160</v>
+      </c>
+      <c r="K36" t="s">
+        <v>74</v>
+      </c>
+      <c r="M36" t="s">
+        <v>825</v>
+      </c>
+      <c r="N36" t="s">
+        <v>826</v>
+      </c>
+      <c r="O36">
+        <v>10</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>189</v>
+      </c>
+      <c r="R36" t="s">
+        <v>838</v>
+      </c>
+      <c r="S36" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="U36" t="s">
+        <v>159</v>
+      </c>
+      <c r="V36" s="30" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y36" s="34"/>
+      <c r="AE36" s="40">
+        <v>43730</v>
+      </c>
+      <c r="AF36" s="41">
+        <f>(AE36-DATE(1970,1,1))*86400</f>
+        <v>1569110400</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7256,8 +7408,8 @@
   <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8823,7 +8975,7 @@
         <v>593</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" ref="I65:I94" si="2">CONCATENATE(A65,B65)</f>
+        <f t="shared" ref="I65:I97" si="2">CONCATENATE(A65,B65)</f>
         <v>22map</v>
       </c>
     </row>
@@ -9539,6 +9691,81 @@
       <c r="I94" t="str">
         <f t="shared" si="2"/>
         <v>33map</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>35</v>
+      </c>
+      <c r="B95" t="s">
+        <v>147</v>
+      </c>
+      <c r="C95" t="s">
+        <v>832</v>
+      </c>
+      <c r="D95" t="s">
+        <v>833</v>
+      </c>
+      <c r="E95" t="s">
+        <v>830</v>
+      </c>
+      <c r="F95" t="s">
+        <v>834</v>
+      </c>
+      <c r="I95" t="str">
+        <f t="shared" si="2"/>
+        <v>35tile</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A96">
+        <v>35</v>
+      </c>
+      <c r="B96" t="s">
+        <v>108</v>
+      </c>
+      <c r="C96" t="s">
+        <v>836</v>
+      </c>
+      <c r="D96" t="s">
+        <v>837</v>
+      </c>
+      <c r="E96" t="s">
+        <v>830</v>
+      </c>
+      <c r="F96" t="s">
+        <v>835</v>
+      </c>
+      <c r="G96">
+        <v>5</v>
+      </c>
+      <c r="I96" t="str">
+        <f t="shared" si="2"/>
+        <v>35topo</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A97">
+        <v>35</v>
+      </c>
+      <c r="B97" t="s">
+        <v>104</v>
+      </c>
+      <c r="C97" t="s">
+        <v>844</v>
+      </c>
+      <c r="D97" t="s">
+        <v>845</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="F97" t="s">
+        <v>593</v>
+      </c>
+      <c r="I97" t="str">
+        <f t="shared" si="2"/>
+        <v>35map</v>
       </c>
     </row>
     <row r="113" spans="9:9" x14ac:dyDescent="0.45">
@@ -9579,18 +9806,19 @@
     <hyperlink ref="E90" r:id="rId5" xr:uid="{59D28AFE-420C-4CA0-BD5D-FC1A4D3B4F21}"/>
     <hyperlink ref="E92" r:id="rId6" xr:uid="{6FFA1984-FD0B-4900-A07C-DD63BA0DAF12}"/>
     <hyperlink ref="E21" r:id="rId7" xr:uid="{13D796E4-2DCC-423A-8465-6FBC7F8F9F51}"/>
+    <hyperlink ref="E97" r:id="rId8" xr:uid="{D9B3E716-EB3F-4800-9BA6-F7CC27A4B929}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10561,6 +10789,35 @@
         <v>29.95</v>
       </c>
     </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" s="3">
+        <v>35</v>
+      </c>
+      <c r="B34" s="5">
+        <v>9780993548628</v>
+      </c>
+      <c r="C34" t="s">
+        <v>842</v>
+      </c>
+      <c r="D34" t="s">
+        <v>215</v>
+      </c>
+      <c r="E34">
+        <v>102</v>
+      </c>
+      <c r="F34" t="s">
+        <v>841</v>
+      </c>
+      <c r="G34" t="s">
+        <v>843</v>
+      </c>
+      <c r="H34" t="s">
+        <v>840</v>
+      </c>
+      <c r="I34">
+        <v>27.95</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1" xr:uid="{14007672-E4E3-4A8F-8DD0-45E59BDCCEDC}"/>
@@ -10574,10 +10831,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11063,15 +11320,38 @@
         <v>812</v>
       </c>
     </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>35</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="C44" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>35</v>
+      </c>
+      <c r="B45" t="s">
+        <v>830</v>
+      </c>
+      <c r="C45" t="s">
+        <v>831</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C40" xr:uid="{9D543331-6ADF-4965-B171-A65876C9201E}"/>
   <hyperlinks>
     <hyperlink ref="B20" r:id="rId1" xr:uid="{B8B4C84F-4B9B-4B98-AA47-BE6674672F64}"/>
     <hyperlink ref="B27" r:id="rId2" location="overview" xr:uid="{AAF53F3C-824D-46A3-8C66-5CFC2A7E56BD}"/>
     <hyperlink ref="B30" r:id="rId3" xr:uid="{22191C32-D6EE-41A0-B31D-B1D036DF0037}"/>
+    <hyperlink ref="B44" r:id="rId4" xr:uid="{5D80DB1F-C872-4D68-9A2E-3246D644E524}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -11398,10 +11678,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745174B4-A8CA-45B8-ACCB-9B5B609F0D5D}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView topLeftCell="A78" zoomScale="94" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15663,6 +15943,138 @@
       </c>
       <c r="N94" s="27">
         <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A95" s="12">
+        <v>35</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="C95" s="12">
+        <v>4</v>
+      </c>
+      <c r="D95" s="12">
+        <v>3</v>
+      </c>
+      <c r="E95" s="12">
+        <v>4</v>
+      </c>
+      <c r="F95" s="12">
+        <v>3</v>
+      </c>
+      <c r="G95" s="12">
+        <v>2</v>
+      </c>
+      <c r="H95" s="12">
+        <v>2</v>
+      </c>
+      <c r="I95" s="12">
+        <v>2</v>
+      </c>
+      <c r="J95" s="12">
+        <v>2</v>
+      </c>
+      <c r="K95" s="12">
+        <v>3</v>
+      </c>
+      <c r="L95" s="12">
+        <v>3</v>
+      </c>
+      <c r="M95" s="12">
+        <v>5</v>
+      </c>
+      <c r="N95" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A96" s="11">
+        <v>35</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C96" s="26">
+        <v>16.2</v>
+      </c>
+      <c r="D96" s="26">
+        <v>17.7</v>
+      </c>
+      <c r="E96" s="26">
+        <v>19.8</v>
+      </c>
+      <c r="F96" s="26">
+        <v>22.5</v>
+      </c>
+      <c r="G96" s="26">
+        <v>24.3</v>
+      </c>
+      <c r="H96" s="26">
+        <v>27.3</v>
+      </c>
+      <c r="I96" s="26">
+        <v>31.3</v>
+      </c>
+      <c r="J96" s="26">
+        <v>31.1</v>
+      </c>
+      <c r="K96" s="26">
+        <v>28</v>
+      </c>
+      <c r="L96" s="26">
+        <v>24.2</v>
+      </c>
+      <c r="M96" s="26">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="N96" s="26">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A97" s="13">
+        <v>35</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="C97" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="D97" s="27">
+        <v>3.7</v>
+      </c>
+      <c r="E97" s="27">
+        <v>6.7</v>
+      </c>
+      <c r="F97" s="27">
+        <v>9.1</v>
+      </c>
+      <c r="G97" s="27">
+        <v>11.5</v>
+      </c>
+      <c r="H97" s="27">
+        <v>13.9</v>
+      </c>
+      <c r="I97" s="27">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="J97" s="27">
+        <v>18</v>
+      </c>
+      <c r="K97" s="27">
+        <v>15.3</v>
+      </c>
+      <c r="L97" s="27">
+        <v>11.5</v>
+      </c>
+      <c r="M97" s="27">
+        <v>7.5</v>
+      </c>
+      <c r="N97" s="27">
+        <v>3.7</v>
       </c>
     </row>
   </sheetData>
@@ -15673,10 +16085,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="87" workbookViewId="0">
-      <selection activeCell="B9" sqref="A9:B9"/>
+    <sheetView topLeftCell="A17" zoomScale="87" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -15956,7 +16368,7 @@
       </c>
       <c r="P5">
         <f>COUNTIF(CLIMBS!J:J,'to-do-score-card'!O5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.5">
@@ -17527,6 +17939,57 @@
       </c>
       <c r="L35" s="25" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A36" t="str">
+        <f>CLIMBS!A36</f>
+        <v>Ksar Rock</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" t="str">
+        <f>CLIMBS!B36</f>
+        <v>publish</v>
+      </c>
+      <c r="D36">
+        <f>IF(CLIMBS!R36&lt;&gt;0,1,0)+IF(CLIMBS!G36&lt;&gt;0,1,0)+IF(CLIMBS!H36&lt;&gt;0,1,0)+IF(CLIMBS!I36&lt;&gt;0,1,0)+IF(CLIMBS!J36&lt;&gt;0,1,0)+IF(CLIMBS!N36&lt;&gt;0,1,0)+IF(CLIMBS!M36&lt;&gt;0,1,0)+IF(CLIMBS!O36&lt;&gt;0,1,0)+IF(CLIMBS!P36&lt;&gt;0,1,0)</f>
+        <v>9</v>
+      </c>
+      <c r="E36">
+        <f>IF(CLIMBS!S36&lt;&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B36,"tile"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B36,"topo"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B36,"map"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <f>SUMIFS(IMAGES!G:G,IMAGES!A:A,'to-do-score-card'!B36,IMAGES!B:B,"topo")</f>
+        <v>5</v>
+      </c>
+      <c r="H36">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B36,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B36,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B36,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <f>IF(VLOOKUP(B36,CLIMBS!C:T,18,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="25" t="str">
+        <f t="shared" ref="L36" si="3">IF(SUM(D36:K36)=22,"DONE","")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
updated sitemap and added new climbs to weather climb json
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C04279-5186-456F-95F8-CB8AE983B2FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDA33BD-ABD6-4E66-8730-48DABE3EA3AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4876,8 +4876,8 @@
   <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y36" sqref="Y36"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -16087,7 +16087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="87" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="87" workbookViewId="0">
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
keyboard accessibility update plus fix for pushstate js error on weather race condition
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDA33BD-ABD6-4E66-8730-48DABE3EA3AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B3C231-683E-4973-8EC1-A9C857AB4B4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4876,8 +4876,8 @@
   <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I9" sqref="I9"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5769,7 +5769,7 @@
         <v>140</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12" t="s">
         <v>39</v>
@@ -7340,7 +7340,7 @@
       <c r="D36" t="s">
         <v>823</v>
       </c>
-      <c r="E36" s="32" t="s">
+      <c r="E36" s="42" t="s">
         <v>827</v>
       </c>
       <c r="F36" t="s">
@@ -16087,7 +16087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="87" workbookViewId="0">
+    <sheetView zoomScale="87" workbookViewId="0">
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ability to wishlist and mark climbs as done - refactored use of local storage - added accessibility around subscribe - added better styles for sliders - added more advanced filters
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A7CB48-6863-4BF0-A8EB-92F0D7B6707C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C2FB03-5AB6-47B1-A9FA-587BEDF673A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="847">
   <si>
     <t>cliff</t>
   </si>
@@ -2833,6 +2833,9 @@
   <si>
     <t>&lt;strong&gt;Approach&lt;/strong&gt;: There is a shuttle bus that runs between Pera in the Val di Fassa and Rufugio Gardenccia (approach time is measured from Rufugio Gardenccia [Gardenccia shelter/mountain refuge]). The service departs from the large carpark by the Ciampedie chairlift in Pera. From here hike to the Rufugio Re Alberto, then follow the well worn path to the towers. Take the path behind Torre Piaz until reaching the gully between the larger towers of Stabeler and Delago. The rout starts from the ledge.&lt;/p&gt;&lt;p&gt;
 &lt;strong&gt;Descent&lt;/strong&gt;: From the east edge of Delago, make a 40m abseil to a notch between the two larger towers (Stabeler and Delago). Make another 40 then 45m abseil to the base of the gully between the towers to the ledge the route started on. From here you can hike back.</t>
+  </si>
+  <si>
+    <t>9780993548628</t>
   </si>
 </sst>
 </file>
@@ -4876,8 +4879,8 @@
   <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S8" sqref="S8"/>
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6347,6 +6350,9 @@
       <c r="U20" t="s">
         <v>158</v>
       </c>
+      <c r="AB20" s="30">
+        <v>1</v>
+      </c>
       <c r="AE20" s="31"/>
     </row>
     <row r="21" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -9817,8 +9823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10793,8 +10799,8 @@
       <c r="A34" s="3">
         <v>35</v>
       </c>
-      <c r="B34" s="5">
-        <v>9780993548628</v>
+      <c r="B34" s="5" t="s">
+        <v>846</v>
       </c>
       <c r="C34" t="s">
         <v>838</v>
@@ -16087,7 +16093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="87" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="87" workbookViewId="0">
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated the readme file
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60342385-8117-4426-8CA6-E22C69369053}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FD8D60-C497-49C7-A702-C8FF075FBEB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="803" yWindow="2363" windowWidth="12577" windowHeight="9532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -4908,7 +4908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="R8" sqref="R8"/>
     </sheetView>
@@ -9866,8 +9866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16208,7 +16208,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G10" sqref="A10:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
updated the contact page and added pictures of our pretty faces! Can remove you if you don't want it.
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FD8D60-C497-49C7-A702-C8FF075FBEB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8255606-61C9-4709-9F55-67956041F645}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="854">
   <si>
     <t>cliff</t>
   </si>
@@ -2866,6 +2866,9 @@
   </si>
   <si>
     <t>The Ordinary Route is the easiest route on the Idwal Slabs, that is however, assuming you manage to stay on route. It represents an ideal introduction to trad multi-pitch climbing. It is also possible to bring up someone with limited climbing experience in a group of 3, but the Descent can prove tricky, especially in wet conditions. Expect some polish on the route as well. The views are stunning, don't underestimate the stamina required despite the easy technical grade.</t>
+  </si>
+  <si>
+    <t>Observatory Ridge</t>
   </si>
 </sst>
 </file>
@@ -4906,11 +4909,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF36"/>
+  <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R8" sqref="R8"/>
+      <selection pane="topRight" activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7443,6 +7446,11 @@
         <v>1569110400</v>
       </c>
     </row>
+    <row r="37" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="32" t="s">
+        <v>853</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9866,7 +9874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -16207,8 +16215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="G10" sqref="A10:G12"/>
+    <sheetView topLeftCell="A15" zoomScale="87" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
fixed the readme file and fixed the sitemap dates. added some styles, can't remember what for but im sure they are beautiful
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8255606-61C9-4709-9F55-67956041F645}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F91AF3-F568-4263-A8BA-98D775CF86F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -4911,8 +4911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
@@ -9874,8 +9874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10425,7 +10425,7 @@
         <v>209</v>
       </c>
       <c r="E19">
-        <v>237</v>
+        <v>327</v>
       </c>
       <c r="F19" t="s">
         <v>847</v>
@@ -16215,8 +16215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="87" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="A6" zoomScale="87" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -16315,8 +16315,8 @@
         <v>0</v>
       </c>
       <c r="L2" s="25" t="str">
-        <f t="shared" ref="L2:L30" si="0">IF(SUM(D2:K2)=22,"DONE","")</f>
-        <v/>
+        <f>IF(SUM(D2:K2)=22,"DONE",IF(SUM(D2:J2)=21,"GOOD",""))</f>
+        <v>GOOD</v>
       </c>
       <c r="O2" t="s">
         <v>722</v>
@@ -16370,7 +16370,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L3:L36" si="0">IF(SUM(D3:K3)=22,"DONE",IF(SUM(D3:J3)=21,"GOOD",""))</f>
         <v>DONE</v>
       </c>
       <c r="O3" t="s">
@@ -16430,7 +16430,7 @@
       </c>
       <c r="L4" s="25" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>GOOD</v>
       </c>
       <c r="O4" t="s">
         <v>355</v>
@@ -16489,7 +16489,7 @@
       </c>
       <c r="L5" s="25" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>GOOD</v>
       </c>
       <c r="O5" t="s">
         <v>154</v>
@@ -16725,7 +16725,7 @@
       </c>
       <c r="L9" s="25" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>GOOD</v>
       </c>
       <c r="O9" t="s">
         <v>364</v>
@@ -16835,7 +16835,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="25" t="str">
-        <f>IF(SUM(D11:K11)=22,"DONE","")</f>
+        <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
     </row>
@@ -17862,7 +17862,7 @@
         <v>1</v>
       </c>
       <c r="L31" s="25" t="str">
-        <f>IF(SUM(D31:K31)=22,"DONE","")</f>
+        <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
     </row>
@@ -17913,7 +17913,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="25" t="str">
-        <f t="shared" ref="L32:L33" si="1">IF(SUM(D32:K32)=22,"DONE","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -17964,7 +17964,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -18015,8 +18015,8 @@
         <v>0</v>
       </c>
       <c r="L34" s="25" t="str">
-        <f t="shared" ref="L34:L35" si="2">IF(SUM(D34:K34)=22,"DONE","")</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>GOOD</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.5">
@@ -18066,7 +18066,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -18117,8 +18117,8 @@
         <v>0</v>
       </c>
       <c r="L36" s="25" t="str">
-        <f t="shared" ref="L36" si="3">IF(SUM(D36:K36)=22,"DONE","")</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>GOOD</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the topo builder and added the topo for Mount Indefatigable in Canada
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F91AF3-F568-4263-A8BA-98D775CF86F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C296214-B63B-44B2-8F73-DF69CCE7B203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="855">
   <si>
     <t>cliff</t>
   </si>
@@ -1230,13 +1230,7 @@
     <t>img: Dow Williams</t>
   </si>
   <si>
-    <t>original: Dow Williams</t>
-  </si>
-  <si>
     <t>Mount Indefatigable topo for Joy route in Canada</t>
-  </si>
-  <si>
-    <t>img/topos/indefatigable/mount-indefatigable-topo.jpg</t>
   </si>
   <si>
     <t>YDS 5.6</t>
@@ -2869,6 +2863,15 @@
   </si>
   <si>
     <t>Observatory Ridge</t>
+  </si>
+  <si>
+    <t>img/topos/indefatigable/joy-climb-mount-indefatigable-topo.jpg</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Mount_Indefatigable</t>
+  </si>
+  <si>
+    <t>original: wikipedia</t>
   </si>
 </sst>
 </file>
@@ -4984,10 +4987,10 @@
         <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>13</v>
@@ -4999,7 +5002,7 @@
         <v>15</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>16</v>
@@ -5008,34 +5011,34 @@
         <v>17</v>
       </c>
       <c r="W1" s="29" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="X1" s="29" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="Y1" s="29" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="Z1" s="29" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="AA1" s="29" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="AB1" s="29" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="AC1" s="29" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="AD1" s="29" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -5088,7 +5091,7 @@
         <v>27</v>
       </c>
       <c r="R2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="S2" t="s">
         <v>28</v>
@@ -5163,13 +5166,13 @@
         <v>39</v>
       </c>
       <c r="R3" s="32" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="S3" s="32" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="T3" s="33" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="U3" s="32" t="s">
         <v>40</v>
@@ -5197,7 +5200,7 @@
     </row>
     <row r="4" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B4" t="s">
         <v>99</v>
@@ -5313,10 +5316,10 @@
         <v>59</v>
       </c>
       <c r="R5" s="32" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="S5" s="35" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="U5" s="32" t="s">
         <v>40</v>
@@ -5517,7 +5520,7 @@
         <v>84</v>
       </c>
       <c r="K8" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="M8" t="s">
         <v>46</v>
@@ -5535,13 +5538,13 @@
         <v>48</v>
       </c>
       <c r="R8" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="S8" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="U8" t="s">
         <v>153</v>
@@ -5604,10 +5607,10 @@
         <v>39</v>
       </c>
       <c r="R9" s="32" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="S9" s="32" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="U9" s="32" t="s">
         <v>153</v>
@@ -5647,7 +5650,7 @@
         <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F10" t="s">
         <v>90</v>
@@ -5668,10 +5671,10 @@
         <v>55</v>
       </c>
       <c r="L10" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="M10" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="N10" t="s">
         <v>161</v>
@@ -5686,10 +5689,10 @@
         <v>39</v>
       </c>
       <c r="R10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="T10" s="2"/>
       <c r="U10" t="s">
@@ -5752,7 +5755,7 @@
         <v>97</v>
       </c>
       <c r="T11" s="32" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="U11" s="32" t="s">
         <v>153</v>
@@ -5886,13 +5889,13 @@
         <v>173</v>
       </c>
       <c r="R13" s="35" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="S13" s="36" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="T13" s="36" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="V13" s="34" t="s">
         <v>154</v>
@@ -5950,7 +5953,7 @@
         <v>65</v>
       </c>
       <c r="N14" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="O14">
         <v>20</v>
@@ -6027,10 +6030,10 @@
         <v>204</v>
       </c>
       <c r="S15" s="35" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="T15" s="36" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="U15" s="32" t="s">
         <v>189</v>
@@ -6090,7 +6093,7 @@
         <v>227</v>
       </c>
       <c r="N16" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="O16">
         <v>5</v>
@@ -6102,10 +6105,10 @@
         <v>228</v>
       </c>
       <c r="R16" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="U16" t="s">
         <v>40</v>
@@ -6170,10 +6173,10 @@
         <v>297</v>
       </c>
       <c r="S17" s="36" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="T17" s="36" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="U17" s="32" t="s">
         <v>153</v>
@@ -6296,7 +6299,7 @@
         <v>355</v>
       </c>
       <c r="K19" s="32" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="M19" s="32" t="s">
         <v>37</v>
@@ -6367,13 +6370,13 @@
         <v>74</v>
       </c>
       <c r="L20" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="M20" t="s">
         <v>375</v>
       </c>
       <c r="N20" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="O20">
         <v>40</v>
@@ -6385,7 +6388,7 @@
         <v>59</v>
       </c>
       <c r="R20" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="S20" t="s">
         <v>380</v>
@@ -6448,13 +6451,13 @@
         <v>39</v>
       </c>
       <c r="R21" s="35" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="S21" s="33" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="T21" s="33" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="V21" s="34" t="s">
         <v>197</v>
@@ -6479,7 +6482,7 @@
     </row>
     <row r="22" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B22" t="s">
         <v>99</v>
@@ -6488,13 +6491,13 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E22" t="s">
+        <v>412</v>
+      </c>
+      <c r="F22" t="s">
         <v>414</v>
-      </c>
-      <c r="F22" t="s">
-        <v>416</v>
       </c>
       <c r="G22">
         <v>80</v>
@@ -6512,10 +6515,10 @@
         <v>325</v>
       </c>
       <c r="M22" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="N22" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="O22">
         <v>40</v>
@@ -6527,13 +6530,13 @@
         <v>39</v>
       </c>
       <c r="R22" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="S22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="U22" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="V22" s="30" t="s">
         <v>41</v>
@@ -6541,7 +6544,7 @@
     </row>
     <row r="23" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="32" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B23" s="32" t="s">
         <v>99</v>
@@ -6553,10 +6556,10 @@
         <v>167</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F23" s="32" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G23" s="32">
         <v>228</v>
@@ -6577,7 +6580,7 @@
         <v>170</v>
       </c>
       <c r="N23" s="32" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="O23" s="32">
         <v>20</v>
@@ -6589,10 +6592,10 @@
         <v>59</v>
       </c>
       <c r="R23" s="32" t="s">
+        <v>452</v>
+      </c>
+      <c r="S23" s="32" t="s">
         <v>454</v>
-      </c>
-      <c r="S23" s="32" t="s">
-        <v>456</v>
       </c>
       <c r="U23" s="32" t="s">
         <v>189</v>
@@ -6613,7 +6616,7 @@
     </row>
     <row r="24" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B24" t="s">
         <v>99</v>
@@ -6622,13 +6625,13 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
+        <v>465</v>
+      </c>
+      <c r="E24" t="s">
         <v>467</v>
       </c>
-      <c r="E24" t="s">
-        <v>469</v>
-      </c>
       <c r="F24" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G24">
         <v>250</v>
@@ -6646,13 +6649,13 @@
         <v>24</v>
       </c>
       <c r="L24" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="M24" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="N24" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="O24">
         <v>21</v>
@@ -6664,10 +6667,10 @@
         <v>173</v>
       </c>
       <c r="R24" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="S24" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="U24" t="s">
         <v>189</v>
@@ -6681,7 +6684,7 @@
     </row>
     <row r="25" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="32" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B25" s="32" t="s">
         <v>99</v>
@@ -6690,13 +6693,13 @@
         <v>24</v>
       </c>
       <c r="D25" s="32" t="s">
+        <v>483</v>
+      </c>
+      <c r="E25" s="32" t="s">
         <v>485</v>
       </c>
-      <c r="E25" s="32" t="s">
-        <v>487</v>
-      </c>
       <c r="F25" s="32" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="G25" s="32">
         <v>350</v>
@@ -6714,13 +6717,13 @@
         <v>55</v>
       </c>
       <c r="L25" s="32" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="M25" s="32" t="s">
+        <v>487</v>
+      </c>
+      <c r="N25" s="32" t="s">
         <v>489</v>
-      </c>
-      <c r="N25" s="32" t="s">
-        <v>491</v>
       </c>
       <c r="O25" s="32">
         <v>190</v>
@@ -6732,10 +6735,10 @@
         <v>39</v>
       </c>
       <c r="R25" s="32" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="S25" s="36" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="T25" s="35"/>
       <c r="U25" s="32" t="s">
@@ -6764,7 +6767,7 @@
     </row>
     <row r="26" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B26" t="s">
         <v>99</v>
@@ -6773,13 +6776,13 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E26" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F26" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="G26">
         <v>230</v>
@@ -6797,13 +6800,13 @@
         <v>181</v>
       </c>
       <c r="L26" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="M26" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="N26" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="O26">
         <v>70</v>
@@ -6815,10 +6818,10 @@
         <v>59</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="S26" s="14" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="T26" s="2"/>
       <c r="U26" t="s">
@@ -6837,7 +6840,7 @@
     </row>
     <row r="27" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="32" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B27" s="32" t="s">
         <v>99</v>
@@ -6849,10 +6852,10 @@
         <v>70</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G27" s="32">
         <v>160</v>
@@ -6867,7 +6870,7 @@
         <v>35</v>
       </c>
       <c r="K27" s="32" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="L27" s="32" t="s">
         <v>75</v>
@@ -6876,7 +6879,7 @@
         <v>76</v>
       </c>
       <c r="N27" s="32" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="O27" s="32">
         <v>80</v>
@@ -6888,10 +6891,10 @@
         <v>78</v>
       </c>
       <c r="R27" s="37" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="S27" s="36" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="T27" s="35"/>
       <c r="U27" s="32" t="s">
@@ -6913,7 +6916,7 @@
     </row>
     <row r="28" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B28" t="s">
         <v>100</v>
@@ -6922,13 +6925,13 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
+        <v>595</v>
+      </c>
+      <c r="E28" t="s">
+        <v>596</v>
+      </c>
+      <c r="F28" t="s">
         <v>597</v>
-      </c>
-      <c r="E28" t="s">
-        <v>598</v>
-      </c>
-      <c r="F28" t="s">
-        <v>599</v>
       </c>
       <c r="G28">
         <v>250</v>
@@ -6946,13 +6949,13 @@
         <v>36</v>
       </c>
       <c r="L28" t="s">
+        <v>598</v>
+      </c>
+      <c r="M28" t="s">
+        <v>593</v>
+      </c>
+      <c r="N28" t="s">
         <v>600</v>
-      </c>
-      <c r="M28" t="s">
-        <v>595</v>
-      </c>
-      <c r="N28" t="s">
-        <v>602</v>
       </c>
       <c r="O28">
         <v>30</v>
@@ -6961,14 +6964,14 @@
         <v>1</v>
       </c>
       <c r="Q28" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
     <row r="29" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="32" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B29" s="32" t="s">
         <v>99</v>
@@ -6977,13 +6980,13 @@
         <v>28</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="G29" s="32">
         <v>115</v>
@@ -7001,13 +7004,13 @@
         <v>181</v>
       </c>
       <c r="L29" s="32" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="M29" s="32" t="s">
         <v>170</v>
       </c>
       <c r="N29" s="32" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="O29" s="32">
         <v>15</v>
@@ -7019,10 +7022,10 @@
         <v>39</v>
       </c>
       <c r="R29" s="35" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="S29" s="36" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="V29" s="34"/>
       <c r="W29" s="34">
@@ -7038,7 +7041,7 @@
     </row>
     <row r="30" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B30" t="s">
         <v>99</v>
@@ -7050,10 +7053,10 @@
         <v>30</v>
       </c>
       <c r="E30" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="F30" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="G30">
         <v>87</v>
@@ -7074,7 +7077,7 @@
         <v>37</v>
       </c>
       <c r="N30" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="O30">
         <v>20</v>
@@ -7086,13 +7089,13 @@
         <v>59</v>
       </c>
       <c r="R30" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="S30" s="14" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="T30" s="3" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="U30" t="s">
         <v>189</v>
@@ -7110,7 +7113,7 @@
     </row>
     <row r="31" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="32" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B31" s="32" t="s">
         <v>99</v>
@@ -7122,10 +7125,10 @@
         <v>30</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G31" s="32">
         <v>67</v>
@@ -7146,7 +7149,7 @@
         <v>37</v>
       </c>
       <c r="N31" s="32" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="O31" s="32">
         <v>1</v>
@@ -7158,13 +7161,13 @@
         <v>59</v>
       </c>
       <c r="R31" s="32" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="S31" s="33" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="T31" s="33" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="U31" s="32" t="s">
         <v>153</v>
@@ -7190,7 +7193,7 @@
     </row>
     <row r="32" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B32" t="s">
         <v>100</v>
@@ -7204,7 +7207,7 @@
     </row>
     <row r="33" spans="1:32" s="32" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="32" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B33" s="32" t="s">
         <v>99</v>
@@ -7213,13 +7216,13 @@
         <v>32</v>
       </c>
       <c r="D33" s="32" t="s">
+        <v>712</v>
+      </c>
+      <c r="E33" s="32" t="s">
         <v>714</v>
       </c>
-      <c r="E33" s="32" t="s">
-        <v>716</v>
-      </c>
       <c r="F33" s="32" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="G33" s="32">
         <v>100</v>
@@ -7237,13 +7240,13 @@
         <v>36</v>
       </c>
       <c r="L33" s="32" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="M33" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="N33" s="32" t="s">
         <v>718</v>
-      </c>
-      <c r="N33" s="32" t="s">
-        <v>720</v>
       </c>
       <c r="O33" s="32">
         <v>20</v>
@@ -7255,10 +7258,10 @@
         <v>59</v>
       </c>
       <c r="R33" s="35" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="S33" s="33" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="V33" s="34" t="s">
         <v>41</v>
@@ -7283,7 +7286,7 @@
     </row>
     <row r="34" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B34" t="s">
         <v>99</v>
@@ -7295,10 +7298,10 @@
         <v>70</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F34" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="G34">
         <v>720</v>
@@ -7313,16 +7316,16 @@
         <v>355</v>
       </c>
       <c r="K34" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L34" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="M34" t="s">
         <v>76</v>
       </c>
       <c r="N34" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="O34">
         <v>60</v>
@@ -7334,10 +7337,10 @@
         <v>78</v>
       </c>
       <c r="R34" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="V34" s="30" t="s">
         <v>154</v>
@@ -7355,7 +7358,7 @@
     </row>
     <row r="35" spans="1:32" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="32" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B35" s="32" t="s">
         <v>100</v>
@@ -7378,7 +7381,7 @@
     </row>
     <row r="36" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B36" t="s">
         <v>99</v>
@@ -7387,13 +7390,13 @@
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E36" s="42" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="F36" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="G36">
         <v>120</v>
@@ -7411,10 +7414,10 @@
         <v>74</v>
       </c>
       <c r="M36" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="N36" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="O36">
         <v>10</v>
@@ -7426,10 +7429,10 @@
         <v>183</v>
       </c>
       <c r="R36" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="U36" t="s">
         <v>153</v>
@@ -7448,7 +7451,7 @@
     </row>
     <row r="37" spans="1:32" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="32" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
   </sheetData>
@@ -7461,9 +7464,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7497,7 +7500,7 @@
         <v>109</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>306</v>
@@ -7511,7 +7514,7 @@
         <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D2" t="s">
         <v>105</v>
@@ -7556,16 +7559,16 @@
         <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D4" t="s">
         <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F4" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -7580,13 +7583,13 @@
         <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D5" t="s">
         <v>115</v>
       </c>
       <c r="E5" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F5" t="s">
         <v>138</v>
@@ -7613,7 +7616,7 @@
         <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F6" t="s">
         <v>138</v>
@@ -7631,16 +7634,16 @@
         <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D7" t="s">
         <v>117</v>
       </c>
       <c r="E7" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F7" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -7658,13 +7661,13 @@
         <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="E8" t="s">
         <v>118</v>
       </c>
       <c r="F8" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -7685,7 +7688,7 @@
         <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -7700,16 +7703,16 @@
         <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D10" t="s">
         <v>121</v>
       </c>
       <c r="E10" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F10" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -7730,7 +7733,7 @@
         <v>144</v>
       </c>
       <c r="E11" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
@@ -7790,16 +7793,16 @@
         <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D14" t="s">
         <v>127</v>
       </c>
       <c r="E14" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F14" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
@@ -7844,7 +7847,7 @@
         <v>128</v>
       </c>
       <c r="E16" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
@@ -7859,16 +7862,16 @@
         <v>102</v>
       </c>
       <c r="C17" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D17" t="s">
         <v>133</v>
       </c>
       <c r="E17" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F17" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -7883,13 +7886,13 @@
         <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="D18" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="E18" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F18" t="s">
         <v>138</v>
@@ -7934,16 +7937,16 @@
         <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D20" t="s">
         <v>135</v>
       </c>
       <c r="E20" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F20" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -7958,16 +7961,16 @@
         <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D21" t="s">
         <v>137</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="F21" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="G21">
         <v>5</v>
@@ -8006,16 +8009,16 @@
         <v>102</v>
       </c>
       <c r="C23" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D23" t="s">
         <v>127</v>
       </c>
       <c r="E23" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F23" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -8030,16 +8033,16 @@
         <v>106</v>
       </c>
       <c r="C24" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D24" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E24" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F24" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
@@ -8078,16 +8081,16 @@
         <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D26" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E26" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F26" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
@@ -8102,13 +8105,13 @@
         <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D27" t="s">
         <v>139</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F27" t="s">
         <v>138</v>
@@ -8147,16 +8150,16 @@
         <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D29" t="s">
         <v>140</v>
       </c>
       <c r="E29" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F29" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
@@ -8219,16 +8222,16 @@
         <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D32" t="s">
         <v>307</v>
       </c>
       <c r="E32" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F32" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="0"/>
@@ -8249,7 +8252,7 @@
         <v>175</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="F33" t="s">
         <v>138</v>
@@ -8294,16 +8297,16 @@
         <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D35" t="s">
         <v>315</v>
       </c>
       <c r="E35" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F35" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="1"/>
@@ -8366,16 +8369,16 @@
         <v>102</v>
       </c>
       <c r="C38" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D38" t="s">
         <v>342</v>
       </c>
       <c r="E38" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F38" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="1"/>
@@ -8438,16 +8441,16 @@
         <v>102</v>
       </c>
       <c r="C41" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D41" t="s">
         <v>313</v>
       </c>
       <c r="E41" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F41" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="1"/>
@@ -8510,16 +8513,16 @@
         <v>102</v>
       </c>
       <c r="C44" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D44" t="s">
         <v>271</v>
       </c>
       <c r="E44" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F44" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="1"/>
@@ -8534,16 +8537,16 @@
         <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D45" t="s">
         <v>286</v>
       </c>
       <c r="E45" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="F45" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="G45">
         <v>5</v>
@@ -8585,16 +8588,16 @@
         <v>102</v>
       </c>
       <c r="C47" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D47" t="s">
         <v>314</v>
       </c>
       <c r="E47" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F47" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="1"/>
@@ -8657,16 +8660,16 @@
         <v>102</v>
       </c>
       <c r="C50" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D50" t="s">
         <v>341</v>
       </c>
       <c r="E50" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F50" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="1"/>
@@ -8687,7 +8690,7 @@
         <v>358</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="F51" t="s">
         <v>103</v>
@@ -8729,16 +8732,16 @@
         <v>102</v>
       </c>
       <c r="C53" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D53" t="s">
         <v>363</v>
       </c>
       <c r="E53" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F53" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="1"/>
@@ -8753,16 +8756,19 @@
         <v>106</v>
       </c>
       <c r="C54" t="s">
-        <v>399</v>
+        <v>852</v>
       </c>
       <c r="D54" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E54" t="s">
-        <v>395</v>
+        <v>853</v>
       </c>
       <c r="F54" t="s">
-        <v>397</v>
+        <v>854</v>
+      </c>
+      <c r="G54">
+        <v>5</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="1"/>
@@ -8801,16 +8807,16 @@
         <v>102</v>
       </c>
       <c r="C56" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D56" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E56" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F56" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I56" t="str">
         <f t="shared" si="1"/>
@@ -8825,13 +8831,13 @@
         <v>106</v>
       </c>
       <c r="C57" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D57" t="s">
         <v>389</v>
       </c>
       <c r="E57" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F57" t="s">
         <v>138</v>
@@ -8852,13 +8858,13 @@
         <v>141</v>
       </c>
       <c r="C58" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D58" t="s">
         <v>388</v>
       </c>
       <c r="E58" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F58" t="s">
         <v>138</v>
@@ -8876,16 +8882,16 @@
         <v>102</v>
       </c>
       <c r="C59" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D59" t="s">
         <v>390</v>
       </c>
       <c r="E59" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F59" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="1"/>
@@ -8900,16 +8906,16 @@
         <v>106</v>
       </c>
       <c r="C60" t="s">
+        <v>424</v>
+      </c>
+      <c r="D60" t="s">
+        <v>425</v>
+      </c>
+      <c r="E60" t="s">
         <v>426</v>
       </c>
-      <c r="D60" t="s">
+      <c r="F60" t="s">
         <v>427</v>
-      </c>
-      <c r="E60" t="s">
-        <v>428</v>
-      </c>
-      <c r="F60" t="s">
-        <v>429</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" si="1"/>
@@ -8924,16 +8930,16 @@
         <v>141</v>
       </c>
       <c r="C61" t="s">
+        <v>420</v>
+      </c>
+      <c r="D61" t="s">
+        <v>421</v>
+      </c>
+      <c r="E61" t="s">
         <v>422</v>
       </c>
-      <c r="D61" t="s">
+      <c r="F61" t="s">
         <v>423</v>
-      </c>
-      <c r="E61" t="s">
-        <v>424</v>
-      </c>
-      <c r="F61" t="s">
-        <v>425</v>
       </c>
       <c r="I61" t="str">
         <f t="shared" si="1"/>
@@ -8948,16 +8954,16 @@
         <v>102</v>
       </c>
       <c r="C62" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D62" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E62" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F62" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I62" t="str">
         <f t="shared" si="1"/>
@@ -8972,16 +8978,16 @@
         <v>106</v>
       </c>
       <c r="C63" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D63" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E63" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F63" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="I63" t="str">
         <f t="shared" si="1"/>
@@ -8996,13 +9002,13 @@
         <v>141</v>
       </c>
       <c r="C64" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D64" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E64" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F64" t="s">
         <v>235</v>
@@ -9020,16 +9026,16 @@
         <v>102</v>
       </c>
       <c r="C65" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D65" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E65" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F65" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I65" t="str">
         <f t="shared" ref="I65:I97" si="2">CONCATENATE(A65,B65)</f>
@@ -9044,16 +9050,16 @@
         <v>106</v>
       </c>
       <c r="C66" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D66" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E66" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F66" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I66" t="str">
         <f t="shared" si="2"/>
@@ -9068,13 +9074,13 @@
         <v>141</v>
       </c>
       <c r="C67" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D67" t="s">
+        <v>472</v>
+      </c>
+      <c r="E67" t="s">
         <v>474</v>
-      </c>
-      <c r="E67" t="s">
-        <v>476</v>
       </c>
       <c r="F67" t="s">
         <v>107</v>
@@ -9092,16 +9098,16 @@
         <v>102</v>
       </c>
       <c r="C68" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D68" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E68" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F68" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I68" t="str">
         <f t="shared" si="2"/>
@@ -9116,16 +9122,16 @@
         <v>106</v>
       </c>
       <c r="C69" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D69" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E69" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F69" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="I69" t="str">
         <f t="shared" si="2"/>
@@ -9140,16 +9146,16 @@
         <v>141</v>
       </c>
       <c r="C70" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D70" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E70" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F70" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" si="2"/>
@@ -9164,16 +9170,16 @@
         <v>102</v>
       </c>
       <c r="C71" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D71" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E71" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F71" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="2"/>
@@ -9188,16 +9194,16 @@
         <v>106</v>
       </c>
       <c r="C72" t="s">
+        <v>531</v>
+      </c>
+      <c r="D72" t="s">
+        <v>532</v>
+      </c>
+      <c r="E72" t="s">
         <v>533</v>
       </c>
-      <c r="D72" t="s">
+      <c r="F72" t="s">
         <v>534</v>
-      </c>
-      <c r="E72" t="s">
-        <v>535</v>
-      </c>
-      <c r="F72" t="s">
-        <v>536</v>
       </c>
       <c r="I72" t="str">
         <f t="shared" si="2"/>
@@ -9212,16 +9218,16 @@
         <v>141</v>
       </c>
       <c r="C73" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D73" t="s">
+        <v>526</v>
+      </c>
+      <c r="E73" t="s">
+        <v>527</v>
+      </c>
+      <c r="F73" t="s">
         <v>528</v>
-      </c>
-      <c r="E73" t="s">
-        <v>529</v>
-      </c>
-      <c r="F73" t="s">
-        <v>530</v>
       </c>
       <c r="I73" t="str">
         <f t="shared" si="2"/>
@@ -9236,16 +9242,16 @@
         <v>102</v>
       </c>
       <c r="C74" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D74" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E74" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F74" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I74" t="str">
         <f t="shared" si="2"/>
@@ -9260,16 +9266,16 @@
         <v>106</v>
       </c>
       <c r="C75" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D75" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E75" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F75" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I75" t="str">
         <f t="shared" si="2"/>
@@ -9284,16 +9290,16 @@
         <v>141</v>
       </c>
       <c r="C76" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D76" t="s">
+        <v>541</v>
+      </c>
+      <c r="E76" t="s">
+        <v>542</v>
+      </c>
+      <c r="F76" t="s">
         <v>543</v>
-      </c>
-      <c r="E76" t="s">
-        <v>544</v>
-      </c>
-      <c r="F76" t="s">
-        <v>545</v>
       </c>
       <c r="I76" t="str">
         <f t="shared" si="2"/>
@@ -9308,16 +9314,16 @@
         <v>102</v>
       </c>
       <c r="C77" t="s">
+        <v>580</v>
+      </c>
+      <c r="D77" t="s">
+        <v>581</v>
+      </c>
+      <c r="E77" t="s">
         <v>582</v>
       </c>
-      <c r="D77" t="s">
+      <c r="F77" t="s">
         <v>583</v>
-      </c>
-      <c r="E77" t="s">
-        <v>584</v>
-      </c>
-      <c r="F77" t="s">
-        <v>585</v>
       </c>
       <c r="I77" t="str">
         <f t="shared" si="2"/>
@@ -9332,16 +9338,16 @@
         <v>106</v>
       </c>
       <c r="C78" t="s">
+        <v>609</v>
+      </c>
+      <c r="D78" t="s">
+        <v>610</v>
+      </c>
+      <c r="E78" s="10" t="s">
         <v>611</v>
       </c>
-      <c r="D78" t="s">
+      <c r="F78" s="14" t="s">
         <v>612</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>613</v>
-      </c>
-      <c r="F78" s="14" t="s">
-        <v>614</v>
       </c>
       <c r="G78" s="14">
         <v>2</v>
@@ -9359,16 +9365,16 @@
         <v>141</v>
       </c>
       <c r="C79" t="s">
+        <v>613</v>
+      </c>
+      <c r="D79" t="s">
+        <v>622</v>
+      </c>
+      <c r="E79" t="s">
         <v>615</v>
       </c>
-      <c r="D79" t="s">
-        <v>624</v>
-      </c>
-      <c r="E79" t="s">
-        <v>617</v>
-      </c>
       <c r="F79" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="I79" t="str">
         <f t="shared" si="2"/>
@@ -9383,16 +9389,16 @@
         <v>102</v>
       </c>
       <c r="C80" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D80" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E80" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F80" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I80" t="str">
         <f t="shared" si="2"/>
@@ -9407,13 +9413,13 @@
         <v>141</v>
       </c>
       <c r="C81" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D81" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E81" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F81" t="s">
         <v>138</v>
@@ -9431,13 +9437,13 @@
         <v>106</v>
       </c>
       <c r="C82" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D82" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="E82" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F82" t="s">
         <v>138</v>
@@ -9458,16 +9464,16 @@
         <v>102</v>
       </c>
       <c r="C83" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D83" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="E83" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F83" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I83" t="str">
         <f t="shared" si="2"/>
@@ -9482,13 +9488,13 @@
         <v>106</v>
       </c>
       <c r="C84" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D84" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="E84" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F84" t="s">
         <v>138</v>
@@ -9509,13 +9515,13 @@
         <v>141</v>
       </c>
       <c r="C85" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D85" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="E85" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F85" t="s">
         <v>138</v>
@@ -9533,16 +9539,16 @@
         <v>102</v>
       </c>
       <c r="C86" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D86" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E86" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F86" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I86" t="str">
         <f t="shared" si="2"/>
@@ -9557,16 +9563,16 @@
         <v>141</v>
       </c>
       <c r="C87" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D87" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="E87" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="F87" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="I87" t="str">
         <f t="shared" si="2"/>
@@ -9581,16 +9587,16 @@
         <v>106</v>
       </c>
       <c r="C88" t="s">
+        <v>725</v>
+      </c>
+      <c r="D88" t="s">
+        <v>726</v>
+      </c>
+      <c r="E88" t="s">
         <v>727</v>
       </c>
-      <c r="D88" t="s">
-        <v>728</v>
-      </c>
-      <c r="E88" t="s">
-        <v>729</v>
-      </c>
       <c r="F88" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="G88">
         <v>5</v>
@@ -9608,16 +9614,16 @@
         <v>102</v>
       </c>
       <c r="C89" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D89" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E89" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F89" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I89" t="str">
         <f t="shared" si="2"/>
@@ -9632,16 +9638,16 @@
         <v>106</v>
       </c>
       <c r="C90" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D90" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="F90" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="G90">
         <v>5</v>
@@ -9659,16 +9665,16 @@
         <v>102</v>
       </c>
       <c r="C91" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D91" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E91" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F91" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I91" t="str">
         <f t="shared" si="2"/>
@@ -9683,16 +9689,16 @@
         <v>141</v>
       </c>
       <c r="C92" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D92" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="E92" s="10" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="F92" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="I92" t="str">
         <f t="shared" si="2"/>
@@ -9707,16 +9713,16 @@
         <v>106</v>
       </c>
       <c r="C93" t="s">
+        <v>774</v>
+      </c>
+      <c r="D93" t="s">
+        <v>775</v>
+      </c>
+      <c r="E93" t="s">
         <v>776</v>
       </c>
-      <c r="D93" t="s">
-        <v>777</v>
-      </c>
-      <c r="E93" t="s">
-        <v>778</v>
-      </c>
       <c r="F93" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="G93">
         <v>5</v>
@@ -9734,16 +9740,16 @@
         <v>102</v>
       </c>
       <c r="C94" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="D94" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E94" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F94" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I94" t="str">
         <f t="shared" si="2"/>
@@ -9758,16 +9764,16 @@
         <v>141</v>
       </c>
       <c r="C95" t="s">
+        <v>819</v>
+      </c>
+      <c r="D95" t="s">
+        <v>820</v>
+      </c>
+      <c r="E95" t="s">
+        <v>817</v>
+      </c>
+      <c r="F95" t="s">
         <v>821</v>
-      </c>
-      <c r="D95" t="s">
-        <v>822</v>
-      </c>
-      <c r="E95" t="s">
-        <v>819</v>
-      </c>
-      <c r="F95" t="s">
-        <v>823</v>
       </c>
       <c r="I95" t="str">
         <f t="shared" si="2"/>
@@ -9782,16 +9788,16 @@
         <v>106</v>
       </c>
       <c r="C96" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D96" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="E96" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="F96" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="G96">
         <v>5</v>
@@ -9809,16 +9815,16 @@
         <v>102</v>
       </c>
       <c r="C97" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D97" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F97" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I97" t="str">
         <f t="shared" si="2"/>
@@ -9874,7 +9880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -9941,7 +9947,7 @@
         <v>240</v>
       </c>
       <c r="H2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I2">
         <v>24.99</v>
@@ -9970,7 +9976,7 @@
         <v>245</v>
       </c>
       <c r="H3" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I3">
         <v>25</v>
@@ -9999,7 +10005,7 @@
         <v>249</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I4">
         <v>24.99</v>
@@ -10028,7 +10034,7 @@
         <v>272</v>
       </c>
       <c r="H5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I5">
         <v>20</v>
@@ -10086,7 +10092,7 @@
         <v>249</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I7">
         <v>24.99</v>
@@ -10115,7 +10121,7 @@
         <v>240</v>
       </c>
       <c r="H8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I8">
         <v>24.99</v>
@@ -10138,13 +10144,13 @@
         <v>34</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G9" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H9" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="I9">
         <v>34.950000000000003</v>
@@ -10173,7 +10179,7 @@
         <v>240</v>
       </c>
       <c r="H10" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I10">
         <v>24.99</v>
@@ -10202,7 +10208,7 @@
         <v>272</v>
       </c>
       <c r="H11" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I11">
         <v>20</v>
@@ -10231,7 +10237,7 @@
         <v>249</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I12">
         <v>24.99</v>
@@ -10260,7 +10266,7 @@
         <v>310</v>
       </c>
       <c r="H13" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="I13">
         <v>25</v>
@@ -10289,7 +10295,7 @@
         <v>240</v>
       </c>
       <c r="H14" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I14">
         <v>24.99</v>
@@ -10318,7 +10324,7 @@
         <v>318</v>
       </c>
       <c r="H15" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="I15">
         <v>34</v>
@@ -10347,7 +10353,7 @@
         <v>331</v>
       </c>
       <c r="H16" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="I16">
         <v>34.99</v>
@@ -10376,7 +10382,7 @@
         <v>369</v>
       </c>
       <c r="H17" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="I17">
         <v>25</v>
@@ -10399,13 +10405,13 @@
         <v>367</v>
       </c>
       <c r="F18" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="G18" t="s">
         <v>372</v>
       </c>
       <c r="H18" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="I18">
         <v>20</v>
@@ -10416,10 +10422,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C19" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D19" t="s">
         <v>209</v>
@@ -10428,13 +10434,13 @@
         <v>327</v>
       </c>
       <c r="F19" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="G19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H19" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="I19">
         <v>34.99</v>
@@ -10445,10 +10451,10 @@
         <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C20" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D20" t="s">
         <v>209</v>
@@ -10457,13 +10463,13 @@
         <v>129</v>
       </c>
       <c r="F20" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G20" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H20" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="I20">
         <v>19.95</v>
@@ -10477,25 +10483,25 @@
         <v>319</v>
       </c>
       <c r="C21" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D21" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E21">
         <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G21" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H21" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I21" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
@@ -10503,10 +10509,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C22" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D22" t="s">
         <v>209</v>
@@ -10515,13 +10521,13 @@
         <v>267</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G22" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H22" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="I22">
         <v>29.95</v>
@@ -10532,10 +10538,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C23" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D23" t="s">
         <v>209</v>
@@ -10544,13 +10550,13 @@
         <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="G23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H23" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I23">
         <v>38</v>
@@ -10561,10 +10567,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C24" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D24" t="s">
         <v>209</v>
@@ -10573,13 +10579,13 @@
         <v>410</v>
       </c>
       <c r="F24" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="G24" t="s">
         <v>508</v>
       </c>
-      <c r="G24" t="s">
-        <v>510</v>
-      </c>
       <c r="H24" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="I24">
         <v>10</v>
@@ -10590,10 +10596,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C25" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D25" t="s">
         <v>209</v>
@@ -10602,13 +10608,13 @@
         <v>300</v>
       </c>
       <c r="F25" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="G25" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H25" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I25">
         <v>38</v>
@@ -10631,7 +10637,7 @@
         <v>86</v>
       </c>
       <c r="F26" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>278</v>
@@ -10648,10 +10654,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C27" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D27" t="s">
         <v>209</v>
@@ -10660,13 +10666,13 @@
         <v>157</v>
       </c>
       <c r="F27" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="H27" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="I27">
         <v>35</v>
@@ -10677,7 +10683,7 @@
         <v>16</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C28" t="s">
         <v>283</v>
@@ -10689,13 +10695,13 @@
         <v>34</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="G28" t="s">
         <v>627</v>
       </c>
-      <c r="G28" t="s">
-        <v>629</v>
-      </c>
       <c r="H28" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="I28">
         <v>10</v>
@@ -10706,10 +10712,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C29" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D29" t="s">
         <v>209</v>
@@ -10718,13 +10724,13 @@
         <v>101</v>
       </c>
       <c r="F29" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G29" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="H29" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="I29">
         <v>25</v>
@@ -10747,13 +10753,13 @@
         <v>53</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="G30" t="s">
         <v>240</v>
       </c>
       <c r="H30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I30">
         <v>24.99</v>
@@ -10767,7 +10773,7 @@
         <v>220</v>
       </c>
       <c r="C31" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="D31" t="s">
         <v>209</v>
@@ -10776,13 +10782,13 @@
         <v>169</v>
       </c>
       <c r="F31" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="G31" t="s">
+        <v>742</v>
+      </c>
+      <c r="H31" t="s">
         <v>741</v>
-      </c>
-      <c r="G31" t="s">
-        <v>744</v>
-      </c>
-      <c r="H31" t="s">
-        <v>743</v>
       </c>
       <c r="I31">
         <v>24.99</v>
@@ -10793,10 +10799,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C32" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D32" t="s">
         <v>209</v>
@@ -10805,13 +10811,13 @@
         <v>20</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="G32" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="H32" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="I32">
         <v>10</v>
@@ -10834,7 +10840,7 @@
         <v>240</v>
       </c>
       <c r="F33" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>278</v>
@@ -10851,10 +10857,10 @@
         <v>35</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C34" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D34" t="s">
         <v>209</v>
@@ -10863,13 +10869,13 @@
         <v>102</v>
       </c>
       <c r="F34" t="s">
+        <v>828</v>
+      </c>
+      <c r="G34" t="s">
         <v>830</v>
       </c>
-      <c r="G34" t="s">
-        <v>832</v>
-      </c>
       <c r="H34" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="I34">
         <v>27.95</v>
@@ -10880,10 +10886,10 @@
         <v>8</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C35" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="D35" t="s">
         <v>209</v>
@@ -10892,13 +10898,13 @@
         <v>160</v>
       </c>
       <c r="F35" t="s">
+        <v>840</v>
+      </c>
+      <c r="G35" t="s">
+        <v>841</v>
+      </c>
+      <c r="H35" s="10" t="s">
         <v>842</v>
-      </c>
-      <c r="G35" t="s">
-        <v>843</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>844</v>
       </c>
       <c r="I35">
         <v>19.989999999999998</v>
@@ -10909,10 +10915,10 @@
         <v>10</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C36" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="D36" t="s">
         <v>209</v>
@@ -10921,13 +10927,13 @@
         <v>187</v>
       </c>
       <c r="F36" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="G36" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="I36">
         <v>19.989999999999998</v>
@@ -11024,7 +11030,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C6" t="s">
         <v>335</v>
@@ -11112,10 +11118,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
@@ -11123,10 +11129,10 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C15" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
@@ -11134,10 +11140,10 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C16" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -11145,10 +11151,10 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -11159,7 +11165,7 @@
         <v>174</v>
       </c>
       <c r="C18" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -11167,10 +11173,10 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C19" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -11178,10 +11184,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C20" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -11189,10 +11195,10 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C21" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -11200,10 +11206,10 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C22" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -11211,10 +11217,10 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
+        <v>641</v>
+      </c>
+      <c r="C23" t="s">
         <v>643</v>
-      </c>
-      <c r="C23" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -11222,7 +11228,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C24" t="s">
         <v>345</v>
@@ -11233,10 +11239,10 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C25" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -11244,10 +11250,10 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C26" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -11255,10 +11261,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C27" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -11266,10 +11272,10 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C28" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -11277,10 +11283,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C29" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
@@ -11288,10 +11294,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C30" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
@@ -11299,10 +11305,10 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C31" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
@@ -11310,10 +11316,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C32" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -11321,10 +11327,10 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C33" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
@@ -11332,10 +11338,10 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C34" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
@@ -11343,10 +11349,10 @@
         <v>2</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C35" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
@@ -11354,10 +11360,10 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C36" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
@@ -11365,10 +11371,10 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C37" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
@@ -11376,10 +11382,10 @@
         <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C38" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
@@ -11387,10 +11393,10 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C39" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
@@ -11398,10 +11404,10 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="C40" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
@@ -11409,10 +11415,10 @@
         <v>8</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C41" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
@@ -11420,10 +11426,10 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C42" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
@@ -11431,10 +11437,10 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C43" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
@@ -11442,10 +11448,10 @@
         <v>35</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C44" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
@@ -11453,10 +11459,10 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C45" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
@@ -11464,10 +11470,10 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C46" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
   </sheetData>
@@ -16246,13 +16252,13 @@
         <v>302</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>303</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>304</v>
@@ -16261,10 +16267,10 @@
         <v>305</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.5">
@@ -16319,7 +16325,7 @@
         <v>GOOD</v>
       </c>
       <c r="O2" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.5">
@@ -17282,7 +17288,7 @@
       </c>
       <c r="G20">
         <f>SUMIFS(IMAGES!G:G,IMAGES!A:A,'to-do-score-card'!B20,IMAGES!B:B,"topo")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H20">
         <f>_xlfn.IFNA(IF(VLOOKUP(B20,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
@@ -17302,7 +17308,7 @@
       </c>
       <c r="L20" s="25" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>GOOD</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
added descriptions for the different grading systems - surprisingly interesting stuff
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC8F99F-FBAD-4B3F-9EAB-72C19016F7D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB2AB95-4518-4CA3-B388-5BFAEEFA7432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="872">
   <si>
     <t>cliff</t>
   </si>
@@ -1716,9 +1716,6 @@
   </si>
   <si>
     <t>The Vejolet Towers topo for Piaz Arete</t>
-  </si>
-  <si>
-    <t>VI+ &amp; (f6b)</t>
   </si>
   <si>
     <t>Piaz Arete Delagokante</t>
@@ -2893,6 +2890,39 @@
   </si>
   <si>
     <t>VS 4c</t>
+  </si>
+  <si>
+    <t>S 4a</t>
+  </si>
+  <si>
+    <t>VS 4b</t>
+  </si>
+  <si>
+    <t>D 3a</t>
+  </si>
+  <si>
+    <t>HS 4a</t>
+  </si>
+  <si>
+    <t>VI+ (f6b)</t>
+  </si>
+  <si>
+    <t>S 4b</t>
+  </si>
+  <si>
+    <t>VD 3c</t>
+  </si>
+  <si>
+    <t>HVS 5b</t>
+  </si>
+  <si>
+    <t>HVS 5c</t>
+  </si>
+  <si>
+    <t>https://www.summitpost.org/traumpfeiler-pillar-of-dreams/292553</t>
+  </si>
+  <si>
+    <t>Climb Info: Summit Post Page</t>
   </si>
 </sst>
 </file>
@@ -4934,9 +4964,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L28" sqref="L28"/>
+      <selection pane="topRight" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4998,10 +5028,10 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>10</v>
@@ -5010,10 +5040,10 @@
         <v>11</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>12</v>
@@ -5025,7 +5055,7 @@
         <v>14</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>15</v>
@@ -5034,34 +5064,34 @@
         <v>16</v>
       </c>
       <c r="X1" s="29" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="Y1" s="29" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="Z1" s="29" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="AA1" s="29" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="AB1" s="29" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="AC1" s="29" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="AD1" s="29" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AE1" s="29" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="AF1" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>704</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -5099,10 +5129,10 @@
         <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M2" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="N2" t="s">
         <v>24</v>
@@ -5180,16 +5210,16 @@
         <v>35</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M3" s="31" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="N3" s="31" t="s">
         <v>36</v>
       </c>
       <c r="O3" s="31" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="P3" s="31">
         <v>10</v>
@@ -5201,13 +5231,13 @@
         <v>37</v>
       </c>
       <c r="S3" s="31" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="T3" s="31" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="U3" s="32" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="V3" s="31" t="s">
         <v>38</v>
@@ -5235,7 +5265,7 @@
     </row>
     <row r="4" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B4" t="s">
         <v>97</v>
@@ -5268,10 +5298,10 @@
         <v>179</v>
       </c>
       <c r="L4" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M4" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="N4" t="s">
         <v>44</v>
@@ -5339,7 +5369,7 @@
         <v>53</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="M5" s="31" t="s">
         <v>54</v>
@@ -5360,10 +5390,10 @@
         <v>57</v>
       </c>
       <c r="S5" s="31" t="s">
+        <v>739</v>
+      </c>
+      <c r="T5" s="34" t="s">
         <v>740</v>
-      </c>
-      <c r="T5" s="34" t="s">
-        <v>741</v>
       </c>
       <c r="V5" s="31" t="s">
         <v>38</v>
@@ -5422,10 +5452,10 @@
         <v>35</v>
       </c>
       <c r="L6" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M6" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="N6" t="s">
         <v>63</v>
@@ -5502,7 +5532,7 @@
         <v>72</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="M7" s="31" t="s">
         <v>73</v>
@@ -5573,13 +5603,13 @@
         <v>82</v>
       </c>
       <c r="K8" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="L8" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M8" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="N8" t="s">
         <v>44</v>
@@ -5597,13 +5627,13 @@
         <v>46</v>
       </c>
       <c r="S8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="T8" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="V8" t="s">
         <v>151</v>
@@ -5651,10 +5681,10 @@
         <v>72</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M9" s="31" t="s">
-        <v>859</v>
+        <v>864</v>
       </c>
       <c r="N9" s="31" t="s">
         <v>36</v>
@@ -5672,10 +5702,10 @@
         <v>37</v>
       </c>
       <c r="S9" s="31" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="T9" s="31" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="V9" s="31" t="s">
         <v>151</v>
@@ -5736,10 +5766,10 @@
         <v>53</v>
       </c>
       <c r="L10" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="M10" t="s">
-        <v>544</v>
+        <v>865</v>
       </c>
       <c r="N10" t="s">
         <v>442</v>
@@ -5802,10 +5832,10 @@
         <v>35</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M11" s="31" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="N11" s="31" t="s">
         <v>36</v>
@@ -5829,7 +5859,7 @@
         <v>95</v>
       </c>
       <c r="U11" s="31" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="V11" s="31" t="s">
         <v>151</v>
@@ -5883,7 +5913,7 @@
         <v>23</v>
       </c>
       <c r="L12" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M12" t="s">
         <v>859</v>
@@ -5951,7 +5981,7 @@
         <v>23</v>
       </c>
       <c r="L13" s="31" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="M13" s="31" t="s">
         <v>169</v>
@@ -5972,13 +6002,13 @@
         <v>171</v>
       </c>
       <c r="S13" s="34" t="s">
+        <v>774</v>
+      </c>
+      <c r="T13" s="35" t="s">
         <v>775</v>
       </c>
-      <c r="T13" s="35" t="s">
-        <v>776</v>
-      </c>
       <c r="U13" s="35" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="W13" s="33" t="s">
         <v>152</v>
@@ -6033,16 +6063,16 @@
         <v>179</v>
       </c>
       <c r="L14" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M14" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="N14" t="s">
         <v>63</v>
       </c>
       <c r="O14" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="P14">
         <v>20</v>
@@ -6101,10 +6131,10 @@
         <v>35</v>
       </c>
       <c r="L15" s="31" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M15" s="31" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="N15" s="31" t="s">
         <v>36</v>
@@ -6125,10 +6155,10 @@
         <v>202</v>
       </c>
       <c r="T15" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="U15" s="35" t="s">
         <v>702</v>
-      </c>
-      <c r="U15" s="35" t="s">
-        <v>703</v>
       </c>
       <c r="V15" s="31" t="s">
         <v>187</v>
@@ -6182,7 +6212,7 @@
         <v>179</v>
       </c>
       <c r="L16" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="M16" s="5">
         <v>5.8</v>
@@ -6191,7 +6221,7 @@
         <v>225</v>
       </c>
       <c r="O16" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="P16">
         <v>5</v>
@@ -6203,10 +6233,10 @@
         <v>226</v>
       </c>
       <c r="S16" t="s">
+        <v>776</v>
+      </c>
+      <c r="T16" s="3" t="s">
         <v>777</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>778</v>
       </c>
       <c r="V16" t="s">
         <v>38</v>
@@ -6253,10 +6283,10 @@
         <v>35</v>
       </c>
       <c r="L17" s="31" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M17" s="31" t="s">
-        <v>859</v>
+        <v>866</v>
       </c>
       <c r="N17" s="31" t="s">
         <v>44</v>
@@ -6277,10 +6307,10 @@
         <v>295</v>
       </c>
       <c r="T17" s="35" t="s">
+        <v>641</v>
+      </c>
+      <c r="U17" s="35" t="s">
         <v>642</v>
-      </c>
-      <c r="U17" s="35" t="s">
-        <v>643</v>
       </c>
       <c r="V17" s="31" t="s">
         <v>151</v>
@@ -6409,10 +6439,10 @@
         <v>535</v>
       </c>
       <c r="L19" s="31" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>859</v>
+        <v>867</v>
       </c>
       <c r="N19" s="31" t="s">
         <v>36</v>
@@ -6483,7 +6513,7 @@
         <v>72</v>
       </c>
       <c r="L20" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="M20" s="5">
         <v>5.7</v>
@@ -6492,7 +6522,7 @@
         <v>372</v>
       </c>
       <c r="O20" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="P20">
         <v>40</v>
@@ -6558,10 +6588,10 @@
         <v>35</v>
       </c>
       <c r="L21" s="31" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="N21" s="31" t="s">
         <v>63</v>
@@ -6579,13 +6609,13 @@
         <v>37</v>
       </c>
       <c r="S21" s="34" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="T21" s="32" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="U21" s="32" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="W21" s="33" t="s">
         <v>195</v>
@@ -6643,10 +6673,10 @@
         <v>323</v>
       </c>
       <c r="L22" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M22" t="s">
-        <v>859</v>
+        <v>868</v>
       </c>
       <c r="N22" t="s">
         <v>411</v>
@@ -6711,10 +6741,10 @@
         <v>53</v>
       </c>
       <c r="L23" s="31" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M23" s="31" t="s">
-        <v>859</v>
+        <v>869</v>
       </c>
       <c r="N23" s="31" t="s">
         <v>168</v>
@@ -6789,7 +6819,7 @@
         <v>23</v>
       </c>
       <c r="L24" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="M24" t="s">
         <v>466</v>
@@ -6813,7 +6843,7 @@
         <v>467</v>
       </c>
       <c r="T24" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="V24" t="s">
         <v>187</v>
@@ -6860,7 +6890,7 @@
         <v>53</v>
       </c>
       <c r="L25" s="31" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="M25" s="31" t="s">
         <v>482</v>
@@ -6884,7 +6914,7 @@
         <v>492</v>
       </c>
       <c r="T25" s="35" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="U25" s="34"/>
       <c r="V25" s="31" t="s">
@@ -6946,7 +6976,7 @@
         <v>179</v>
       </c>
       <c r="L26" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="M26" t="s">
         <v>520</v>
@@ -6970,7 +7000,7 @@
         <v>531</v>
       </c>
       <c r="T26" s="14" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="U26" s="2"/>
       <c r="V26" t="s">
@@ -7004,7 +7034,7 @@
         <v>534</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G27" s="31">
         <v>160</v>
@@ -7022,7 +7052,7 @@
         <v>72</v>
       </c>
       <c r="L27" s="31" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="M27" s="31" t="s">
         <v>73</v>
@@ -7046,7 +7076,7 @@
         <v>536</v>
       </c>
       <c r="T27" s="35" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="U27" s="34"/>
       <c r="V27" s="31" t="s">
@@ -7075,7 +7105,7 @@
     </row>
     <row r="28" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B28" t="s">
         <v>98</v>
@@ -7084,13 +7114,13 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
+        <v>589</v>
+      </c>
+      <c r="E28" t="s">
         <v>590</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>591</v>
-      </c>
-      <c r="F28" t="s">
-        <v>592</v>
       </c>
       <c r="G28">
         <v>250</v>
@@ -7108,16 +7138,16 @@
         <v>35</v>
       </c>
       <c r="L28" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="M28" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="N28" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="O28" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P28">
         <v>30</v>
@@ -7126,14 +7156,14 @@
         <v>1</v>
       </c>
       <c r="R28" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
     </row>
     <row r="29" spans="1:33" s="31" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="31" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>97</v>
@@ -7142,13 +7172,13 @@
         <v>28</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F29" s="31" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G29" s="31">
         <v>115</v>
@@ -7166,7 +7196,7 @@
         <v>179</v>
       </c>
       <c r="L29" s="31" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="M29" s="31" t="s">
         <v>466</v>
@@ -7175,7 +7205,7 @@
         <v>168</v>
       </c>
       <c r="O29" s="31" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="P29" s="31">
         <v>15</v>
@@ -7187,10 +7217,10 @@
         <v>37</v>
       </c>
       <c r="S29" s="34" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="T29" s="35" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="W29" s="33"/>
       <c r="X29" s="33">
@@ -7206,7 +7236,7 @@
     </row>
     <row r="30" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B30" t="s">
         <v>97</v>
@@ -7218,10 +7248,10 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
+        <v>646</v>
+      </c>
+      <c r="F30" t="s">
         <v>647</v>
-      </c>
-      <c r="F30" t="s">
-        <v>648</v>
       </c>
       <c r="G30">
         <v>87</v>
@@ -7239,16 +7269,16 @@
         <v>35</v>
       </c>
       <c r="L30" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M30" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="N30" t="s">
         <v>36</v>
       </c>
       <c r="O30" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="P30">
         <v>20</v>
@@ -7260,13 +7290,13 @@
         <v>57</v>
       </c>
       <c r="S30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="T30" s="14" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="U30" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="V30" t="s">
         <v>187</v>
@@ -7284,7 +7314,7 @@
     </row>
     <row r="31" spans="1:33" s="31" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="31" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B31" s="31" t="s">
         <v>97</v>
@@ -7296,10 +7326,10 @@
         <v>29</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="F31" s="31" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G31" s="31">
         <v>67</v>
@@ -7317,16 +7347,16 @@
         <v>72</v>
       </c>
       <c r="L31" s="31" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M31" s="31" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="N31" s="31" t="s">
         <v>36</v>
       </c>
       <c r="O31" s="31" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="P31" s="31">
         <v>1</v>
@@ -7338,13 +7368,13 @@
         <v>57</v>
       </c>
       <c r="S31" s="31" t="s">
+        <v>689</v>
+      </c>
+      <c r="T31" s="32" t="s">
+        <v>783</v>
+      </c>
+      <c r="U31" s="32" t="s">
         <v>690</v>
-      </c>
-      <c r="T31" s="32" t="s">
-        <v>784</v>
-      </c>
-      <c r="U31" s="32" t="s">
-        <v>691</v>
       </c>
       <c r="V31" s="31" t="s">
         <v>151</v>
@@ -7370,7 +7400,7 @@
     </row>
     <row r="32" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B32" t="s">
         <v>98</v>
@@ -7382,15 +7412,12 @@
         <v>318</v>
       </c>
       <c r="L32" t="s">
-        <v>854</v>
-      </c>
-      <c r="M32" t="s">
-        <v>859</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:33" s="31" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="31" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B33" s="31" t="s">
         <v>97</v>
@@ -7399,13 +7426,13 @@
         <v>32</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E33" s="31" t="s">
+        <v>708</v>
+      </c>
+      <c r="F33" s="31" t="s">
         <v>709</v>
-      </c>
-      <c r="F33" s="31" t="s">
-        <v>710</v>
       </c>
       <c r="G33" s="31">
         <v>100</v>
@@ -7423,16 +7450,16 @@
         <v>35</v>
       </c>
       <c r="L33" s="31" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="M33" s="31" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="N33" s="31" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="O33" s="31" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="P33" s="31">
         <v>20</v>
@@ -7444,10 +7471,10 @@
         <v>57</v>
       </c>
       <c r="S33" s="34" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="T33" s="32" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="W33" s="33" t="s">
         <v>39</v>
@@ -7472,7 +7499,7 @@
     </row>
     <row r="34" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B34" t="s">
         <v>97</v>
@@ -7487,7 +7514,7 @@
         <v>534</v>
       </c>
       <c r="F34" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G34">
         <v>720</v>
@@ -7505,16 +7532,16 @@
         <v>395</v>
       </c>
       <c r="L34" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="M34" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="N34" t="s">
         <v>74</v>
       </c>
       <c r="O34" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="P34">
         <v>60</v>
@@ -7526,10 +7553,10 @@
         <v>76</v>
       </c>
       <c r="S34" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="T34" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="W34" s="30" t="s">
         <v>152</v>
@@ -7547,7 +7574,7 @@
     </row>
     <row r="35" spans="1:33" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="31" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>98</v>
@@ -7557,6 +7584,9 @@
       </c>
       <c r="D35" s="31" t="s">
         <v>18</v>
+      </c>
+      <c r="L35" s="31" t="s">
+        <v>853</v>
       </c>
       <c r="W35" s="33"/>
       <c r="X35" s="33"/>
@@ -7570,7 +7600,7 @@
     </row>
     <row r="36" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B36" t="s">
         <v>97</v>
@@ -7579,13 +7609,13 @@
         <v>35</v>
       </c>
       <c r="D36" t="s">
+        <v>804</v>
+      </c>
+      <c r="E36" s="41" t="s">
+        <v>808</v>
+      </c>
+      <c r="F36" t="s">
         <v>805</v>
-      </c>
-      <c r="E36" s="41" t="s">
-        <v>809</v>
-      </c>
-      <c r="F36" t="s">
-        <v>806</v>
       </c>
       <c r="G36">
         <v>120</v>
@@ -7603,16 +7633,16 @@
         <v>72</v>
       </c>
       <c r="L36" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M36" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="N36" t="s">
+        <v>806</v>
+      </c>
+      <c r="O36" t="s">
         <v>807</v>
-      </c>
-      <c r="O36" t="s">
-        <v>808</v>
       </c>
       <c r="P36">
         <v>10</v>
@@ -7624,10 +7654,10 @@
         <v>181</v>
       </c>
       <c r="S36" t="s">
+        <v>819</v>
+      </c>
+      <c r="T36" s="3" t="s">
         <v>820</v>
-      </c>
-      <c r="T36" s="3" t="s">
-        <v>821</v>
       </c>
       <c r="V36" t="s">
         <v>151</v>
@@ -7646,7 +7676,10 @@
     </row>
     <row r="37" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="31" t="s">
-        <v>846</v>
+        <v>845</v>
+      </c>
+      <c r="L37" s="31" t="s">
+        <v>853</v>
       </c>
     </row>
   </sheetData>
@@ -7695,7 +7728,7 @@
         <v>107</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>304</v>
@@ -7709,7 +7742,7 @@
         <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D2" t="s">
         <v>103</v>
@@ -7754,16 +7787,16 @@
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D4" t="s">
         <v>99</v>
       </c>
       <c r="E4" t="s">
+        <v>576</v>
+      </c>
+      <c r="F4" t="s">
         <v>577</v>
-      </c>
-      <c r="F4" t="s">
-        <v>578</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -7778,13 +7811,13 @@
         <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D5" t="s">
         <v>113</v>
       </c>
       <c r="E5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F5" t="s">
         <v>136</v>
@@ -7811,7 +7844,7 @@
         <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F6" t="s">
         <v>136</v>
@@ -7829,16 +7862,16 @@
         <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D7" t="s">
         <v>115</v>
       </c>
       <c r="E7" t="s">
+        <v>576</v>
+      </c>
+      <c r="F7" t="s">
         <v>577</v>
-      </c>
-      <c r="F7" t="s">
-        <v>578</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -7856,13 +7889,13 @@
         <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E8" t="s">
         <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -7883,7 +7916,7 @@
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -7898,16 +7931,16 @@
         <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D10" t="s">
         <v>119</v>
       </c>
       <c r="E10" t="s">
+        <v>576</v>
+      </c>
+      <c r="F10" t="s">
         <v>577</v>
-      </c>
-      <c r="F10" t="s">
-        <v>578</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -7928,7 +7961,7 @@
         <v>142</v>
       </c>
       <c r="E11" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
@@ -7988,16 +8021,16 @@
         <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D14" t="s">
         <v>125</v>
       </c>
       <c r="E14" t="s">
+        <v>576</v>
+      </c>
+      <c r="F14" t="s">
         <v>577</v>
-      </c>
-      <c r="F14" t="s">
-        <v>578</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
@@ -8042,7 +8075,7 @@
         <v>126</v>
       </c>
       <c r="E16" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
@@ -8057,16 +8090,16 @@
         <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D17" t="s">
         <v>131</v>
       </c>
       <c r="E17" t="s">
+        <v>576</v>
+      </c>
+      <c r="F17" t="s">
         <v>577</v>
-      </c>
-      <c r="F17" t="s">
-        <v>578</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -8081,13 +8114,13 @@
         <v>104</v>
       </c>
       <c r="C18" t="s">
+        <v>840</v>
+      </c>
+      <c r="D18" t="s">
         <v>841</v>
       </c>
-      <c r="D18" t="s">
-        <v>842</v>
-      </c>
       <c r="E18" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F18" t="s">
         <v>136</v>
@@ -8132,16 +8165,16 @@
         <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D20" t="s">
         <v>133</v>
       </c>
       <c r="E20" t="s">
+        <v>576</v>
+      </c>
+      <c r="F20" t="s">
         <v>577</v>
-      </c>
-      <c r="F20" t="s">
-        <v>578</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -8156,16 +8189,16 @@
         <v>104</v>
       </c>
       <c r="C21" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D21" t="s">
         <v>135</v>
       </c>
       <c r="E21" s="10" t="s">
+        <v>797</v>
+      </c>
+      <c r="F21" t="s">
         <v>798</v>
-      </c>
-      <c r="F21" t="s">
-        <v>799</v>
       </c>
       <c r="G21">
         <v>5</v>
@@ -8204,16 +8237,16 @@
         <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D23" t="s">
         <v>125</v>
       </c>
       <c r="E23" t="s">
+        <v>576</v>
+      </c>
+      <c r="F23" t="s">
         <v>577</v>
-      </c>
-      <c r="F23" t="s">
-        <v>578</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -8276,16 +8309,16 @@
         <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D26" t="s">
         <v>433</v>
       </c>
       <c r="E26" t="s">
+        <v>576</v>
+      </c>
+      <c r="F26" t="s">
         <v>577</v>
-      </c>
-      <c r="F26" t="s">
-        <v>578</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
@@ -8300,13 +8333,13 @@
         <v>104</v>
       </c>
       <c r="C27" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D27" t="s">
         <v>137</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F27" t="s">
         <v>136</v>
@@ -8345,16 +8378,16 @@
         <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D29" t="s">
         <v>138</v>
       </c>
       <c r="E29" t="s">
+        <v>576</v>
+      </c>
+      <c r="F29" t="s">
         <v>577</v>
-      </c>
-      <c r="F29" t="s">
-        <v>578</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
@@ -8417,16 +8450,16 @@
         <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D32" t="s">
         <v>305</v>
       </c>
       <c r="E32" t="s">
+        <v>576</v>
+      </c>
+      <c r="F32" t="s">
         <v>577</v>
-      </c>
-      <c r="F32" t="s">
-        <v>578</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="0"/>
@@ -8447,7 +8480,7 @@
         <v>173</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F33" t="s">
         <v>136</v>
@@ -8492,16 +8525,16 @@
         <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D35" t="s">
         <v>313</v>
       </c>
       <c r="E35" t="s">
+        <v>576</v>
+      </c>
+      <c r="F35" t="s">
         <v>577</v>
-      </c>
-      <c r="F35" t="s">
-        <v>578</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="1"/>
@@ -8564,16 +8597,16 @@
         <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D38" t="s">
         <v>340</v>
       </c>
       <c r="E38" t="s">
+        <v>576</v>
+      </c>
+      <c r="F38" t="s">
         <v>577</v>
-      </c>
-      <c r="F38" t="s">
-        <v>578</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="1"/>
@@ -8636,16 +8669,16 @@
         <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D41" t="s">
         <v>311</v>
       </c>
       <c r="E41" t="s">
+        <v>576</v>
+      </c>
+      <c r="F41" t="s">
         <v>577</v>
-      </c>
-      <c r="F41" t="s">
-        <v>578</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="1"/>
@@ -8708,16 +8741,16 @@
         <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D44" t="s">
         <v>269</v>
       </c>
       <c r="E44" t="s">
+        <v>576</v>
+      </c>
+      <c r="F44" t="s">
         <v>577</v>
-      </c>
-      <c r="F44" t="s">
-        <v>578</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="1"/>
@@ -8732,16 +8765,16 @@
         <v>104</v>
       </c>
       <c r="C45" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D45" t="s">
         <v>284</v>
       </c>
       <c r="E45" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F45" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G45">
         <v>5</v>
@@ -8783,16 +8816,16 @@
         <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D47" t="s">
         <v>312</v>
       </c>
       <c r="E47" t="s">
+        <v>576</v>
+      </c>
+      <c r="F47" t="s">
         <v>577</v>
-      </c>
-      <c r="F47" t="s">
-        <v>578</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="1"/>
@@ -8855,16 +8888,16 @@
         <v>100</v>
       </c>
       <c r="C50" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D50" t="s">
         <v>339</v>
       </c>
       <c r="E50" t="s">
+        <v>576</v>
+      </c>
+      <c r="F50" t="s">
         <v>577</v>
-      </c>
-      <c r="F50" t="s">
-        <v>578</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="1"/>
@@ -8885,7 +8918,7 @@
         <v>356</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F51" t="s">
         <v>101</v>
@@ -8927,16 +8960,16 @@
         <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D53" t="s">
         <v>361</v>
       </c>
       <c r="E53" t="s">
+        <v>576</v>
+      </c>
+      <c r="F53" t="s">
         <v>577</v>
-      </c>
-      <c r="F53" t="s">
-        <v>578</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="1"/>
@@ -8951,16 +8984,16 @@
         <v>104</v>
       </c>
       <c r="C54" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D54" t="s">
         <v>394</v>
       </c>
       <c r="E54" t="s">
+        <v>847</v>
+      </c>
+      <c r="F54" t="s">
         <v>848</v>
-      </c>
-      <c r="F54" t="s">
-        <v>849</v>
       </c>
       <c r="G54">
         <v>5</v>
@@ -9002,16 +9035,16 @@
         <v>100</v>
       </c>
       <c r="C56" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D56" t="s">
         <v>397</v>
       </c>
       <c r="E56" t="s">
+        <v>576</v>
+      </c>
+      <c r="F56" t="s">
         <v>577</v>
-      </c>
-      <c r="F56" t="s">
-        <v>578</v>
       </c>
       <c r="I56" t="str">
         <f t="shared" si="1"/>
@@ -9026,13 +9059,13 @@
         <v>104</v>
       </c>
       <c r="C57" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D57" t="s">
         <v>386</v>
       </c>
       <c r="E57" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F57" t="s">
         <v>136</v>
@@ -9053,13 +9086,13 @@
         <v>139</v>
       </c>
       <c r="C58" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D58" t="s">
         <v>385</v>
       </c>
       <c r="E58" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F58" t="s">
         <v>136</v>
@@ -9077,16 +9110,16 @@
         <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D59" t="s">
         <v>387</v>
       </c>
       <c r="E59" t="s">
+        <v>576</v>
+      </c>
+      <c r="F59" t="s">
         <v>577</v>
-      </c>
-      <c r="F59" t="s">
-        <v>578</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="1"/>
@@ -9149,16 +9182,16 @@
         <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D62" t="s">
         <v>426</v>
       </c>
       <c r="E62" t="s">
+        <v>576</v>
+      </c>
+      <c r="F62" t="s">
         <v>577</v>
-      </c>
-      <c r="F62" t="s">
-        <v>578</v>
       </c>
       <c r="I62" t="str">
         <f t="shared" si="1"/>
@@ -9221,16 +9254,16 @@
         <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D65" t="s">
         <v>459</v>
       </c>
       <c r="E65" t="s">
+        <v>576</v>
+      </c>
+      <c r="F65" t="s">
         <v>577</v>
-      </c>
-      <c r="F65" t="s">
-        <v>578</v>
       </c>
       <c r="I65" t="str">
         <f t="shared" ref="I65:I97" si="2">CONCATENATE(A65,B65)</f>
@@ -9293,16 +9326,16 @@
         <v>100</v>
       </c>
       <c r="C68" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D68" t="s">
         <v>473</v>
       </c>
       <c r="E68" t="s">
+        <v>576</v>
+      </c>
+      <c r="F68" t="s">
         <v>577</v>
-      </c>
-      <c r="F68" t="s">
-        <v>578</v>
       </c>
       <c r="I68" t="str">
         <f t="shared" si="2"/>
@@ -9365,16 +9398,16 @@
         <v>100</v>
       </c>
       <c r="C71" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D71" t="s">
         <v>493</v>
       </c>
       <c r="E71" t="s">
+        <v>576</v>
+      </c>
+      <c r="F71" t="s">
         <v>577</v>
-      </c>
-      <c r="F71" t="s">
-        <v>578</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="2"/>
@@ -9437,16 +9470,16 @@
         <v>100</v>
       </c>
       <c r="C74" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D74" t="s">
         <v>526</v>
       </c>
       <c r="E74" t="s">
+        <v>576</v>
+      </c>
+      <c r="F74" t="s">
         <v>577</v>
-      </c>
-      <c r="F74" t="s">
-        <v>578</v>
       </c>
       <c r="I74" t="str">
         <f t="shared" si="2"/>
@@ -9461,7 +9494,7 @@
         <v>104</v>
       </c>
       <c r="C75" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D75" t="s">
         <v>543</v>
@@ -9512,16 +9545,16 @@
         <v>100</v>
       </c>
       <c r="C77" t="s">
+        <v>574</v>
+      </c>
+      <c r="D77" t="s">
         <v>575</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>576</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>577</v>
-      </c>
-      <c r="F77" t="s">
-        <v>578</v>
       </c>
       <c r="I77" t="str">
         <f t="shared" si="2"/>
@@ -9536,16 +9569,16 @@
         <v>104</v>
       </c>
       <c r="C78" t="s">
+        <v>603</v>
+      </c>
+      <c r="D78" t="s">
         <v>604</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" s="10" t="s">
         <v>605</v>
       </c>
-      <c r="E78" s="10" t="s">
+      <c r="F78" s="14" t="s">
         <v>606</v>
-      </c>
-      <c r="F78" s="14" t="s">
-        <v>607</v>
       </c>
       <c r="G78" s="14">
         <v>2</v>
@@ -9563,16 +9596,16 @@
         <v>139</v>
       </c>
       <c r="C79" t="s">
+        <v>607</v>
+      </c>
+      <c r="D79" t="s">
+        <v>616</v>
+      </c>
+      <c r="E79" t="s">
+        <v>609</v>
+      </c>
+      <c r="F79" t="s">
         <v>608</v>
-      </c>
-      <c r="D79" t="s">
-        <v>617</v>
-      </c>
-      <c r="E79" t="s">
-        <v>610</v>
-      </c>
-      <c r="F79" t="s">
-        <v>609</v>
       </c>
       <c r="I79" t="str">
         <f t="shared" si="2"/>
@@ -9587,16 +9620,16 @@
         <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D80" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E80" t="s">
+        <v>576</v>
+      </c>
+      <c r="F80" t="s">
         <v>577</v>
-      </c>
-      <c r="F80" t="s">
-        <v>578</v>
       </c>
       <c r="I80" t="str">
         <f t="shared" si="2"/>
@@ -9611,13 +9644,13 @@
         <v>139</v>
       </c>
       <c r="C81" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D81" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E81" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F81" t="s">
         <v>136</v>
@@ -9635,13 +9668,13 @@
         <v>104</v>
       </c>
       <c r="C82" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D82" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E82" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F82" t="s">
         <v>136</v>
@@ -9662,16 +9695,16 @@
         <v>100</v>
       </c>
       <c r="C83" t="s">
+        <v>651</v>
+      </c>
+      <c r="D83" t="s">
         <v>652</v>
       </c>
-      <c r="D83" t="s">
-        <v>653</v>
-      </c>
       <c r="E83" t="s">
+        <v>576</v>
+      </c>
+      <c r="F83" t="s">
         <v>577</v>
-      </c>
-      <c r="F83" t="s">
-        <v>578</v>
       </c>
       <c r="I83" t="str">
         <f t="shared" si="2"/>
@@ -9686,13 +9719,13 @@
         <v>104</v>
       </c>
       <c r="C84" t="s">
+        <v>681</v>
+      </c>
+      <c r="D84" t="s">
         <v>682</v>
       </c>
-      <c r="D84" t="s">
-        <v>683</v>
-      </c>
       <c r="E84" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F84" t="s">
         <v>136</v>
@@ -9713,13 +9746,13 @@
         <v>139</v>
       </c>
       <c r="C85" t="s">
+        <v>683</v>
+      </c>
+      <c r="D85" t="s">
         <v>684</v>
       </c>
-      <c r="D85" t="s">
-        <v>685</v>
-      </c>
       <c r="E85" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F85" t="s">
         <v>136</v>
@@ -9737,16 +9770,16 @@
         <v>100</v>
       </c>
       <c r="C86" t="s">
+        <v>687</v>
+      </c>
+      <c r="D86" t="s">
         <v>688</v>
       </c>
-      <c r="D86" t="s">
-        <v>689</v>
-      </c>
       <c r="E86" t="s">
+        <v>576</v>
+      </c>
+      <c r="F86" t="s">
         <v>577</v>
-      </c>
-      <c r="F86" t="s">
-        <v>578</v>
       </c>
       <c r="I86" t="str">
         <f t="shared" si="2"/>
@@ -9761,16 +9794,16 @@
         <v>139</v>
       </c>
       <c r="C87" t="s">
+        <v>717</v>
+      </c>
+      <c r="D87" t="s">
         <v>718</v>
       </c>
-      <c r="D87" t="s">
-        <v>719</v>
-      </c>
       <c r="E87" t="s">
+        <v>715</v>
+      </c>
+      <c r="F87" t="s">
         <v>716</v>
-      </c>
-      <c r="F87" t="s">
-        <v>717</v>
       </c>
       <c r="I87" t="str">
         <f t="shared" si="2"/>
@@ -9785,16 +9818,16 @@
         <v>104</v>
       </c>
       <c r="C88" t="s">
+        <v>719</v>
+      </c>
+      <c r="D88" t="s">
         <v>720</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>721</v>
       </c>
-      <c r="E88" t="s">
-        <v>722</v>
-      </c>
       <c r="F88" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="G88">
         <v>5</v>
@@ -9812,16 +9845,16 @@
         <v>100</v>
       </c>
       <c r="C89" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D89" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E89" t="s">
+        <v>576</v>
+      </c>
+      <c r="F89" t="s">
         <v>577</v>
-      </c>
-      <c r="F89" t="s">
-        <v>578</v>
       </c>
       <c r="I89" t="str">
         <f t="shared" si="2"/>
@@ -9836,16 +9869,16 @@
         <v>104</v>
       </c>
       <c r="C90" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D90" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F90" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G90">
         <v>5</v>
@@ -9863,16 +9896,16 @@
         <v>100</v>
       </c>
       <c r="C91" t="s">
+        <v>737</v>
+      </c>
+      <c r="D91" t="s">
         <v>738</v>
       </c>
-      <c r="D91" t="s">
-        <v>739</v>
-      </c>
       <c r="E91" t="s">
+        <v>576</v>
+      </c>
+      <c r="F91" t="s">
         <v>577</v>
-      </c>
-      <c r="F91" t="s">
-        <v>578</v>
       </c>
       <c r="I91" t="str">
         <f t="shared" si="2"/>
@@ -9887,16 +9920,16 @@
         <v>139</v>
       </c>
       <c r="C92" t="s">
+        <v>760</v>
+      </c>
+      <c r="D92" t="s">
         <v>761</v>
       </c>
-      <c r="D92" t="s">
-        <v>762</v>
-      </c>
       <c r="E92" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F92" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I92" t="str">
         <f t="shared" si="2"/>
@@ -9911,13 +9944,13 @@
         <v>104</v>
       </c>
       <c r="C93" t="s">
+        <v>768</v>
+      </c>
+      <c r="D93" t="s">
         <v>769</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>770</v>
-      </c>
-      <c r="E93" t="s">
-        <v>771</v>
       </c>
       <c r="F93" t="s">
         <v>542</v>
@@ -9938,16 +9971,16 @@
         <v>100</v>
       </c>
       <c r="C94" t="s">
+        <v>786</v>
+      </c>
+      <c r="D94" t="s">
         <v>787</v>
       </c>
-      <c r="D94" t="s">
-        <v>788</v>
-      </c>
       <c r="E94" t="s">
+        <v>576</v>
+      </c>
+      <c r="F94" t="s">
         <v>577</v>
-      </c>
-      <c r="F94" t="s">
-        <v>578</v>
       </c>
       <c r="I94" t="str">
         <f t="shared" si="2"/>
@@ -9962,16 +9995,16 @@
         <v>139</v>
       </c>
       <c r="C95" t="s">
+        <v>813</v>
+      </c>
+      <c r="D95" t="s">
         <v>814</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
+        <v>811</v>
+      </c>
+      <c r="F95" t="s">
         <v>815</v>
-      </c>
-      <c r="E95" t="s">
-        <v>812</v>
-      </c>
-      <c r="F95" t="s">
-        <v>816</v>
       </c>
       <c r="I95" t="str">
         <f t="shared" si="2"/>
@@ -9986,16 +10019,16 @@
         <v>104</v>
       </c>
       <c r="C96" t="s">
+        <v>817</v>
+      </c>
+      <c r="D96" t="s">
         <v>818</v>
       </c>
-      <c r="D96" t="s">
-        <v>819</v>
-      </c>
       <c r="E96" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F96" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="G96">
         <v>5</v>
@@ -10013,16 +10046,16 @@
         <v>100</v>
       </c>
       <c r="C97" t="s">
+        <v>825</v>
+      </c>
+      <c r="D97" t="s">
         <v>826</v>
       </c>
-      <c r="D97" t="s">
-        <v>827</v>
-      </c>
       <c r="E97" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="F97" t="s">
         <v>577</v>
-      </c>
-      <c r="F97" t="s">
-        <v>578</v>
       </c>
       <c r="I97" t="str">
         <f t="shared" si="2"/>
@@ -10603,7 +10636,7 @@
         <v>365</v>
       </c>
       <c r="F18" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G18" t="s">
         <v>370</v>
@@ -10632,7 +10665,7 @@
         <v>327</v>
       </c>
       <c r="F19" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="G19" t="s">
         <v>400</v>
@@ -10835,7 +10868,7 @@
         <v>86</v>
       </c>
       <c r="F26" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>276</v>
@@ -10852,10 +10885,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C27" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D27" t="s">
         <v>207</v>
@@ -10864,13 +10897,13 @@
         <v>157</v>
       </c>
       <c r="F27" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G27" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="H27" t="s">
         <v>581</v>
-      </c>
-      <c r="H27" t="s">
-        <v>582</v>
       </c>
       <c r="I27">
         <v>35</v>
@@ -10881,7 +10914,7 @@
         <v>16</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C28" t="s">
         <v>281</v>
@@ -10893,13 +10926,13 @@
         <v>34</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="G28" t="s">
+        <v>621</v>
+      </c>
+      <c r="H28" t="s">
         <v>620</v>
-      </c>
-      <c r="G28" t="s">
-        <v>622</v>
-      </c>
-      <c r="H28" t="s">
-        <v>621</v>
       </c>
       <c r="I28">
         <v>10</v>
@@ -10910,10 +10943,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="C29" t="s">
         <v>661</v>
-      </c>
-      <c r="C29" t="s">
-        <v>662</v>
       </c>
       <c r="D29" t="s">
         <v>207</v>
@@ -10922,13 +10955,13 @@
         <v>101</v>
       </c>
       <c r="F29" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G29" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H29" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I29">
         <v>25</v>
@@ -10951,7 +10984,7 @@
         <v>53</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G30" t="s">
         <v>238</v>
@@ -10971,7 +11004,7 @@
         <v>218</v>
       </c>
       <c r="C31" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D31" t="s">
         <v>207</v>
@@ -10980,13 +11013,13 @@
         <v>169</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G31" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="H31" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I31">
         <v>24.99</v>
@@ -10997,10 +11030,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="C32" t="s">
         <v>744</v>
-      </c>
-      <c r="C32" t="s">
-        <v>745</v>
       </c>
       <c r="D32" t="s">
         <v>207</v>
@@ -11009,13 +11042,13 @@
         <v>20</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G32" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="H32" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I32">
         <v>10</v>
@@ -11038,7 +11071,7 @@
         <v>240</v>
       </c>
       <c r="F33" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>276</v>
@@ -11055,10 +11088,10 @@
         <v>35</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C34" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D34" t="s">
         <v>207</v>
@@ -11067,13 +11100,13 @@
         <v>102</v>
       </c>
       <c r="F34" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="G34" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="H34" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="I34">
         <v>27.95</v>
@@ -11084,10 +11117,10 @@
         <v>8</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C35" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D35" t="s">
         <v>207</v>
@@ -11096,13 +11129,13 @@
         <v>160</v>
       </c>
       <c r="F35" t="s">
+        <v>834</v>
+      </c>
+      <c r="G35" t="s">
         <v>835</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" s="10" t="s">
         <v>836</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>837</v>
       </c>
       <c r="I35">
         <v>19.989999999999998</v>
@@ -11113,10 +11146,10 @@
         <v>10</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C36" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D36" t="s">
         <v>207</v>
@@ -11125,13 +11158,13 @@
         <v>187</v>
       </c>
       <c r="F36" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="G36" t="s">
+        <v>835</v>
+      </c>
+      <c r="H36" s="10" t="s">
         <v>836</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>837</v>
       </c>
       <c r="I36">
         <v>19.989999999999998</v>
@@ -11152,9 +11185,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -11349,10 +11382,10 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
+        <v>600</v>
+      </c>
+      <c r="C17" t="s">
         <v>601</v>
-      </c>
-      <c r="C17" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -11363,7 +11396,7 @@
         <v>172</v>
       </c>
       <c r="C18" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -11371,10 +11404,10 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
+        <v>610</v>
+      </c>
+      <c r="C19" t="s">
         <v>611</v>
-      </c>
-      <c r="C19" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -11382,10 +11415,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>626</v>
+      </c>
+      <c r="C20" t="s">
         <v>627</v>
-      </c>
-      <c r="C20" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -11393,10 +11426,10 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
+        <v>623</v>
+      </c>
+      <c r="C21" t="s">
         <v>624</v>
-      </c>
-      <c r="C21" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -11404,10 +11437,10 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
+        <v>635</v>
+      </c>
+      <c r="C22" t="s">
         <v>636</v>
-      </c>
-      <c r="C22" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -11415,10 +11448,10 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C23" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -11426,7 +11459,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C24" t="s">
         <v>343</v>
@@ -11437,10 +11470,10 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
+        <v>643</v>
+      </c>
+      <c r="C25" t="s">
         <v>644</v>
-      </c>
-      <c r="C25" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -11448,10 +11481,10 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
+        <v>654</v>
+      </c>
+      <c r="C26" t="s">
         <v>655</v>
-      </c>
-      <c r="C26" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -11459,10 +11492,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C27" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -11470,10 +11503,10 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
+        <v>668</v>
+      </c>
+      <c r="C28" t="s">
         <v>669</v>
-      </c>
-      <c r="C28" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -11481,10 +11514,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C29" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
@@ -11492,10 +11525,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="C30" t="s">
         <v>673</v>
-      </c>
-      <c r="C30" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
@@ -11503,10 +11536,10 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>674</v>
+      </c>
+      <c r="C31" t="s">
         <v>675</v>
-      </c>
-      <c r="C31" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
@@ -11514,10 +11547,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
+        <v>685</v>
+      </c>
+      <c r="C32" t="s">
         <v>686</v>
-      </c>
-      <c r="C32" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -11525,10 +11558,10 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
+        <v>695</v>
+      </c>
+      <c r="C33" t="s">
         <v>696</v>
-      </c>
-      <c r="C33" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
@@ -11536,10 +11569,10 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
+        <v>697</v>
+      </c>
+      <c r="C34" t="s">
         <v>698</v>
-      </c>
-      <c r="C34" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
@@ -11547,10 +11580,10 @@
         <v>2</v>
       </c>
       <c r="B35" s="28" t="s">
+        <v>699</v>
+      </c>
+      <c r="C35" t="s">
         <v>700</v>
-      </c>
-      <c r="C35" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
@@ -11558,10 +11591,10 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
+        <v>726</v>
+      </c>
+      <c r="C36" t="s">
         <v>727</v>
-      </c>
-      <c r="C36" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
@@ -11569,10 +11602,10 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
+        <v>729</v>
+      </c>
+      <c r="C37" t="s">
         <v>730</v>
-      </c>
-      <c r="C37" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
@@ -11580,10 +11613,10 @@
         <v>33</v>
       </c>
       <c r="B38" t="s">
+        <v>766</v>
+      </c>
+      <c r="C38" t="s">
         <v>767</v>
-      </c>
-      <c r="C38" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
@@ -11591,10 +11624,10 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
+        <v>772</v>
+      </c>
+      <c r="C39" t="s">
         <v>773</v>
-      </c>
-      <c r="C39" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
@@ -11602,10 +11635,10 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
+        <v>793</v>
+      </c>
+      <c r="C40" t="s">
         <v>794</v>
-      </c>
-      <c r="C40" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
@@ -11613,10 +11646,10 @@
         <v>8</v>
       </c>
       <c r="B41" s="10" t="s">
+        <v>801</v>
+      </c>
+      <c r="C41" t="s">
         <v>802</v>
-      </c>
-      <c r="C41" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
@@ -11624,10 +11657,10 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C42" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
@@ -11635,10 +11668,10 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C43" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
@@ -11646,10 +11679,10 @@
         <v>35</v>
       </c>
       <c r="B44" s="10" t="s">
+        <v>809</v>
+      </c>
+      <c r="C44" t="s">
         <v>810</v>
-      </c>
-      <c r="C44" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
@@ -11657,10 +11690,10 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
+        <v>811</v>
+      </c>
+      <c r="C45" t="s">
         <v>812</v>
-      </c>
-      <c r="C45" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
@@ -11668,10 +11701,21 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C46" t="s">
-        <v>667</v>
+        <v>666</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>23</v>
+      </c>
+      <c r="B47" t="s">
+        <v>870</v>
+      </c>
+      <c r="C47" t="s">
+        <v>871</v>
       </c>
     </row>
   </sheetData>
@@ -16419,8 +16463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="87" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:K20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="87" workbookViewId="0">
+      <selection activeCell="K24" sqref="B24:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -16450,13 +16494,13 @@
         <v>300</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>301</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>302</v>
@@ -16465,10 +16509,10 @@
         <v>303</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.5">
@@ -16523,7 +16567,7 @@
         <v>DONE</v>
       </c>
       <c r="O2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.5">
@@ -17702,7 +17746,7 @@
       </c>
       <c r="J24">
         <f>_xlfn.IFNA(IF(VLOOKUP(B24,REFERANCES!A:A,1,FALSE),1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24">
         <f>IF(VLOOKUP(B24,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>

</xml_diff>

<commit_message>
feature rich grade conversion in real time based on quite complex logic, also auto tool tips for abbr tags
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB2AB95-4518-4CA3-B388-5BFAEEFA7432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165B2090-79BA-4500-A931-0535A7C20462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -4964,9 +4965,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M37" sqref="M37"/>
+      <selection pane="topRight" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -16463,8 +16464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="87" workbookViewId="0">
-      <selection activeCell="K24" sqref="B24:K24"/>
+    <sheetView topLeftCell="A13" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
added Amzkhssan wall climb
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D7207C-0331-4839-AA2C-81F200016A6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18838428-8D62-4383-AC15-32857A3555E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">REFERANCES!$A$1:$C$43</definedName>
   </definedNames>
   <calcPr calcId="181029" iterateDelta="0" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="915">
   <si>
     <t>cliff</t>
   </si>
@@ -3046,6 +3047,44 @@
   </si>
   <si>
     <t xml:space="preserve">A fantastic guidebook to the quartzite trad climbing around the Jebel el Kest and Jebel Taskra massifs and Tafraout Grabite. The book covers mostly multi-pitch climbs including some mountain routes over a kilometer long. This is a selective guide that describes 79 of the best crags, and offers comprehensive coverage of the key route or two on those crags. It covers the High Sierra climb in exceptional detail. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Pinnacle Slab starts about 10m right of the Amzkhssan Rib climb (graded V. Diff itself) which follows most obvious break up the middle of the wall. The goal is climb up to a small black overhang split by a crack, the climber passes this and heads up the wall to create a second anchor at the pinnacle, with the final pitch taking the easiest line through the steep overlap to the top. 
+&lt;br/&gt;
+&lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;50m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;Start 10m right of the main break and a meter or two left from the outcropping bulge at the base of the wall. Climb up the slabs as far as the rope and any rope drag will allow, until you reach a suitable belay. 
+&lt;br/&gt;
+&lt;strong class="pitch-title"&gt;Pitch 2 –&lt;span class="length"&gt;50m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;Continue up the slab heading to the obvious pinnacle not too far from the top of the wall. 
+&lt;br/&gt;
+&lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;There are a few options to get though the steeper overlap at the top. Take the easier line directly above the pinnacle to create the belay at the top of the wall. </t>
+  </si>
+  <si>
+    <t>29.84265,-9.02353</t>
+  </si>
+  <si>
+    <t>Morocco Rock offers great information for climbing on the Amzkhssan Wall. The descriptions and photography for his wall are both on the smaller side, but it’s still more than clear enough to get up the wall. The book overall also offers an incredible about of information on the routes and climbing in the Jebel El Kest.</t>
+  </si>
+  <si>
+    <t>The Amzkhssan Wall in Morocco offers easy rock climbing</t>
+  </si>
+  <si>
+    <t>img/topos/amzkhssan/amzkhssan-wall-pinnacle-slab-climb-morocco.jpg</t>
+  </si>
+  <si>
+    <t>The Amzkhssan Wall's Pinnacle Slab climb in Morocco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Pinnacle Slab on the Amzkhssan Wall offers around 130m of enjoyable climbing with little technical difficulty. The Amzkhssan Wall could be climbed hundreds of times without ever using the same holds. Although this particular route is only graded &lt;abbr title="Difficult"&gt;Diff&lt;/abbr&gt;, it should not be underestimated. Finding gear in the quartzite rock can be difficult and the leader can easily be enticed off the route in pursuit of placements, leading to serious rope drag quite quickly. In addition, route finding is more or less impossible to follow once on the wall. That said the climbing doesn’t go above V. Diff / Severe anywhere on the right side of the rock face. A confident leader with a mixed rack, particularly smaller gear, will be rewarded with enjoyable and easy climbing, an ideal option for a short warm up climb, especially given its easy approach and nearby parking. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Approach&lt;/strong&gt;: Parking can be found on the higher side of the nearest hairpin bend. There is space for 2 cars. From here it’s a short walk around the corner to the base of the Amzkhssan Wall.
+&lt;br /&gt;
+&lt;strong&gt;Descent&lt;/strong&gt;: From the summit move over the back and trend North West (left with your back to the climb). This will allow the climbers an easy scramble down to a path that moves around the west side of the wall bringing climbers back towards the road. </t>
+  </si>
+  <si>
+    <t>img/topos/amzkhssan/maps/</t>
+  </si>
+  <si>
+    <t>The location of the Amzkhssan Wall in the Jebel El Kest Mountains</t>
   </si>
 </sst>
 </file>
@@ -5090,9 +5129,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F42" sqref="F42"/>
+    <sheetView topLeftCell="B1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7906,7 +7945,7 @@
         <v>877</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C39" s="31">
         <v>38</v>
@@ -7924,7 +7963,7 @@
         <v>130</v>
       </c>
       <c r="H39" s="31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I39" s="31">
         <v>1</v>
@@ -7944,6 +7983,9 @@
       <c r="N39" s="31" t="s">
         <v>805</v>
       </c>
+      <c r="O39" s="31" t="s">
+        <v>906</v>
+      </c>
       <c r="P39" s="31">
         <v>5</v>
       </c>
@@ -7953,8 +7995,27 @@
       <c r="R39" s="31" t="s">
         <v>880</v>
       </c>
+      <c r="S39" s="31" t="s">
+        <v>911</v>
+      </c>
+      <c r="T39" s="32" t="s">
+        <v>912</v>
+      </c>
+      <c r="U39" s="32" t="s">
+        <v>905</v>
+      </c>
+      <c r="V39" s="31" t="s">
+        <v>150</v>
+      </c>
       <c r="W39" s="31" t="s">
         <v>151</v>
+      </c>
+      <c r="AF39" s="38">
+        <v>43806</v>
+      </c>
+      <c r="AG39" s="37">
+        <f>(AF39-DATE(1970,1,1))*86400</f>
+        <v>1575676800</v>
       </c>
     </row>
     <row r="40" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -8056,9 +8117,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0812394-7A25-4828-BAB3-74F65E9FB495}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C94" sqref="C94"/>
+      <selection pane="bottomLeft" activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9630,7 +9691,7 @@
         <v>576</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" ref="I65:I101" si="2">CONCATENATE(A65,B65)</f>
+        <f t="shared" ref="I65:I104" si="2">CONCATENATE(A65,B65)</f>
         <v>22map</v>
       </c>
     </row>
@@ -10523,6 +10584,81 @@
       <c r="I101" t="str">
         <f t="shared" si="2"/>
         <v>37map</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>38</v>
+      </c>
+      <c r="B102" t="s">
+        <v>138</v>
+      </c>
+      <c r="C102" t="s">
+        <v>886</v>
+      </c>
+      <c r="D102" t="s">
+        <v>908</v>
+      </c>
+      <c r="E102" t="s">
+        <v>724</v>
+      </c>
+      <c r="F102" t="s">
+        <v>135</v>
+      </c>
+      <c r="I102" t="str">
+        <f t="shared" si="2"/>
+        <v>38tile</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>38</v>
+      </c>
+      <c r="B103" t="s">
+        <v>103</v>
+      </c>
+      <c r="C103" t="s">
+        <v>909</v>
+      </c>
+      <c r="D103" t="s">
+        <v>910</v>
+      </c>
+      <c r="E103" t="s">
+        <v>724</v>
+      </c>
+      <c r="F103" t="s">
+        <v>135</v>
+      </c>
+      <c r="G103">
+        <v>5</v>
+      </c>
+      <c r="I103" t="str">
+        <f t="shared" si="2"/>
+        <v>38topo</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>38</v>
+      </c>
+      <c r="B104" t="s">
+        <v>99</v>
+      </c>
+      <c r="C104" t="s">
+        <v>913</v>
+      </c>
+      <c r="D104" t="s">
+        <v>914</v>
+      </c>
+      <c r="E104" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="F104" t="s">
+        <v>576</v>
+      </c>
+      <c r="I104" t="str">
+        <f t="shared" si="2"/>
+        <v>38map</v>
       </c>
     </row>
     <row r="113" spans="9:9" x14ac:dyDescent="0.45">
@@ -10565,18 +10701,19 @@
     <hyperlink ref="E21" r:id="rId7" xr:uid="{13D796E4-2DCC-423A-8465-6FBC7F8F9F51}"/>
     <hyperlink ref="E97" r:id="rId8" xr:uid="{D9B3E716-EB3F-4800-9BA6-F7CC27A4B929}"/>
     <hyperlink ref="E101" r:id="rId9" xr:uid="{100D2796-C308-4072-A193-26516BF1698F}"/>
+    <hyperlink ref="E104" r:id="rId10" xr:uid="{B966E3D2-A42D-4B1E-B741-5BF7C80D8894}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11721,6 +11858,35 @@
         <v>27.95</v>
       </c>
     </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>898</v>
+      </c>
+      <c r="C40" t="s">
+        <v>899</v>
+      </c>
+      <c r="D40" t="s">
+        <v>206</v>
+      </c>
+      <c r="E40">
+        <v>107</v>
+      </c>
+      <c r="F40" t="s">
+        <v>907</v>
+      </c>
+      <c r="G40" t="s">
+        <v>901</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>900</v>
+      </c>
+      <c r="I40">
+        <v>27.5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1" xr:uid="{14007672-E4E3-4A8F-8DD0-45E59BDCCEDC}"/>
@@ -11730,9 +11896,10 @@
     <hyperlink ref="H36" r:id="rId5" xr:uid="{F68D8C59-CEB7-45D1-A038-A5572E263335}"/>
     <hyperlink ref="H37" r:id="rId6" xr:uid="{D04069F0-0DAA-4A4C-A8AA-26AB11C3BD56}"/>
     <hyperlink ref="H38" r:id="rId7" xr:uid="{E4D07885-E59B-43A1-8072-9E773C85A997}"/>
+    <hyperlink ref="H40" r:id="rId8" xr:uid="{F25B0F60-BB7D-4EAD-838E-387765FC9868}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -12618,10 +12785,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745174B4-A8CA-45B8-ACCB-9B5B609F0D5D}">
-  <dimension ref="A1:V100"/>
+  <dimension ref="A1:V103"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView topLeftCell="A80" zoomScale="94" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17147,6 +17314,138 @@
       </c>
       <c r="N100" s="27">
         <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A101" s="12">
+        <v>38</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="C101" s="12">
+        <v>4</v>
+      </c>
+      <c r="D101" s="12">
+        <v>3</v>
+      </c>
+      <c r="E101" s="12">
+        <v>4</v>
+      </c>
+      <c r="F101" s="12">
+        <v>3</v>
+      </c>
+      <c r="G101" s="12">
+        <v>2</v>
+      </c>
+      <c r="H101" s="12">
+        <v>2</v>
+      </c>
+      <c r="I101" s="12">
+        <v>2</v>
+      </c>
+      <c r="J101" s="12">
+        <v>2</v>
+      </c>
+      <c r="K101" s="12">
+        <v>3</v>
+      </c>
+      <c r="L101" s="12">
+        <v>3</v>
+      </c>
+      <c r="M101" s="12">
+        <v>5</v>
+      </c>
+      <c r="N101" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A102" s="11">
+        <v>38</v>
+      </c>
+      <c r="B102" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C102" s="26">
+        <v>16.2</v>
+      </c>
+      <c r="D102" s="26">
+        <v>17.7</v>
+      </c>
+      <c r="E102" s="26">
+        <v>19.8</v>
+      </c>
+      <c r="F102" s="26">
+        <v>22.5</v>
+      </c>
+      <c r="G102" s="26">
+        <v>24.3</v>
+      </c>
+      <c r="H102" s="26">
+        <v>27.3</v>
+      </c>
+      <c r="I102" s="26">
+        <v>31.3</v>
+      </c>
+      <c r="J102" s="26">
+        <v>31.1</v>
+      </c>
+      <c r="K102" s="26">
+        <v>28</v>
+      </c>
+      <c r="L102" s="26">
+        <v>24.2</v>
+      </c>
+      <c r="M102" s="26">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="N102" s="26">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A103" s="13">
+        <v>38</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="C103" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="D103" s="27">
+        <v>3.7</v>
+      </c>
+      <c r="E103" s="27">
+        <v>6.7</v>
+      </c>
+      <c r="F103" s="27">
+        <v>9.1</v>
+      </c>
+      <c r="G103" s="27">
+        <v>11.5</v>
+      </c>
+      <c r="H103" s="27">
+        <v>13.9</v>
+      </c>
+      <c r="I103" s="27">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="J103" s="27">
+        <v>18</v>
+      </c>
+      <c r="K103" s="27">
+        <v>15.3</v>
+      </c>
+      <c r="L103" s="27">
+        <v>11.5</v>
+      </c>
+      <c r="M103" s="27">
+        <v>7.5</v>
+      </c>
+      <c r="N103" s="27">
+        <v>3.7</v>
       </c>
     </row>
   </sheetData>
@@ -17159,8 +17458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="87" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A21" zoomScale="87" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -19177,33 +19476,33 @@
       </c>
       <c r="C39" t="str">
         <f>CLIMBS!B39</f>
-        <v>draft</v>
+        <v>publish</v>
       </c>
       <c r="D39">
         <f>IF(CLIMBS!S39&lt;&gt;0,1,0)+IF(CLIMBS!G39&lt;&gt;0,1,0)+IF(CLIMBS!H39&lt;&gt;0,1,0)+IF(CLIMBS!I39&lt;&gt;0,1,0)+IF(CLIMBS!J39&lt;&gt;0,1,0)+IF(CLIMBS!O39&lt;&gt;0,1,0)+IF(CLIMBS!N39&lt;&gt;0,1,0)+IF(CLIMBS!P39&lt;&gt;0,1,0)+IF(CLIMBS!Q39&lt;&gt;0,1,0)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E39">
         <f>IF(CLIMBS!T39&lt;&gt;0,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F39" t="str">
+        <v>1</v>
+      </c>
+      <c r="F39">
         <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B39,"tile"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B39,"topo"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B39,"map"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
-        <v>missing</v>
+        <v>3</v>
       </c>
       <c r="G39">
         <f>SUMIFS(IMAGES!G:G,IMAGES!A:A,'to-do-score-card'!B39,IMAGES!B:B,"topo")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H39">
         <f>_xlfn.IFNA(IF(VLOOKUP(B39,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39">
         <f>_xlfn.IFNA(IF(VLOOKUP(B39,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39">
         <f>_xlfn.IFNA(IF(VLOOKUP(B39,REFERANCES!A:A,1,FALSE),1,0),0)</f>
@@ -19211,7 +19510,7 @@
       </c>
       <c r="K39">
         <f>IF(VLOOKUP(B39,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" s="25" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
added Donkey topo data
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F071E426-7DC9-42C8-9A8B-C412C9ACC208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F232BEFC-D0EC-4A6A-9120-6789D343531D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="924">
   <si>
     <t>cliff</t>
   </si>
@@ -3111,6 +3111,33 @@
   </si>
   <si>
     <t>Lower Eagle Crag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donkey Serenades takes the easiest line and obvious sweeping weakness up the more prominent part of the Lower Eagle Crag buttress. There are two possible starts and two different finishes depending which guidebook you use. The Oxford Alpine Club guide takes the easier start, which follows the first pitch of Pink Lady. There are also some options for variation throughout this multi-pitch climb.
+&lt;br/&gt;
+&lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;25m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;3b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Follow the broken right leading crack up to the ledge below the little overhang. From here head left up the easy slab to belay on one of the ledges. 
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 2 –&lt;span class="length"&gt;40m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;3c&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+There are a few options for getting to the so-called party time belay. The route takes the left side of the pillar and moves around to finish on the large ledge system. However, the climber could take the crack on the right side of the pillar in two pitches to follow Pink Lady graded &lt;abbr title="Very Severe"&gt;VS&lt;/abbr&gt; 4c. Alternatively the vegetated corner further right sill, follows the Real Men Wear Pink route, also VS. An additional option is to take the clean slab between these two VS lines for some exceptional climbing, with some decent gear options (not graded but also feels like VS). 
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Follow the right side of the broken slab above the party time belay ledge until reaching a steeper slab covered in black moss, usually in the shadow of the headwall. Build a traditional belay here.
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 4 –&lt;span class="length"&gt;25m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;3c&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Head up and slightly left on the black mossy slab. There are lots of options for climbing this wall. When approaching the top, look for one of the vertical blocks. Belays can be built around one of the blocks using slings and other gear. 
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 5 –&lt;span class="length"&gt;25m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Walk left along the ledge. The climber can follow the low-level crack higher up on the wall, or walk on a lower section. It’s possible to make this into a longer pitch. The 3 pitches (this pitch and the following 2 pitches) can be linked into 2 longer ones if required or if the climbers are short of time. 
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 6 –&lt;span class="length"&gt;25m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;3c&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Follow the steeper right, shady side of the next face. A belay can be created below the next headwall, or if linking pitches, aim to go all the way to the belay ledge below the now obvious, large pinnacle. 
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 7 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Move left towards the short ledges below the large pinnacle. Create an anchor here. Depending on the approach to the next pitch, create the belay further left or right if possible. 
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 8 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;3c&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+The Oxford Alpine guide suggests taking the route left and around the pinnacle, from the top of which the climber can scramble higher to build a final belay. The Morocco Rock guide suggests the climber should take the right grove around the right side of the pinnacle to reach the broken scramble above. A third option is to tackle the pinnacle directly for a much harder but much more impressive finish. The rock looks loose and very steep from below, but upon attacking the pinnacle directly the climber will be surprised to find the rock is solid and there are a number of good stances from which protection can be placed. The Donkey Direct finish is not listed in the guides but is likely not harder than VS and will offer the best possible end to the route if the climber is feeling unchallenged by the climbing up to that point. After building a belay on the ledges above to bring up the last of the party, then the climbers can scramble up to the summit paths without difficulty. </t>
   </si>
 </sst>
 </file>
@@ -5155,9 +5182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+      <selection pane="bottomLeft" activeCell="AF40" sqref="AF40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8105,6 +8132,9 @@
       <c r="T40" s="3" t="s">
         <v>917</v>
       </c>
+      <c r="U40" s="3" t="s">
+        <v>923</v>
+      </c>
       <c r="V40" t="s">
         <v>150</v>
       </c>
@@ -8112,11 +8142,11 @@
         <v>916</v>
       </c>
       <c r="AF40" s="39">
-        <v>43808</v>
+        <v>43810</v>
       </c>
       <c r="AG40" s="40">
         <f>(AF40-DATE(1970,1,1))*86400</f>
-        <v>1575849600</v>
+        <v>1576022400</v>
       </c>
     </row>
     <row r="41" spans="1:33" s="31" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -8161,7 +8191,7 @@
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D107" sqref="D107:F107"/>
+      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17708,7 +17738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="87" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="87" workbookViewId="0">
       <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
published old man of hoy
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896383D5-F36B-49A6-B612-408279AA2892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5C3CCB-62E7-4F50-87E4-833299602200}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1727" uniqueCount="952">
   <si>
     <t>cliff</t>
   </si>
@@ -2541,9 +2541,6 @@
 </t>
   </si>
   <si>
-    <t>Old man of Hoy</t>
-  </si>
-  <si>
     <t>img: Silvia Mazzani</t>
   </si>
   <si>
@@ -2708,9 +2705,6 @@
   </si>
   <si>
     <t>29.81270,-9.06676</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Souss-Massa</t>
   </si>
   <si>
     <t>https://issuu.com/oxfordalpineclub/docs/100cc_preview_reduced</t>
@@ -3082,9 +3076,6 @@
   </si>
   <si>
     <t>Lower Eagle Crag in the Anti-Atlas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Lower Eagle Crag in the Jebel El Kest mountain range offers some of the best rock climbing in the anti-atlas. The rock climbing is clean and the quartzite is generally very solid. Many routes ascend to around 300m with grades starting from V. Diff, like this classic route, Donkey Serenades. Pink Lady and Real Men wear Pink are nearby &lt;abbr title="Very Severe"&gt;VS&lt;/abbr&gt; climbs. Sir Chris Bonington’s climb, Black Beauty offers an exceptional E1 climb further down the crag. Routes from the Lower Eagle Crag can also be linked up with routes on the shorter Upper Eagle Crag for extended adventures. The Route Donkey Serenades covered here, weaves its way up the north facing slabs, making use of the natural breaks and slopes in the rock to reach the top. There is little technical difficulty (depending of which line you take), but it does require solid mountaineering experience because all anchors need to be built from trad gear. Many of the pitches will be in the shade until later in the afternoon, giving a shadier option if you want to avoid the worst of the Morocco sun. </t>
   </si>
   <si>
     <t>NE</t>
@@ -3138,6 +3129,101 @@
   </si>
   <si>
     <t>Its possible to park at Ristorante Pian Schiavaneis (46.503278,11.802140). From there, head North and slightly East to Sass Pordoi. Start 50m left of the prominent black streak, directly below the huge boulder on the upper ledge. Climb easy scree and rocks to a scree basin where the climb starts.</t>
+  </si>
+  <si>
+    <t>The Lower Eagle Crag in the Jebel El Kest mountain range offers some of the best rock climbing in the anti-atlas. The rock climbing is clean and the quartzite is generally very solid. Many routes ascend to around 300m with grades starting from V. Diff, like this classic route, Donkey Serenades. Pink Lady and Real Men wear Pink are nearby &lt;abbr title="Very Severe"&gt;VS&lt;/abbr&gt; climbs. Sir Chris Bonington’s climb, Black Beauty offers an exceptional E1 climb further down the crag. Routes from the Lower Eagle Crag can also be linked up with routes on the shorter Upper Eagle Crag for extended adventures. The route Donkey Serenades covered here, weaves its way up the north facing slabs, making use of the natural breaks and slopes in the rock to reach the top. There is little technical difficulty (depending of which line you take), but it does require solid mountaineering experience because all anchors need to be built from trad gear. Many of the pitches will be in the shade until later in the afternoon, giving a shadier option if you want to avoid the worst of the Morocco sun.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morocco Rock is a quality guidebook and one of the original for the region. The imagery and description are clear and the book contains an incredible number of routes in all key trad climbing areas. The guide covers climbing graded from Diff up to E6. The guide covers the whole Eagle Rock section and specifically the climb Donkey Serenades in good detail. The route in this guide shows a start further left (East) on the crag graded 4a. I also has finish that takes the right side of the final pinnacle.  The book is great value for money but not as well organised as The Oxford Alpine club books for this region. </t>
+  </si>
+  <si>
+    <t>58.8836982,-3.4304736</t>
+  </si>
+  <si>
+    <t>Orkney</t>
+  </si>
+  <si>
+    <t>https://www.independent.co.uk/news/uk/home-news/jesse-dufton-blind-climber-record-orkney-old-man-hoy-sheer-cliff-a8949946.html</t>
+  </si>
+  <si>
+    <t>https://www.ukclimbing.com/articles/destinations/the_old_man_of_hoy-69</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/paul_stephenson/5927357279</t>
+  </si>
+  <si>
+    <t>originl: Paul Stephenson</t>
+  </si>
+  <si>
+    <t>The Old Man of Hoy Rock Climbing Stack</t>
+  </si>
+  <si>
+    <t>img/topos/hoy/the-original-route-on-the-old-man-of-hoy-stack.jpg</t>
+  </si>
+  <si>
+    <t>img/tiles/old-man-of-hoy-climb.jpg</t>
+  </si>
+  <si>
+    <t>Old Man of Hoy</t>
+  </si>
+  <si>
+    <t>E1 5b</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wNzUtvy0lsI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Ruvzhhg_B-s</t>
+  </si>
+  <si>
+    <t>Video: Catherine Destivelle soloing The Old Man of Hoy</t>
+  </si>
+  <si>
+    <t>Video: BBC documentry from 1992 focused on The Old Man of Hoy</t>
+  </si>
+  <si>
+    <t>Climb Info: Climbs on The Old Man of Hoy</t>
+  </si>
+  <si>
+    <t>Souss-Massa</t>
+  </si>
+  <si>
+    <t>https://www.ukclimbing.com/articles/features/the_blind_man_of_hoy-5602</t>
+  </si>
+  <si>
+    <t>Article: Blind Man Leads Old Man of Hoy</t>
+  </si>
+  <si>
+    <t>https://www.thebmc.co.uk/eight-year-old-climbed-old-man-of-hoy-receives-award</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article: 8 year old climbs Old Man of Hoy for charity </t>
+  </si>
+  <si>
+    <t>Article: The Blind Man of Hoy</t>
+  </si>
+  <si>
+    <t>The Original Route up The Old Man of Hoy is a classic climb amongst classic climbs. Originally climbed in 1966 by Rusty Baillie, Chris Bonington and Tom Patey, this iconic multi-pitch has been the centre of some of the most focused media attention around climbing in the late 1990’s. The route climbs the east landward face, of this northern Scottish sandstone stack. It’s technically not a sea stack (because it’s attached to the mainland), but is usually referred to as such. The route requires a mix of technical climbing, including a short down climb, a traverse, as well as crack climbing and bridging skills. The route is made harder by nesting Fulmars who don’t like climbers around their nests. Decent from the top requires abseiling back down the route. The Original Route is listed in Ken Wilsons Hard Rock book, sitting alongside other UK classics in the &lt;abbr title="Very Severe"&gt;HVS&lt;/abbr&gt; to &lt;abbr title="Extremely Severe"&gt;E1&lt;/abbr&gt; range. The route has seen some incredible accents over the year including being climbed by Red Szell as the first blind man to climb up The Old Man of Hoy and in more decent years Jesse Dufton, also blind, climbed it on lead. Chris Bonington also made recent repeat of this stack, now in his 80’s, over 50 years after his first accent. He climbed the stack with Leo Holding this time. The climb was originally graded HVS but most recent guidebooks list it as E1. Although some pitches are straightforward, it would be easy to underestimate the complexity of getting up and back down safely. The exposure is incredible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Approach&lt;/strong&gt;: Head up the hill behind Rackwick Hostel until reaching the cottage at the top from which a well-constructed path will lead to the viewing promontory across from the Old Man of Hoy. Head North 120m from here and take the small well-worn path down to the rubble scramble to the stack at the base. 
+&lt;/p&gt;&lt;p&gt;
+&lt;strong&gt;Descent&lt;/strong&gt;: There are two options for descent. The first is to abseil each pitch. Typically, there will be slings left behind to rap from at each anchor point. The climber should come prepared to replace them if they are not in a suitable condition. There is also sometimes a rope in situ to help with the pitch two traverse. If the party is not using 60m ropes, and there is not a rope in situ on pitch two, then climbers should be prepared to leave a spare rope behind on ascent, in order to facilitate the descent here. Alternatively, if the party is using a pair of 60m ropes, these can be used to rappel to the end of pitch 3. Then a short rappel to the end of pitch two. Then a longer rappel, free hanging, should take the climbers to the base of the stack. It should go without saying, but climbers should have a pair of prusik cords during the abseil. One to back up the abseil, the other in case the climber needs to ascend the rope for some reason. </t>
+  </si>
+  <si>
+    <t>Old man of Hoy Located on the Isle of Hoy</t>
+  </si>
+  <si>
+    <t>img/topos/hoy/maps/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/p300njb/43950216932</t>
+  </si>
+  <si>
+    <t>originl: Rab Lawrence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An extensive and well-made guidebook covering every worthwhile crag in Northern Scotland. The guides are clear with generally very good photography. The climb on the Old Man of Hoy has a good amount of detail. The guide also covers key Scottish sea stacks like The Old Man of Stoer and Am Buachaille. A guide that comes highly recomended. </t>
   </si>
 </sst>
 </file>
@@ -4116,7 +4202,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5182,9 +5268,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T7" sqref="T7"/>
+    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5246,10 +5332,10 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>10</v>
@@ -5282,7 +5368,7 @@
         <v>16</v>
       </c>
       <c r="X1" s="29" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="Y1" s="29" t="s">
         <v>570</v>
@@ -5347,10 +5433,10 @@
         <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M2" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="N2" t="s">
         <v>24</v>
@@ -5365,7 +5451,7 @@
         <v>3</v>
       </c>
       <c r="R2" t="s">
-        <v>26</v>
+        <v>586</v>
       </c>
       <c r="S2" t="s">
         <v>472</v>
@@ -5428,16 +5514,16 @@
         <v>35</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M3" s="31" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="N3" s="31" t="s">
         <v>36</v>
       </c>
       <c r="O3" s="31" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="P3" s="31">
         <v>10</v>
@@ -5483,7 +5569,7 @@
     </row>
     <row r="4" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B4" t="s">
         <v>95</v>
@@ -5516,10 +5602,10 @@
         <v>177</v>
       </c>
       <c r="L4" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M4" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="N4" t="s">
         <v>44</v>
@@ -5587,7 +5673,7 @@
         <v>53</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="M5" s="31" t="s">
         <v>54</v>
@@ -5670,10 +5756,10 @@
         <v>35</v>
       </c>
       <c r="L6" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M6" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="N6" t="s">
         <v>63</v>
@@ -5750,7 +5836,7 @@
         <v>72</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="M7" s="31" t="s">
         <v>73</v>
@@ -5774,7 +5860,7 @@
         <v>77</v>
       </c>
       <c r="T7" s="31" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="V7" s="31" t="s">
         <v>38</v>
@@ -5824,10 +5910,10 @@
         <v>597</v>
       </c>
       <c r="L8" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M8" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="N8" t="s">
         <v>44</v>
@@ -5845,13 +5931,13 @@
         <v>46</v>
       </c>
       <c r="S8" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="T8" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="V8" t="s">
         <v>149</v>
@@ -5899,10 +5985,10 @@
         <v>72</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M9" s="31" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="N9" s="31" t="s">
         <v>36</v>
@@ -5920,10 +6006,10 @@
         <v>37</v>
       </c>
       <c r="S9" s="31" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="T9" s="31" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="V9" s="31" t="s">
         <v>149</v>
@@ -5984,10 +6070,10 @@
         <v>53</v>
       </c>
       <c r="L10" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="M10" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="N10" t="s">
         <v>440</v>
@@ -6050,10 +6136,10 @@
         <v>35</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M11" s="31" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="N11" s="31" t="s">
         <v>36</v>
@@ -6071,7 +6157,7 @@
         <v>92</v>
       </c>
       <c r="S11" s="31" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="T11" s="31" t="s">
         <v>93</v>
@@ -6131,10 +6217,10 @@
         <v>23</v>
       </c>
       <c r="L12" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M12" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="N12" t="s">
         <v>24</v>
@@ -6199,7 +6285,7 @@
         <v>23</v>
       </c>
       <c r="L13" s="31" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="M13" s="31" t="s">
         <v>167</v>
@@ -6220,10 +6306,10 @@
         <v>169</v>
       </c>
       <c r="S13" s="34" t="s">
+        <v>771</v>
+      </c>
+      <c r="T13" s="35" t="s">
         <v>772</v>
-      </c>
-      <c r="T13" s="35" t="s">
-        <v>773</v>
       </c>
       <c r="U13" s="35" t="s">
         <v>638</v>
@@ -6281,10 +6367,10 @@
         <v>177</v>
       </c>
       <c r="L14" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M14" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="N14" t="s">
         <v>63</v>
@@ -6349,10 +6435,10 @@
         <v>35</v>
       </c>
       <c r="L15" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M15" s="31" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="N15" s="31" t="s">
         <v>36</v>
@@ -6430,7 +6516,7 @@
         <v>177</v>
       </c>
       <c r="L16" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="M16" s="5">
         <v>5.8</v>
@@ -6451,10 +6537,10 @@
         <v>224</v>
       </c>
       <c r="S16" t="s">
+        <v>773</v>
+      </c>
+      <c r="T16" s="3" t="s">
         <v>774</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>775</v>
       </c>
       <c r="V16" t="s">
         <v>38</v>
@@ -6501,10 +6587,10 @@
         <v>35</v>
       </c>
       <c r="L17" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M17" s="31" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="N17" s="31" t="s">
         <v>44</v>
@@ -6657,10 +6743,10 @@
         <v>533</v>
       </c>
       <c r="L19" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="N19" s="31" t="s">
         <v>36</v>
@@ -6731,7 +6817,7 @@
         <v>72</v>
       </c>
       <c r="L20" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="M20" s="5">
         <v>5.7</v>
@@ -6806,10 +6892,10 @@
         <v>35</v>
       </c>
       <c r="L21" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="N21" s="31" t="s">
         <v>63</v>
@@ -6830,7 +6916,7 @@
         <v>745</v>
       </c>
       <c r="T21" s="32" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="U21" s="32" t="s">
         <v>754</v>
@@ -6891,10 +6977,10 @@
         <v>321</v>
       </c>
       <c r="L22" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M22" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="N22" t="s">
         <v>409</v>
@@ -6959,10 +7045,10 @@
         <v>53</v>
       </c>
       <c r="L23" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M23" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="N23" s="31" t="s">
         <v>166</v>
@@ -7037,7 +7123,7 @@
         <v>23</v>
       </c>
       <c r="L24" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="M24" t="s">
         <v>464</v>
@@ -7061,7 +7147,7 @@
         <v>465</v>
       </c>
       <c r="T24" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="V24" t="s">
         <v>185</v>
@@ -7108,7 +7194,7 @@
         <v>53</v>
       </c>
       <c r="L25" s="31" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="M25" s="31" t="s">
         <v>480</v>
@@ -7132,7 +7218,7 @@
         <v>490</v>
       </c>
       <c r="T25" s="35" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="U25" s="34"/>
       <c r="V25" s="31" t="s">
@@ -7194,7 +7280,7 @@
         <v>177</v>
       </c>
       <c r="L26" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M26" t="s">
         <v>518</v>
@@ -7218,7 +7304,7 @@
         <v>529</v>
       </c>
       <c r="T26" s="14" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="U26" s="2"/>
       <c r="V26" t="s">
@@ -7270,7 +7356,7 @@
         <v>72</v>
       </c>
       <c r="L27" s="31" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="M27" s="31" t="s">
         <v>73</v>
@@ -7294,7 +7380,7 @@
         <v>534</v>
       </c>
       <c r="T27" s="35" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="U27" s="34"/>
       <c r="V27" s="31" t="s">
@@ -7356,7 +7442,7 @@
         <v>35</v>
       </c>
       <c r="L28" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="M28" t="s">
         <v>590</v>
@@ -7414,7 +7500,7 @@
         <v>177</v>
       </c>
       <c r="L29" s="31" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="M29" s="31" t="s">
         <v>464</v>
@@ -7438,7 +7524,7 @@
         <v>610</v>
       </c>
       <c r="T29" s="35" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="W29" s="33"/>
       <c r="X29" s="33">
@@ -7487,10 +7573,10 @@
         <v>35</v>
       </c>
       <c r="L30" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M30" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="N30" t="s">
         <v>36</v>
@@ -7565,10 +7651,10 @@
         <v>72</v>
       </c>
       <c r="L31" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M31" s="31" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="N31" s="31" t="s">
         <v>36</v>
@@ -7589,7 +7675,7 @@
         <v>687</v>
       </c>
       <c r="T31" s="32" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="U31" s="32" t="s">
         <v>688</v>
@@ -7668,7 +7754,7 @@
         <v>35</v>
       </c>
       <c r="L33" s="31" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M33" s="31" t="s">
         <v>711</v>
@@ -7692,7 +7778,7 @@
         <v>722</v>
       </c>
       <c r="T33" s="32" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="W33" s="33" t="s">
         <v>39</v>
@@ -7717,7 +7803,7 @@
     </row>
     <row r="34" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B34" t="s">
         <v>95</v>
@@ -7732,7 +7818,7 @@
         <v>532</v>
       </c>
       <c r="F34" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G34">
         <v>720</v>
@@ -7750,16 +7836,16 @@
         <v>393</v>
       </c>
       <c r="L34" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="M34" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="N34" t="s">
         <v>74</v>
       </c>
       <c r="O34" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="P34">
         <v>60</v>
@@ -7771,10 +7857,10 @@
         <v>76</v>
       </c>
       <c r="S34" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="T34" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="W34" s="30" t="s">
         <v>150</v>
@@ -7792,10 +7878,10 @@
     </row>
     <row r="35" spans="1:33" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="31" t="s">
-        <v>755</v>
+        <v>932</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C35" s="31">
         <v>34</v>
@@ -7803,22 +7889,82 @@
       <c r="D35" s="31" t="s">
         <v>18</v>
       </c>
+      <c r="E35" s="31" t="s">
+        <v>924</v>
+      </c>
+      <c r="F35" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="31">
+        <v>137</v>
+      </c>
+      <c r="H35" s="31">
+        <v>5</v>
+      </c>
+      <c r="I35" s="31">
+        <v>7</v>
+      </c>
+      <c r="J35" s="31" t="s">
+        <v>360</v>
+      </c>
+      <c r="K35" s="31" t="s">
+        <v>321</v>
+      </c>
       <c r="L35" s="31" t="s">
-        <v>848</v>
-      </c>
-      <c r="W35" s="33"/>
-      <c r="X35" s="33"/>
-      <c r="Y35" s="33"/>
+        <v>846</v>
+      </c>
+      <c r="M35" s="31" t="s">
+        <v>933</v>
+      </c>
+      <c r="N35" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="O35" s="31" t="s">
+        <v>923</v>
+      </c>
+      <c r="P35" s="31">
+        <v>45</v>
+      </c>
+      <c r="Q35" s="31">
+        <v>2</v>
+      </c>
+      <c r="R35" s="31" t="s">
+        <v>586</v>
+      </c>
+      <c r="S35" s="31" t="s">
+        <v>945</v>
+      </c>
+      <c r="T35" s="32" t="s">
+        <v>946</v>
+      </c>
+      <c r="W35" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="X35" s="33">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="33">
+        <v>1</v>
+      </c>
       <c r="Z35" s="33"/>
-      <c r="AA35" s="33"/>
+      <c r="AA35" s="33">
+        <v>1</v>
+      </c>
       <c r="AB35" s="33"/>
       <c r="AC35" s="33"/>
       <c r="AD35" s="33"/>
       <c r="AE35" s="33"/>
+      <c r="AF35" s="38">
+        <v>43814</v>
+      </c>
+      <c r="AG35" s="37">
+        <f>(AF35-DATE(1970,1,1))*86400</f>
+        <v>1576368000</v>
+      </c>
     </row>
     <row r="36" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B36" t="s">
         <v>95</v>
@@ -7827,13 +7973,13 @@
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E36" s="41" t="s">
-        <v>805</v>
+        <v>939</v>
       </c>
       <c r="F36" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="G36">
         <v>120</v>
@@ -7851,16 +7997,16 @@
         <v>35</v>
       </c>
       <c r="L36" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M36" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="N36" t="s">
+        <v>802</v>
+      </c>
+      <c r="O36" t="s">
         <v>803</v>
-      </c>
-      <c r="O36" t="s">
-        <v>804</v>
       </c>
       <c r="P36">
         <v>10</v>
@@ -7872,13 +8018,13 @@
         <v>179</v>
       </c>
       <c r="S36" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="U36" s="3" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="V36" t="s">
         <v>185</v>
@@ -7897,7 +8043,7 @@
     </row>
     <row r="37" spans="1:33" s="31" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="31" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B37" s="31" t="s">
         <v>96</v>
@@ -7909,12 +8055,12 @@
         <v>18</v>
       </c>
       <c r="L37" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="38" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="B38" t="s">
         <v>95</v>
@@ -7923,13 +8069,13 @@
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E38" t="s">
+        <v>869</v>
+      </c>
+      <c r="F38" t="s">
         <v>871</v>
-      </c>
-      <c r="F38" t="s">
-        <v>873</v>
       </c>
       <c r="G38">
         <v>120</v>
@@ -7947,16 +8093,16 @@
         <v>23</v>
       </c>
       <c r="L38" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M38" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="N38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="O38" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="P38">
         <v>15</v>
@@ -7968,13 +8114,13 @@
         <v>37</v>
       </c>
       <c r="S38" t="s">
+        <v>886</v>
+      </c>
+      <c r="T38" s="3" t="s">
         <v>888</v>
       </c>
-      <c r="T38" s="3" t="s">
-        <v>890</v>
-      </c>
       <c r="U38" s="3" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="V38" t="s">
         <v>149</v>
@@ -7995,7 +8141,7 @@
     </row>
     <row r="39" spans="1:33" s="31" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="31" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>95</v>
@@ -8004,13 +8150,13 @@
         <v>38</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F39" s="31" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="G39" s="31">
         <v>130</v>
@@ -8028,16 +8174,16 @@
         <v>393</v>
       </c>
       <c r="L39" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M39" s="31" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="N39" s="31" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="O39" s="31" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="P39" s="31">
         <v>5</v>
@@ -8046,16 +8192,16 @@
         <v>1</v>
       </c>
       <c r="R39" s="31" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="S39" s="31" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="T39" s="32" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="U39" s="32" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="V39" s="31" t="s">
         <v>149</v>
@@ -8073,7 +8219,7 @@
     </row>
     <row r="40" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="B40" t="s">
         <v>95</v>
@@ -8082,13 +8228,13 @@
         <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E40" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F40" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="G40">
         <v>270</v>
@@ -8106,16 +8252,16 @@
         <v>533</v>
       </c>
       <c r="L40" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="M40" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="N40" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="O40" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="P40">
         <v>15</v>
@@ -8124,22 +8270,22 @@
         <v>1</v>
       </c>
       <c r="R40" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="S40" t="s">
-        <v>914</v>
+        <v>921</v>
       </c>
       <c r="T40" s="3" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="U40" s="3" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="V40" t="s">
         <v>149</v>
       </c>
       <c r="W40" s="30" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="AF40" s="39">
         <v>43810</v>
@@ -8191,7 +8337,7 @@
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
+      <selection pane="bottomLeft" activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8386,7 +8532,7 @@
         <v>116</v>
       </c>
       <c r="D8" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E8" t="s">
         <v>114</v>
@@ -8413,7 +8559,7 @@
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -8611,10 +8757,10 @@
         <v>102</v>
       </c>
       <c r="C18" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="D18" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="E18" t="s">
         <v>723</v>
@@ -8686,16 +8832,16 @@
         <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D21" t="s">
         <v>133</v>
       </c>
       <c r="E21" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="F21" t="s">
         <v>795</v>
-      </c>
-      <c r="F21" t="s">
-        <v>796</v>
       </c>
       <c r="G21">
         <v>5</v>
@@ -9481,16 +9627,16 @@
         <v>102</v>
       </c>
       <c r="C54" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="D54" t="s">
         <v>392</v>
       </c>
       <c r="E54" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="F54" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="G54">
         <v>5</v>
@@ -9763,7 +9909,7 @@
         <v>575</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" ref="I65:I107" si="2">CONCATENATE(A65,B65)</f>
+        <f t="shared" ref="I65:I110" si="2">CONCATENATE(A65,B65)</f>
         <v>22map</v>
       </c>
     </row>
@@ -9991,7 +10137,7 @@
         <v>102</v>
       </c>
       <c r="C75" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D75" t="s">
         <v>541</v>
@@ -10417,16 +10563,16 @@
         <v>137</v>
       </c>
       <c r="C92" t="s">
+        <v>757</v>
+      </c>
+      <c r="D92" t="s">
         <v>758</v>
       </c>
-      <c r="D92" t="s">
-        <v>759</v>
-      </c>
       <c r="E92" s="10" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F92" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="I92" t="str">
         <f t="shared" si="2"/>
@@ -10441,13 +10587,13 @@
         <v>102</v>
       </c>
       <c r="C93" t="s">
+        <v>765</v>
+      </c>
+      <c r="D93" t="s">
         <v>766</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>767</v>
-      </c>
-      <c r="E93" t="s">
-        <v>768</v>
       </c>
       <c r="F93" t="s">
         <v>540</v>
@@ -10468,10 +10614,10 @@
         <v>98</v>
       </c>
       <c r="C94" t="s">
+        <v>783</v>
+      </c>
+      <c r="D94" t="s">
         <v>784</v>
-      </c>
-      <c r="D94" t="s">
-        <v>785</v>
       </c>
       <c r="E94" t="s">
         <v>574</v>
@@ -10492,16 +10638,16 @@
         <v>137</v>
       </c>
       <c r="C95" t="s">
+        <v>808</v>
+      </c>
+      <c r="D95" t="s">
+        <v>809</v>
+      </c>
+      <c r="E95" t="s">
+        <v>806</v>
+      </c>
+      <c r="F95" t="s">
         <v>810</v>
-      </c>
-      <c r="D95" t="s">
-        <v>811</v>
-      </c>
-      <c r="E95" t="s">
-        <v>808</v>
-      </c>
-      <c r="F95" t="s">
-        <v>812</v>
       </c>
       <c r="I95" t="str">
         <f t="shared" si="2"/>
@@ -10516,16 +10662,16 @@
         <v>102</v>
       </c>
       <c r="C96" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D96" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="E96" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="F96" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="G96">
         <v>5</v>
@@ -10543,10 +10689,10 @@
         <v>98</v>
       </c>
       <c r="C97" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="D97" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>574</v>
@@ -10567,10 +10713,10 @@
         <v>137</v>
       </c>
       <c r="C98" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="D98" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="E98" t="s">
         <v>723</v>
@@ -10591,10 +10737,10 @@
         <v>137</v>
       </c>
       <c r="C99" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="D99" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="E99" t="s">
         <v>723</v>
@@ -10615,10 +10761,10 @@
         <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="D100" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="E100" t="s">
         <v>723</v>
@@ -10642,10 +10788,10 @@
         <v>98</v>
       </c>
       <c r="C101" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="D101" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E101" s="10" t="s">
         <v>574</v>
@@ -10666,10 +10812,10 @@
         <v>137</v>
       </c>
       <c r="C102" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="D102" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E102" t="s">
         <v>723</v>
@@ -10690,10 +10836,10 @@
         <v>102</v>
       </c>
       <c r="C103" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="D103" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="E103" t="s">
         <v>723</v>
@@ -10717,10 +10863,10 @@
         <v>98</v>
       </c>
       <c r="C104" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="D104" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="E104" s="10" t="s">
         <v>574</v>
@@ -10741,10 +10887,10 @@
         <v>137</v>
       </c>
       <c r="C105" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="D105" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E105" t="s">
         <v>723</v>
@@ -10765,10 +10911,10 @@
         <v>102</v>
       </c>
       <c r="C106" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="D106" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="E106" t="s">
         <v>723</v>
@@ -10792,10 +10938,10 @@
         <v>98</v>
       </c>
       <c r="C107" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="D107" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="E107" s="10" t="s">
         <v>574</v>
@@ -10806,6 +10952,81 @@
       <c r="I107" t="str">
         <f t="shared" si="2"/>
         <v>39map</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>34</v>
+      </c>
+      <c r="B108" t="s">
+        <v>137</v>
+      </c>
+      <c r="C108" t="s">
+        <v>931</v>
+      </c>
+      <c r="D108" t="s">
+        <v>929</v>
+      </c>
+      <c r="E108" t="s">
+        <v>949</v>
+      </c>
+      <c r="F108" t="s">
+        <v>950</v>
+      </c>
+      <c r="I108" t="str">
+        <f t="shared" si="2"/>
+        <v>34tile</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>34</v>
+      </c>
+      <c r="B109" t="s">
+        <v>102</v>
+      </c>
+      <c r="C109" t="s">
+        <v>930</v>
+      </c>
+      <c r="D109" t="s">
+        <v>929</v>
+      </c>
+      <c r="E109" t="s">
+        <v>927</v>
+      </c>
+      <c r="F109" t="s">
+        <v>928</v>
+      </c>
+      <c r="G109">
+        <v>4</v>
+      </c>
+      <c r="I109" t="str">
+        <f t="shared" si="2"/>
+        <v>34topo</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>34</v>
+      </c>
+      <c r="B110" t="s">
+        <v>98</v>
+      </c>
+      <c r="C110" t="s">
+        <v>948</v>
+      </c>
+      <c r="D110" t="s">
+        <v>947</v>
+      </c>
+      <c r="E110" s="10" t="s">
+        <v>574</v>
+      </c>
+      <c r="F110" t="s">
+        <v>575</v>
+      </c>
+      <c r="I110" t="str">
+        <f t="shared" si="2"/>
+        <v>34map</v>
       </c>
     </row>
     <row r="113" spans="9:9" x14ac:dyDescent="0.45">
@@ -10850,18 +11071,19 @@
     <hyperlink ref="E101" r:id="rId9" xr:uid="{100D2796-C308-4072-A193-26516BF1698F}"/>
     <hyperlink ref="E104" r:id="rId10" xr:uid="{B966E3D2-A42D-4B1E-B741-5BF7C80D8894}"/>
     <hyperlink ref="E107" r:id="rId11" xr:uid="{EED9F4AD-44D3-4EB4-BE7F-A87AA21B96A6}"/>
+    <hyperlink ref="E110" r:id="rId12" xr:uid="{80395FA3-9005-4540-BB40-1F4F5512E758}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11414,7 +11636,7 @@
         <v>327</v>
       </c>
       <c r="F19" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="G19" t="s">
         <v>398</v>
@@ -11820,7 +12042,7 @@
         <v>240</v>
       </c>
       <c r="F33" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>274</v>
@@ -11837,10 +12059,10 @@
         <v>35</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="C34" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="D34" t="s">
         <v>205</v>
@@ -11849,13 +12071,13 @@
         <v>102</v>
       </c>
       <c r="F34" t="s">
+        <v>815</v>
+      </c>
+      <c r="G34" t="s">
         <v>817</v>
       </c>
-      <c r="G34" t="s">
-        <v>819</v>
-      </c>
       <c r="H34" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="I34">
         <v>27.95</v>
@@ -11866,10 +12088,10 @@
         <v>8</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C35" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D35" t="s">
         <v>205</v>
@@ -11878,13 +12100,13 @@
         <v>160</v>
       </c>
       <c r="F35" t="s">
+        <v>827</v>
+      </c>
+      <c r="G35" t="s">
+        <v>828</v>
+      </c>
+      <c r="H35" s="10" t="s">
         <v>829</v>
-      </c>
-      <c r="G35" t="s">
-        <v>830</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>831</v>
       </c>
       <c r="I35">
         <v>19.989999999999998</v>
@@ -11895,10 +12117,10 @@
         <v>10</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C36" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D36" t="s">
         <v>205</v>
@@ -11907,13 +12129,13 @@
         <v>187</v>
       </c>
       <c r="F36" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="G36" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="I36">
         <v>19.989999999999998</v>
@@ -11924,10 +12146,10 @@
         <v>14</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C37" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D37" t="s">
         <v>205</v>
@@ -11936,13 +12158,13 @@
         <v>261</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="G37" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="I37">
         <v>19.989999999999998</v>
@@ -11953,10 +12175,10 @@
         <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="C38" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="D38" t="s">
         <v>205</v>
@@ -11965,13 +12187,13 @@
         <v>244</v>
       </c>
       <c r="F38" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="G38" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="I38">
         <v>27.5</v>
@@ -11982,10 +12204,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="C39" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="D39" t="s">
         <v>205</v>
@@ -11994,13 +12216,13 @@
         <v>137</v>
       </c>
       <c r="F39" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="G39" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="H39" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="I39">
         <v>27.95</v>
@@ -12011,10 +12233,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="C40" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="D40" t="s">
         <v>205</v>
@@ -12023,16 +12245,74 @@
         <v>107</v>
       </c>
       <c r="F40" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="G40" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="I40">
         <v>27.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A41" s="3">
+        <v>39</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="C41" t="s">
+        <v>893</v>
+      </c>
+      <c r="D41" t="s">
+        <v>205</v>
+      </c>
+      <c r="E41">
+        <v>190</v>
+      </c>
+      <c r="F41" t="s">
+        <v>922</v>
+      </c>
+      <c r="G41" t="s">
+        <v>895</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>894</v>
+      </c>
+      <c r="I41">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A42" s="3">
+        <v>34</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C42" t="s">
+        <v>206</v>
+      </c>
+      <c r="D42" t="s">
+        <v>205</v>
+      </c>
+      <c r="E42">
+        <v>459</v>
+      </c>
+      <c r="F42" t="s">
+        <v>951</v>
+      </c>
+      <c r="G42" t="s">
+        <v>241</v>
+      </c>
+      <c r="H42" t="s">
+        <v>474</v>
+      </c>
+      <c r="I42">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -12045,18 +12325,19 @@
     <hyperlink ref="H37" r:id="rId6" xr:uid="{D04069F0-0DAA-4A4C-A8AA-26AB11C3BD56}"/>
     <hyperlink ref="H38" r:id="rId7" xr:uid="{E4D07885-E59B-43A1-8072-9E773C85A997}"/>
     <hyperlink ref="H40" r:id="rId8" xr:uid="{F25B0F60-BB7D-4EAD-838E-387765FC9868}"/>
+    <hyperlink ref="H41" r:id="rId9" xr:uid="{E07B9E34-2ABF-468E-AFD3-1F8D19956346}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12481,10 +12762,10 @@
         <v>33</v>
       </c>
       <c r="B38" t="s">
+        <v>763</v>
+      </c>
+      <c r="C38" t="s">
         <v>764</v>
-      </c>
-      <c r="C38" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
@@ -12492,10 +12773,10 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
+        <v>769</v>
+      </c>
+      <c r="C39" t="s">
         <v>770</v>
-      </c>
-      <c r="C39" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
@@ -12503,10 +12784,10 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
+        <v>790</v>
+      </c>
+      <c r="C40" t="s">
         <v>791</v>
-      </c>
-      <c r="C40" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
@@ -12514,10 +12795,10 @@
         <v>8</v>
       </c>
       <c r="B41" s="10" t="s">
+        <v>798</v>
+      </c>
+      <c r="C41" t="s">
         <v>799</v>
-      </c>
-      <c r="C41" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
@@ -12525,10 +12806,10 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C42" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
@@ -12536,10 +12817,10 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C43" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
@@ -12547,10 +12828,10 @@
         <v>35</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="C44" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
@@ -12558,10 +12839,10 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C45" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
@@ -12569,7 +12850,7 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C46" t="s">
         <v>664</v>
@@ -12580,10 +12861,10 @@
         <v>23</v>
       </c>
       <c r="B47" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="C47" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
@@ -12591,10 +12872,76 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="C48" t="s">
-        <v>899</v>
+        <v>897</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>34</v>
+      </c>
+      <c r="B49" t="s">
+        <v>926</v>
+      </c>
+      <c r="C49" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>34</v>
+      </c>
+      <c r="B50" t="s">
+        <v>934</v>
+      </c>
+      <c r="C50" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s">
+        <v>935</v>
+      </c>
+      <c r="C51" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>34</v>
+      </c>
+      <c r="B52" t="s">
+        <v>940</v>
+      </c>
+      <c r="C52" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>34</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>925</v>
+      </c>
+      <c r="C53" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>34</v>
+      </c>
+      <c r="B54" t="s">
+        <v>942</v>
+      </c>
+      <c r="C54" t="s">
+        <v>943</v>
       </c>
     </row>
   </sheetData>
@@ -12604,9 +12951,10 @@
     <hyperlink ref="B27" r:id="rId2" location="overview" xr:uid="{AAF53F3C-824D-46A3-8C66-5CFC2A7E56BD}"/>
     <hyperlink ref="B30" r:id="rId3" xr:uid="{22191C32-D6EE-41A0-B31D-B1D036DF0037}"/>
     <hyperlink ref="B44" r:id="rId4" xr:uid="{5D80DB1F-C872-4D68-9A2E-3246D644E524}"/>
+    <hyperlink ref="B53" r:id="rId5" xr:uid="{A501B9A2-7BC1-4D6C-B3CA-355CCB1697AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -12933,10 +13281,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745174B4-A8CA-45B8-ACCB-9B5B609F0D5D}">
-  <dimension ref="A1:V106"/>
+  <dimension ref="A1:V109"/>
   <sheetViews>
     <sheetView topLeftCell="A86" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+      <selection activeCell="N109" sqref="N109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17726,6 +18074,138 @@
       </c>
       <c r="N106" s="27">
         <v>3.7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A107" s="12">
+        <v>34</v>
+      </c>
+      <c r="B107" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C107" s="12">
+        <v>20</v>
+      </c>
+      <c r="D107" s="12">
+        <v>14</v>
+      </c>
+      <c r="E107" s="12">
+        <v>15</v>
+      </c>
+      <c r="F107" s="12">
+        <v>13</v>
+      </c>
+      <c r="G107" s="12">
+        <v>11</v>
+      </c>
+      <c r="H107" s="12">
+        <v>10</v>
+      </c>
+      <c r="I107" s="12">
+        <v>10</v>
+      </c>
+      <c r="J107" s="12">
+        <v>12</v>
+      </c>
+      <c r="K107" s="12">
+        <v>14</v>
+      </c>
+      <c r="L107" s="12">
+        <v>17</v>
+      </c>
+      <c r="M107" s="12">
+        <v>20</v>
+      </c>
+      <c r="N107" s="12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A108" s="11">
+        <v>34</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C108" s="26">
+        <v>5</v>
+      </c>
+      <c r="D108" s="26">
+        <v>5</v>
+      </c>
+      <c r="E108" s="26">
+        <v>5</v>
+      </c>
+      <c r="F108" s="26">
+        <v>7</v>
+      </c>
+      <c r="G108" s="26">
+        <v>10</v>
+      </c>
+      <c r="H108" s="26">
+        <v>12</v>
+      </c>
+      <c r="I108" s="26">
+        <v>14</v>
+      </c>
+      <c r="J108" s="26">
+        <v>14</v>
+      </c>
+      <c r="K108" s="26">
+        <v>11</v>
+      </c>
+      <c r="L108" s="26">
+        <v>9</v>
+      </c>
+      <c r="M108" s="26">
+        <v>7</v>
+      </c>
+      <c r="N108" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A109" s="13">
+        <v>34</v>
+      </c>
+      <c r="B109" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C109" s="27">
+        <v>2</v>
+      </c>
+      <c r="D109" s="27">
+        <v>2</v>
+      </c>
+      <c r="E109" s="27">
+        <v>2</v>
+      </c>
+      <c r="F109" s="27">
+        <v>4</v>
+      </c>
+      <c r="G109" s="27">
+        <v>6</v>
+      </c>
+      <c r="H109" s="27">
+        <v>8</v>
+      </c>
+      <c r="I109" s="27">
+        <v>10</v>
+      </c>
+      <c r="J109" s="27">
+        <v>10</v>
+      </c>
+      <c r="K109" s="27">
+        <v>8</v>
+      </c>
+      <c r="L109" s="27">
+        <v>7</v>
+      </c>
+      <c r="M109" s="27">
+        <v>4</v>
+      </c>
+      <c r="N109" s="27">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -17738,8 +18218,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="87" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -17834,12 +18315,12 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <f>IF(VLOOKUP(B2,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B2,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L2" s="25" t="str">
         <f>IF(SUM(D2:K2)=22,"DONE",IF(SUM(D2:J2)=21,"GOOD",""))</f>
-        <v>DONE</v>
+        <v>GOOD</v>
       </c>
       <c r="O2" t="s">
         <v>712</v>
@@ -17889,7 +18370,7 @@
         <v>1</v>
       </c>
       <c r="K3">
-        <f>IF(VLOOKUP(B3,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B3,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L3" s="25" t="str">
@@ -17948,12 +18429,12 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <f>IF(VLOOKUP(B4,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B4,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L4" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>DONE</v>
+        <v>GOOD</v>
       </c>
       <c r="O4" t="s">
         <v>351</v>
@@ -18007,12 +18488,12 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <f>IF(VLOOKUP(B5,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B5,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L5" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>DONE</v>
+        <v>GOOD</v>
       </c>
       <c r="O5" t="s">
         <v>150</v>
@@ -18066,8 +18547,8 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <f>IF(VLOOKUP(B6,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B6,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L6" s="25" t="str">
         <f t="shared" si="0"/>
@@ -18125,8 +18606,8 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <f>IF(VLOOKUP(B7,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B7,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L7" s="25" t="str">
         <f t="shared" si="0"/>
@@ -18184,7 +18665,7 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <f>IF(VLOOKUP(B8,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B8,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L8" s="25" t="str">
@@ -18243,19 +18724,19 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <f>IF(VLOOKUP(B9,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B9,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L9" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>DONE</v>
+        <v>GOOD</v>
       </c>
       <c r="O9" t="s">
         <v>360</v>
       </c>
       <c r="P9">
         <f>COUNTIF(CLIMBS!J:J,'to-do-score-card'!O9)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.5">
@@ -18302,8 +18783,8 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <f>IF(VLOOKUP(B10,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B10,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L10" s="25" t="str">
         <f t="shared" si="0"/>
@@ -18354,7 +18835,7 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <f>IF(VLOOKUP(B11,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B11,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L11" s="25" t="str">
@@ -18406,8 +18887,8 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <f>IF(VLOOKUP(B12,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B12,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L12" s="25" t="str">
         <f t="shared" si="0"/>
@@ -18458,7 +18939,7 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <f>IF(VLOOKUP(B13,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B13,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L13" s="25" t="str">
@@ -18510,8 +18991,8 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <f>IF(VLOOKUP(B14,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B14,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L14" s="25" t="str">
         <f t="shared" si="0"/>
@@ -18562,7 +19043,7 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <f>IF(VLOOKUP(B15,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B15,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L15" s="25" t="str">
@@ -18614,8 +19095,8 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <f>IF(VLOOKUP(B16,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B16,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L16" s="25" t="str">
         <f t="shared" si="0"/>
@@ -18666,7 +19147,7 @@
         <v>1</v>
       </c>
       <c r="K17">
-        <f>IF(VLOOKUP(B17,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B17,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L17" s="25" t="str">
@@ -18718,8 +19199,8 @@
         <v>1</v>
       </c>
       <c r="K18">
-        <f>IF(VLOOKUP(B18,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B18,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L18" s="25" t="str">
         <f t="shared" si="0"/>
@@ -18769,8 +19250,8 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <f>IF(VLOOKUP(B19,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B19,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L19" s="25" t="str">
         <f t="shared" si="0"/>
@@ -18820,12 +19301,12 @@
         <v>1</v>
       </c>
       <c r="K20">
-        <f>IF(VLOOKUP(B20,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B20,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L20" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>DONE</v>
+        <v>GOOD</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.5">
@@ -18871,7 +19352,7 @@
         <v>1</v>
       </c>
       <c r="K21">
-        <f>IF(VLOOKUP(B21,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B21,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L21" s="25" t="str">
@@ -18922,8 +19403,8 @@
         <v>1</v>
       </c>
       <c r="K22">
-        <f>IF(VLOOKUP(B22,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B22,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L22" s="25" t="str">
         <f t="shared" si="0"/>
@@ -18973,8 +19454,8 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <f>IF(VLOOKUP(B23,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B23,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L23" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19024,8 +19505,8 @@
         <v>1</v>
       </c>
       <c r="K24">
-        <f>IF(VLOOKUP(B24,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B24,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L24" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19075,8 +19556,8 @@
         <v>1</v>
       </c>
       <c r="K25">
-        <f>IF(VLOOKUP(B25,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B25,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L25" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19126,8 +19607,8 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <f>IF(VLOOKUP(B26,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B26,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L26" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19177,8 +19658,8 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <f>IF(VLOOKUP(B27,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B27,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L27" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19228,7 +19709,7 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <f>IF(VLOOKUP(B28,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B28,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="L28" s="25" t="str">
@@ -19279,8 +19760,8 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <f>IF(VLOOKUP(B29,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B29,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L29" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19330,7 +19811,7 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <f>IF(VLOOKUP(B30,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B30,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L30" s="25" t="str">
@@ -19381,7 +19862,7 @@
         <v>1</v>
       </c>
       <c r="K31">
-        <f>IF(VLOOKUP(B31,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B31,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L31" s="25" t="str">
@@ -19432,7 +19913,7 @@
         <v>1</v>
       </c>
       <c r="K32">
-        <f>IF(VLOOKUP(B32,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B32,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="L32" s="25" t="str">
@@ -19483,8 +19964,8 @@
         <v>0</v>
       </c>
       <c r="K33">
-        <f>IF(VLOOKUP(B33,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B33,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L33" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19534,58 +20015,57 @@
         <v>1</v>
       </c>
       <c r="K34">
-        <f>IF(VLOOKUP(B34,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
-        <v>1</v>
+        <f>IF(VLOOKUP(B34,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>0</v>
       </c>
       <c r="L34" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>DONE</v>
+        <v>GOOD</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A35" t="str">
         <f>CLIMBS!A35</f>
-        <v>Old man of Hoy</v>
+        <v>Old Man of Hoy</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
       <c r="C35" t="str">
         <f>CLIMBS!B35</f>
-        <v>draft</v>
+        <v>publish</v>
       </c>
       <c r="D35">
         <f>IF(CLIMBS!S35&lt;&gt;0,1,0)+IF(CLIMBS!G35&lt;&gt;0,1,0)+IF(CLIMBS!H35&lt;&gt;0,1,0)+IF(CLIMBS!I35&lt;&gt;0,1,0)+IF(CLIMBS!J35&lt;&gt;0,1,0)+IF(CLIMBS!O35&lt;&gt;0,1,0)+IF(CLIMBS!N35&lt;&gt;0,1,0)+IF(CLIMBS!P35&lt;&gt;0,1,0)+IF(CLIMBS!Q35&lt;&gt;0,1,0)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E35">
         <f>IF(CLIMBS!T35&lt;&gt;0,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F35" t="str">
+        <v>1</v>
+      </c>
+      <c r="F35">
         <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B35,"tile"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B35,"topo"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
 IF(VLOOKUP(CONCATENATE(B35,"map"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
-        <v>missing</v>
+        <v>3</v>
       </c>
       <c r="G35">
-        <f>SUMIFS(IMAGES!G:G,IMAGES!A:A,'to-do-score-card'!B35,IMAGES!B:B,"topo")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H35">
         <f>_xlfn.IFNA(IF(VLOOKUP(B35,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <f>_xlfn.IFNA(IF(VLOOKUP(B35,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35">
         <f>_xlfn.IFNA(IF(VLOOKUP(B35,REFERANCES!A:A,1,FALSE),1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35">
-        <f>IF(VLOOKUP(B35,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B35,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="L35" s="25" t="str">
@@ -19636,7 +20116,7 @@
         <v>1</v>
       </c>
       <c r="K36">
-        <f>IF(VLOOKUP(B36,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B36,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L36" s="25" t="str">
@@ -19687,7 +20167,7 @@
         <v>0</v>
       </c>
       <c r="K37">
-        <f>IF(VLOOKUP(B37,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B37,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="L37" s="25" t="str">
@@ -19738,7 +20218,7 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <f>IF(VLOOKUP(B38,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B38,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L38" s="25" t="str">
@@ -19789,7 +20269,7 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <f>IF(VLOOKUP(B39,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B39,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L39" s="25" t="str">
@@ -19829,7 +20309,7 @@
       </c>
       <c r="H40">
         <f>_xlfn.IFNA(IF(VLOOKUP(B40,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40">
         <f>_xlfn.IFNA(IF(VLOOKUP(B40,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
@@ -19840,7 +20320,7 @@
         <v>0</v>
       </c>
       <c r="K40">
-        <f>IF(VLOOKUP(B40,CLIMBS!C:U,18,FALSE)&gt;0,1,0)</f>
+        <f>IF(VLOOKUP(B40,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="L40" s="25" t="str">

</xml_diff>

<commit_message>
added cliff face direction - some questionable CSS -__-
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5C3CCB-62E7-4F50-87E4-833299602200}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00ECE58-BB26-43AB-B7E2-52ABE88791F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -5268,9 +5268,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="84" zoomScaleNormal="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -13283,7 +13283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745174B4-A8CA-45B8-ACCB-9B5B609F0D5D}">
   <dimension ref="A1:V109"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" zoomScale="94" workbookViewId="0">
+    <sheetView topLeftCell="A88" zoomScale="94" workbookViewId="0">
       <selection activeCell="N109" sqref="N109"/>
     </sheetView>
   </sheetViews>
@@ -18218,9 +18218,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+    <sheetView zoomScale="87" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
+      <selection pane="bottomLeft" activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
some wording corrections for the old man of Hoy"
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00ECE58-BB26-43AB-B7E2-52ABE88791F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370A527B-76FA-422C-9AE7-2DD5371E02AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3203,9 +3203,6 @@
     <t>Article: The Blind Man of Hoy</t>
   </si>
   <si>
-    <t>The Original Route up The Old Man of Hoy is a classic climb amongst classic climbs. Originally climbed in 1966 by Rusty Baillie, Chris Bonington and Tom Patey, this iconic multi-pitch has been the centre of some of the most focused media attention around climbing in the late 1990’s. The route climbs the east landward face, of this northern Scottish sandstone stack. It’s technically not a sea stack (because it’s attached to the mainland), but is usually referred to as such. The route requires a mix of technical climbing, including a short down climb, a traverse, as well as crack climbing and bridging skills. The route is made harder by nesting Fulmars who don’t like climbers around their nests. Decent from the top requires abseiling back down the route. The Original Route is listed in Ken Wilsons Hard Rock book, sitting alongside other UK classics in the &lt;abbr title="Very Severe"&gt;HVS&lt;/abbr&gt; to &lt;abbr title="Extremely Severe"&gt;E1&lt;/abbr&gt; range. The route has seen some incredible accents over the year including being climbed by Red Szell as the first blind man to climb up The Old Man of Hoy and in more decent years Jesse Dufton, also blind, climbed it on lead. Chris Bonington also made recent repeat of this stack, now in his 80’s, over 50 years after his first accent. He climbed the stack with Leo Holding this time. The climb was originally graded HVS but most recent guidebooks list it as E1. Although some pitches are straightforward, it would be easy to underestimate the complexity of getting up and back down safely. The exposure is incredible.</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;strong&gt;Approach&lt;/strong&gt;: Head up the hill behind Rackwick Hostel until reaching the cottage at the top from which a well-constructed path will lead to the viewing promontory across from the Old Man of Hoy. Head North 120m from here and take the small well-worn path down to the rubble scramble to the stack at the base. 
 &lt;/p&gt;&lt;p&gt;
 &lt;strong&gt;Descent&lt;/strong&gt;: There are two options for descent. The first is to abseil each pitch. Typically, there will be slings left behind to rap from at each anchor point. The climber should come prepared to replace them if they are not in a suitable condition. There is also sometimes a rope in situ to help with the pitch two traverse. If the party is not using 60m ropes, and there is not a rope in situ on pitch two, then climbers should be prepared to leave a spare rope behind on ascent, in order to facilitate the descent here. Alternatively, if the party is using a pair of 60m ropes, these can be used to rappel to the end of pitch 3. Then a short rappel to the end of pitch two. Then a longer rappel, free hanging, should take the climbers to the base of the stack. It should go without saying, but climbers should have a pair of prusik cords during the abseil. One to back up the abseil, the other in case the climber needs to ascend the rope for some reason. </t>
@@ -3224,6 +3221,9 @@
   </si>
   <si>
     <t xml:space="preserve">An extensive and well-made guidebook covering every worthwhile crag in Northern Scotland. The guides are clear with generally very good photography. The climb on the Old Man of Hoy has a good amount of detail. The guide also covers key Scottish sea stacks like The Old Man of Stoer and Am Buachaille. A guide that comes highly recomended. </t>
+  </si>
+  <si>
+    <t>The Original Route up The Old Man of Hoy is a classic climb amongst classic climbs. Originally climbed in 1966 by Rusty Baillie, Chris Bonington and Tom Patey, this iconic multi-pitch has been the centre of some of the most focused media attention around climbing in the late 1990’s. The route climbs the east landward face, of this northern Scottish sandstone stack. It’s technically not a sea stack (because it’s attached to the mainland), but is usually referred to as such. The route requires a mix of technical climbing, including a short down climb, a traverse, as well as crack climbing and bridging skills. The route is made harder by nesting Fulmars who don’t like climbers around their nests. Descent from the top requires abseiling back down the route. The Original Route is listed in Ken Wilsons Hard Rock book, sitting alongside other UK classics in the &lt;abbr title="Very Severe"&gt;HVS&lt;/abbr&gt; to &lt;abbr title="Extremely Severe"&gt;E1&lt;/abbr&gt; range. The route has seen some incredible accents over the years, including being climbed by Red Szell as the first blind man to climb up The Old Man of Hoy. In more recent years Jesse Dufton, also blind, went one step further and climbed it on lead. Chris Bonington also made recent repeat of this stack while in his 80’s, over 50 years after his first accent, he climbed the stack with Leo Holding. The climb was originally graded HVS, but most recent guidebooks list it as E1. Although some pitches are straightforward, it would be easy to underestimate the complexity of getting up and back down safely. The exposure is incredible.</t>
   </si>
 </sst>
 </file>
@@ -5268,9 +5268,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="84" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7932,10 +7932,10 @@
         <v>586</v>
       </c>
       <c r="S35" s="31" t="s">
+        <v>951</v>
+      </c>
+      <c r="T35" s="32" t="s">
         <v>945</v>
-      </c>
-      <c r="T35" s="32" t="s">
-        <v>946</v>
       </c>
       <c r="W35" s="33" t="s">
         <v>272</v>
@@ -10968,10 +10968,10 @@
         <v>929</v>
       </c>
       <c r="E108" t="s">
+        <v>948</v>
+      </c>
+      <c r="F108" t="s">
         <v>949</v>
-      </c>
-      <c r="F108" t="s">
-        <v>950</v>
       </c>
       <c r="I108" t="str">
         <f t="shared" si="2"/>
@@ -11013,10 +11013,10 @@
         <v>98</v>
       </c>
       <c r="C110" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D110" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="E110" s="10" t="s">
         <v>574</v>
@@ -12303,7 +12303,7 @@
         <v>459</v>
       </c>
       <c r="F42" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="G42" t="s">
         <v>241</v>

</xml_diff>

<commit_message>
publshing agan - works locally
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370A527B-76FA-422C-9AE7-2DD5371E02AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E47DC23-FF9A-444A-ADB4-7388941FC0DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1727" uniqueCount="952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="953">
   <si>
     <t>cliff</t>
   </si>
@@ -3224,6 +3224,9 @@
   </si>
   <si>
     <t>The Original Route up The Old Man of Hoy is a classic climb amongst classic climbs. Originally climbed in 1966 by Rusty Baillie, Chris Bonington and Tom Patey, this iconic multi-pitch has been the centre of some of the most focused media attention around climbing in the late 1990’s. The route climbs the east landward face, of this northern Scottish sandstone stack. It’s technically not a sea stack (because it’s attached to the mainland), but is usually referred to as such. The route requires a mix of technical climbing, including a short down climb, a traverse, as well as crack climbing and bridging skills. The route is made harder by nesting Fulmars who don’t like climbers around their nests. Descent from the top requires abseiling back down the route. The Original Route is listed in Ken Wilsons Hard Rock book, sitting alongside other UK classics in the &lt;abbr title="Very Severe"&gt;HVS&lt;/abbr&gt; to &lt;abbr title="Extremely Severe"&gt;E1&lt;/abbr&gt; range. The route has seen some incredible accents over the years, including being climbed by Red Szell as the first blind man to climb up The Old Man of Hoy. In more recent years Jesse Dufton, also blind, went one step further and climbed it on lead. Chris Bonington also made recent repeat of this stack while in his 80’s, over 50 years after his first accent, he climbed the stack with Leo Holding. The climb was originally graded HVS, but most recent guidebooks list it as E1. Although some pitches are straightforward, it would be easy to underestimate the complexity of getting up and back down safely. The exposure is incredible.</t>
+  </si>
+  <si>
+    <t>NW</t>
   </si>
 </sst>
 </file>
@@ -5268,9 +5271,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S35" sqref="S35"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="84" zoomScaleNormal="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5288,8 +5291,7 @@
     <col min="11" max="13" width="9.3984375" customWidth="1"/>
     <col min="14" max="14" width="9.59765625" customWidth="1"/>
     <col min="15" max="15" width="12.73046875" customWidth="1"/>
-    <col min="16" max="16" width="11.265625" customWidth="1"/>
-    <col min="17" max="17" width="15.1328125" customWidth="1"/>
+    <col min="16" max="17" width="6.53125" customWidth="1"/>
     <col min="18" max="22" width="15.265625" customWidth="1"/>
     <col min="23" max="30" width="7.265625" style="30" customWidth="1"/>
     <col min="31" max="31" width="10.796875" style="30" customWidth="1"/>
@@ -5462,6 +5464,9 @@
       <c r="V2" t="s">
         <v>38</v>
       </c>
+      <c r="W2" s="30" t="s">
+        <v>292</v>
+      </c>
       <c r="X2" s="30">
         <v>1</v>
       </c>
@@ -5865,7 +5870,9 @@
       <c r="V7" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="W7" s="33"/>
+      <c r="W7" s="33" t="s">
+        <v>952</v>
+      </c>
       <c r="X7" s="33"/>
       <c r="Y7" s="33"/>
       <c r="Z7" s="33"/>
@@ -5941,6 +5948,9 @@
       </c>
       <c r="V8" t="s">
         <v>149</v>
+      </c>
+      <c r="W8" s="30" t="s">
+        <v>952</v>
       </c>
       <c r="AF8" s="39">
         <v>43736</v>
@@ -6100,6 +6110,9 @@
       <c r="V10" t="s">
         <v>38</v>
       </c>
+      <c r="W10" s="30" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="11" spans="1:33" s="31" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="31" t="s">
@@ -6168,7 +6181,9 @@
       <c r="V11" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="W11" s="33"/>
+      <c r="W11" s="33" t="s">
+        <v>150</v>
+      </c>
       <c r="X11" s="33"/>
       <c r="Y11" s="33"/>
       <c r="Z11" s="33"/>

</xml_diff>

<commit_message>
added sort order to localstorage and fixed the image size query string
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E47DC23-FF9A-444A-ADB4-7388941FC0DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3BAD76-56BB-47FF-A004-9204A2458D6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2961,17 +2961,6 @@
     <t>29.80866,-9.06435</t>
   </si>
   <si>
-    <t>The route is described as esoteric in some guides for good reason. The first few moves of the climb require friction stepping, on steep rock with very few and very small handholds. It can seem outrageously hard for the technical grade of 5a. These first moves are unlikely to get easier as the route weathers years of climber’s feet, that said the sticky rubber of climbing shoes adheres to the granite in a way that defies sense. The first pitch can be avoided by approaching from further left or aided using the two starting bolts. After this the climb then offers a wonderful undercut pitch that is reminiscent of &lt;a href="/climbs/doorpost-on-bosigran/"&gt;Doorpost’s first pitch at Bosigran&lt;/a&gt;, only bigger and longer. The third pitch offers some initial friction climbing that leads to an incredible and rather unique waist height flake. The final pitch is a short climb onto the nearby summit boulders. 
-&lt;br/&gt;
-&lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;5a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;Climb the block right the right corner to gain a left sloping ramp. Walk along this ramp to the first bolt. Make the aforementioned hard moves, relying on small holds for both hands and feet. After a couple of tricky moves onto the block the second bolt can be clipped. From here the route moves up and right to increasingly better holds, with some options for gear placements at the top of the slab. From there move onto the right block then left to the bolted anchor. Alternatively, the climber can move past the bolted anchor onto the ledge and create a quick traditional anchor in the start of the second pitch using the crack system and nearby wedged blocks. 
-&lt;br/&gt;
-&lt;strong class="pitch-title"&gt;Pitch 2 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;Climb the exceptional sloping crack using mostly undercuts all the way around the corner to a traditional gear belay in the corner before the rising flack of the 3rd pitch. Large cams are particularly helpful for protecting this pitch. 
-&lt;br/&gt;
-&lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;45m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;Some delicate friction-based climbing on the low angle slab takes the climber to a bolt. Moving up from here a large flake can be used to comfortably move up the slab. Slings on the granite spikes on the top an edge of the flake can offer some additional protection as the climber moves up. The are also some options for gear higher in the giant flake. As the flake moves right the climber can pull up and slightly left onto the flake where there is a single bolt. From here the climber moved up to a crack then a bolted anchor. 
-&lt;br/&gt;
-&lt;strong class="pitch-title"&gt;Pitch 4 –&lt;span class="length"&gt;15m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;From the previous anchor move onto the large plateau. There will be a large boulder with 2 additional smaller boulders on it, one of which has the summit boulder on top. Climb the large wall of the main boulder using the 3 bolts for protection. From here there is easier climbing to the summit boulder and its 2 anchor bolts with an abseil malion. Reaching this is a little runout. From the summit the climbers can abseil back to the plateau and walk off. Whilst there should be a malion on the summit anchor, carrying a spare one would be prudent.</t>
-  </si>
-  <si>
     <t>img/tiles/amzkhassan-wall-climb-in-morocco.jpg</t>
   </si>
   <si>
@@ -2994,11 +2983,6 @@
   </si>
   <si>
     <t>Ksar rock offers great multi-pitch rock climbing up to around 150 meters with plenty of climbs in grades from Severe to E1. This is a popular destination for its quick approach, easy access and quality routes that get great winter sun on the south face. The East Buttress route is one of the easier climbs up Ksar Rock, graded as severe in some guides and hard severe in others, the route can be upgraded to very severe by taking some direct variations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;strong&gt;Approach&lt;/strong&gt;: The approach to the High Sierra Dome is a straightforward walk from the &amp;quot;car park&amp;quot;. Drive into and through the village of Aguerd Oudad, under Napoleon’s Hat. Follow a dirt path out of the back of the village until you see the High Sierra Dome on the right. The climb can be approached directly with a scramble on the boulders to gain the base of the climb. 
-&lt;/p&gt;&lt;p&gt;
-&lt;strong&gt;Descent&lt;/strong&gt;: Upon reaching the summit boulder, abseil back to the main plateau. Whilst it’s possible to lower off of the malion, the climber’s rope will undoubtably have picked up a lot of fine granite dust and sand along the route, meaning that running the weighted rope though the malion when lowering off, will wear through the metal (and damage your rope) faster. This will mean both need replacing more frequently. When abseiling, the rope sits statically on the malion reducing wear. From the plateau, walk east and behind the summit boulder. i.e. rom the end of the abseil, turn to face the 3rd pitch anchor and walk forwards and left around the summit boulder. From here the climber walks past an incredible boulder shaped like the letter n. The climber carries onto the back of the plateau and walks of to the left (West) side to scramble down and back around. </t>
   </si>
   <si>
     <t>img/topos/high-sierra/maps/</t>
@@ -3227,6 +3211,22 @@
   </si>
   <si>
     <t>NW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Approach&lt;/strong&gt;: The approach to the High Sierra Dome is a straightforward walk from the &amp;quot;car park&amp;quot;. Drive into and through the village of Aguerd Oudad, under Napoleon’s Hat. Follow a dirt path out of the back of the village until you see the High Sierra Dome on the right. The climb can be approached directly with a scramble on the boulders to gain the base of the climb. 
+&lt;/p&gt;&lt;p&gt;
+&lt;strong&gt;Descent&lt;/strong&gt;: Upon reaching the summit boulder, abseil back to the main plateau. Whilst it’s possible to lower off of the malion, the climber’s rope will undoubtably have picked up a lot of fine granite dust and sand along the route, meaning that running the weighted rope though the malion when lowering off, will wear through the metal (and damage your rope) faster. This will mean both need replacing more frequently. When abseiling, the rope sits statically on the malion reducing wear. From the plateau, walk east and behind the summit boulder. i.e. from the end of the abseil, turn to face the 3rd pitch anchor and walk forwards and left around the summit boulder. From here the climber walks past an incredible boulder shaped like the letter n. The climber carries onto the back of the plateau and walks of to the left (West) side to scramble down and back around. </t>
+  </si>
+  <si>
+    <t>The route is described as esoteric in some guides for good reason. The first few moves of the climb require friction stepping, on steep rock with very few and very small handholds. It can seem outrageously hard for the technical grade of 5a. These first moves are unlikely to get easier as the route weathers years of climber’s feet, that said the sticky rubber of climbing shoes adheres to the granite in a way that defies sense. The first pitch can be avoided by approaching from further left or aided using the two starting bolts. After this the climb then offers a wonderful undercut pitch that is reminiscent of &lt;a href="/climbs/doorpost-on-bosigran/"&gt;Doorpost’s first pitch at Bosigran&lt;/a&gt;, only bigger and longer. The third pitch offers some initial friction climbing that leads to an incredible and rather unique waist height flake. The final pitch is a short climb onto the nearby summit boulders. 
+&lt;br/&gt;
+&lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;5a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;Climb the block right the right corner to gain a left sloping ramp. Walk along this ramp to the first bolt. Make the aforementioned hard moves, relying on small holds for both hands and feet. After a couple of tricky moves onto the block the second bolt can be clipped. From here the route moves up and right to increasingly better holds, with some options for gear placements at the top of the slab. From there move onto the right block then left to the bolted anchor. Alternatively, the climber can move past the bolted anchor onto the ledge and create a quick traditional anchor in the start of the second pitch using the crack system and nearby wedged blocks. 
+&lt;br/&gt;
+&lt;strong class="pitch-title"&gt;Pitch 2 –&lt;span class="length"&gt;30m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;Climb the exceptional sloping crack using mostly undercuts all the way around the corner to a traditional gear belay in the corner before the rising flake of the 3rd pitch. Large cams are particularly helpful for protecting this pitch. 
+&lt;br/&gt;
+&lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;45m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;Some delicate friction-based climbing on the low angle slab takes the climber to a bolt. Moving up from here a large flake can be used to comfortably move up the slab. Slings on the granite spikes on the top an edge of the flake can offer some additional protection as the climber moves up. The are also some options for gear higher in the giant flake. As the flake moves right the climber can pull up and slightly left onto the flake where there is a single bolt. From here the climber moves up to a crack then a bolted anchor. 
+&lt;br/&gt;
+&lt;strong class="pitch-title"&gt;Pitch 4 –&lt;span class="length"&gt;15m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;From the previous anchor move onto the large plateau. There will be a large boulder with 2 additional smaller boulders on it, one of which has the summit boulder on top. Climb the large wall of the main boulder using the 3 bolts for protection. From here there is easier climbing to the summit boulder and its 2 anchor bolts with an abseil malion. Reaching this is a little runout. From the summit the climbers can abseil back to the plateau and walk off. Whilst there should be a malion on the summit anchor, carrying a spare one would be prudent.</t>
   </si>
 </sst>
 </file>
@@ -5272,8 +5272,8 @@
   <dimension ref="A1:AG43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="84" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W14" sqref="W14"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5865,13 +5865,13 @@
         <v>77</v>
       </c>
       <c r="T7" s="31" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="V7" s="31" t="s">
         <v>38</v>
       </c>
       <c r="W7" s="33" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="X7" s="33"/>
       <c r="Y7" s="33"/>
@@ -5950,7 +5950,7 @@
         <v>149</v>
       </c>
       <c r="W8" s="30" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="AF8" s="39">
         <v>43736</v>
@@ -7893,7 +7893,7 @@
     </row>
     <row r="35" spans="1:33" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="31" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>95</v>
@@ -7905,7 +7905,7 @@
         <v>18</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>20</v>
@@ -7929,13 +7929,13 @@
         <v>846</v>
       </c>
       <c r="M35" s="31" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="N35" s="31" t="s">
         <v>24</v>
       </c>
       <c r="O35" s="31" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="P35" s="31">
         <v>45</v>
@@ -7947,10 +7947,10 @@
         <v>586</v>
       </c>
       <c r="S35" s="31" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="T35" s="32" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="W35" s="33" t="s">
         <v>272</v>
@@ -7991,10 +7991,10 @@
         <v>801</v>
       </c>
       <c r="E36" s="41" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="F36" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="G36">
         <v>120</v>
@@ -8033,7 +8033,7 @@
         <v>179</v>
       </c>
       <c r="S36" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="T36" s="3" t="s">
         <v>867</v>
@@ -8129,13 +8129,13 @@
         <v>37</v>
       </c>
       <c r="S38" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="T38" s="3" t="s">
-        <v>888</v>
+        <v>951</v>
       </c>
       <c r="U38" s="3" t="s">
-        <v>879</v>
+        <v>952</v>
       </c>
       <c r="V38" t="s">
         <v>149</v>
@@ -8192,13 +8192,13 @@
         <v>846</v>
       </c>
       <c r="M39" s="31" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="N39" s="31" t="s">
         <v>802</v>
       </c>
       <c r="O39" s="31" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="P39" s="31">
         <v>5</v>
@@ -8210,13 +8210,13 @@
         <v>876</v>
       </c>
       <c r="S39" s="31" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="T39" s="32" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="U39" s="32" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="V39" s="31" t="s">
         <v>149</v>
@@ -8249,7 +8249,7 @@
         <v>874</v>
       </c>
       <c r="F40" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="G40">
         <v>270</v>
@@ -8288,19 +8288,19 @@
         <v>876</v>
       </c>
       <c r="S40" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="T40" s="3" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="U40" s="3" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="V40" t="s">
         <v>149</v>
       </c>
       <c r="W40" s="30" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="AF40" s="39">
         <v>43810</v>
@@ -10728,10 +10728,10 @@
         <v>137</v>
       </c>
       <c r="C98" t="s">
+        <v>879</v>
+      </c>
+      <c r="D98" t="s">
         <v>880</v>
-      </c>
-      <c r="D98" t="s">
-        <v>881</v>
       </c>
       <c r="E98" t="s">
         <v>723</v>
@@ -10752,10 +10752,10 @@
         <v>137</v>
       </c>
       <c r="C99" t="s">
+        <v>881</v>
+      </c>
+      <c r="D99" t="s">
         <v>882</v>
-      </c>
-      <c r="D99" t="s">
-        <v>883</v>
       </c>
       <c r="E99" t="s">
         <v>723</v>
@@ -10776,10 +10776,10 @@
         <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="D100" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="E100" t="s">
         <v>723</v>
@@ -10803,10 +10803,10 @@
         <v>98</v>
       </c>
       <c r="C101" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="D101" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E101" s="10" t="s">
         <v>574</v>
@@ -10827,10 +10827,10 @@
         <v>137</v>
       </c>
       <c r="C102" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="D102" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E102" t="s">
         <v>723</v>
@@ -10851,10 +10851,10 @@
         <v>102</v>
       </c>
       <c r="C103" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D103" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E103" t="s">
         <v>723</v>
@@ -10878,10 +10878,10 @@
         <v>98</v>
       </c>
       <c r="C104" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="D104" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E104" s="10" t="s">
         <v>574</v>
@@ -10902,10 +10902,10 @@
         <v>137</v>
       </c>
       <c r="C105" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D105" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E105" t="s">
         <v>723</v>
@@ -10926,10 +10926,10 @@
         <v>102</v>
       </c>
       <c r="C106" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D106" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="E106" t="s">
         <v>723</v>
@@ -10953,10 +10953,10 @@
         <v>98</v>
       </c>
       <c r="C107" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="D107" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="E107" s="10" t="s">
         <v>574</v>
@@ -10977,16 +10977,16 @@
         <v>137</v>
       </c>
       <c r="C108" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D108" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="E108" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="F108" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="I108" t="str">
         <f t="shared" si="2"/>
@@ -11001,16 +11001,16 @@
         <v>102</v>
       </c>
       <c r="C109" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="D109" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="E109" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="F109" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G109">
         <v>4</v>
@@ -11028,10 +11028,10 @@
         <v>98</v>
       </c>
       <c r="C110" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D110" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="E110" s="10" t="s">
         <v>574</v>
@@ -12190,10 +12190,10 @@
         <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C38" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D38" t="s">
         <v>205</v>
@@ -12202,13 +12202,13 @@
         <v>244</v>
       </c>
       <c r="F38" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="G38" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="I38">
         <v>27.5</v>
@@ -12231,7 +12231,7 @@
         <v>137</v>
       </c>
       <c r="F39" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="G39" t="s">
         <v>817</v>
@@ -12248,10 +12248,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C40" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D40" t="s">
         <v>205</v>
@@ -12260,13 +12260,13 @@
         <v>107</v>
       </c>
       <c r="F40" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="G40" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="I40">
         <v>27.5</v>
@@ -12277,10 +12277,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C41" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D41" t="s">
         <v>205</v>
@@ -12289,13 +12289,13 @@
         <v>190</v>
       </c>
       <c r="F41" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="G41" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="I41">
         <v>27.5</v>
@@ -12318,7 +12318,7 @@
         <v>459</v>
       </c>
       <c r="F42" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="G42" t="s">
         <v>241</v>
@@ -12887,10 +12887,10 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="C48" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
@@ -12898,10 +12898,10 @@
         <v>34</v>
       </c>
       <c r="B49" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C49" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
@@ -12909,10 +12909,10 @@
         <v>34</v>
       </c>
       <c r="B50" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C50" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
@@ -12920,10 +12920,10 @@
         <v>34</v>
       </c>
       <c r="B51" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="C51" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
@@ -12931,10 +12931,10 @@
         <v>34</v>
       </c>
       <c r="B52" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C52" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
@@ -12942,10 +12942,10 @@
         <v>34</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C53" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
@@ -12953,10 +12953,10 @@
         <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C54" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed morocco crag names
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3BAD76-56BB-47FF-A004-9204A2458D6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C075B451-D6C4-4375-90C9-520E128E8E21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5271,9 +5271,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="84" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U38" sqref="U38"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8075,7 +8075,7 @@
     </row>
     <row r="38" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B38" t="s">
         <v>95</v>
@@ -8090,7 +8090,7 @@
         <v>869</v>
       </c>
       <c r="F38" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="G38">
         <v>120</v>
@@ -8156,7 +8156,7 @@
     </row>
     <row r="39" spans="1:33" s="31" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="31" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>95</v>
@@ -8171,7 +8171,7 @@
         <v>874</v>
       </c>
       <c r="F39" s="31" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G39" s="31">
         <v>130</v>
@@ -8234,7 +8234,7 @@
     </row>
     <row r="40" spans="1:33" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>877</v>
+        <v>916</v>
       </c>
       <c r="B40" t="s">
         <v>95</v>
@@ -8249,7 +8249,7 @@
         <v>874</v>
       </c>
       <c r="F40" t="s">
-        <v>916</v>
+        <v>877</v>
       </c>
       <c r="G40">
         <v>270</v>
@@ -20192,7 +20192,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A38" t="str">
-        <f>CLIMBS!A38</f>
+        <f>CLIMBS!F38</f>
         <v xml:space="preserve">High Sierra </v>
       </c>
       <c r="B38">
@@ -20243,7 +20243,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A39" t="str">
-        <f>CLIMBS!A39</f>
+        <f>CLIMBS!F39</f>
         <v>Pinnacle Slab</v>
       </c>
       <c r="B39">
@@ -20294,7 +20294,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A40" t="str">
-        <f>CLIMBS!A40</f>
+        <f>CLIMBS!F40</f>
         <v xml:space="preserve">Donkey Serenades </v>
       </c>
       <c r="B40">

</xml_diff>

<commit_message>
so... I changed a lot of things. The main one is some SEO content pages under /climbing-tips/. this is just the start of a lot of content, but more will come. I also added the native lazy load feature to the homepage. I also tweaked the about page Ialso changed the grade conversion page. There may be some bugs and i didn't add any automation yet so best not push to prod just yet. But i think its a good update.
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C075B451-D6C4-4375-90C9-520E128E8E21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CFAF6B-BF62-48B3-962F-7F66D1C99B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="957">
   <si>
     <t>cliff</t>
   </si>
@@ -3227,6 +3227,18 @@
 &lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;45m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;Some delicate friction-based climbing on the low angle slab takes the climber to a bolt. Moving up from here a large flake can be used to comfortably move up the slab. Slings on the granite spikes on the top an edge of the flake can offer some additional protection as the climber moves up. The are also some options for gear higher in the giant flake. As the flake moves right the climber can pull up and slightly left onto the flake where there is a single bolt. From here the climber moves up to a crack then a bolted anchor. 
 &lt;br/&gt;
 &lt;strong class="pitch-title"&gt;Pitch 4 –&lt;span class="length"&gt;15m&lt;/span&gt; &lt;span class="pitchGrade brit"&gt;4b&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;From the previous anchor move onto the large plateau. There will be a large boulder with 2 additional smaller boulders on it, one of which has the summit boulder on top. Climb the large wall of the main boulder using the 3 bolts for protection. From here there is easier climbing to the summit boulder and its 2 anchor bolts with an abseil malion. Reaching this is a little runout. From the summit the climbers can abseil back to the plateau and walk off. Whilst there should be a malion on the summit anchor, carrying a spare one would be prudent.</t>
+  </si>
+  <si>
+    <t>Gower</t>
+  </si>
+  <si>
+    <t>Great Tor</t>
+  </si>
+  <si>
+    <t>East Ridge</t>
+  </si>
+  <si>
+    <t>S 3c</t>
   </si>
 </sst>
 </file>
@@ -4193,7 +4205,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
@@ -5272,8 +5284,8 @@
   <dimension ref="A1:AG43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8311,6 +8323,48 @@
       </c>
     </row>
     <row r="41" spans="1:33" s="31" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="31" t="s">
+        <v>954</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="31">
+        <v>40</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>953</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>955</v>
+      </c>
+      <c r="G41" s="31">
+        <v>71</v>
+      </c>
+      <c r="H41" s="31">
+        <v>4</v>
+      </c>
+      <c r="I41" s="31">
+        <v>3</v>
+      </c>
+      <c r="J41" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="K41" s="31" t="s">
+        <v>533</v>
+      </c>
+      <c r="L41" s="31" t="s">
+        <v>846</v>
+      </c>
+      <c r="M41" s="31" t="s">
+        <v>956</v>
+      </c>
+      <c r="N41" s="31" t="s">
+        <v>44</v>
+      </c>
       <c r="T41" s="35"/>
       <c r="U41" s="34"/>
       <c r="W41" s="33"/>
@@ -11070,7 +11124,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I116" xr:uid="{8A9CCE92-9934-4A85-9799-3C2EFD57E833}">
-    <sortState ref="A2:H116">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H116">
       <sortCondition ref="A1:A116"/>
     </sortState>
   </autoFilter>
@@ -18515,7 +18569,7 @@
       </c>
       <c r="P5">
         <f>COUNTIF(CLIMBS!J:J,'to-do-score-card'!O5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
fixed build - broken published climb (forgot i haven't finished great tor in wales yet
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CFAF6B-BF62-48B3-962F-7F66D1C99B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA07C8DF-6158-49BC-9289-357C357B84AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5284,8 +5284,8 @@
   <dimension ref="A1:AG43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O41" sqref="O41"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8327,7 +8327,7 @@
         <v>954</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C41" s="31">
         <v>40</v>

</xml_diff>

<commit_message>
finally added the climb in gower. Also fixed a minor bug where the decent lines were drawn as dotted on the canvas rather than solid
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA07C8DF-6158-49BC-9289-357C357B84AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4039046A-3E36-44BA-9622-CADE10C2C125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="976">
   <si>
     <t>cliff</t>
   </si>
@@ -3239,6 +3239,82 @@
   </si>
   <si>
     <t>S 3c</t>
+  </si>
+  <si>
+    <t>51.568422,-4.122578</t>
+  </si>
+  <si>
+    <t>img/topos/gower/east-buttress-climb-on-high-tor-gower.jpg</t>
+  </si>
+  <si>
+    <t>East Buttress Climb on Great Tor in Gower.</t>
+  </si>
+  <si>
+    <t>img/tiles/great-tor-in-gower-south-wales.jpg</t>
+  </si>
+  <si>
+    <t>Great Tor climb on the beach in South Wales</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/swansealocalboy/14697940249/</t>
+  </si>
+  <si>
+    <t>Gareth Lovering</t>
+  </si>
+  <si>
+    <t>The East Ridge of Great Tor offers easy climbing right above the beach of Three Cliffs Bay. The route is non-tidal, but approaching from the beach is only possible at low tide. A not so straightforward scramble down or abseil from a nearby block are alternative options for reaching the base of the climb. The route is broken up by 3 significant ledges. Although it’s set as 4 pitches, linking pitch 2 and 3 or even 3 and 4 makes the pitches a bit more significant. There are also some variations that up the difficulty to Very Severe, although the variations avoids the dramatic south east edge overlooking the beaches and sea. Although Great Tor is the most significant multi-pitch climb in the area, the nearby 3 cliffs bay has a multitude of shorter trad climbs.</t>
+  </si>
+  <si>
+    <t>img/topos/gower/maps/</t>
+  </si>
+  <si>
+    <t>Great Tor location on Three Cliffs Bay</t>
+  </si>
+  <si>
+    <t>https://swcw.org.uk/wiki/Great_Tor_Proper</t>
+  </si>
+  <si>
+    <t>Climb Info: South Wales Climbing Wiki Great Tor page</t>
+  </si>
+  <si>
+    <t>9781906095369</t>
+  </si>
+  <si>
+    <t>Gower Rock Selected Rock Climbs</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3bpSwzI</t>
+  </si>
+  <si>
+    <t>This is a selective rock climbing guide to the Gower peninsula in South Wales. Gower Rock aims to showcase the depth and quality of rock climbing on this wild, beautiful yet somewhat unknown peninsula. The book does a good job highlighting the best of the area, including a short section on Great Tor. The directions to find the climbs in the book seem to be inaccurate because they rely on landmarks that change (the white house near Paviland is not white anymore and the bench on the way to Great Tor is no where to be found). The book is good value for money for the climber planning a passing visit to Gower.</t>
+  </si>
+  <si>
+    <t>img/guidebooks/gower-rock-selected-rock-climbs.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Tor is a limestone tower that divides Three Cliffs Bay to the East from Oxwich Bay to the West. The Tor rises out of the sand between these beaches and can be climbed on all faces. While steep in places, the holds are usually plentiful and solid. Protection is also mostly easy to come by. 
+&lt;br /&gt;
+&lt;strong class="pitch-title"&gt;Pitch 1 –&lt;span class="length"&gt;18m&lt;/span&gt; &lt;span class="pitchGrade bas"&gt;3c&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+The first pitch follows a crack surrounded by good holds. Upon reaching the bulge before the ledge, this can be talked directly using good handholds or the climber can pass it on the right. An anchor can be built in the wall at the back of the large ledge. 
+&lt;br /&gt;&lt;strong class="pitch-title"&gt;Pitch 2 –&lt;span class="length"&gt;16m&lt;/span&gt; &lt;span class="pitchGrade bas"&gt;3a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+Step out from the ledge to the south east ridge, where a grove will take the climber up the arête (edge) to anther large ledge. The climber can build an anchor here which offers more protection, or continue up pitch 3 to the next ledge.
+&lt;br /&gt;&lt;strong class="pitch-title"&gt;Pitch 3 –&lt;span class="length"&gt;13m&lt;/span&gt; &lt;span class="pitchGrade bas"&gt;3a&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+A short pitch on its own, that once again takes the arête (edge / ridge) up to the next ledge. The climbing is easy and the views and are incredible. An anchor can be made before the final steep pitch. Alternatively pitch 3 &amp; 4 can be linked. 
+&lt;br /&gt;&lt;strong class="pitch-title"&gt;Pitch 4 –&lt;span class="length"&gt;24m&lt;/span&gt; &lt;span class="pitchGrade bas"&gt;3c&lt;/span&gt;&lt;/strong&gt;&lt;br /&gt;
+The final pitch offers a short steep wall before giving way to much easier climbing up the ledges to the summit of Great Tor. An anchor can be built on the top with creative use of various protection and slinging one of the larger summit blocks. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Approach&lt;/strong&gt;:&lt;br /&gt;
+From the National Trust Car Park at Penmaen (postcode: SA3 2HH), head back to the main road, go right up hill, then cross over to the smaller parking area and bus stop. Through the gate, follow the path towards Three Cliffs Bay. &lt;br /&gt;
+&lt;strong&gt;Option A – Abseil &amp; Scramble Down&lt;/strong&gt;:&lt;br /&gt;
+Take the first right at the fork in the path, then at the next fork take the left. Follow the path west along the coast and follow it out towards Great Tor. Before scrambling up onto the Tor proper (rocky peak), there is a large block, that at the time of writing, was suitable for a gearless &amp; retrievable abseil. This may be the most appropriate option if the grass is wet and the tide is in. 50m of abseil reaches the rocky ledges. From there, it’s possible to scramble across to the base of the climb.&lt;br /&gt;
+&lt;strong&gt;Option B –  Low Tide Beach Approach&lt;/strong&gt;:&lt;br /&gt;
+Take the left at the first fork in the road and head down all the way down to Three Cliffs Bay.  Hug the right side of the beach all the way to the base of Great Tor and scramble up to the non-tidal start of the route.&lt;br /&gt;
+&lt;strong&gt;Option C –  Scramble Down&lt;/strong&gt;:&lt;br /&gt;
+Follow the instructions of option A, but keep on over the first outcrop until the gully between the two peaks. From here it’s possible to scramble down carefully to the base of the climb. Not recommended un-roped in wet conditions. &lt;br /&gt;
+&lt;br /&gt;&lt;strong&gt;Descent&lt;/strong&gt;:&lt;br /&gt;
+Scramble off the Tor to the North, following the work path down into the gully then back up and out on the path. Take care on the polished limestone. </t>
   </si>
 </sst>
 </file>
@@ -5284,8 +5360,8 @@
   <dimension ref="A1:AG43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T41" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8327,7 +8403,7 @@
         <v>954</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C41" s="31">
         <v>40</v>
@@ -8365,9 +8441,33 @@
       <c r="N41" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="T41" s="35"/>
-      <c r="U41" s="34"/>
-      <c r="W41" s="33"/>
+      <c r="O41" s="31" t="s">
+        <v>957</v>
+      </c>
+      <c r="P41" s="31">
+        <v>25</v>
+      </c>
+      <c r="Q41" s="31">
+        <v>1</v>
+      </c>
+      <c r="R41" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="S41" s="31" t="s">
+        <v>964</v>
+      </c>
+      <c r="T41" s="35" t="s">
+        <v>975</v>
+      </c>
+      <c r="U41" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="V41" t="s">
+        <v>185</v>
+      </c>
+      <c r="W41" s="33" t="s">
+        <v>292</v>
+      </c>
       <c r="X41" s="33"/>
       <c r="Y41" s="33"/>
       <c r="Z41" s="33"/>
@@ -8376,8 +8476,13 @@
       <c r="AC41" s="33"/>
       <c r="AD41" s="33"/>
       <c r="AE41" s="33"/>
-      <c r="AF41" s="38"/>
-      <c r="AG41" s="37"/>
+      <c r="AF41" s="38">
+        <v>43940</v>
+      </c>
+      <c r="AG41" s="37">
+        <f>(AF41-DATE(1970,1,1))*86400</f>
+        <v>1587254400</v>
+      </c>
     </row>
     <row r="43" spans="1:33" s="31" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="T43" s="35"/>
@@ -8405,8 +8510,8 @@
   <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F108" sqref="F108"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9978,7 +10083,7 @@
         <v>575</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" ref="I65:I110" si="2">CONCATENATE(A65,B65)</f>
+        <f t="shared" ref="I65:I112" si="2">CONCATENATE(A65,B65)</f>
         <v>22map</v>
       </c>
     </row>
@@ -11098,25 +11203,94 @@
         <v>34map</v>
       </c>
     </row>
-    <row r="113" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>40</v>
+      </c>
+      <c r="B111" t="s">
+        <v>102</v>
+      </c>
+      <c r="C111" t="s">
+        <v>958</v>
+      </c>
+      <c r="D111" t="s">
+        <v>959</v>
+      </c>
+      <c r="E111" t="s">
+        <v>723</v>
+      </c>
+      <c r="F111" t="s">
+        <v>134</v>
+      </c>
+      <c r="G111">
+        <v>5</v>
+      </c>
+      <c r="I111" t="str">
+        <f t="shared" si="2"/>
+        <v>40topo</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>40</v>
+      </c>
+      <c r="B112" t="s">
+        <v>137</v>
+      </c>
+      <c r="C112" t="s">
+        <v>960</v>
+      </c>
+      <c r="D112" t="s">
+        <v>961</v>
+      </c>
+      <c r="E112" s="10" t="s">
+        <v>962</v>
+      </c>
+      <c r="F112" t="s">
+        <v>963</v>
+      </c>
+      <c r="I112" t="str">
+        <f t="shared" si="2"/>
+        <v>40tile</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>40</v>
+      </c>
+      <c r="B113" t="s">
+        <v>98</v>
+      </c>
+      <c r="C113" t="s">
+        <v>965</v>
+      </c>
+      <c r="D113" t="s">
+        <v>966</v>
+      </c>
+      <c r="E113" s="10" t="s">
+        <v>574</v>
+      </c>
+      <c r="F113" t="s">
+        <v>575</v>
+      </c>
       <c r="I113" t="str">
         <f>CONCATENATE(A113,B113)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="114" spans="9:9" x14ac:dyDescent="0.45">
+        <v>40map</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I114" t="str">
         <f>CONCATENATE(A114,B114)</f>
         <v/>
       </c>
     </row>
-    <row r="115" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I115" t="str">
         <f>CONCATENATE(A115,B115)</f>
         <v/>
       </c>
     </row>
-    <row r="116" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I116" t="str">
         <f>CONCATENATE(A116,B116)</f>
         <v/>
@@ -11141,18 +11315,20 @@
     <hyperlink ref="E104" r:id="rId10" xr:uid="{B966E3D2-A42D-4B1E-B741-5BF7C80D8894}"/>
     <hyperlink ref="E107" r:id="rId11" xr:uid="{EED9F4AD-44D3-4EB4-BE7F-A87AA21B96A6}"/>
     <hyperlink ref="E110" r:id="rId12" xr:uid="{80395FA3-9005-4540-BB40-1F4F5512E758}"/>
+    <hyperlink ref="E112" r:id="rId13" xr:uid="{B51D1FAF-B2C0-4F11-A276-D652E30B2B35}"/>
+    <hyperlink ref="E113" r:id="rId14" xr:uid="{2D210F36-D435-4B6F-AE7E-BD16837D52FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB58989-DB9B-42B8-8BEA-AD863D94E91D}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12382,6 +12558,35 @@
       </c>
       <c r="I42">
         <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A43" s="3">
+        <v>40</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="C43" t="s">
+        <v>970</v>
+      </c>
+      <c r="D43" t="s">
+        <v>205</v>
+      </c>
+      <c r="E43">
+        <v>87</v>
+      </c>
+      <c r="F43" t="s">
+        <v>972</v>
+      </c>
+      <c r="G43" t="s">
+        <v>973</v>
+      </c>
+      <c r="H43" t="s">
+        <v>971</v>
+      </c>
+      <c r="I43">
+        <v>12.99</v>
       </c>
     </row>
   </sheetData>
@@ -12403,10 +12608,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091284CD-7BE4-40C5-8B13-8EF65FF7D256}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:C54"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13011,6 +13216,17 @@
       </c>
       <c r="C54" t="s">
         <v>941</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>40</v>
+      </c>
+      <c r="B55" t="s">
+        <v>967</v>
+      </c>
+      <c r="C55" t="s">
+        <v>968</v>
       </c>
     </row>
   </sheetData>
@@ -13350,10 +13566,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745174B4-A8CA-45B8-ACCB-9B5B609F0D5D}">
-  <dimension ref="A1:V109"/>
+  <dimension ref="A1:V112"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="94" workbookViewId="0">
-      <selection activeCell="N109" sqref="N109"/>
+    <sheetView topLeftCell="A92" zoomScale="94" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18275,6 +18491,138 @@
       </c>
       <c r="N109" s="27">
         <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A110" s="12">
+        <v>40</v>
+      </c>
+      <c r="B110" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C110" s="12">
+        <v>16</v>
+      </c>
+      <c r="D110" s="12">
+        <v>13</v>
+      </c>
+      <c r="E110" s="12">
+        <v>8</v>
+      </c>
+      <c r="F110" s="12">
+        <v>12</v>
+      </c>
+      <c r="G110" s="12">
+        <v>10</v>
+      </c>
+      <c r="H110" s="12">
+        <v>13</v>
+      </c>
+      <c r="I110" s="12">
+        <v>9</v>
+      </c>
+      <c r="J110" s="12">
+        <v>12</v>
+      </c>
+      <c r="K110" s="12">
+        <v>9</v>
+      </c>
+      <c r="L110" s="12">
+        <v>15</v>
+      </c>
+      <c r="M110" s="12">
+        <v>16</v>
+      </c>
+      <c r="N110" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A111" s="11">
+        <v>40</v>
+      </c>
+      <c r="B111" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C111" s="26">
+        <v>8</v>
+      </c>
+      <c r="D111" s="26">
+        <v>8</v>
+      </c>
+      <c r="E111" s="26">
+        <v>9</v>
+      </c>
+      <c r="F111" s="26">
+        <v>12</v>
+      </c>
+      <c r="G111" s="26">
+        <v>15</v>
+      </c>
+      <c r="H111" s="26">
+        <v>18</v>
+      </c>
+      <c r="I111" s="26">
+        <v>19</v>
+      </c>
+      <c r="J111" s="26">
+        <v>19</v>
+      </c>
+      <c r="K111" s="26">
+        <v>17</v>
+      </c>
+      <c r="L111" s="26">
+        <v>14</v>
+      </c>
+      <c r="M111" s="26">
+        <v>11</v>
+      </c>
+      <c r="N111" s="26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A112" s="13">
+        <v>40</v>
+      </c>
+      <c r="B112" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C112" s="27">
+        <v>4</v>
+      </c>
+      <c r="D112" s="27">
+        <v>4</v>
+      </c>
+      <c r="E112" s="27">
+        <v>5</v>
+      </c>
+      <c r="F112" s="27">
+        <v>6</v>
+      </c>
+      <c r="G112" s="27">
+        <v>9</v>
+      </c>
+      <c r="H112" s="27">
+        <v>12</v>
+      </c>
+      <c r="I112" s="27">
+        <v>14</v>
+      </c>
+      <c r="J112" s="27">
+        <v>14</v>
+      </c>
+      <c r="K112" s="27">
+        <v>12</v>
+      </c>
+      <c r="L112" s="27">
+        <v>10</v>
+      </c>
+      <c r="M112" s="27">
+        <v>7</v>
+      </c>
+      <c r="N112" s="27">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -18285,11 +18633,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDF4E69-F28E-4F52-8319-FE157D3A6CAD}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView zoomScale="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P24" sqref="P24"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -20397,8 +20745,59 @@
         <v/>
       </c>
     </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A41" t="str">
+        <f>CLIMBS!F41</f>
+        <v>East Ridge</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41" t="str">
+        <f>CLIMBS!B41</f>
+        <v>publish</v>
+      </c>
+      <c r="D41">
+        <f>IF(CLIMBS!S41&lt;&gt;0,1,0)+IF(CLIMBS!G41&lt;&gt;0,1,0)+IF(CLIMBS!H41&lt;&gt;0,1,0)+IF(CLIMBS!I41&lt;&gt;0,1,0)+IF(CLIMBS!J41&lt;&gt;0,1,0)+IF(CLIMBS!O41&lt;&gt;0,1,0)+IF(CLIMBS!N41&lt;&gt;0,1,0)+IF(CLIMBS!P41&lt;&gt;0,1,0)+IF(CLIMBS!Q41&lt;&gt;0,1,0)</f>
+        <v>9</v>
+      </c>
+      <c r="E41">
+        <f>IF(CLIMBS!T41&lt;&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <f>_xlfn.IFNA(IF(VLOOKUP(CONCATENATE(B41,"tile"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B41,"topo"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0)+
+IF(VLOOKUP(CONCATENATE(B41,"map"),IMAGES!I:I,1,FALSE)&lt;&gt;0,1,0),"missing")</f>
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <f>SUMIFS(IMAGES!G:G,IMAGES!A:A,'to-do-score-card'!B41,IMAGES!B:B,"topo")</f>
+        <v>5</v>
+      </c>
+      <c r="H41">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B41,GUIDEBOOKS!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B41,WEATHER!A:A,1,FALSE) &lt;&gt; 0,1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <f>_xlfn.IFNA(IF(VLOOKUP(B41,REFERANCES!A:A,1,FALSE),1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <f>IF(VLOOKUP(B41,CLIMBS!C:U,19,FALSE)&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L41" s="25" t="str">
+        <f t="shared" ref="L41" si="3">IF(SUM(D41:K41)=22,"DONE",IF(SUM(D41:J41)=21,"GOOD",""))</f>
+        <v>DONE</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D40">
+  <conditionalFormatting sqref="D2:D41">
     <cfRule type="cellIs" dxfId="16" priority="16" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
@@ -20406,7 +20805,7 @@
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C40">
+  <conditionalFormatting sqref="C2:C41">
     <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"draft"</formula>
     </cfRule>
@@ -20416,12 +20815,12 @@
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C40">
+  <conditionalFormatting sqref="C3:C41">
     <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"publish"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E40">
+  <conditionalFormatting sqref="E2:E41">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -20429,7 +20828,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:G40">
+  <conditionalFormatting sqref="F2:G41">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
@@ -20437,7 +20836,7 @@
       <formula>"missing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:J40">
+  <conditionalFormatting sqref="H2:J41">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -20445,7 +20844,7 @@
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K40">
+  <conditionalFormatting sqref="K2:K41">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -20453,7 +20852,7 @@
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G41">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>1</formula>
       <formula>4</formula>
@@ -20465,7 +20864,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F40">
+  <conditionalFormatting sqref="F2:F41">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>3</formula>
     </cfRule>

</xml_diff>

<commit_message>
making the site wider on large 1920 screens so grid is 4 climbs wide. changed footer to use video for smalller files size removed a LOT of un-used bootstrap grid css added / updated Great Tor climb Updated site map generation
</commit_message>
<xml_diff>
--- a/working-files/multi-pitch-data.xlsx
+++ b/working-files/multi-pitch-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inver\Desktop\forAWS\multi-pitch\working-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4039046A-3E36-44BA-9622-CADE10C2C125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E808B6E1-60AE-41D7-AF20-E100B9A6E047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-4890" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIMBS" sheetId="1" r:id="rId1"/>
@@ -3306,15 +3306,15 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;strong&gt;Approach&lt;/strong&gt;:&lt;br /&gt;
-From the National Trust Car Park at Penmaen (postcode: SA3 2HH), head back to the main road, go right up hill, then cross over to the smaller parking area and bus stop. Through the gate, follow the path towards Three Cliffs Bay. &lt;br /&gt;
+From the National Trust Car Park at Penmaen (postcode: SA3 2HH), head back to the main road, turn right up the hill, then cross over to the smaller parking area and bus stop. Through the gate, follow the path towards Three Cliffs Bay. &lt;br /&gt;
 &lt;strong&gt;Option A – Abseil &amp; Scramble Down&lt;/strong&gt;:&lt;br /&gt;
-Take the first right at the fork in the path, then at the next fork take the left. Follow the path west along the coast and follow it out towards Great Tor. Before scrambling up onto the Tor proper (rocky peak), there is a large block, that at the time of writing, was suitable for a gearless &amp; retrievable abseil. This may be the most appropriate option if the grass is wet and the tide is in. 50m of abseil reaches the rocky ledges. From there, it’s possible to scramble across to the base of the climb.&lt;br /&gt;
+Take the first right at the fork in the path, then at the next fork take the left. Follow the path west along the coast until it heads out towards Great Tor. Before scrambling up onto the Tor proper (tor = rocky peak), there is a large block, that at the time of writing, was suitable for a gearless &amp; retrievable abseil. This may be the most appropriate option if the grass is wet and the tide is in. 50m of abseil reaches the rocky ledges. From there, it’s possible to scramble across to the base of the climb.&lt;br /&gt;
 &lt;strong&gt;Option B –  Low Tide Beach Approach&lt;/strong&gt;:&lt;br /&gt;
-Take the left at the first fork in the road and head down all the way down to Three Cliffs Bay.  Hug the right side of the beach all the way to the base of Great Tor and scramble up to the non-tidal start of the route.&lt;br /&gt;
+Take the left at the first fork in the path and head down, all the way down to Three Cliffs Bay beach.  Keep to the right side of the beach, following it all the way to the base of Great Tor and scramble up to the non-tidal start of the route. &lt;em&gt;The tide has to be at it's lowest for this option.&lt;/em&gt;&lt;br /&gt;
 &lt;strong&gt;Option C –  Scramble Down&lt;/strong&gt;:&lt;br /&gt;
-Follow the instructions of option A, but keep on over the first outcrop until the gully between the two peaks. From here it’s possible to scramble down carefully to the base of the climb. Not recommended un-roped in wet conditions. &lt;br /&gt;
+Follow the instructions of option A, but carry on over the first outcrop until the gully between the two peaks. From here it’s possible to scramble down carefully to the base of the climb. Not recommended un-roped in wet conditions. &lt;br /&gt;
 &lt;br /&gt;&lt;strong&gt;Descent&lt;/strong&gt;:&lt;br /&gt;
-Scramble off the Tor to the North, following the work path down into the gully then back up and out on the path. Take care on the polished limestone. </t>
+Scramble off the Tor to the North, following the worn path down into the gully then back up and out, onto the foot path. Take care on the polished limestone. </t>
   </si>
 </sst>
 </file>

</xml_diff>